<commit_message>
RPA datasets push 2023-09-12
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="237">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -530,12 +530,18 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
     <t>유투바이오</t>
   </si>
   <si>
     <t>퀄리타스반도체</t>
   </si>
   <si>
+    <t>컨텍</t>
+  </si>
+  <si>
     <t>신성에스티</t>
   </si>
   <si>
@@ -584,7 +590,7 @@
     <t>유안타스팩11호</t>
   </si>
   <si>
-    <t>대신밸런스스팩15호</t>
+    <t>2023.10.19~10.25</t>
   </si>
   <si>
     <t>2023.10.18~10.19</t>
@@ -632,10 +638,7 @@
     <t>2023.08.16~08.17</t>
   </si>
   <si>
-    <t>2023.08.14~08.16</t>
-  </si>
-  <si>
-    <t>2023.08.08~08.09</t>
+    <t>9,100~11,000</t>
   </si>
   <si>
     <t>3,300~3,900</t>
@@ -644,6 +647,9 @@
     <t>13,000~15,000</t>
   </si>
   <si>
+    <t>20,300~22,500</t>
+  </si>
+  <si>
     <t>22,000~25,000</t>
   </si>
   <si>
@@ -674,13 +680,10 @@
     <t>10,500~12,000</t>
   </si>
   <si>
-    <t>9,200~10,600</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
-    <t>12000</t>
+    <t>IBK투자증권</t>
   </si>
   <si>
     <t>신한투자증권</t>
@@ -689,6 +692,9 @@
     <t>한국투자증권</t>
   </si>
   <si>
+    <t>대신증권</t>
+  </si>
+  <si>
     <t>미래에셋증권</t>
   </si>
   <si>
@@ -717,9 +723,6 @@
   </si>
   <si>
     <t>한화투자증권</t>
-  </si>
-  <si>
-    <t>대신증권</t>
   </si>
   <si>
     <t>유안타증권</t>
@@ -3049,7 +3052,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
         <v>207</v>
@@ -3058,7 +3061,7 @@
         <v>130</v>
       </c>
       <c r="E2">
-        <v>3724</v>
+        <v>10920</v>
       </c>
       <c r="F2" t="s">
         <v>222</v>
@@ -3069,7 +3072,7 @@
         <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
         <v>208</v>
@@ -3078,7 +3081,7 @@
         <v>130</v>
       </c>
       <c r="E3">
-        <v>23400</v>
+        <v>3724</v>
       </c>
       <c r="F3" t="s">
         <v>223</v>
@@ -3089,7 +3092,7 @@
         <v>173</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>209</v>
@@ -3098,7 +3101,7 @@
         <v>130</v>
       </c>
       <c r="E4">
-        <v>44000</v>
+        <v>23400</v>
       </c>
       <c r="F4" t="s">
         <v>224</v>
@@ -3118,10 +3121,10 @@
         <v>130</v>
       </c>
       <c r="E5">
-        <v>36405</v>
+        <v>41818</v>
       </c>
       <c r="F5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3138,10 +3141,10 @@
         <v>130</v>
       </c>
       <c r="E6">
-        <v>8000</v>
+        <v>44000</v>
       </c>
       <c r="F6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3158,7 +3161,7 @@
         <v>130</v>
       </c>
       <c r="E7">
-        <v>6314</v>
+        <v>36405</v>
       </c>
       <c r="F7" t="s">
         <v>226</v>
@@ -3172,16 +3175,16 @@
         <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
         <v>130</v>
       </c>
       <c r="E8">
-        <v>36000</v>
+        <v>8000</v>
       </c>
       <c r="F8" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3192,16 +3195,16 @@
         <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D9" t="s">
         <v>130</v>
       </c>
       <c r="E9">
-        <v>25760</v>
+        <v>6314</v>
       </c>
       <c r="F9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3209,19 +3212,19 @@
         <v>179</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
         <v>130</v>
       </c>
       <c r="E10">
-        <v>340200</v>
+        <v>36000</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3229,7 +3232,7 @@
         <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s">
         <v>215</v>
@@ -3238,7 +3241,7 @@
         <v>130</v>
       </c>
       <c r="E11">
-        <v>13350</v>
+        <v>25760</v>
       </c>
       <c r="F11" t="s">
         <v>229</v>
@@ -3258,10 +3261,10 @@
         <v>130</v>
       </c>
       <c r="E12">
-        <v>30000</v>
+        <v>340200</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3278,10 +3281,10 @@
         <v>130</v>
       </c>
       <c r="E13">
-        <v>22000</v>
+        <v>13350</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3289,7 +3292,7 @@
         <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C14" t="s">
         <v>218</v>
@@ -3298,10 +3301,10 @@
         <v>130</v>
       </c>
       <c r="E14">
-        <v>16590</v>
+        <v>30000</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3309,16 +3312,16 @@
         <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E15">
-        <v>9000</v>
+        <v>22000</v>
       </c>
       <c r="F15" t="s">
         <v>232</v>
@@ -3332,13 +3335,13 @@
         <v>202</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="E16">
-        <v>9500</v>
+        <v>16590</v>
       </c>
       <c r="F16" t="s">
         <v>233</v>
@@ -3352,13 +3355,13 @@
         <v>203</v>
       </c>
       <c r="C17" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E17">
-        <v>13000</v>
+        <v>9000</v>
       </c>
       <c r="F17" t="s">
         <v>234</v>
@@ -3372,16 +3375,16 @@
         <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E18">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="F18" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3389,19 +3392,19 @@
         <v>188</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C19" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E19">
-        <v>10000</v>
+        <v>13000</v>
       </c>
       <c r="F19" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3409,39 +3412,39 @@
         <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E20">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
         <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D21" t="s">
         <v>221</v>
       </c>
       <c r="E21">
-        <v>10671</v>
+        <v>10000</v>
       </c>
       <c r="F21" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-09-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="243">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -536,12 +536,21 @@
     <t>유투바이오</t>
   </si>
   <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>서울보증보험</t>
+  </si>
+  <si>
     <t>퀄리타스반도체</t>
   </si>
   <si>
     <t>컨텍</t>
   </si>
   <si>
+    <t>워트</t>
+  </si>
+  <si>
     <t>신성에스티</t>
   </si>
   <si>
@@ -581,24 +590,24 @@
     <t>한화플러스스팩4호</t>
   </si>
   <si>
-    <t>대신밸런스스팩16호</t>
-  </si>
-  <si>
-    <t>한국스팩12호</t>
-  </si>
-  <si>
-    <t>유안타스팩11호</t>
-  </si>
-  <si>
     <t>2023.10.19~10.25</t>
   </si>
   <si>
     <t>2023.10.18~10.19</t>
   </si>
   <si>
+    <t>2023.10.18~10.24</t>
+  </si>
+  <si>
+    <t>2023.10.13~10.19</t>
+  </si>
+  <si>
     <t>2023.10.06~10.13</t>
   </si>
   <si>
+    <t>2023.10.05~10.12</t>
+  </si>
+  <si>
     <t>2023.09.22~10.04</t>
   </si>
   <si>
@@ -632,24 +641,27 @@
     <t>2023.08.24~08.25</t>
   </si>
   <si>
-    <t>2023.08.17~08.18</t>
-  </si>
-  <si>
-    <t>2023.08.16~08.17</t>
-  </si>
-  <si>
     <t>9,100~11,000</t>
   </si>
   <si>
     <t>3,300~3,900</t>
   </si>
   <si>
+    <t>29,800~33,500</t>
+  </si>
+  <si>
+    <t>39,500~51,800</t>
+  </si>
+  <si>
     <t>13,000~15,000</t>
   </si>
   <si>
     <t>20,300~22,500</t>
   </si>
   <si>
+    <t>5,000~5,600</t>
+  </si>
+  <si>
     <t>22,000~25,000</t>
   </si>
   <si>
@@ -680,6 +692,9 @@
     <t>10,500~12,000</t>
   </si>
   <si>
+    <t>24000</t>
+  </si>
+  <si>
     <t>2000</t>
   </si>
   <si>
@@ -689,12 +704,18 @@
     <t>신한투자증권</t>
   </si>
   <si>
+    <t>미래에셋증권,삼성증권</t>
+  </si>
+  <si>
     <t>한국투자증권</t>
   </si>
   <si>
     <t>대신증권</t>
   </si>
   <si>
+    <t>키움증권</t>
+  </si>
+  <si>
     <t>미래에셋증권</t>
   </si>
   <si>
@@ -723,9 +744,6 @@
   </si>
   <si>
     <t>한화투자증권</t>
-  </si>
-  <si>
-    <t>유안타증권</t>
   </si>
 </sst>
 </file>
@@ -3055,7 +3073,7 @@
         <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
         <v>130</v>
@@ -3064,7 +3082,7 @@
         <v>10920</v>
       </c>
       <c r="F2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3075,7 +3093,7 @@
         <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D3" t="s">
         <v>130</v>
@@ -3084,7 +3102,7 @@
         <v>3724</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3095,16 +3113,16 @@
         <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
         <v>130</v>
       </c>
       <c r="E4">
-        <v>23400</v>
+        <v>47680</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3112,19 +3130,19 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D5" t="s">
         <v>130</v>
       </c>
       <c r="E5">
-        <v>41818</v>
+        <v>275795</v>
       </c>
       <c r="F5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3132,19 +3150,19 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
         <v>130</v>
       </c>
       <c r="E6">
-        <v>44000</v>
+        <v>23400</v>
       </c>
       <c r="F6" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3155,16 +3173,16 @@
         <v>195</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
         <v>130</v>
       </c>
       <c r="E7">
-        <v>36405</v>
+        <v>41818</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3175,16 +3193,16 @@
         <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D8" t="s">
         <v>130</v>
       </c>
       <c r="E8">
-        <v>8000</v>
+        <v>20000</v>
       </c>
       <c r="F8" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3195,16 +3213,16 @@
         <v>197</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
         <v>130</v>
       </c>
       <c r="E9">
-        <v>6314</v>
+        <v>44000</v>
       </c>
       <c r="F9" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3215,16 +3233,16 @@
         <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D10" t="s">
         <v>130</v>
       </c>
       <c r="E10">
-        <v>36000</v>
+        <v>36405</v>
       </c>
       <c r="F10" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3235,16 +3253,16 @@
         <v>199</v>
       </c>
       <c r="C11" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
         <v>130</v>
       </c>
       <c r="E11">
-        <v>25760</v>
+        <v>8000</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3252,19 +3270,19 @@
         <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
         <v>130</v>
       </c>
       <c r="E12">
-        <v>340200</v>
+        <v>6314</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3272,7 +3290,7 @@
         <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
         <v>217</v>
@@ -3281,10 +3299,10 @@
         <v>130</v>
       </c>
       <c r="E13">
-        <v>13350</v>
+        <v>36000</v>
       </c>
       <c r="F13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3292,19 +3310,19 @@
         <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D14" t="s">
         <v>130</v>
       </c>
       <c r="E14">
-        <v>30000</v>
+        <v>25760</v>
       </c>
       <c r="F14" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3315,16 +3333,16 @@
         <v>202</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D15" t="s">
         <v>130</v>
       </c>
       <c r="E15">
-        <v>22000</v>
+        <v>340200</v>
       </c>
       <c r="F15" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3332,19 +3350,19 @@
         <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D16" t="s">
         <v>130</v>
       </c>
       <c r="E16">
-        <v>16590</v>
+        <v>13350</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3352,19 +3370,19 @@
         <v>186</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D17" t="s">
-        <v>221</v>
+        <v>130</v>
       </c>
       <c r="E17">
-        <v>9000</v>
+        <v>30000</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3372,19 +3390,19 @@
         <v>187</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E18">
-        <v>9500</v>
+        <v>22000</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3395,16 +3413,16 @@
         <v>205</v>
       </c>
       <c r="C19" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>130</v>
       </c>
       <c r="E19">
-        <v>13000</v>
+        <v>16590</v>
       </c>
       <c r="F19" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3415,16 +3433,16 @@
         <v>206</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E20">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="F20" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3432,19 +3450,19 @@
         <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E21">
-        <v>10000</v>
+        <v>9500</v>
       </c>
       <c r="F21" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-11
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -131,9 +131,6 @@
     <t>2023-08-02</t>
   </si>
   <si>
-    <t>2023-07-26</t>
-  </si>
-  <si>
     <t>2023-09-15</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>2023-08-03</t>
   </si>
   <si>
-    <t>2023-07-27</t>
-  </si>
-  <si>
     <t>2023-10-05</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t>2023-08-21</t>
   </si>
   <si>
-    <t>2023-08-11</t>
-  </si>
-  <si>
     <t>한국, 미래</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
     <t>하나</t>
   </si>
   <si>
-    <t>SK</t>
-  </si>
-  <si>
     <t>두산로보틱스</t>
   </si>
   <si>
@@ -284,9 +272,6 @@
     <t>넥스틸</t>
   </si>
   <si>
-    <t>SK증권제10호스팩</t>
-  </si>
-  <si>
     <t>272.03:1</t>
   </si>
   <si>
@@ -335,9 +320,6 @@
     <t>235.56:1</t>
   </si>
   <si>
-    <t>1205.00:1</t>
-  </si>
-  <si>
     <t>51.60%</t>
   </si>
   <si>
@@ -384,9 +366,6 @@
   </si>
   <si>
     <t>0.60%</t>
-  </si>
-  <si>
-    <t>0.66%</t>
   </si>
   <si>
     <t>협동로봇</t>
@@ -999,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1087,16 +1066,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F2">
         <v>16200000</v>
@@ -1123,10 +1102,10 @@
         <v>26000</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="P2">
         <v>36980</v>
@@ -1156,7 +1135,7 @@
         <v>-9333</v>
       </c>
       <c r="Y2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1164,16 +1143,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F3">
         <v>18000000</v>
@@ -1200,10 +1179,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1233,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1244,13 +1223,13 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F4">
         <v>1500000</v>
@@ -1277,10 +1256,10 @@
         <v>12500</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="O4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P4">
         <v>18408761227</v>
@@ -1310,7 +1289,7 @@
         <v>592903151</v>
       </c>
       <c r="Y4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1318,16 +1297,16 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F5">
         <v>2240000</v>
@@ -1354,10 +1333,10 @@
         <v>15000</v>
       </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="P5">
         <v>22818451349</v>
@@ -1387,7 +1366,7 @@
         <v>1929682988</v>
       </c>
       <c r="Y5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1395,16 +1374,16 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F6">
         <v>1580000</v>
@@ -1431,10 +1410,10 @@
         <v>14000</v>
       </c>
       <c r="N6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="P6">
         <v>7327878427</v>
@@ -1464,7 +1443,7 @@
         <v>-550600734</v>
       </c>
       <c r="Y6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1472,16 +1451,16 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F7">
         <v>1500000</v>
@@ -1508,10 +1487,10 @@
         <v>23000</v>
       </c>
       <c r="N7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="O7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="P7">
         <v>28857</v>
@@ -1541,7 +1520,7 @@
         <v>5128</v>
       </c>
       <c r="Y7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1549,16 +1528,16 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>1100000</v>
@@ -1585,10 +1564,10 @@
         <v>24000</v>
       </c>
       <c r="N8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="P8">
         <v>32608351</v>
@@ -1618,7 +1597,7 @@
         <v>180579</v>
       </c>
       <c r="Y8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1626,16 +1605,16 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F9">
         <v>4500000</v>
@@ -1662,10 +1641,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="O9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1695,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1703,16 +1682,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F10">
         <v>4750000</v>
@@ -1739,10 +1718,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="O10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1772,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1780,16 +1759,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F11">
         <v>6500000</v>
@@ -1816,10 +1795,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1849,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1860,13 +1839,13 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F12">
         <v>5000000</v>
@@ -1893,10 +1872,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1926,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1937,13 +1916,13 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F13">
         <v>4000000</v>
@@ -1970,10 +1949,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="O13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -2003,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2014,13 +1993,13 @@
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F14">
         <v>6500000</v>
@@ -2047,10 +2026,10 @@
         <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="O14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2080,7 +2059,7 @@
         <v>-25255133</v>
       </c>
       <c r="Y14" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2088,16 +2067,16 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F15">
         <v>1333885</v>
@@ -2124,10 +2103,10 @@
         <v>12000</v>
       </c>
       <c r="N15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="O15" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="P15">
         <v>1188142585</v>
@@ -2157,7 +2136,7 @@
         <v>-5441928110</v>
       </c>
       <c r="Y15" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2168,13 +2147,13 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F16">
         <v>2220000</v>
@@ -2201,10 +2180,10 @@
         <v>8000</v>
       </c>
       <c r="N16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="O16" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P16">
         <v>4679062361</v>
@@ -2234,7 +2213,7 @@
         <v>-7737792622</v>
       </c>
       <c r="Y16" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2242,16 +2221,16 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F17">
         <v>7000000</v>
@@ -2278,10 +2257,10 @@
         <v>11500</v>
       </c>
       <c r="N17" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="P17">
         <v>214793831184</v>
@@ -2311,84 +2290,7 @@
         <v>144193113559</v>
       </c>
       <c r="Y17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18">
-        <v>3000000</v>
-      </c>
-      <c r="G18">
-        <v>3000000</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>2000</v>
-      </c>
-      <c r="J18">
-        <v>2000</v>
-      </c>
-      <c r="K18">
-        <v>3310000</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>2000</v>
-      </c>
-      <c r="N18" t="s">
-        <v>106</v>
-      </c>
-      <c r="O18" t="s">
-        <v>123</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2406,422 +2308,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E2">
         <v>13500</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E3">
         <v>26800</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E4">
         <v>524031</v>
       </c>
       <c r="F4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E5">
         <v>5107</v>
       </c>
       <c r="F5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E6">
         <v>14950</v>
       </c>
       <c r="F6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E7">
         <v>8000</v>
       </c>
       <c r="F7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E8">
         <v>18040</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E9">
         <v>50353</v>
       </c>
       <c r="F9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E10">
         <v>8400</v>
       </c>
       <c r="F10" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E11">
         <v>41818</v>
       </c>
       <c r="F11" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E12">
         <v>47680</v>
       </c>
       <c r="F12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E13">
         <v>18200</v>
       </c>
       <c r="F13" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E14">
         <v>10920</v>
       </c>
       <c r="F14" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E15">
         <v>25000</v>
       </c>
       <c r="F15" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E16">
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E17">
         <v>3724</v>
       </c>
       <c r="F17" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E18">
         <v>18000</v>
       </c>
       <c r="F18" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E19">
         <v>275795</v>
       </c>
       <c r="F19" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E20">
         <v>13433</v>
       </c>
       <c r="F20" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E21">
         <v>23400</v>
       </c>
       <c r="F21" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="203">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -576,6 +576,9 @@
   </si>
   <si>
     <t>3,300~3,900</t>
+  </si>
+  <si>
+    <t>5,000~7,000</t>
   </si>
   <si>
     <t>39,500~51,800</t>
@@ -2343,7 +2346,7 @@
         <v>13500</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2363,7 +2366,7 @@
         <v>26800</v>
       </c>
       <c r="F3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2383,7 +2386,7 @@
         <v>524031</v>
       </c>
       <c r="F4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2403,7 +2406,7 @@
         <v>5107</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2423,7 +2426,7 @@
         <v>14950</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2443,7 +2446,7 @@
         <v>8000</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2463,7 +2466,7 @@
         <v>18040</v>
       </c>
       <c r="F8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2483,7 +2486,7 @@
         <v>50353</v>
       </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2503,7 +2506,7 @@
         <v>8400</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2523,7 +2526,7 @@
         <v>41818</v>
       </c>
       <c r="F11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2543,7 +2546,7 @@
         <v>47680</v>
       </c>
       <c r="F12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2563,7 +2566,7 @@
         <v>18200</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2583,7 +2586,7 @@
         <v>10920</v>
       </c>
       <c r="F14" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2603,7 +2606,7 @@
         <v>25000</v>
       </c>
       <c r="F15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2623,7 +2626,7 @@
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2643,7 +2646,7 @@
         <v>3724</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2654,7 +2657,7 @@
         <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
@@ -2663,7 +2666,7 @@
         <v>18000</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2674,7 +2677,7 @@
         <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
         <v>108</v>
@@ -2683,7 +2686,7 @@
         <v>275795</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2694,7 +2697,7 @@
         <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D20" t="s">
         <v>108</v>
@@ -2703,7 +2706,7 @@
         <v>13433</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2714,7 +2717,7 @@
         <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
         <v>108</v>
@@ -2723,7 +2726,7 @@
         <v>23400</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-17
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -431,9 +431,21 @@
     <t>와이바이오로직스</t>
   </si>
   <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연(유가)</t>
+  </si>
+  <si>
     <t>스톰테크</t>
   </si>
   <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
     <t>에코프로머티리얼즈</t>
   </si>
   <si>
@@ -470,27 +482,21 @@
     <t>KB스팩27호</t>
   </si>
   <si>
-    <t>에코아이</t>
-  </si>
-  <si>
     <t>유투바이오</t>
   </si>
   <si>
     <t>쏘닉스</t>
   </si>
   <si>
-    <t>서울보증보험</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
     <t>2023.11.10~11.16</t>
   </si>
   <si>
+    <t>2023.11.02~11.08</t>
+  </si>
+  <si>
+    <t>2023.11.01~11.07</t>
+  </si>
+  <si>
     <t>2023.10.31~11.06</t>
   </si>
   <si>
@@ -524,21 +530,24 @@
     <t>2023.10.17~10.23</t>
   </si>
   <si>
-    <t>2023.10.13~10.19</t>
-  </si>
-  <si>
-    <t>2023.10.11~10.17</t>
-  </si>
-  <si>
-    <t>2023.10.06~10.13</t>
-  </si>
-  <si>
     <t>9,000~11,000</t>
   </si>
   <si>
+    <t>5,200~6,000</t>
+  </si>
+  <si>
+    <t>28,500~34,700</t>
+  </si>
+  <si>
+    <t>33,000~37,000</t>
+  </si>
+  <si>
     <t>8,000~9,500</t>
   </si>
   <si>
+    <t>15,000~19,000</t>
+  </si>
+  <si>
     <t>36,200~44,000</t>
   </si>
   <si>
@@ -572,36 +581,33 @@
     <t>9,100~11,000</t>
   </si>
   <si>
-    <t>28,500~34,700</t>
-  </si>
-  <si>
     <t>3,300~3,900</t>
   </si>
   <si>
     <t>5,000~7,000</t>
   </si>
   <si>
-    <t>39,500~51,800</t>
-  </si>
-  <si>
-    <t>12,800~14,500</t>
-  </si>
-  <si>
-    <t>13,000~15,000</t>
-  </si>
-  <si>
     <t>유안타증권</t>
   </si>
   <si>
+    <t>대신증권</t>
+  </si>
+  <si>
+    <t>KB증권</t>
+  </si>
+  <si>
+    <t>NH투자증권</t>
+  </si>
+  <si>
     <t>하이투자증권</t>
   </si>
   <si>
+    <t>하나증권,키움증권</t>
+  </si>
+  <si>
     <t>미래에셋증권,NH투자증권,하이투자증권</t>
   </si>
   <si>
-    <t>NH투자증권</t>
-  </si>
-  <si>
     <t>하나증권</t>
   </si>
   <si>
@@ -609,12 +615,6 @@
   </si>
   <si>
     <t>삼성증권</t>
-  </si>
-  <si>
-    <t>KB증권</t>
-  </si>
-  <si>
-    <t>대신증권</t>
   </si>
   <si>
     <t>미래에셋증권,삼성증권</t>
@@ -2337,7 +2337,7 @@
         <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
         <v>108</v>
@@ -2346,7 +2346,7 @@
         <v>13500</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2357,16 +2357,16 @@
         <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
         <v>108</v>
       </c>
       <c r="E3">
-        <v>26800</v>
+        <v>22100</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2377,16 +2377,16 @@
         <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
         <v>108</v>
       </c>
       <c r="E4">
-        <v>524031</v>
+        <v>59251</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2394,19 +2394,19 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
         <v>108</v>
       </c>
       <c r="E5">
-        <v>5107</v>
+        <v>60654</v>
       </c>
       <c r="F5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2417,16 +2417,16 @@
         <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
         <v>108</v>
       </c>
       <c r="E6">
-        <v>14950</v>
+        <v>26800</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2434,19 +2434,19 @@
         <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
         <v>108</v>
       </c>
       <c r="E7">
-        <v>8000</v>
+        <v>21000</v>
       </c>
       <c r="F7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2454,19 +2454,19 @@
         <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
         <v>108</v>
       </c>
       <c r="E8">
-        <v>18040</v>
+        <v>524031</v>
       </c>
       <c r="F8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2474,19 +2474,19 @@
         <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
         <v>108</v>
       </c>
       <c r="E9">
-        <v>50353</v>
+        <v>5107</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2494,19 +2494,19 @@
         <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
         <v>108</v>
       </c>
       <c r="E10">
-        <v>8400</v>
+        <v>14950</v>
       </c>
       <c r="F10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2514,19 +2514,19 @@
         <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
         <v>108</v>
       </c>
       <c r="E11">
-        <v>41818</v>
+        <v>8000</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2537,16 +2537,16 @@
         <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
         <v>108</v>
       </c>
       <c r="E12">
-        <v>47680</v>
+        <v>18040</v>
       </c>
       <c r="F12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2554,19 +2554,19 @@
         <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
         <v>108</v>
       </c>
       <c r="E13">
-        <v>18200</v>
+        <v>50353</v>
       </c>
       <c r="F13" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2577,16 +2577,16 @@
         <v>165</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D14" t="s">
         <v>108</v>
       </c>
       <c r="E14">
-        <v>10920</v>
+        <v>8400</v>
       </c>
       <c r="F14" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2597,16 +2597,16 @@
         <v>166</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
         <v>108</v>
       </c>
       <c r="E15">
-        <v>25000</v>
+        <v>41818</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2614,7 +2614,7 @@
         <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
         <v>185</v>
@@ -2623,10 +2623,10 @@
         <v>108</v>
       </c>
       <c r="E16">
-        <v>59251</v>
+        <v>47680</v>
       </c>
       <c r="F16" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2634,7 +2634,7 @@
         <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
         <v>186</v>
@@ -2643,10 +2643,10 @@
         <v>108</v>
       </c>
       <c r="E17">
-        <v>3724</v>
+        <v>18200</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2654,7 +2654,7 @@
         <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18" t="s">
         <v>187</v>
@@ -2663,10 +2663,10 @@
         <v>108</v>
       </c>
       <c r="E18">
-        <v>18000</v>
+        <v>10920</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2674,19 +2674,19 @@
         <v>154</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
         <v>108</v>
       </c>
       <c r="E19">
-        <v>275795</v>
+        <v>25000</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2694,19 +2694,19 @@
         <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
         <v>108</v>
       </c>
       <c r="E20">
-        <v>13433</v>
+        <v>3724</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2714,19 +2714,19 @@
         <v>156</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s">
         <v>108</v>
       </c>
       <c r="E21">
-        <v>23400</v>
+        <v>18000</v>
       </c>
       <c r="F21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-11
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="234">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -642,6 +642,12 @@
   </si>
   <si>
     <t>20,300~22,500</t>
+  </si>
+  <si>
+    <t>17000</t>
+  </si>
+  <si>
+    <t>7000</t>
   </si>
   <si>
     <t>34700</t>
@@ -2741,7 +2747,7 @@
         <v>21000</v>
       </c>
       <c r="F2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2761,7 +2767,7 @@
         <v>64350</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2781,7 +2787,7 @@
         <v>20000</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2801,7 +2807,7 @@
         <v>7000</v>
       </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2821,7 +2827,7 @@
         <v>14250</v>
       </c>
       <c r="F6" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2841,7 +2847,7 @@
         <v>16000</v>
       </c>
       <c r="F7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2861,7 +2867,7 @@
         <v>13500</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2881,7 +2887,7 @@
         <v>14950</v>
       </c>
       <c r="F9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2901,7 +2907,7 @@
         <v>29547</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2915,13 +2921,13 @@
         <v>199</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>18040</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2935,13 +2941,13 @@
         <v>200</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
       <c r="E12">
         <v>22100</v>
       </c>
       <c r="F12" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2955,13 +2961,13 @@
         <v>201</v>
       </c>
       <c r="D13" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E13">
         <v>59251</v>
       </c>
       <c r="F13" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2975,13 +2981,13 @@
         <v>202</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E14">
         <v>60654</v>
       </c>
       <c r="F14" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2995,13 +3001,13 @@
         <v>203</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E15">
         <v>26800</v>
       </c>
       <c r="F15" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3015,13 +3021,13 @@
         <v>204</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E16">
         <v>524031</v>
       </c>
       <c r="F16" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3035,13 +3041,13 @@
         <v>205</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E17">
         <v>6384</v>
       </c>
       <c r="F17" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3055,13 +3061,13 @@
         <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3075,13 +3081,13 @@
         <v>206</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E19">
         <v>50353</v>
       </c>
       <c r="F19" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3095,13 +3101,13 @@
         <v>207</v>
       </c>
       <c r="D20" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E20">
         <v>8400</v>
       </c>
       <c r="F20" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3115,13 +3121,13 @@
         <v>208</v>
       </c>
       <c r="D21" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E21">
         <v>41818</v>
       </c>
       <c r="F21" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="240">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -95,6 +95,12 @@
     <t>2023-10-20</t>
   </si>
   <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-25</t>
+  </si>
+  <si>
     <t>2023-10-19</t>
   </si>
   <si>
@@ -140,10 +146,7 @@
     <t>2023-10-26</t>
   </si>
   <si>
-    <t>2023-10-25</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
+    <t>2023-10-27</t>
   </si>
   <si>
     <t>2023-10-13</t>
@@ -167,6 +170,9 @@
     <t>2023-11-09</t>
   </si>
   <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
     <t>2023-11-10</t>
   </si>
   <si>
@@ -179,9 +185,6 @@
     <t>2023-11-02</t>
   </si>
   <si>
-    <t>2023-10-27</t>
-  </si>
-  <si>
     <t>2023-10-10</t>
   </si>
   <si>
@@ -194,6 +197,12 @@
     <t>미래, 삼성</t>
   </si>
   <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -209,9 +218,6 @@
     <t>신한</t>
   </si>
   <si>
-    <t>한국</t>
-  </si>
-  <si>
     <t>키움</t>
   </si>
   <si>
@@ -224,9 +230,6 @@
     <t>한국, 미래</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
     <t>유안타</t>
   </si>
   <si>
@@ -239,6 +242,12 @@
     <t>큐로셀</t>
   </si>
   <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
     <t>메가터치</t>
   </si>
   <si>
@@ -299,6 +308,12 @@
     <t>20.88:1</t>
   </si>
   <si>
+    <t>490.02:1</t>
+  </si>
+  <si>
+    <t>745.80:1</t>
+  </si>
+  <si>
     <t>765.86:1</t>
   </si>
   <si>
@@ -359,6 +374,12 @@
     <t>4.74%</t>
   </si>
   <si>
+    <t>22.38%</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>9.25%</t>
   </si>
   <si>
@@ -371,9 +392,6 @@
     <t>1.39%</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>17.63%</t>
   </si>
   <si>
@@ -413,6 +431,12 @@
     <t>CAR-T 세포치료제</t>
   </si>
   <si>
+    <t>비메모리 반도체 설계및 제조, 전자회로 연구, 설계, 레이아웃 등</t>
+  </si>
+  <si>
+    <t>기업인수합병</t>
+  </si>
+  <si>
     <t>배터리 핀, 반도체 핀</t>
   </si>
   <si>
@@ -425,9 +449,6 @@
     <t>RF필터 파운드리</t>
   </si>
   <si>
-    <t>기업인수합병</t>
-  </si>
-  <si>
     <t>이차전지 정밀금형 외</t>
   </si>
   <si>
@@ -537,9 +558,6 @@
   </si>
   <si>
     <t>한국스팩13호</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
   </si>
   <si>
     <t>에스와이스틸텍</t>
@@ -1074,7 +1092,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1162,16 +1180,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F2">
         <v>1600000</v>
@@ -1198,10 +1216,10 @@
         <v>20000</v>
       </c>
       <c r="N2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1231,546 +1249,546 @@
         <v>-12610702106</v>
       </c>
       <c r="Y2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3">
-        <v>5200000</v>
+        <v>2636330</v>
       </c>
       <c r="G3">
-        <v>5200000</v>
+        <v>2636330</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>3500</v>
+        <v>19100</v>
       </c>
       <c r="J3">
-        <v>4000</v>
+        <v>21400</v>
       </c>
       <c r="K3">
-        <v>20771000</v>
+        <v>10585320</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>4800</v>
+        <v>25000</v>
       </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="P3">
-        <v>39450601</v>
+        <v>45195788</v>
       </c>
       <c r="Q3">
-        <v>49044883</v>
+        <v>69629209</v>
       </c>
       <c r="R3">
-        <v>21826468</v>
+        <v>35634471</v>
       </c>
       <c r="S3">
-        <v>2477559</v>
+        <v>2751277</v>
       </c>
       <c r="T3">
-        <v>8094900</v>
+        <v>11449731</v>
       </c>
       <c r="U3">
-        <v>215154</v>
+        <v>2482194</v>
       </c>
       <c r="V3">
-        <v>3427734</v>
+        <v>2092692</v>
       </c>
       <c r="W3">
-        <v>6575528</v>
+        <v>5149538</v>
       </c>
       <c r="X3">
-        <v>349843</v>
+        <v>2327401</v>
       </c>
       <c r="Y3" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4">
-        <v>2060000</v>
+        <v>4000000</v>
       </c>
       <c r="G4">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="H4">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>20300</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>22500</v>
+        <v>2000</v>
       </c>
       <c r="K4">
-        <v>14384224</v>
+        <v>4320000</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>22500</v>
+        <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="P4">
-        <v>5787300240</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1914633847</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>3156092272</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>-1798278694</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>-1453689952</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>-4067648306</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>-12449932055</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>-7426231074</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>-52132058866</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F5">
-        <v>1200000</v>
+        <v>5200000</v>
       </c>
       <c r="G5">
-        <v>1200000</v>
+        <v>5200000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>9100</v>
+        <v>3500</v>
       </c>
       <c r="J5">
-        <v>11000</v>
+        <v>4000</v>
       </c>
       <c r="K5">
-        <v>7206940</v>
+        <v>20771000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="P5">
-        <v>20924</v>
+        <v>39450601</v>
       </c>
       <c r="Q5">
-        <v>27659</v>
+        <v>49044883</v>
       </c>
       <c r="R5">
-        <v>11818</v>
+        <v>21826468</v>
       </c>
       <c r="S5">
-        <v>2838</v>
+        <v>2477559</v>
       </c>
       <c r="T5">
-        <v>4563</v>
+        <v>8094900</v>
       </c>
       <c r="U5">
-        <v>-1222</v>
+        <v>215154</v>
       </c>
       <c r="V5">
-        <v>2413</v>
+        <v>3427734</v>
       </c>
       <c r="W5">
-        <v>3190</v>
+        <v>6575528</v>
       </c>
       <c r="X5">
-        <v>-862</v>
+        <v>349843</v>
       </c>
       <c r="Y5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6">
-        <v>3600000</v>
+        <v>2060000</v>
       </c>
       <c r="G6">
-        <v>3600000</v>
+        <v>2000000</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I6">
-        <v>5000</v>
+        <v>20300</v>
       </c>
       <c r="J6">
-        <v>7000</v>
+        <v>22500</v>
       </c>
       <c r="K6">
-        <v>17306490</v>
+        <v>14384224</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="P6">
-        <v>21976760922</v>
+        <v>5787300240</v>
       </c>
       <c r="Q6">
-        <v>15839004968</v>
+        <v>1914633847</v>
       </c>
       <c r="R6">
-        <v>6887755932</v>
+        <v>3156092272</v>
       </c>
       <c r="S6">
-        <v>-2217897363</v>
+        <v>-1798278694</v>
       </c>
       <c r="T6">
-        <v>-3403228196</v>
+        <v>-1453689952</v>
       </c>
       <c r="U6">
-        <v>-2758864194</v>
+        <v>-4067648306</v>
       </c>
       <c r="V6">
-        <v>-5110677395</v>
+        <v>-12449932055</v>
       </c>
       <c r="W6">
-        <v>-29510193610</v>
+        <v>-7426231074</v>
       </c>
       <c r="X6">
-        <v>-2514471056</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y6" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F7">
-        <v>12500000</v>
+        <v>1200000</v>
       </c>
       <c r="G7">
-        <v>12500000</v>
+        <v>1200000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>9100</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K7">
-        <v>12905000</v>
+        <v>7206940</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O7" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>20924</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>27659</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>11818</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>2838</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>4563</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>-1222</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>2413</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>3190</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>-862</v>
       </c>
       <c r="Y7" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F8">
-        <v>1049482</v>
+        <v>3600000</v>
       </c>
       <c r="G8">
-        <v>944534</v>
+        <v>3600000</v>
       </c>
       <c r="H8">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>12800</v>
+        <v>5000</v>
       </c>
       <c r="J8">
-        <v>14500</v>
+        <v>7000</v>
       </c>
       <c r="K8">
-        <v>6261485</v>
+        <v>17306490</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O8" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="P8">
-        <v>34557425427</v>
+        <v>21976760922</v>
       </c>
       <c r="Q8">
-        <v>39824841246</v>
+        <v>15839004968</v>
       </c>
       <c r="R8">
-        <v>23231897516</v>
+        <v>6887755932</v>
       </c>
       <c r="S8">
-        <v>3011651602</v>
+        <v>-2217897363</v>
       </c>
       <c r="T8">
-        <v>2384643399</v>
+        <v>-3403228196</v>
       </c>
       <c r="U8">
-        <v>4436005255</v>
+        <v>-2758864194</v>
       </c>
       <c r="V8">
-        <v>2755379556</v>
+        <v>-5110677395</v>
       </c>
       <c r="W8">
-        <v>1176755354</v>
+        <v>-29510193610</v>
       </c>
       <c r="X8">
-        <v>4046949430</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y8" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F9">
-        <v>1128720</v>
+        <v>12500000</v>
       </c>
       <c r="G9">
-        <v>1128720</v>
+        <v>12500000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>3300</v>
+        <v>2000</v>
       </c>
       <c r="J9">
-        <v>3900</v>
+        <v>2000</v>
       </c>
       <c r="K9">
-        <v>11287196</v>
+        <v>12905000</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O9" t="s">
         <v>120</v>
       </c>
       <c r="P9">
-        <v>50552623684</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>69013134090</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>16887814423</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>9027232647</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>15707796256</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>555562560</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>9236341465</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>13159994846</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>1236029732</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1778,34 +1796,34 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F10">
-        <v>1800000</v>
+        <v>1049482</v>
       </c>
       <c r="G10">
-        <v>1800000</v>
+        <v>944534</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I10">
-        <v>13000</v>
+        <v>12800</v>
       </c>
       <c r="J10">
-        <v>15000</v>
+        <v>14500</v>
       </c>
       <c r="K10">
-        <v>10193520</v>
+        <v>6261485</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1814,40 +1832,40 @@
         <v>17000</v>
       </c>
       <c r="N10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="P10">
-        <v>3952070068</v>
+        <v>34557425427</v>
       </c>
       <c r="Q10">
-        <v>10789274729</v>
+        <v>39824841246</v>
       </c>
       <c r="R10">
-        <v>6040367765</v>
+        <v>23231897516</v>
       </c>
       <c r="S10">
-        <v>-4741577598</v>
+        <v>3011651602</v>
       </c>
       <c r="T10">
-        <v>-3671026788</v>
+        <v>2384643399</v>
       </c>
       <c r="U10">
-        <v>-3292521363</v>
+        <v>4436005255</v>
       </c>
       <c r="V10">
-        <v>-3654889267</v>
+        <v>2755379556</v>
       </c>
       <c r="W10">
-        <v>-2281074471</v>
+        <v>1176755354</v>
       </c>
       <c r="X10">
-        <v>-2539505707</v>
+        <v>4046949430</v>
       </c>
       <c r="Y10" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1858,73 +1876,73 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F11">
-        <v>4000000</v>
+        <v>1128720</v>
       </c>
       <c r="G11">
-        <v>4000000</v>
+        <v>1128720</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>5000</v>
+        <v>3300</v>
       </c>
       <c r="J11">
-        <v>5600</v>
+        <v>3900</v>
       </c>
       <c r="K11">
-        <v>16120000</v>
+        <v>11287196</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O11" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="P11">
-        <v>26691070764</v>
+        <v>50552623684</v>
       </c>
       <c r="Q11">
-        <v>22835113396</v>
+        <v>69013134090</v>
       </c>
       <c r="R11">
-        <v>7519073723</v>
+        <v>16887814423</v>
       </c>
       <c r="S11">
-        <v>6041270235</v>
+        <v>9027232647</v>
       </c>
       <c r="T11">
-        <v>6705120210</v>
+        <v>15707796256</v>
       </c>
       <c r="U11">
-        <v>982044017</v>
+        <v>555562560</v>
       </c>
       <c r="V11">
-        <v>5119066139</v>
+        <v>9236341465</v>
       </c>
       <c r="W11">
-        <v>5870093710</v>
+        <v>13159994846</v>
       </c>
       <c r="X11">
-        <v>1198587470</v>
+        <v>1236029732</v>
       </c>
       <c r="Y11" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1932,76 +1950,76 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F12">
-        <v>770000</v>
+        <v>1800000</v>
       </c>
       <c r="G12">
-        <v>770000</v>
+        <v>1800000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>8200</v>
+        <v>13000</v>
       </c>
       <c r="J12">
-        <v>9400</v>
+        <v>15000</v>
       </c>
       <c r="K12">
-        <v>7674103</v>
+        <v>10193520</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O12" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="P12">
-        <v>8242508010</v>
+        <v>3952070068</v>
       </c>
       <c r="Q12">
-        <v>10751900430</v>
+        <v>10789274729</v>
       </c>
       <c r="R12">
-        <v>4416778965</v>
+        <v>6040367765</v>
       </c>
       <c r="S12">
-        <v>426234451</v>
+        <v>-4741577598</v>
       </c>
       <c r="T12">
-        <v>2423749751</v>
+        <v>-3671026788</v>
       </c>
       <c r="U12">
-        <v>677048172</v>
+        <v>-3292521363</v>
       </c>
       <c r="V12">
-        <v>57890953</v>
+        <v>-3654889267</v>
       </c>
       <c r="W12">
-        <v>2826043673</v>
+        <v>-2281074471</v>
       </c>
       <c r="X12">
-        <v>990121873</v>
+        <v>-2539505707</v>
       </c>
       <c r="Y12" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2009,76 +2027,76 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F13">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="G13">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>22000</v>
+        <v>5000</v>
       </c>
       <c r="J13">
-        <v>25000</v>
+        <v>5600</v>
       </c>
       <c r="K13">
-        <v>9039778</v>
+        <v>16120000</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O13" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P13">
-        <v>104225113285</v>
+        <v>26691070764</v>
       </c>
       <c r="Q13">
-        <v>106505634411</v>
+        <v>22835113396</v>
       </c>
       <c r="R13">
-        <v>66424930568</v>
+        <v>7519073723</v>
       </c>
       <c r="S13">
-        <v>6291020806</v>
+        <v>6041270235</v>
       </c>
       <c r="T13">
-        <v>7893242769</v>
+        <v>6705120210</v>
       </c>
       <c r="U13">
-        <v>7661497240</v>
+        <v>982044017</v>
       </c>
       <c r="V13">
-        <v>7319368873</v>
+        <v>5119066139</v>
       </c>
       <c r="W13">
-        <v>9286891982</v>
+        <v>5870093710</v>
       </c>
       <c r="X13">
-        <v>7334816490</v>
+        <v>1198587470</v>
       </c>
       <c r="Y13" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2086,76 +2104,76 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F14">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="G14">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>21000</v>
+        <v>8200</v>
       </c>
       <c r="J14">
-        <v>26000</v>
+        <v>9400</v>
       </c>
       <c r="K14">
-        <v>64819980</v>
+        <v>7674103</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O14" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="P14">
-        <v>36980</v>
+        <v>8242508010</v>
       </c>
       <c r="Q14">
-        <v>44954</v>
+        <v>10751900430</v>
       </c>
       <c r="R14">
-        <v>23652</v>
+        <v>4416778965</v>
       </c>
       <c r="S14">
-        <v>-7085</v>
+        <v>426234451</v>
       </c>
       <c r="T14">
-        <v>-13228</v>
+        <v>2423749751</v>
       </c>
       <c r="U14">
-        <v>-9932</v>
+        <v>677048172</v>
       </c>
       <c r="V14">
-        <v>-7417</v>
+        <v>57890953</v>
       </c>
       <c r="W14">
-        <v>-12548</v>
+        <v>2826043673</v>
       </c>
       <c r="X14">
-        <v>-9333</v>
+        <v>990121873</v>
       </c>
       <c r="Y14" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2166,73 +2184,73 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15">
-        <v>18000000</v>
+        <v>2000000</v>
       </c>
       <c r="G15">
-        <v>18000000</v>
+        <v>2000000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="K15">
-        <v>18905000</v>
+        <v>9039778</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>104225113285</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>106505634411</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>66424930568</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>6291020806</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>7893242769</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>7661497240</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>7319368873</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>9286891982</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>7334816490</v>
       </c>
       <c r="Y15" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2240,461 +2258,615 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="G16">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8900</v>
+        <v>21000</v>
       </c>
       <c r="J16">
-        <v>11000</v>
+        <v>26000</v>
       </c>
       <c r="K16">
-        <v>5447675</v>
+        <v>64819980</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N16" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="O16" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="P16">
-        <v>18408761227</v>
+        <v>36980</v>
       </c>
       <c r="Q16">
-        <v>21902816604</v>
+        <v>44954</v>
       </c>
       <c r="R16">
-        <v>8176918465</v>
+        <v>23652</v>
       </c>
       <c r="S16">
-        <v>3669182465</v>
+        <v>-7085</v>
       </c>
       <c r="T16">
-        <v>1851925471</v>
+        <v>-13228</v>
       </c>
       <c r="U16">
-        <v>590566592</v>
+        <v>-9932</v>
       </c>
       <c r="V16">
-        <v>3633973594</v>
+        <v>-7417</v>
       </c>
       <c r="W16">
-        <v>2205418963</v>
+        <v>-12548</v>
       </c>
       <c r="X16">
-        <v>592903151</v>
+        <v>-9333</v>
       </c>
       <c r="Y16" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F17">
-        <v>2240000</v>
+        <v>18000000</v>
       </c>
       <c r="G17">
-        <v>1640000</v>
+        <v>18000000</v>
       </c>
       <c r="H17">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="J17">
-        <v>13200</v>
+        <v>2000</v>
       </c>
       <c r="K17">
-        <v>10969386</v>
+        <v>18905000</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="N17" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P17">
-        <v>22818451349</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>30491967755</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>18040053709</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>2313787613</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>4014101926</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>1878997667</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>559427078</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>-711183147</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>1929682988</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F18">
-        <v>1580000</v>
+        <v>1500000</v>
       </c>
       <c r="G18">
-        <v>1580000</v>
+        <v>1500000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>10500</v>
+        <v>8900</v>
       </c>
       <c r="J18">
-        <v>12000</v>
+        <v>11000</v>
       </c>
       <c r="K18">
-        <v>7874611</v>
+        <v>5447675</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>14000</v>
+        <v>12500</v>
       </c>
       <c r="N18" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O18" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="P18">
-        <v>7327878427</v>
+        <v>18408761227</v>
       </c>
       <c r="Q18">
-        <v>10756717708</v>
+        <v>21902816604</v>
       </c>
       <c r="R18">
-        <v>4113702647</v>
+        <v>8176918465</v>
       </c>
       <c r="S18">
-        <v>-588932080</v>
+        <v>3669182465</v>
       </c>
       <c r="T18">
-        <v>254042570</v>
+        <v>1851925471</v>
       </c>
       <c r="U18">
-        <v>-738698858</v>
+        <v>590566592</v>
       </c>
       <c r="V18">
-        <v>-569358529</v>
+        <v>3633973594</v>
       </c>
       <c r="W18">
-        <v>-429546963</v>
+        <v>2205418963</v>
       </c>
       <c r="X18">
-        <v>-550600734</v>
+        <v>592903151</v>
       </c>
       <c r="Y18" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F19">
-        <v>1500000</v>
+        <v>2240000</v>
       </c>
       <c r="G19">
-        <v>1500000</v>
+        <v>1640000</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="I19">
-        <v>20000</v>
+        <v>11500</v>
       </c>
       <c r="J19">
-        <v>23000</v>
+        <v>13200</v>
       </c>
       <c r="K19">
-        <v>8110389</v>
+        <v>10969386</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>23000</v>
+        <v>15000</v>
       </c>
       <c r="N19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O19" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="P19">
-        <v>28857</v>
+        <v>22818451349</v>
       </c>
       <c r="Q19">
-        <v>45830</v>
+        <v>30491967755</v>
       </c>
       <c r="R19">
-        <v>25997</v>
+        <v>18040053709</v>
       </c>
       <c r="S19">
-        <v>-14511</v>
+        <v>2313787613</v>
       </c>
       <c r="T19">
-        <v>4169</v>
+        <v>4014101926</v>
       </c>
       <c r="U19">
-        <v>4958</v>
+        <v>1878997667</v>
       </c>
       <c r="V19">
-        <v>-34842</v>
+        <v>559427078</v>
       </c>
       <c r="W19">
-        <v>13350</v>
+        <v>-711183147</v>
       </c>
       <c r="X19">
-        <v>5128</v>
+        <v>1929682988</v>
       </c>
       <c r="Y19" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F20">
-        <v>1100000</v>
+        <v>1580000</v>
       </c>
       <c r="G20">
-        <v>900000</v>
+        <v>1580000</v>
       </c>
       <c r="H20">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J20">
-        <v>24000</v>
+        <v>12000</v>
       </c>
       <c r="K20">
-        <v>4901526</v>
+        <v>7874611</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>24000</v>
+        <v>14000</v>
       </c>
       <c r="N20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="O20" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P20">
-        <v>32608351</v>
+        <v>7327878427</v>
       </c>
       <c r="Q20">
-        <v>43629717</v>
+        <v>10756717708</v>
       </c>
       <c r="R20">
-        <v>14011366</v>
+        <v>4113702647</v>
       </c>
       <c r="S20">
-        <v>4301870</v>
+        <v>-588932080</v>
       </c>
       <c r="T20">
-        <v>7039261</v>
+        <v>254042570</v>
       </c>
       <c r="U20">
-        <v>316611</v>
+        <v>-738698858</v>
       </c>
       <c r="V20">
-        <v>4422483</v>
+        <v>-569358529</v>
       </c>
       <c r="W20">
-        <v>5391712</v>
+        <v>-429546963</v>
       </c>
       <c r="X20">
-        <v>180579</v>
+        <v>-550600734</v>
       </c>
       <c r="Y20" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21">
+        <v>1500000</v>
+      </c>
+      <c r="G21">
+        <v>1500000</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>20000</v>
+      </c>
+      <c r="J21">
+        <v>23000</v>
+      </c>
+      <c r="K21">
+        <v>8110389</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>23000</v>
+      </c>
+      <c r="N21" t="s">
+        <v>115</v>
+      </c>
+      <c r="O21" t="s">
+        <v>135</v>
+      </c>
+      <c r="P21">
+        <v>28857</v>
+      </c>
+      <c r="Q21">
+        <v>45830</v>
+      </c>
+      <c r="R21">
+        <v>25997</v>
+      </c>
+      <c r="S21">
+        <v>-14511</v>
+      </c>
+      <c r="T21">
+        <v>4169</v>
+      </c>
+      <c r="U21">
+        <v>4958</v>
+      </c>
+      <c r="V21">
+        <v>-34842</v>
+      </c>
+      <c r="W21">
+        <v>13350</v>
+      </c>
+      <c r="X21">
+        <v>5128</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22">
+        <v>1100000</v>
+      </c>
+      <c r="G22">
+        <v>900000</v>
+      </c>
+      <c r="H22">
+        <v>200000</v>
+      </c>
+      <c r="I22">
+        <v>20000</v>
+      </c>
+      <c r="J22">
+        <v>24000</v>
+      </c>
+      <c r="K22">
+        <v>4901526</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>24000</v>
+      </c>
+      <c r="N22" t="s">
+        <v>116</v>
+      </c>
+      <c r="O22" t="s">
+        <v>136</v>
+      </c>
+      <c r="P22">
+        <v>32608351</v>
+      </c>
+      <c r="Q22">
+        <v>43629717</v>
+      </c>
+      <c r="R22">
+        <v>14011366</v>
+      </c>
+      <c r="S22">
+        <v>4301870</v>
+      </c>
+      <c r="T22">
+        <v>7039261</v>
+      </c>
+      <c r="U22">
+        <v>316611</v>
+      </c>
+      <c r="V22">
+        <v>4422483</v>
+      </c>
+      <c r="W22">
+        <v>5391712</v>
+      </c>
+      <c r="X22">
+        <v>180579</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23">
         <v>4500000</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>4500000</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>2000</v>
       </c>
-      <c r="J21">
+      <c r="J23">
         <v>2000</v>
       </c>
-      <c r="K21">
+      <c r="K23">
         <v>5220000</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
         <v>2000</v>
       </c>
-      <c r="N21" t="s">
-        <v>112</v>
-      </c>
-      <c r="O21" t="s">
-        <v>118</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>150</v>
+      <c r="N23" t="s">
+        <v>117</v>
+      </c>
+      <c r="O23" t="s">
+        <v>120</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2712,422 +2884,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E2">
         <v>21000</v>
       </c>
       <c r="F2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E3">
         <v>64350</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E4">
         <v>20000</v>
       </c>
       <c r="F4" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E5">
         <v>7000</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E6">
         <v>14250</v>
       </c>
       <c r="F6" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E7">
         <v>16000</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E8">
         <v>13500</v>
       </c>
       <c r="F8" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E9">
         <v>14950</v>
       </c>
       <c r="F9" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E10">
         <v>29547</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E11">
         <v>18040</v>
       </c>
       <c r="F11" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E12">
         <v>22100</v>
       </c>
       <c r="F12" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E13">
         <v>59251</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D14" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E14">
         <v>60654</v>
       </c>
       <c r="F14" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="E15">
         <v>26800</v>
       </c>
       <c r="F15" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E16">
         <v>524031</v>
       </c>
       <c r="F16" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E17">
         <v>6384</v>
       </c>
       <c r="F17" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E19">
         <v>50353</v>
       </c>
       <c r="F19" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E20">
         <v>8400</v>
       </c>
       <c r="F20" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E21">
         <v>41818</v>
       </c>
       <c r="F21" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-15
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="243">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2023-10-26</t>
+  </si>
+  <si>
     <t>2023-10-20</t>
   </si>
   <si>
@@ -140,7 +143,7 @@
     <t>2023-09-07</t>
   </si>
   <si>
-    <t>2023-10-26</t>
+    <t>2023-11-01</t>
   </si>
   <si>
     <t>2023-10-27</t>
@@ -161,6 +164,9 @@
     <t>2023-09-13</t>
   </si>
   <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
     <t>2023-11-09</t>
   </si>
   <si>
@@ -191,6 +197,9 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>미래, 삼성</t>
   </si>
   <si>
@@ -203,9 +212,6 @@
     <t>KB</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>대신</t>
   </si>
   <si>
@@ -233,6 +239,9 @@
     <t>신영</t>
   </si>
   <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
     <t>큐로셀</t>
   </si>
   <si>
@@ -299,6 +308,9 @@
     <t>인스웨이브시스템즈</t>
   </si>
   <si>
+    <t>952.78</t>
+  </si>
+  <si>
     <t>20.88:1</t>
   </si>
   <si>
@@ -365,6 +377,9 @@
     <t>672.42:1</t>
   </si>
   <si>
+    <t>0.19%</t>
+  </si>
+  <si>
     <t>4.74%</t>
   </si>
   <si>
@@ -425,6 +440,9 @@
     <t>7.46%</t>
   </si>
   <si>
+    <t>벤처투자조합 등 조합 결성 및 운영</t>
+  </si>
+  <si>
     <t>CAR-T 세포치료제</t>
   </si>
   <si>
@@ -549,9 +567,6 @@
   </si>
   <si>
     <t>에코프로머티리얼즈(유가)</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
   </si>
   <si>
     <t>한국스팩13호</t>
@@ -1086,7 +1101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1174,76 +1189,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="G2">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>29800</v>
+        <v>3200</v>
       </c>
       <c r="J2">
-        <v>33500</v>
+        <v>3600</v>
       </c>
       <c r="K2">
-        <v>13612736</v>
+        <v>13346380</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>7668281979</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>7100921456</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1207846478</v>
       </c>
       <c r="S2">
-        <v>-15286512079</v>
+        <v>5659403971</v>
       </c>
       <c r="T2">
-        <v>-21424611321</v>
+        <v>6124121466</v>
       </c>
       <c r="U2">
-        <v>-139745251263</v>
+        <v>940668827</v>
       </c>
       <c r="V2">
-        <v>-53575668634</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>-38885125426</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>-12610702106</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1251,76 +1266,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F3">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="G3">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>19100</v>
+        <v>29800</v>
       </c>
       <c r="J3">
-        <v>21400</v>
+        <v>33500</v>
       </c>
       <c r="K3">
-        <v>10585320</v>
+        <v>13612736</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P3">
-        <v>45195788</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>69629209</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>35634471</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>2751277</v>
+        <v>-15286512079</v>
       </c>
       <c r="T3">
-        <v>11449731</v>
+        <v>-21424611321</v>
       </c>
       <c r="U3">
-        <v>2482194</v>
+        <v>-139745251263</v>
       </c>
       <c r="V3">
-        <v>2092692</v>
+        <v>-53575668634</v>
       </c>
       <c r="W3">
-        <v>5149538</v>
+        <v>-38885125426</v>
       </c>
       <c r="X3">
-        <v>2327401</v>
+        <v>-12610702106</v>
       </c>
       <c r="Y3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1328,384 +1343,384 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="G4">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>19100</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>21400</v>
       </c>
       <c r="K4">
-        <v>4320000</v>
+        <v>10585320</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>45195788</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>69629209</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>35634471</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>2751277</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>11449731</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2482194</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>2092692</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>5149538</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>2327401</v>
       </c>
       <c r="Y4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F5">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="G5">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>30610000</v>
+        <v>4320000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P5">
-        <v>67332006578</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>100050838794</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>63366010569</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>1140243099</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>8333440685</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>7415958936</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>668088159</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>5930478364</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>5666583221</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F6">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="G6">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>3500</v>
+        <v>1200</v>
       </c>
       <c r="J6">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="K6">
-        <v>20771000</v>
+        <v>30610000</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="P6">
-        <v>39450601</v>
+        <v>67332006578</v>
       </c>
       <c r="Q6">
-        <v>49044883</v>
+        <v>100050838794</v>
       </c>
       <c r="R6">
-        <v>21826468</v>
+        <v>63366010569</v>
       </c>
       <c r="S6">
-        <v>2477559</v>
+        <v>1140243099</v>
       </c>
       <c r="T6">
-        <v>8094900</v>
+        <v>8333440685</v>
       </c>
       <c r="U6">
-        <v>215154</v>
+        <v>7415958936</v>
       </c>
       <c r="V6">
-        <v>3427734</v>
+        <v>668088159</v>
       </c>
       <c r="W6">
-        <v>6575528</v>
+        <v>5930478364</v>
       </c>
       <c r="X6">
-        <v>349843</v>
+        <v>5666583221</v>
       </c>
       <c r="Y6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F7">
-        <v>2060000</v>
+        <v>5200000</v>
       </c>
       <c r="G7">
-        <v>2000000</v>
+        <v>5200000</v>
       </c>
       <c r="H7">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>20300</v>
+        <v>3500</v>
       </c>
       <c r="J7">
-        <v>22500</v>
+        <v>4000</v>
       </c>
       <c r="K7">
-        <v>14384224</v>
+        <v>20771000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O7" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="P7">
-        <v>5787300240</v>
+        <v>39450601</v>
       </c>
       <c r="Q7">
-        <v>1914633847</v>
+        <v>49044883</v>
       </c>
       <c r="R7">
-        <v>3156092272</v>
+        <v>21826468</v>
       </c>
       <c r="S7">
-        <v>-1798278694</v>
+        <v>2477559</v>
       </c>
       <c r="T7">
-        <v>-1453689952</v>
+        <v>8094900</v>
       </c>
       <c r="U7">
-        <v>-4067648306</v>
+        <v>215154</v>
       </c>
       <c r="V7">
-        <v>-12449932055</v>
+        <v>3427734</v>
       </c>
       <c r="W7">
-        <v>-7426231074</v>
+        <v>6575528</v>
       </c>
       <c r="X7">
-        <v>-52132058866</v>
+        <v>349843</v>
       </c>
       <c r="Y7" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F8">
-        <v>1200000</v>
+        <v>2060000</v>
       </c>
       <c r="G8">
-        <v>1200000</v>
+        <v>2000000</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I8">
-        <v>9100</v>
+        <v>20300</v>
       </c>
       <c r="J8">
-        <v>11000</v>
+        <v>22500</v>
       </c>
       <c r="K8">
-        <v>7206940</v>
+        <v>14384224</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="P8">
-        <v>20924</v>
+        <v>5787300240</v>
       </c>
       <c r="Q8">
-        <v>27659</v>
+        <v>1914633847</v>
       </c>
       <c r="R8">
-        <v>11818</v>
+        <v>3156092272</v>
       </c>
       <c r="S8">
-        <v>2838</v>
+        <v>-1798278694</v>
       </c>
       <c r="T8">
-        <v>4563</v>
+        <v>-1453689952</v>
       </c>
       <c r="U8">
-        <v>-1222</v>
+        <v>-4067648306</v>
       </c>
       <c r="V8">
-        <v>2413</v>
+        <v>-12449932055</v>
       </c>
       <c r="W8">
-        <v>3190</v>
+        <v>-7426231074</v>
       </c>
       <c r="X8">
-        <v>-862</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y8" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1713,227 +1728,227 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F9">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="G9">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>5000</v>
+        <v>9100</v>
       </c>
       <c r="J9">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="K9">
-        <v>17306490</v>
+        <v>7206940</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O9" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="P9">
-        <v>21976760922</v>
+        <v>20924</v>
       </c>
       <c r="Q9">
-        <v>15839004968</v>
+        <v>27659</v>
       </c>
       <c r="R9">
-        <v>6887755932</v>
+        <v>11818</v>
       </c>
       <c r="S9">
-        <v>-2217897363</v>
+        <v>2838</v>
       </c>
       <c r="T9">
-        <v>-3403228196</v>
+        <v>4563</v>
       </c>
       <c r="U9">
-        <v>-2758864194</v>
+        <v>-1222</v>
       </c>
       <c r="V9">
-        <v>-5110677395</v>
+        <v>2413</v>
       </c>
       <c r="W9">
-        <v>-29510193610</v>
+        <v>3190</v>
       </c>
       <c r="X9">
-        <v>-2514471056</v>
+        <v>-862</v>
       </c>
       <c r="Y9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F10">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="G10">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K10">
-        <v>12905000</v>
+        <v>17306490</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O10" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>21976760922</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>15839004968</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>6887755932</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>-2217897363</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>-3403228196</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>-2758864194</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>-5110677395</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>-29510193610</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y10" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11">
-        <v>1049482</v>
+        <v>12500000</v>
       </c>
       <c r="G11">
-        <v>944534</v>
+        <v>12500000</v>
       </c>
       <c r="H11">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>12800</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="K11">
-        <v>6261485</v>
+        <v>12905000</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P11">
-        <v>34557425427</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>39824841246</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>23231897516</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>3011651602</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>2384643399</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>4436005255</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>2755379556</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>1176755354</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>4046949430</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="s">
         <v>144</v>
@@ -1944,76 +1959,76 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F12">
-        <v>1128720</v>
+        <v>1049482</v>
       </c>
       <c r="G12">
-        <v>1128720</v>
+        <v>944534</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I12">
-        <v>3300</v>
+        <v>12800</v>
       </c>
       <c r="J12">
-        <v>3900</v>
+        <v>14500</v>
       </c>
       <c r="K12">
-        <v>11287196</v>
+        <v>6261485</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O12" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="P12">
-        <v>50552623684</v>
+        <v>34557425427</v>
       </c>
       <c r="Q12">
-        <v>69013134090</v>
+        <v>39824841246</v>
       </c>
       <c r="R12">
-        <v>16887814423</v>
+        <v>23231897516</v>
       </c>
       <c r="S12">
-        <v>9027232647</v>
+        <v>3011651602</v>
       </c>
       <c r="T12">
-        <v>15707796256</v>
+        <v>2384643399</v>
       </c>
       <c r="U12">
-        <v>555562560</v>
+        <v>4436005255</v>
       </c>
       <c r="V12">
-        <v>9236341465</v>
+        <v>2755379556</v>
       </c>
       <c r="W12">
-        <v>13159994846</v>
+        <v>1176755354</v>
       </c>
       <c r="X12">
-        <v>1236029732</v>
+        <v>4046949430</v>
       </c>
       <c r="Y12" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2021,76 +2036,76 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F13">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="G13">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>13000</v>
+        <v>3300</v>
       </c>
       <c r="J13">
-        <v>15000</v>
+        <v>3900</v>
       </c>
       <c r="K13">
-        <v>10193520</v>
+        <v>11287196</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O13" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="P13">
-        <v>3952070068</v>
+        <v>50552623684</v>
       </c>
       <c r="Q13">
-        <v>10789274729</v>
+        <v>69013134090</v>
       </c>
       <c r="R13">
-        <v>6040367765</v>
+        <v>16887814423</v>
       </c>
       <c r="S13">
-        <v>-4741577598</v>
+        <v>9027232647</v>
       </c>
       <c r="T13">
-        <v>-3671026788</v>
+        <v>15707796256</v>
       </c>
       <c r="U13">
-        <v>-3292521363</v>
+        <v>555562560</v>
       </c>
       <c r="V13">
-        <v>-3654889267</v>
+        <v>9236341465</v>
       </c>
       <c r="W13">
-        <v>-2281074471</v>
+        <v>13159994846</v>
       </c>
       <c r="X13">
-        <v>-2539505707</v>
+        <v>1236029732</v>
       </c>
       <c r="Y13" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2098,76 +2113,76 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F14">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="G14">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J14">
-        <v>5600</v>
+        <v>15000</v>
       </c>
       <c r="K14">
-        <v>16120000</v>
+        <v>10193520</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="O14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="P14">
-        <v>26691070764</v>
+        <v>3952070068</v>
       </c>
       <c r="Q14">
-        <v>22835113396</v>
+        <v>10789274729</v>
       </c>
       <c r="R14">
-        <v>7519073723</v>
+        <v>6040367765</v>
       </c>
       <c r="S14">
-        <v>6041270235</v>
+        <v>-4741577598</v>
       </c>
       <c r="T14">
-        <v>6705120210</v>
+        <v>-3671026788</v>
       </c>
       <c r="U14">
-        <v>982044017</v>
+        <v>-3292521363</v>
       </c>
       <c r="V14">
-        <v>5119066139</v>
+        <v>-3654889267</v>
       </c>
       <c r="W14">
-        <v>5870093710</v>
+        <v>-2281074471</v>
       </c>
       <c r="X14">
-        <v>1198587470</v>
+        <v>-2539505707</v>
       </c>
       <c r="Y14" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2175,76 +2190,76 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F15">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="G15">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>8200</v>
+        <v>5000</v>
       </c>
       <c r="J15">
-        <v>9400</v>
+        <v>5600</v>
       </c>
       <c r="K15">
-        <v>7674103</v>
+        <v>16120000</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="O15" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="P15">
-        <v>8242508010</v>
+        <v>26691070764</v>
       </c>
       <c r="Q15">
-        <v>10751900430</v>
+        <v>22835113396</v>
       </c>
       <c r="R15">
-        <v>4416778965</v>
+        <v>7519073723</v>
       </c>
       <c r="S15">
-        <v>426234451</v>
+        <v>6041270235</v>
       </c>
       <c r="T15">
-        <v>2423749751</v>
+        <v>6705120210</v>
       </c>
       <c r="U15">
-        <v>677048172</v>
+        <v>982044017</v>
       </c>
       <c r="V15">
-        <v>57890953</v>
+        <v>5119066139</v>
       </c>
       <c r="W15">
-        <v>2826043673</v>
+        <v>5870093710</v>
       </c>
       <c r="X15">
-        <v>990121873</v>
+        <v>1198587470</v>
       </c>
       <c r="Y15" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2252,76 +2267,76 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F16">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="G16">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>22000</v>
+        <v>8200</v>
       </c>
       <c r="J16">
-        <v>25000</v>
+        <v>9400</v>
       </c>
       <c r="K16">
-        <v>9039778</v>
+        <v>7674103</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N16" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O16" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="P16">
-        <v>104225113285</v>
+        <v>8242508010</v>
       </c>
       <c r="Q16">
-        <v>106505634411</v>
+        <v>10751900430</v>
       </c>
       <c r="R16">
-        <v>66424930568</v>
+        <v>4416778965</v>
       </c>
       <c r="S16">
-        <v>6291020806</v>
+        <v>426234451</v>
       </c>
       <c r="T16">
-        <v>7893242769</v>
+        <v>2423749751</v>
       </c>
       <c r="U16">
-        <v>7661497240</v>
+        <v>677048172</v>
       </c>
       <c r="V16">
-        <v>7319368873</v>
+        <v>57890953</v>
       </c>
       <c r="W16">
-        <v>9286891982</v>
+        <v>2826043673</v>
       </c>
       <c r="X16">
-        <v>7334816490</v>
+        <v>990121873</v>
       </c>
       <c r="Y16" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2332,31 +2347,31 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F17">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="G17">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="J17">
-        <v>26000</v>
+        <v>25000</v>
       </c>
       <c r="K17">
-        <v>64819980</v>
+        <v>9039778</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2365,40 +2380,40 @@
         <v>26000</v>
       </c>
       <c r="N17" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="P17">
-        <v>36980</v>
+        <v>104225113285</v>
       </c>
       <c r="Q17">
-        <v>44954</v>
+        <v>106505634411</v>
       </c>
       <c r="R17">
-        <v>23652</v>
+        <v>66424930568</v>
       </c>
       <c r="S17">
-        <v>-7085</v>
+        <v>6291020806</v>
       </c>
       <c r="T17">
-        <v>-13228</v>
+        <v>7893242769</v>
       </c>
       <c r="U17">
-        <v>-9932</v>
+        <v>7661497240</v>
       </c>
       <c r="V17">
-        <v>-7417</v>
+        <v>7319368873</v>
       </c>
       <c r="W17">
-        <v>-12548</v>
+        <v>9286891982</v>
       </c>
       <c r="X17">
-        <v>-9333</v>
+        <v>7334816490</v>
       </c>
       <c r="Y17" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2406,76 +2421,76 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="G18">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K18">
-        <v>18905000</v>
+        <v>64819980</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N18" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O18" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>36980</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>44954</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>23652</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>-7085</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>-13228</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>-9932</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>-7417</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>-12548</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>-9333</v>
       </c>
       <c r="Y18" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2483,230 +2498,230 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F19">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="G19">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J19">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K19">
-        <v>5447675</v>
+        <v>18905000</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N19" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="O19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="P19">
-        <v>18408761227</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>21902816604</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>8176918465</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>3669182465</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <v>1851925471</v>
+        <v>0</v>
       </c>
       <c r="U19">
-        <v>590566592</v>
+        <v>0</v>
       </c>
       <c r="V19">
-        <v>3633973594</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <v>2205418963</v>
+        <v>0</v>
       </c>
       <c r="X19">
-        <v>592903151</v>
+        <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F20">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="G20">
-        <v>1640000</v>
+        <v>1500000</v>
       </c>
       <c r="H20">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J20">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K20">
-        <v>10969386</v>
+        <v>5447675</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N20" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="O20" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="P20">
-        <v>22818451349</v>
+        <v>18408761227</v>
       </c>
       <c r="Q20">
-        <v>30491967755</v>
+        <v>21902816604</v>
       </c>
       <c r="R20">
-        <v>18040053709</v>
+        <v>8176918465</v>
       </c>
       <c r="S20">
-        <v>2313787613</v>
+        <v>3669182465</v>
       </c>
       <c r="T20">
-        <v>4014101926</v>
+        <v>1851925471</v>
       </c>
       <c r="U20">
-        <v>1878997667</v>
+        <v>590566592</v>
       </c>
       <c r="V20">
-        <v>559427078</v>
+        <v>3633973594</v>
       </c>
       <c r="W20">
-        <v>-711183147</v>
+        <v>2205418963</v>
       </c>
       <c r="X20">
-        <v>1929682988</v>
+        <v>592903151</v>
       </c>
       <c r="Y20" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F21">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="G21">
-        <v>1580000</v>
+        <v>1640000</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="I21">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J21">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K21">
-        <v>7874611</v>
+        <v>10969386</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N21" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O21" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="P21">
-        <v>7327878427</v>
+        <v>22818451349</v>
       </c>
       <c r="Q21">
-        <v>10756717708</v>
+        <v>30491967755</v>
       </c>
       <c r="R21">
-        <v>4113702647</v>
+        <v>18040053709</v>
       </c>
       <c r="S21">
-        <v>-588932080</v>
+        <v>2313787613</v>
       </c>
       <c r="T21">
-        <v>254042570</v>
+        <v>4014101926</v>
       </c>
       <c r="U21">
-        <v>-738698858</v>
+        <v>1878997667</v>
       </c>
       <c r="V21">
-        <v>-569358529</v>
+        <v>559427078</v>
       </c>
       <c r="W21">
-        <v>-429546963</v>
+        <v>-711183147</v>
       </c>
       <c r="X21">
-        <v>-550600734</v>
+        <v>1929682988</v>
       </c>
       <c r="Y21" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2717,150 +2732,227 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F22">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="G22">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J22">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K22">
-        <v>8110389</v>
+        <v>7874611</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="O22" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="P22">
-        <v>28857</v>
+        <v>7327878427</v>
       </c>
       <c r="Q22">
-        <v>45830</v>
+        <v>10756717708</v>
       </c>
       <c r="R22">
-        <v>25997</v>
+        <v>4113702647</v>
       </c>
       <c r="S22">
-        <v>-14511</v>
+        <v>-588932080</v>
       </c>
       <c r="T22">
-        <v>4169</v>
+        <v>254042570</v>
       </c>
       <c r="U22">
-        <v>4958</v>
+        <v>-738698858</v>
       </c>
       <c r="V22">
-        <v>-34842</v>
+        <v>-569358529</v>
       </c>
       <c r="W22">
-        <v>13350</v>
+        <v>-429546963</v>
       </c>
       <c r="X22">
-        <v>5128</v>
+        <v>-550600734</v>
       </c>
       <c r="Y22" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F23">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="G23">
-        <v>900000</v>
+        <v>1500000</v>
       </c>
       <c r="H23">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>20000</v>
       </c>
       <c r="J23">
+        <v>23000</v>
+      </c>
+      <c r="K23">
+        <v>8110389</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>23000</v>
+      </c>
+      <c r="N23" t="s">
+        <v>118</v>
+      </c>
+      <c r="O23" t="s">
+        <v>139</v>
+      </c>
+      <c r="P23">
+        <v>28857</v>
+      </c>
+      <c r="Q23">
+        <v>45830</v>
+      </c>
+      <c r="R23">
+        <v>25997</v>
+      </c>
+      <c r="S23">
+        <v>-14511</v>
+      </c>
+      <c r="T23">
+        <v>4169</v>
+      </c>
+      <c r="U23">
+        <v>4958</v>
+      </c>
+      <c r="V23">
+        <v>-34842</v>
+      </c>
+      <c r="W23">
+        <v>13350</v>
+      </c>
+      <c r="X23">
+        <v>5128</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24">
+        <v>1100000</v>
+      </c>
+      <c r="G24">
+        <v>900000</v>
+      </c>
+      <c r="H24">
+        <v>200000</v>
+      </c>
+      <c r="I24">
+        <v>20000</v>
+      </c>
+      <c r="J24">
         <v>24000</v>
       </c>
-      <c r="K23">
+      <c r="K24">
         <v>4901526</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>24000</v>
       </c>
-      <c r="N23" t="s">
-        <v>115</v>
-      </c>
-      <c r="O23" t="s">
-        <v>135</v>
-      </c>
-      <c r="P23">
+      <c r="N24" t="s">
+        <v>119</v>
+      </c>
+      <c r="O24" t="s">
+        <v>140</v>
+      </c>
+      <c r="P24">
         <v>32608351</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>43629717</v>
       </c>
-      <c r="R23">
+      <c r="R24">
         <v>14011366</v>
       </c>
-      <c r="S23">
+      <c r="S24">
         <v>4301870</v>
       </c>
-      <c r="T23">
+      <c r="T24">
         <v>7039261</v>
       </c>
-      <c r="U23">
+      <c r="U24">
         <v>316611</v>
       </c>
-      <c r="V23">
+      <c r="V24">
         <v>4422483</v>
       </c>
-      <c r="W23">
+      <c r="W24">
         <v>5391712</v>
       </c>
-      <c r="X23">
+      <c r="X24">
         <v>180579</v>
       </c>
-      <c r="Y23" t="s">
-        <v>156</v>
+      <c r="Y24" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2878,422 +2970,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E2">
         <v>21000</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E3">
         <v>64350</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E4">
         <v>20000</v>
       </c>
       <c r="F4" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E5">
         <v>7000</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E6">
         <v>14250</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E7">
         <v>16000</v>
       </c>
       <c r="F7" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E8">
         <v>13500</v>
       </c>
       <c r="F8" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E9">
         <v>14950</v>
       </c>
       <c r="F9" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E10">
         <v>29547</v>
       </c>
       <c r="F10" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E11">
         <v>18040</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D12" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E12">
         <v>22100</v>
       </c>
       <c r="F12" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E13">
         <v>59251</v>
       </c>
       <c r="F13" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E14">
         <v>60654</v>
       </c>
       <c r="F14" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E15">
         <v>26800</v>
       </c>
       <c r="F15" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="E16">
         <v>524031</v>
       </c>
       <c r="F16" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E17">
         <v>6384</v>
       </c>
       <c r="F17" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E19">
         <v>50353</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D20" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E20">
         <v>8400</v>
       </c>
       <c r="F20" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D21" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E21">
         <v>41818</v>
       </c>
       <c r="F21" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-20
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="253">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
     <t>2023-10-26</t>
   </si>
   <si>
@@ -143,6 +146,9 @@
     <t>2023-09-07</t>
   </si>
   <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
     <t>2023-11-01</t>
   </si>
   <si>
@@ -164,6 +170,9 @@
     <t>2023-09-13</t>
   </si>
   <si>
+    <t>2023-11-20</t>
+  </si>
+  <si>
     <t>2023-11-15</t>
   </si>
   <si>
@@ -197,6 +206,9 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>하이</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -239,6 +251,9 @@
     <t>신영</t>
   </si>
   <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
     <t>캡스톤파트너스</t>
   </si>
   <si>
@@ -308,6 +323,9 @@
     <t>인스웨이브시스템즈</t>
   </si>
   <si>
+    <t>573.97:1</t>
+  </si>
+  <si>
     <t>952.78</t>
   </si>
   <si>
@@ -377,6 +395,9 @@
     <t>672.42:1</t>
   </si>
   <si>
+    <t>3.24%</t>
+  </si>
+  <si>
     <t>0.19%</t>
   </si>
   <si>
@@ -440,6 +461,9 @@
     <t>7.46%</t>
   </si>
   <si>
+    <t>정수기 피팅, 밸브, 파우셋 등 부품</t>
+  </si>
+  <si>
     <t>벤처투자조합 등 조합 결성 및 운영</t>
   </si>
   <si>
@@ -570,9 +594,6 @@
   </si>
   <si>
     <t>동인기연(유가)</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
   </si>
   <si>
     <t>에코프로머티리얼즈(유가)</t>
@@ -1110,7 +1131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1198,76 +1219,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F2">
-        <v>1596000</v>
+        <v>3350000</v>
       </c>
       <c r="G2">
-        <v>1596000</v>
+        <v>3350000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>3200</v>
+        <v>8000</v>
       </c>
       <c r="J2">
-        <v>3600</v>
+        <v>9500</v>
       </c>
       <c r="K2">
-        <v>13346380</v>
+        <v>13436499</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>4000</v>
+        <v>11000</v>
       </c>
       <c r="N2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="O2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="P2">
-        <v>7668281979</v>
+        <v>47984</v>
       </c>
       <c r="Q2">
-        <v>7100921456</v>
+        <v>51031</v>
       </c>
       <c r="R2">
-        <v>1207846478</v>
+        <v>29425</v>
       </c>
       <c r="S2">
-        <v>5659403971</v>
+        <v>10526</v>
       </c>
       <c r="T2">
-        <v>6124121466</v>
+        <v>11804</v>
       </c>
       <c r="U2">
-        <v>940668827</v>
+        <v>7008</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>8661</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>9582</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>5612</v>
       </c>
       <c r="Y2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1275,76 +1296,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F3">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="G3">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>29800</v>
+        <v>3200</v>
       </c>
       <c r="J3">
-        <v>33500</v>
+        <v>3600</v>
       </c>
       <c r="K3">
-        <v>13612736</v>
+        <v>13346380</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="O3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>7668281979</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>7100921456</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1207846478</v>
       </c>
       <c r="S3">
-        <v>-15286512079</v>
+        <v>5659403971</v>
       </c>
       <c r="T3">
-        <v>-21424611321</v>
+        <v>6124121466</v>
       </c>
       <c r="U3">
-        <v>-139745251263</v>
+        <v>940668827</v>
       </c>
       <c r="V3">
-        <v>-53575668634</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>-38885125426</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>-12610702106</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1352,76 +1373,76 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F4">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="G4">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>19100</v>
+        <v>29800</v>
       </c>
       <c r="J4">
-        <v>21400</v>
+        <v>33500</v>
       </c>
       <c r="K4">
-        <v>10585320</v>
+        <v>13612736</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="O4" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="P4">
-        <v>45195788</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>69629209</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>35634471</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>2751277</v>
+        <v>-15286512079</v>
       </c>
       <c r="T4">
-        <v>11449731</v>
+        <v>-21424611321</v>
       </c>
       <c r="U4">
-        <v>2482194</v>
+        <v>-139745251263</v>
       </c>
       <c r="V4">
-        <v>2092692</v>
+        <v>-53575668634</v>
       </c>
       <c r="W4">
-        <v>5149538</v>
+        <v>-38885125426</v>
       </c>
       <c r="X4">
-        <v>2327401</v>
+        <v>-12610702106</v>
       </c>
       <c r="Y4" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1429,384 +1450,384 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F5">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>19100</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>21400</v>
       </c>
       <c r="K5">
-        <v>4320000</v>
+        <v>10585320</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="O5" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>45195788</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>69629209</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>35634471</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2751277</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>11449731</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>2482194</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>2092692</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>5149538</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>2327401</v>
       </c>
       <c r="Y5" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F6">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="G6">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K6">
-        <v>30610000</v>
+        <v>4320000</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="O6" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="P6">
-        <v>67332006578</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>100050838794</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>63366010569</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1140243099</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>8333440685</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>7415958936</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>668088159</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>5930478364</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>5666583221</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F7">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="G7">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>3500</v>
+        <v>1200</v>
       </c>
       <c r="J7">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="K7">
-        <v>20771000</v>
+        <v>30610000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="O7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="P7">
-        <v>39450601</v>
+        <v>67332006578</v>
       </c>
       <c r="Q7">
-        <v>49044883</v>
+        <v>100050838794</v>
       </c>
       <c r="R7">
-        <v>21826468</v>
+        <v>63366010569</v>
       </c>
       <c r="S7">
-        <v>2477559</v>
+        <v>1140243099</v>
       </c>
       <c r="T7">
-        <v>8094900</v>
+        <v>8333440685</v>
       </c>
       <c r="U7">
-        <v>215154</v>
+        <v>7415958936</v>
       </c>
       <c r="V7">
-        <v>3427734</v>
+        <v>668088159</v>
       </c>
       <c r="W7">
-        <v>6575528</v>
+        <v>5930478364</v>
       </c>
       <c r="X7">
-        <v>349843</v>
+        <v>5666583221</v>
       </c>
       <c r="Y7" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F8">
-        <v>2060000</v>
+        <v>5200000</v>
       </c>
       <c r="G8">
-        <v>2000000</v>
+        <v>5200000</v>
       </c>
       <c r="H8">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>20300</v>
+        <v>3500</v>
       </c>
       <c r="J8">
-        <v>22500</v>
+        <v>4000</v>
       </c>
       <c r="K8">
-        <v>14384224</v>
+        <v>20771000</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N8" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="O8" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="P8">
-        <v>5787300240</v>
+        <v>39450601</v>
       </c>
       <c r="Q8">
-        <v>1914633847</v>
+        <v>49044883</v>
       </c>
       <c r="R8">
-        <v>3156092272</v>
+        <v>21826468</v>
       </c>
       <c r="S8">
-        <v>-1798278694</v>
+        <v>2477559</v>
       </c>
       <c r="T8">
-        <v>-1453689952</v>
+        <v>8094900</v>
       </c>
       <c r="U8">
-        <v>-4067648306</v>
+        <v>215154</v>
       </c>
       <c r="V8">
-        <v>-12449932055</v>
+        <v>3427734</v>
       </c>
       <c r="W8">
-        <v>-7426231074</v>
+        <v>6575528</v>
       </c>
       <c r="X8">
-        <v>-52132058866</v>
+        <v>349843</v>
       </c>
       <c r="Y8" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F9">
-        <v>1200000</v>
+        <v>2060000</v>
       </c>
       <c r="G9">
-        <v>1200000</v>
+        <v>2000000</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I9">
-        <v>9100</v>
+        <v>20300</v>
       </c>
       <c r="J9">
-        <v>11000</v>
+        <v>22500</v>
       </c>
       <c r="K9">
-        <v>7206940</v>
+        <v>14384224</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="O9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="P9">
-        <v>20924</v>
+        <v>5787300240</v>
       </c>
       <c r="Q9">
-        <v>27659</v>
+        <v>1914633847</v>
       </c>
       <c r="R9">
-        <v>11818</v>
+        <v>3156092272</v>
       </c>
       <c r="S9">
-        <v>2838</v>
+        <v>-1798278694</v>
       </c>
       <c r="T9">
-        <v>4563</v>
+        <v>-1453689952</v>
       </c>
       <c r="U9">
-        <v>-1222</v>
+        <v>-4067648306</v>
       </c>
       <c r="V9">
-        <v>2413</v>
+        <v>-12449932055</v>
       </c>
       <c r="W9">
-        <v>3190</v>
+        <v>-7426231074</v>
       </c>
       <c r="X9">
-        <v>-862</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y9" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1814,230 +1835,230 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F10">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="G10">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>5000</v>
+        <v>9100</v>
       </c>
       <c r="J10">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="K10">
-        <v>17306490</v>
+        <v>7206940</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N10" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="O10" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="P10">
-        <v>21976760922</v>
+        <v>20924</v>
       </c>
       <c r="Q10">
-        <v>15839004968</v>
+        <v>27659</v>
       </c>
       <c r="R10">
-        <v>6887755932</v>
+        <v>11818</v>
       </c>
       <c r="S10">
-        <v>-2217897363</v>
+        <v>2838</v>
       </c>
       <c r="T10">
-        <v>-3403228196</v>
+        <v>4563</v>
       </c>
       <c r="U10">
-        <v>-2758864194</v>
+        <v>-1222</v>
       </c>
       <c r="V10">
-        <v>-5110677395</v>
+        <v>2413</v>
       </c>
       <c r="W10">
-        <v>-29510193610</v>
+        <v>3190</v>
       </c>
       <c r="X10">
-        <v>-2514471056</v>
+        <v>-862</v>
       </c>
       <c r="Y10" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F11">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="G11">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K11">
-        <v>12905000</v>
+        <v>17306490</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N11" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O11" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>21976760922</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>15839004968</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>6887755932</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>-2217897363</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>-3403228196</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>-2758864194</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>-5110677395</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>-29510193610</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y11" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F12">
-        <v>1049482</v>
+        <v>12500000</v>
       </c>
       <c r="G12">
-        <v>944534</v>
+        <v>12500000</v>
       </c>
       <c r="H12">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>12800</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>6261485</v>
+        <v>12905000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="O12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="P12">
-        <v>34557425427</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>39824841246</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>23231897516</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>3011651602</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>2384643399</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>4436005255</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>2755379556</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>1176755354</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>4046949430</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2045,76 +2066,76 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F13">
-        <v>1128720</v>
+        <v>1049482</v>
       </c>
       <c r="G13">
-        <v>1128720</v>
+        <v>944534</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I13">
-        <v>3300</v>
+        <v>12800</v>
       </c>
       <c r="J13">
-        <v>3900</v>
+        <v>14500</v>
       </c>
       <c r="K13">
-        <v>11287196</v>
+        <v>6261485</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N13" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="O13" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="P13">
-        <v>50552623684</v>
+        <v>34557425427</v>
       </c>
       <c r="Q13">
-        <v>69013134090</v>
+        <v>39824841246</v>
       </c>
       <c r="R13">
-        <v>16887814423</v>
+        <v>23231897516</v>
       </c>
       <c r="S13">
-        <v>9027232647</v>
+        <v>3011651602</v>
       </c>
       <c r="T13">
-        <v>15707796256</v>
+        <v>2384643399</v>
       </c>
       <c r="U13">
-        <v>555562560</v>
+        <v>4436005255</v>
       </c>
       <c r="V13">
-        <v>9236341465</v>
+        <v>2755379556</v>
       </c>
       <c r="W13">
-        <v>13159994846</v>
+        <v>1176755354</v>
       </c>
       <c r="X13">
-        <v>1236029732</v>
+        <v>4046949430</v>
       </c>
       <c r="Y13" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2122,76 +2143,76 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F14">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="G14">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>13000</v>
+        <v>3300</v>
       </c>
       <c r="J14">
-        <v>15000</v>
+        <v>3900</v>
       </c>
       <c r="K14">
-        <v>10193520</v>
+        <v>11287196</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N14" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="O14" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="P14">
-        <v>3952070068</v>
+        <v>50552623684</v>
       </c>
       <c r="Q14">
-        <v>10789274729</v>
+        <v>69013134090</v>
       </c>
       <c r="R14">
-        <v>6040367765</v>
+        <v>16887814423</v>
       </c>
       <c r="S14">
-        <v>-4741577598</v>
+        <v>9027232647</v>
       </c>
       <c r="T14">
-        <v>-3671026788</v>
+        <v>15707796256</v>
       </c>
       <c r="U14">
-        <v>-3292521363</v>
+        <v>555562560</v>
       </c>
       <c r="V14">
-        <v>-3654889267</v>
+        <v>9236341465</v>
       </c>
       <c r="W14">
-        <v>-2281074471</v>
+        <v>13159994846</v>
       </c>
       <c r="X14">
-        <v>-2539505707</v>
+        <v>1236029732</v>
       </c>
       <c r="Y14" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2199,76 +2220,76 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F15">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="G15">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J15">
-        <v>5600</v>
+        <v>15000</v>
       </c>
       <c r="K15">
-        <v>16120000</v>
+        <v>10193520</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N15" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="O15" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="P15">
-        <v>26691070764</v>
+        <v>3952070068</v>
       </c>
       <c r="Q15">
-        <v>22835113396</v>
+        <v>10789274729</v>
       </c>
       <c r="R15">
-        <v>7519073723</v>
+        <v>6040367765</v>
       </c>
       <c r="S15">
-        <v>6041270235</v>
+        <v>-4741577598</v>
       </c>
       <c r="T15">
-        <v>6705120210</v>
+        <v>-3671026788</v>
       </c>
       <c r="U15">
-        <v>982044017</v>
+        <v>-3292521363</v>
       </c>
       <c r="V15">
-        <v>5119066139</v>
+        <v>-3654889267</v>
       </c>
       <c r="W15">
-        <v>5870093710</v>
+        <v>-2281074471</v>
       </c>
       <c r="X15">
-        <v>1198587470</v>
+        <v>-2539505707</v>
       </c>
       <c r="Y15" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2276,76 +2297,76 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F16">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="G16">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8200</v>
+        <v>5000</v>
       </c>
       <c r="J16">
-        <v>9400</v>
+        <v>5600</v>
       </c>
       <c r="K16">
-        <v>7674103</v>
+        <v>16120000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N16" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="P16">
-        <v>8242508010</v>
+        <v>26691070764</v>
       </c>
       <c r="Q16">
-        <v>10751900430</v>
+        <v>22835113396</v>
       </c>
       <c r="R16">
-        <v>4416778965</v>
+        <v>7519073723</v>
       </c>
       <c r="S16">
-        <v>426234451</v>
+        <v>6041270235</v>
       </c>
       <c r="T16">
-        <v>2423749751</v>
+        <v>6705120210</v>
       </c>
       <c r="U16">
-        <v>677048172</v>
+        <v>982044017</v>
       </c>
       <c r="V16">
-        <v>57890953</v>
+        <v>5119066139</v>
       </c>
       <c r="W16">
-        <v>2826043673</v>
+        <v>5870093710</v>
       </c>
       <c r="X16">
-        <v>990121873</v>
+        <v>1198587470</v>
       </c>
       <c r="Y16" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2353,76 +2374,76 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F17">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="G17">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>22000</v>
+        <v>8200</v>
       </c>
       <c r="J17">
-        <v>25000</v>
+        <v>9400</v>
       </c>
       <c r="K17">
-        <v>9039778</v>
+        <v>7674103</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N17" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="O17" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="P17">
-        <v>104225113285</v>
+        <v>8242508010</v>
       </c>
       <c r="Q17">
-        <v>106505634411</v>
+        <v>10751900430</v>
       </c>
       <c r="R17">
-        <v>66424930568</v>
+        <v>4416778965</v>
       </c>
       <c r="S17">
-        <v>6291020806</v>
+        <v>426234451</v>
       </c>
       <c r="T17">
-        <v>7893242769</v>
+        <v>2423749751</v>
       </c>
       <c r="U17">
-        <v>7661497240</v>
+        <v>677048172</v>
       </c>
       <c r="V17">
-        <v>7319368873</v>
+        <v>57890953</v>
       </c>
       <c r="W17">
-        <v>9286891982</v>
+        <v>2826043673</v>
       </c>
       <c r="X17">
-        <v>7334816490</v>
+        <v>990121873</v>
       </c>
       <c r="Y17" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2430,34 +2451,34 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F18">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="G18">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="J18">
-        <v>26000</v>
+        <v>25000</v>
       </c>
       <c r="K18">
-        <v>64819980</v>
+        <v>9039778</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2466,40 +2487,40 @@
         <v>26000</v>
       </c>
       <c r="N18" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="O18" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="P18">
-        <v>36980</v>
+        <v>104225113285</v>
       </c>
       <c r="Q18">
-        <v>44954</v>
+        <v>106505634411</v>
       </c>
       <c r="R18">
-        <v>23652</v>
+        <v>66424930568</v>
       </c>
       <c r="S18">
-        <v>-7085</v>
+        <v>6291020806</v>
       </c>
       <c r="T18">
-        <v>-13228</v>
+        <v>7893242769</v>
       </c>
       <c r="U18">
-        <v>-9932</v>
+        <v>7661497240</v>
       </c>
       <c r="V18">
-        <v>-7417</v>
+        <v>7319368873</v>
       </c>
       <c r="W18">
-        <v>-12548</v>
+        <v>9286891982</v>
       </c>
       <c r="X18">
-        <v>-9333</v>
+        <v>7334816490</v>
       </c>
       <c r="Y18" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2507,76 +2528,76 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F19">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="G19">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K19">
-        <v>18905000</v>
+        <v>64819980</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N19" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="O19" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>36980</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>44954</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>23652</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>-7085</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>-13228</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>-9932</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>-7417</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>-12548</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>-9333</v>
       </c>
       <c r="Y19" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2584,230 +2605,230 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F20">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="G20">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J20">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K20">
-        <v>5447675</v>
+        <v>18905000</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N20" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="O20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P20">
-        <v>18408761227</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>21902816604</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>8176918465</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>3669182465</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>1851925471</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>590566592</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>3633973594</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>2205418963</v>
+        <v>0</v>
       </c>
       <c r="X20">
-        <v>592903151</v>
+        <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F21">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="G21">
-        <v>1640000</v>
+        <v>1500000</v>
       </c>
       <c r="H21">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J21">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K21">
-        <v>10969386</v>
+        <v>5447675</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N21" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="P21">
-        <v>22818451349</v>
+        <v>18408761227</v>
       </c>
       <c r="Q21">
-        <v>30491967755</v>
+        <v>21902816604</v>
       </c>
       <c r="R21">
-        <v>18040053709</v>
+        <v>8176918465</v>
       </c>
       <c r="S21">
-        <v>2313787613</v>
+        <v>3669182465</v>
       </c>
       <c r="T21">
-        <v>4014101926</v>
+        <v>1851925471</v>
       </c>
       <c r="U21">
-        <v>1878997667</v>
+        <v>590566592</v>
       </c>
       <c r="V21">
-        <v>559427078</v>
+        <v>3633973594</v>
       </c>
       <c r="W21">
-        <v>-711183147</v>
+        <v>2205418963</v>
       </c>
       <c r="X21">
-        <v>1929682988</v>
+        <v>592903151</v>
       </c>
       <c r="Y21" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F22">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="G22">
-        <v>1580000</v>
+        <v>1640000</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="I22">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J22">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K22">
-        <v>7874611</v>
+        <v>10969386</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N22" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="O22" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="P22">
-        <v>7327878427</v>
+        <v>22818451349</v>
       </c>
       <c r="Q22">
-        <v>10756717708</v>
+        <v>30491967755</v>
       </c>
       <c r="R22">
-        <v>4113702647</v>
+        <v>18040053709</v>
       </c>
       <c r="S22">
-        <v>-588932080</v>
+        <v>2313787613</v>
       </c>
       <c r="T22">
-        <v>254042570</v>
+        <v>4014101926</v>
       </c>
       <c r="U22">
-        <v>-738698858</v>
+        <v>1878997667</v>
       </c>
       <c r="V22">
-        <v>-569358529</v>
+        <v>559427078</v>
       </c>
       <c r="W22">
-        <v>-429546963</v>
+        <v>-711183147</v>
       </c>
       <c r="X22">
-        <v>-550600734</v>
+        <v>1929682988</v>
       </c>
       <c r="Y22" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2815,153 +2836,230 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F23">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="G23">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J23">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K23">
-        <v>8110389</v>
+        <v>7874611</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N23" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="O23" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="P23">
-        <v>28857</v>
+        <v>7327878427</v>
       </c>
       <c r="Q23">
-        <v>45830</v>
+        <v>10756717708</v>
       </c>
       <c r="R23">
-        <v>25997</v>
+        <v>4113702647</v>
       </c>
       <c r="S23">
-        <v>-14511</v>
+        <v>-588932080</v>
       </c>
       <c r="T23">
-        <v>4169</v>
+        <v>254042570</v>
       </c>
       <c r="U23">
-        <v>4958</v>
+        <v>-738698858</v>
       </c>
       <c r="V23">
-        <v>-34842</v>
+        <v>-569358529</v>
       </c>
       <c r="W23">
-        <v>13350</v>
+        <v>-429546963</v>
       </c>
       <c r="X23">
-        <v>5128</v>
+        <v>-550600734</v>
       </c>
       <c r="Y23" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F24">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="G24">
-        <v>900000</v>
+        <v>1500000</v>
       </c>
       <c r="H24">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>20000</v>
       </c>
       <c r="J24">
+        <v>23000</v>
+      </c>
+      <c r="K24">
+        <v>8110389</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>23000</v>
+      </c>
+      <c r="N24" t="s">
+        <v>124</v>
+      </c>
+      <c r="O24" t="s">
+        <v>146</v>
+      </c>
+      <c r="P24">
+        <v>28857</v>
+      </c>
+      <c r="Q24">
+        <v>45830</v>
+      </c>
+      <c r="R24">
+        <v>25997</v>
+      </c>
+      <c r="S24">
+        <v>-14511</v>
+      </c>
+      <c r="T24">
+        <v>4169</v>
+      </c>
+      <c r="U24">
+        <v>4958</v>
+      </c>
+      <c r="V24">
+        <v>-34842</v>
+      </c>
+      <c r="W24">
+        <v>13350</v>
+      </c>
+      <c r="X24">
+        <v>5128</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25">
+        <v>1100000</v>
+      </c>
+      <c r="G25">
+        <v>900000</v>
+      </c>
+      <c r="H25">
+        <v>200000</v>
+      </c>
+      <c r="I25">
+        <v>20000</v>
+      </c>
+      <c r="J25">
         <v>24000</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <v>4901526</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>24000</v>
       </c>
-      <c r="N24" t="s">
-        <v>119</v>
-      </c>
-      <c r="O24" t="s">
-        <v>140</v>
-      </c>
-      <c r="P24">
+      <c r="N25" t="s">
+        <v>125</v>
+      </c>
+      <c r="O25" t="s">
+        <v>147</v>
+      </c>
+      <c r="P25">
         <v>32608351</v>
       </c>
-      <c r="Q24">
+      <c r="Q25">
         <v>43629717</v>
       </c>
-      <c r="R24">
+      <c r="R25">
         <v>14011366</v>
       </c>
-      <c r="S24">
+      <c r="S25">
         <v>4301870</v>
       </c>
-      <c r="T24">
+      <c r="T25">
         <v>7039261</v>
       </c>
-      <c r="U24">
+      <c r="U25">
         <v>316611</v>
       </c>
-      <c r="V24">
+      <c r="V25">
         <v>4422483</v>
       </c>
-      <c r="W24">
+      <c r="W25">
         <v>5391712</v>
       </c>
-      <c r="X24">
+      <c r="X25">
         <v>180579</v>
       </c>
-      <c r="Y24" t="s">
-        <v>162</v>
+      <c r="Y25" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2979,422 +3077,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E2">
         <v>14000</v>
       </c>
       <c r="F2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E3">
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E4">
         <v>96380</v>
       </c>
       <c r="F4" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E5">
         <v>21000</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E6">
         <v>64350</v>
       </c>
       <c r="F6" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E7">
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E9">
         <v>14250</v>
       </c>
       <c r="F9" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E10">
         <v>16000</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E11">
         <v>13500</v>
       </c>
       <c r="F11" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="E12">
         <v>14950</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E13">
         <v>29547</v>
       </c>
       <c r="F13" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D14" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E14">
         <v>18040</v>
       </c>
       <c r="F14" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="E15">
         <v>22100</v>
       </c>
       <c r="F15" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E16">
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E17">
         <v>60654</v>
       </c>
       <c r="F17" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D18" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="E18">
         <v>26800</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D19" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="E19">
         <v>524031</v>
       </c>
       <c r="F19" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="D20" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E20">
         <v>6384</v>
       </c>
       <c r="F20" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E21">
         <v>8000</v>
       </c>
       <c r="F21" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-23
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -3298,7 +3298,7 @@
         <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="E7">
         <v>20000</v>
@@ -3318,7 +3318,7 @@
         <v>216</v>
       </c>
       <c r="D8" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="E8">
         <v>7000</v>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-27
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="254">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -152,9 +152,6 @@
     <t>2023-09-06</t>
   </si>
   <si>
-    <t>2023-09-07</t>
-  </si>
-  <si>
     <t>2023-11-09</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>2023-09-12</t>
   </si>
   <si>
-    <t>2023-09-13</t>
-  </si>
-  <si>
     <t>2023-11-24</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>2023-10-10</t>
   </si>
   <si>
-    <t>2023-09-27</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
@@ -329,9 +320,6 @@
     <t>아이엠티</t>
   </si>
   <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
     <t>753.19:1</t>
   </si>
   <si>
@@ -407,9 +395,6 @@
     <t>753.50:1</t>
   </si>
   <si>
-    <t>619.24:1</t>
-  </si>
-  <si>
     <t>5.39%</t>
   </si>
   <si>
@@ -479,9 +464,6 @@
     <t>22.20%</t>
   </si>
   <si>
-    <t>5.76%</t>
-  </si>
-  <si>
     <t>반도체 및 디스플레이 장비 보호코팅 및 소재</t>
   </si>
   <si>
@@ -552,9 +534,6 @@
   </si>
   <si>
     <t>건식세정 장비 및 EUV Mask Baking Laser</t>
-  </si>
-  <si>
-    <t>전자책 정기구독 서비스</t>
   </si>
   <si>
     <t>종목명</t>
@@ -1155,7 +1134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1243,16 +1222,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F2">
         <v>1640000</v>
@@ -1279,10 +1258,10 @@
         <v>17000</v>
       </c>
       <c r="N2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="O2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="P2">
         <v>13660</v>
@@ -1312,7 +1291,7 @@
         <v>1666</v>
       </c>
       <c r="Y2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1320,16 +1299,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F3">
         <v>3350000</v>
@@ -1356,10 +1335,10 @@
         <v>11000</v>
       </c>
       <c r="N3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="O3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P3">
         <v>47984</v>
@@ -1389,7 +1368,7 @@
         <v>5612</v>
       </c>
       <c r="Y3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1397,16 +1376,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4">
         <v>4250000</v>
@@ -1433,10 +1412,10 @@
         <v>7000</v>
       </c>
       <c r="N4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="O4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="P4">
         <v>27199897007</v>
@@ -1466,7 +1445,7 @@
         <v>3402334635</v>
       </c>
       <c r="Y4" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1474,16 +1453,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5">
         <v>2079000</v>
@@ -1510,10 +1489,10 @@
         <v>34700</v>
       </c>
       <c r="N5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="P5">
         <v>26994234332</v>
@@ -1543,7 +1522,7 @@
         <v>15932218050</v>
       </c>
       <c r="Y5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1554,13 +1533,13 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F6">
         <v>1596000</v>
@@ -1587,10 +1566,10 @@
         <v>4000</v>
       </c>
       <c r="N6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="O6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P6">
         <v>7668281979</v>
@@ -1620,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1631,13 +1610,13 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F7">
         <v>1600000</v>
@@ -1664,10 +1643,10 @@
         <v>20000</v>
       </c>
       <c r="N7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1697,7 +1676,7 @@
         <v>-12610702106</v>
       </c>
       <c r="Y7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1705,16 +1684,16 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F8">
         <v>2636330</v>
@@ -1741,10 +1720,10 @@
         <v>25000</v>
       </c>
       <c r="N8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="P8">
         <v>45195788</v>
@@ -1774,7 +1753,7 @@
         <v>2327401</v>
       </c>
       <c r="Y8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1785,13 +1764,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1818,10 +1797,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1851,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1859,16 +1838,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F10">
         <v>7000000</v>
@@ -1895,10 +1874,10 @@
         <v>1800</v>
       </c>
       <c r="N10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P10">
         <v>67332006578</v>
@@ -1928,7 +1907,7 @@
         <v>5666583221</v>
       </c>
       <c r="Y10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1939,13 +1918,13 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="D11" t="s">
-        <v>65</v>
-      </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11">
         <v>5200000</v>
@@ -1972,10 +1951,10 @@
         <v>4800</v>
       </c>
       <c r="N11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P11">
         <v>39450601</v>
@@ -2005,7 +1984,7 @@
         <v>349843</v>
       </c>
       <c r="Y11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -2016,13 +1995,13 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F12">
         <v>2060000</v>
@@ -2049,10 +2028,10 @@
         <v>22500</v>
       </c>
       <c r="N12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O12" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P12">
         <v>5787300240</v>
@@ -2082,7 +2061,7 @@
         <v>-52132058866</v>
       </c>
       <c r="Y12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2093,13 +2072,13 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13">
         <v>1200000</v>
@@ -2126,10 +2105,10 @@
         <v>13000</v>
       </c>
       <c r="N13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P13">
         <v>20924</v>
@@ -2159,7 +2138,7 @@
         <v>-862</v>
       </c>
       <c r="Y13" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2170,13 +2149,13 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F14">
         <v>3600000</v>
@@ -2203,10 +2182,10 @@
         <v>7500</v>
       </c>
       <c r="N14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="O14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P14">
         <v>21976760922</v>
@@ -2236,7 +2215,7 @@
         <v>-2514471056</v>
       </c>
       <c r="Y14" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2250,10 +2229,10 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F15">
         <v>12500000</v>
@@ -2280,10 +2259,10 @@
         <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2313,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2327,10 +2306,10 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F16">
         <v>1049482</v>
@@ -2357,10 +2336,10 @@
         <v>17000</v>
       </c>
       <c r="N16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P16">
         <v>34557425427</v>
@@ -2390,7 +2369,7 @@
         <v>4046949430</v>
       </c>
       <c r="Y16" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2404,10 +2383,10 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F17">
         <v>1128720</v>
@@ -2434,10 +2413,10 @@
         <v>4400</v>
       </c>
       <c r="N17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="P17">
         <v>50552623684</v>
@@ -2467,7 +2446,7 @@
         <v>1236029732</v>
       </c>
       <c r="Y17" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2475,16 +2454,16 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F18">
         <v>1800000</v>
@@ -2511,10 +2490,10 @@
         <v>17000</v>
       </c>
       <c r="N18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O18" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="P18">
         <v>3952070068</v>
@@ -2544,7 +2523,7 @@
         <v>-2539505707</v>
       </c>
       <c r="Y18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2558,10 +2537,10 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F19">
         <v>4000000</v>
@@ -2588,10 +2567,10 @@
         <v>6500</v>
       </c>
       <c r="N19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P19">
         <v>26691070764</v>
@@ -2621,7 +2600,7 @@
         <v>1198587470</v>
       </c>
       <c r="Y19" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2635,10 +2614,10 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F20">
         <v>770000</v>
@@ -2665,10 +2644,10 @@
         <v>7000</v>
       </c>
       <c r="N20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O20" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P20">
         <v>8242508010</v>
@@ -2698,7 +2677,7 @@
         <v>990121873</v>
       </c>
       <c r="Y20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2706,16 +2685,16 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F21">
         <v>2000000</v>
@@ -2742,10 +2721,10 @@
         <v>26000</v>
       </c>
       <c r="N21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O21" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="P21">
         <v>104225113285</v>
@@ -2775,7 +2754,7 @@
         <v>7334816490</v>
       </c>
       <c r="Y21" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2783,16 +2762,16 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F22">
         <v>16200000</v>
@@ -2819,10 +2798,10 @@
         <v>26000</v>
       </c>
       <c r="N22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P22">
         <v>36980</v>
@@ -2852,7 +2831,7 @@
         <v>-9333</v>
       </c>
       <c r="Y22" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2860,16 +2839,16 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F23">
         <v>18000000</v>
@@ -2896,10 +2875,10 @@
         <v>2000</v>
       </c>
       <c r="N23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P23">
         <v>0</v>
@@ -2929,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="Y23" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2940,13 +2919,13 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F24">
         <v>1500000</v>
@@ -2973,10 +2952,10 @@
         <v>12500</v>
       </c>
       <c r="N24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O24" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P24">
         <v>18408761227</v>
@@ -3006,7 +2985,7 @@
         <v>592903151</v>
       </c>
       <c r="Y24" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -3014,16 +2993,16 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F25">
         <v>2240000</v>
@@ -3050,10 +3029,10 @@
         <v>15000</v>
       </c>
       <c r="N25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="P25">
         <v>22818451349</v>
@@ -3083,7 +3062,7 @@
         <v>1929682988</v>
       </c>
       <c r="Y25" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -3091,16 +3070,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F26">
         <v>1580000</v>
@@ -3127,10 +3106,10 @@
         <v>14000</v>
       </c>
       <c r="N26" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O26" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="P26">
         <v>7327878427</v>
@@ -3160,84 +3139,7 @@
         <v>-550600734</v>
       </c>
       <c r="Y26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27">
-        <v>1500000</v>
-      </c>
-      <c r="G27">
-        <v>1500000</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>20000</v>
-      </c>
-      <c r="J27">
-        <v>23000</v>
-      </c>
-      <c r="K27">
-        <v>8110389</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>23000</v>
-      </c>
-      <c r="N27" t="s">
-        <v>130</v>
-      </c>
-      <c r="O27" t="s">
-        <v>154</v>
-      </c>
-      <c r="P27">
-        <v>28857</v>
-      </c>
-      <c r="Q27">
-        <v>45830</v>
-      </c>
-      <c r="R27">
-        <v>25997</v>
-      </c>
-      <c r="S27">
-        <v>-14511</v>
-      </c>
-      <c r="T27">
-        <v>4169</v>
-      </c>
-      <c r="U27">
-        <v>4958</v>
-      </c>
-      <c r="V27">
-        <v>-34842</v>
-      </c>
-      <c r="W27">
-        <v>13350</v>
-      </c>
-      <c r="X27">
-        <v>5128</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3255,422 +3157,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E2">
         <v>14000</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E3">
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E4">
         <v>96380</v>
       </c>
       <c r="F4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E5">
         <v>21000</v>
       </c>
       <c r="F5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E6">
         <v>64350</v>
       </c>
       <c r="F6" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E7">
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E8">
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E9">
         <v>14250</v>
       </c>
       <c r="F9" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E10">
         <v>16000</v>
       </c>
       <c r="F10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D11" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="E11">
         <v>13500</v>
       </c>
       <c r="F11" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D12" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E12">
         <v>14950</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E13">
         <v>29547</v>
       </c>
       <c r="F13" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E14">
         <v>18040</v>
       </c>
       <c r="F14" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D15" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E15">
         <v>22100</v>
       </c>
       <c r="F15" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E16">
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C17" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D17" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E17">
         <v>60654</v>
       </c>
       <c r="F17" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E18">
         <v>26800</v>
       </c>
       <c r="F18" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E19">
         <v>524031</v>
       </c>
       <c r="F19" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E20">
         <v>6384</v>
       </c>
       <c r="F20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E21">
         <v>8000</v>
       </c>
       <c r="F21" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-28
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="258">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2023-11-07</t>
+  </si>
+  <si>
     <t>2023-11-03</t>
   </si>
   <si>
@@ -152,6 +155,9 @@
     <t>2023-09-06</t>
   </si>
   <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
     <t>2023-11-09</t>
   </si>
   <si>
@@ -161,9 +167,6 @@
     <t>2023-11-08</t>
   </si>
   <si>
-    <t>2023-11-07</t>
-  </si>
-  <si>
     <t>2023-10-27</t>
   </si>
   <si>
@@ -179,6 +182,9 @@
     <t>2023-09-12</t>
   </si>
   <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
     <t>2023-11-24</t>
   </si>
   <si>
@@ -191,9 +197,6 @@
     <t>2023-11-15</t>
   </si>
   <si>
-    <t>2023-11-13</t>
-  </si>
-  <si>
     <t>2023-11-14</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
     <t>2023-10-10</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -236,15 +242,15 @@
     <t>하나</t>
   </si>
   <si>
-    <t>미래</t>
-  </si>
-  <si>
     <t>한국, 미래</t>
   </si>
   <si>
     <t>유안타</t>
   </si>
   <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
     <t>그린리소스</t>
   </si>
   <si>
@@ -320,6 +326,9 @@
     <t>아이엠티</t>
   </si>
   <si>
+    <t>629.95:1</t>
+  </si>
+  <si>
     <t>753.19:1</t>
   </si>
   <si>
@@ -395,6 +404,9 @@
     <t>753.50:1</t>
   </si>
   <si>
+    <t>8.66%</t>
+  </si>
+  <si>
     <t>5.39%</t>
   </si>
   <si>
@@ -464,6 +476,9 @@
     <t>22.20%</t>
   </si>
   <si>
+    <t>자외선 차단제 유기 원료</t>
+  </si>
+  <si>
     <t>반도체 및 디스플레이 장비 보호코팅 및 소재</t>
   </si>
   <si>
@@ -585,9 +600,6 @@
   </si>
   <si>
     <t>에이텀</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
   </si>
   <si>
     <t>동인기연(유가)</t>
@@ -1134,7 +1146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1222,76 +1234,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2">
-        <v>1640000</v>
+        <v>1407000</v>
       </c>
       <c r="G2">
-        <v>1640000</v>
+        <v>844000</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>563000</v>
       </c>
       <c r="I2">
-        <v>11000</v>
+        <v>21000</v>
       </c>
       <c r="J2">
-        <v>14000</v>
+        <v>25000</v>
       </c>
       <c r="K2">
-        <v>8183944</v>
+        <v>5657215</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>17000</v>
+        <v>28000</v>
       </c>
       <c r="N2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="P2">
-        <v>13660</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>25085</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>8905</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>3108</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>3731</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>2219</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1157</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>3465</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1666</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1299,76 +1311,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F3">
-        <v>3350000</v>
+        <v>1640000</v>
       </c>
       <c r="G3">
-        <v>3350000</v>
+        <v>1640000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="J3">
-        <v>9500</v>
+        <v>14000</v>
       </c>
       <c r="K3">
-        <v>13436499</v>
+        <v>8183944</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="P3">
-        <v>47984</v>
+        <v>13660</v>
       </c>
       <c r="Q3">
-        <v>51031</v>
+        <v>25085</v>
       </c>
       <c r="R3">
-        <v>29425</v>
+        <v>8905</v>
       </c>
       <c r="S3">
-        <v>10526</v>
+        <v>3108</v>
       </c>
       <c r="T3">
-        <v>11804</v>
+        <v>3731</v>
       </c>
       <c r="U3">
-        <v>7008</v>
+        <v>2219</v>
       </c>
       <c r="V3">
-        <v>8661</v>
+        <v>1157</v>
       </c>
       <c r="W3">
-        <v>9582</v>
+        <v>3465</v>
       </c>
       <c r="X3">
-        <v>5612</v>
+        <v>1666</v>
       </c>
       <c r="Y3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1376,76 +1388,76 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F4">
-        <v>4250000</v>
+        <v>3350000</v>
       </c>
       <c r="G4">
-        <v>4250000</v>
+        <v>3350000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>5200</v>
+        <v>8000</v>
       </c>
       <c r="J4">
-        <v>6000</v>
+        <v>9500</v>
       </c>
       <c r="K4">
-        <v>17002500</v>
+        <v>13436499</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="N4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="P4">
-        <v>27199897007</v>
+        <v>47984</v>
       </c>
       <c r="Q4">
-        <v>40971122327</v>
+        <v>51031</v>
       </c>
       <c r="R4">
-        <v>25300714406</v>
+        <v>29425</v>
       </c>
       <c r="S4">
-        <v>2887034102</v>
+        <v>10526</v>
       </c>
       <c r="T4">
-        <v>7167697077</v>
+        <v>11804</v>
       </c>
       <c r="U4">
-        <v>4740280453</v>
+        <v>7008</v>
       </c>
       <c r="V4">
-        <v>2399514033</v>
+        <v>8661</v>
       </c>
       <c r="W4">
-        <v>5498221693</v>
+        <v>9582</v>
       </c>
       <c r="X4">
-        <v>3402334635</v>
+        <v>5612</v>
       </c>
       <c r="Y4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1453,76 +1465,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5">
-        <v>2079000</v>
+        <v>4250000</v>
       </c>
       <c r="G5">
-        <v>2079000</v>
+        <v>4250000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>28500</v>
+        <v>5200</v>
       </c>
       <c r="J5">
-        <v>34700</v>
+        <v>6000</v>
       </c>
       <c r="K5">
-        <v>9877043</v>
+        <v>17002500</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>34700</v>
+        <v>7000</v>
       </c>
       <c r="N5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="P5">
-        <v>26994234332</v>
+        <v>27199897007</v>
       </c>
       <c r="Q5">
-        <v>60121142197</v>
+        <v>40971122327</v>
       </c>
       <c r="R5">
-        <v>53305665235</v>
+        <v>25300714406</v>
       </c>
       <c r="S5">
-        <v>10162848799</v>
+        <v>2887034102</v>
       </c>
       <c r="T5">
-        <v>20033029594</v>
+        <v>7167697077</v>
       </c>
       <c r="U5">
-        <v>19806683734</v>
+        <v>4740280453</v>
       </c>
       <c r="V5">
-        <v>7996520497</v>
+        <v>2399514033</v>
       </c>
       <c r="W5">
-        <v>15559454518</v>
+        <v>5498221693</v>
       </c>
       <c r="X5">
-        <v>15932218050</v>
+        <v>3402334635</v>
       </c>
       <c r="Y5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1530,76 +1542,76 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6">
-        <v>1596000</v>
+        <v>2079000</v>
       </c>
       <c r="G6">
-        <v>1596000</v>
+        <v>2079000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>3200</v>
+        <v>28500</v>
       </c>
       <c r="J6">
-        <v>3600</v>
+        <v>34700</v>
       </c>
       <c r="K6">
-        <v>13346380</v>
+        <v>9877043</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>4000</v>
+        <v>34700</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="P6">
-        <v>7668281979</v>
+        <v>26994234332</v>
       </c>
       <c r="Q6">
-        <v>7100921456</v>
+        <v>60121142197</v>
       </c>
       <c r="R6">
-        <v>1207846478</v>
+        <v>53305665235</v>
       </c>
       <c r="S6">
-        <v>5659403971</v>
+        <v>10162848799</v>
       </c>
       <c r="T6">
-        <v>6124121466</v>
+        <v>20033029594</v>
       </c>
       <c r="U6">
-        <v>940668827</v>
+        <v>19806683734</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>7996520497</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>15559454518</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>15932218050</v>
       </c>
       <c r="Y6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1610,73 +1622,73 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F7">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="G7">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>29800</v>
+        <v>3200</v>
       </c>
       <c r="J7">
-        <v>33500</v>
+        <v>3600</v>
       </c>
       <c r="K7">
-        <v>13612736</v>
+        <v>13346380</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>7668281979</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>7100921456</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1207846478</v>
       </c>
       <c r="S7">
-        <v>-15286512079</v>
+        <v>5659403971</v>
       </c>
       <c r="T7">
-        <v>-21424611321</v>
+        <v>6124121466</v>
       </c>
       <c r="U7">
-        <v>-139745251263</v>
+        <v>940668827</v>
       </c>
       <c r="V7">
-        <v>-53575668634</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>-38885125426</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>-12610702106</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1684,76 +1696,76 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F8">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="G8">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>19100</v>
+        <v>29800</v>
       </c>
       <c r="J8">
-        <v>21400</v>
+        <v>33500</v>
       </c>
       <c r="K8">
-        <v>10585320</v>
+        <v>13612736</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="P8">
-        <v>45195788</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>69629209</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>35634471</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>2751277</v>
+        <v>-15286512079</v>
       </c>
       <c r="T8">
-        <v>11449731</v>
+        <v>-21424611321</v>
       </c>
       <c r="U8">
-        <v>2482194</v>
+        <v>-139745251263</v>
       </c>
       <c r="V8">
-        <v>2092692</v>
+        <v>-53575668634</v>
       </c>
       <c r="W8">
-        <v>5149538</v>
+        <v>-38885125426</v>
       </c>
       <c r="X8">
-        <v>2327401</v>
+        <v>-12610702106</v>
       </c>
       <c r="Y8" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1761,384 +1773,384 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F9">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="G9">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>19100</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>21400</v>
       </c>
       <c r="K9">
-        <v>4320000</v>
+        <v>10585320</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="O9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>45195788</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>69629209</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>35634471</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>2751277</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>11449731</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>2482194</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>2092692</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>5149538</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>2327401</v>
       </c>
       <c r="Y9" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F10">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="G10">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K10">
-        <v>30610000</v>
+        <v>4320000</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="O10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="P10">
-        <v>67332006578</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>100050838794</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>63366010569</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>1140243099</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>8333440685</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <v>7415958936</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>668088159</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>5930478364</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>5666583221</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="G11">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>3500</v>
+        <v>1200</v>
       </c>
       <c r="J11">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="K11">
-        <v>20771000</v>
+        <v>30610000</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="O11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="P11">
-        <v>39450601</v>
+        <v>67332006578</v>
       </c>
       <c r="Q11">
-        <v>49044883</v>
+        <v>100050838794</v>
       </c>
       <c r="R11">
-        <v>21826468</v>
+        <v>63366010569</v>
       </c>
       <c r="S11">
-        <v>2477559</v>
+        <v>1140243099</v>
       </c>
       <c r="T11">
-        <v>8094900</v>
+        <v>8333440685</v>
       </c>
       <c r="U11">
-        <v>215154</v>
+        <v>7415958936</v>
       </c>
       <c r="V11">
-        <v>3427734</v>
+        <v>668088159</v>
       </c>
       <c r="W11">
-        <v>6575528</v>
+        <v>5930478364</v>
       </c>
       <c r="X11">
-        <v>349843</v>
+        <v>5666583221</v>
       </c>
       <c r="Y11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
         <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F12">
-        <v>2060000</v>
+        <v>5200000</v>
       </c>
       <c r="G12">
-        <v>2000000</v>
+        <v>5200000</v>
       </c>
       <c r="H12">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>20300</v>
+        <v>3500</v>
       </c>
       <c r="J12">
-        <v>22500</v>
+        <v>4000</v>
       </c>
       <c r="K12">
-        <v>14384224</v>
+        <v>20771000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="O12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="P12">
-        <v>5787300240</v>
+        <v>39450601</v>
       </c>
       <c r="Q12">
-        <v>1914633847</v>
+        <v>49044883</v>
       </c>
       <c r="R12">
-        <v>3156092272</v>
+        <v>21826468</v>
       </c>
       <c r="S12">
-        <v>-1798278694</v>
+        <v>2477559</v>
       </c>
       <c r="T12">
-        <v>-1453689952</v>
+        <v>8094900</v>
       </c>
       <c r="U12">
-        <v>-4067648306</v>
+        <v>215154</v>
       </c>
       <c r="V12">
-        <v>-12449932055</v>
+        <v>3427734</v>
       </c>
       <c r="W12">
-        <v>-7426231074</v>
+        <v>6575528</v>
       </c>
       <c r="X12">
-        <v>-52132058866</v>
+        <v>349843</v>
       </c>
       <c r="Y12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F13">
-        <v>1200000</v>
+        <v>2060000</v>
       </c>
       <c r="G13">
-        <v>1200000</v>
+        <v>2000000</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I13">
-        <v>9100</v>
+        <v>20300</v>
       </c>
       <c r="J13">
-        <v>11000</v>
+        <v>22500</v>
       </c>
       <c r="K13">
-        <v>7206940</v>
+        <v>14384224</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O13" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="P13">
-        <v>20924</v>
+        <v>5787300240</v>
       </c>
       <c r="Q13">
-        <v>27659</v>
+        <v>1914633847</v>
       </c>
       <c r="R13">
-        <v>11818</v>
+        <v>3156092272</v>
       </c>
       <c r="S13">
-        <v>2838</v>
+        <v>-1798278694</v>
       </c>
       <c r="T13">
-        <v>4563</v>
+        <v>-1453689952</v>
       </c>
       <c r="U13">
-        <v>-1222</v>
+        <v>-4067648306</v>
       </c>
       <c r="V13">
-        <v>2413</v>
+        <v>-12449932055</v>
       </c>
       <c r="W13">
-        <v>3190</v>
+        <v>-7426231074</v>
       </c>
       <c r="X13">
-        <v>-862</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y13" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2146,230 +2158,230 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F14">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="G14">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>5000</v>
+        <v>9100</v>
       </c>
       <c r="J14">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="K14">
-        <v>17306490</v>
+        <v>7206940</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="O14" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="P14">
-        <v>21976760922</v>
+        <v>20924</v>
       </c>
       <c r="Q14">
-        <v>15839004968</v>
+        <v>27659</v>
       </c>
       <c r="R14">
-        <v>6887755932</v>
+        <v>11818</v>
       </c>
       <c r="S14">
-        <v>-2217897363</v>
+        <v>2838</v>
       </c>
       <c r="T14">
-        <v>-3403228196</v>
+        <v>4563</v>
       </c>
       <c r="U14">
-        <v>-2758864194</v>
+        <v>-1222</v>
       </c>
       <c r="V14">
-        <v>-5110677395</v>
+        <v>2413</v>
       </c>
       <c r="W14">
-        <v>-29510193610</v>
+        <v>3190</v>
       </c>
       <c r="X14">
-        <v>-2514471056</v>
+        <v>-862</v>
       </c>
       <c r="Y14" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F15">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="G15">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K15">
-        <v>12905000</v>
+        <v>17306490</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="O15" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>21976760922</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>15839004968</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>6887755932</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>-2217897363</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>-3403228196</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>-2758864194</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>-5110677395</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>-29510193610</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y15" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F16">
-        <v>1049482</v>
+        <v>12500000</v>
       </c>
       <c r="G16">
-        <v>944534</v>
+        <v>12500000</v>
       </c>
       <c r="H16">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>12800</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="K16">
-        <v>6261485</v>
+        <v>12905000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="O16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P16">
-        <v>34557425427</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>39824841246</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>23231897516</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>3011651602</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>2384643399</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>4436005255</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>2755379556</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>1176755354</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>4046949430</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2377,76 +2389,76 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17">
-        <v>1128720</v>
+        <v>1049482</v>
       </c>
       <c r="G17">
-        <v>1128720</v>
+        <v>944534</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I17">
-        <v>3300</v>
+        <v>12800</v>
       </c>
       <c r="J17">
-        <v>3900</v>
+        <v>14500</v>
       </c>
       <c r="K17">
-        <v>11287196</v>
+        <v>6261485</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="O17" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P17">
-        <v>50552623684</v>
+        <v>34557425427</v>
       </c>
       <c r="Q17">
-        <v>69013134090</v>
+        <v>39824841246</v>
       </c>
       <c r="R17">
-        <v>16887814423</v>
+        <v>23231897516</v>
       </c>
       <c r="S17">
-        <v>9027232647</v>
+        <v>3011651602</v>
       </c>
       <c r="T17">
-        <v>15707796256</v>
+        <v>2384643399</v>
       </c>
       <c r="U17">
-        <v>555562560</v>
+        <v>4436005255</v>
       </c>
       <c r="V17">
-        <v>9236341465</v>
+        <v>2755379556</v>
       </c>
       <c r="W17">
-        <v>13159994846</v>
+        <v>1176755354</v>
       </c>
       <c r="X17">
-        <v>1236029732</v>
+        <v>4046949430</v>
       </c>
       <c r="Y17" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2454,76 +2466,76 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F18">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="G18">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>13000</v>
+        <v>3300</v>
       </c>
       <c r="J18">
-        <v>15000</v>
+        <v>3900</v>
       </c>
       <c r="K18">
-        <v>10193520</v>
+        <v>11287196</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="O18" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="P18">
-        <v>3952070068</v>
+        <v>50552623684</v>
       </c>
       <c r="Q18">
-        <v>10789274729</v>
+        <v>69013134090</v>
       </c>
       <c r="R18">
-        <v>6040367765</v>
+        <v>16887814423</v>
       </c>
       <c r="S18">
-        <v>-4741577598</v>
+        <v>9027232647</v>
       </c>
       <c r="T18">
-        <v>-3671026788</v>
+        <v>15707796256</v>
       </c>
       <c r="U18">
-        <v>-3292521363</v>
+        <v>555562560</v>
       </c>
       <c r="V18">
-        <v>-3654889267</v>
+        <v>9236341465</v>
       </c>
       <c r="W18">
-        <v>-2281074471</v>
+        <v>13159994846</v>
       </c>
       <c r="X18">
-        <v>-2539505707</v>
+        <v>1236029732</v>
       </c>
       <c r="Y18" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2531,76 +2543,76 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F19">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="G19">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J19">
-        <v>5600</v>
+        <v>15000</v>
       </c>
       <c r="K19">
-        <v>16120000</v>
+        <v>10193520</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="O19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="P19">
-        <v>26691070764</v>
+        <v>3952070068</v>
       </c>
       <c r="Q19">
-        <v>22835113396</v>
+        <v>10789274729</v>
       </c>
       <c r="R19">
-        <v>7519073723</v>
+        <v>6040367765</v>
       </c>
       <c r="S19">
-        <v>6041270235</v>
+        <v>-4741577598</v>
       </c>
       <c r="T19">
-        <v>6705120210</v>
+        <v>-3671026788</v>
       </c>
       <c r="U19">
-        <v>982044017</v>
+        <v>-3292521363</v>
       </c>
       <c r="V19">
-        <v>5119066139</v>
+        <v>-3654889267</v>
       </c>
       <c r="W19">
-        <v>5870093710</v>
+        <v>-2281074471</v>
       </c>
       <c r="X19">
-        <v>1198587470</v>
+        <v>-2539505707</v>
       </c>
       <c r="Y19" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2608,76 +2620,76 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="G20">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>8200</v>
+        <v>5000</v>
       </c>
       <c r="J20">
-        <v>9400</v>
+        <v>5600</v>
       </c>
       <c r="K20">
-        <v>7674103</v>
+        <v>16120000</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N20" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="O20" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="P20">
-        <v>8242508010</v>
+        <v>26691070764</v>
       </c>
       <c r="Q20">
-        <v>10751900430</v>
+        <v>22835113396</v>
       </c>
       <c r="R20">
-        <v>4416778965</v>
+        <v>7519073723</v>
       </c>
       <c r="S20">
-        <v>426234451</v>
+        <v>6041270235</v>
       </c>
       <c r="T20">
-        <v>2423749751</v>
+        <v>6705120210</v>
       </c>
       <c r="U20">
-        <v>677048172</v>
+        <v>982044017</v>
       </c>
       <c r="V20">
-        <v>57890953</v>
+        <v>5119066139</v>
       </c>
       <c r="W20">
-        <v>2826043673</v>
+        <v>5870093710</v>
       </c>
       <c r="X20">
-        <v>990121873</v>
+        <v>1198587470</v>
       </c>
       <c r="Y20" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2685,76 +2697,76 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F21">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="G21">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>22000</v>
+        <v>8200</v>
       </c>
       <c r="J21">
-        <v>25000</v>
+        <v>9400</v>
       </c>
       <c r="K21">
-        <v>9039778</v>
+        <v>7674103</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N21" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O21" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="P21">
-        <v>104225113285</v>
+        <v>8242508010</v>
       </c>
       <c r="Q21">
-        <v>106505634411</v>
+        <v>10751900430</v>
       </c>
       <c r="R21">
-        <v>66424930568</v>
+        <v>4416778965</v>
       </c>
       <c r="S21">
-        <v>6291020806</v>
+        <v>426234451</v>
       </c>
       <c r="T21">
-        <v>7893242769</v>
+        <v>2423749751</v>
       </c>
       <c r="U21">
-        <v>7661497240</v>
+        <v>677048172</v>
       </c>
       <c r="V21">
-        <v>7319368873</v>
+        <v>57890953</v>
       </c>
       <c r="W21">
-        <v>9286891982</v>
+        <v>2826043673</v>
       </c>
       <c r="X21">
-        <v>7334816490</v>
+        <v>990121873</v>
       </c>
       <c r="Y21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2765,31 +2777,31 @@
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F22">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="G22">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>21000</v>
+        <v>22000</v>
       </c>
       <c r="J22">
-        <v>26000</v>
+        <v>25000</v>
       </c>
       <c r="K22">
-        <v>64819980</v>
+        <v>9039778</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2798,40 +2810,40 @@
         <v>26000</v>
       </c>
       <c r="N22" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="O22" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="P22">
-        <v>36980</v>
+        <v>104225113285</v>
       </c>
       <c r="Q22">
-        <v>44954</v>
+        <v>106505634411</v>
       </c>
       <c r="R22">
-        <v>23652</v>
+        <v>66424930568</v>
       </c>
       <c r="S22">
-        <v>-7085</v>
+        <v>6291020806</v>
       </c>
       <c r="T22">
-        <v>-13228</v>
+        <v>7893242769</v>
       </c>
       <c r="U22">
-        <v>-9932</v>
+        <v>7661497240</v>
       </c>
       <c r="V22">
-        <v>-7417</v>
+        <v>7319368873</v>
       </c>
       <c r="W22">
-        <v>-12548</v>
+        <v>9286891982</v>
       </c>
       <c r="X22">
-        <v>-9333</v>
+        <v>7334816490</v>
       </c>
       <c r="Y22" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2839,76 +2851,76 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F23">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="G23">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J23">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K23">
-        <v>18905000</v>
+        <v>64819980</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O23" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>36980</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>44954</v>
       </c>
       <c r="R23">
-        <v>0</v>
+        <v>23652</v>
       </c>
       <c r="S23">
-        <v>0</v>
+        <v>-7085</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>-13228</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>-9932</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>-7417</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>-12548</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>-9333</v>
       </c>
       <c r="Y23" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2916,230 +2928,307 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="G24">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J24">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K24">
-        <v>5447675</v>
+        <v>18905000</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="O24" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P24">
-        <v>18408761227</v>
+        <v>0</v>
       </c>
       <c r="Q24">
-        <v>21902816604</v>
+        <v>0</v>
       </c>
       <c r="R24">
-        <v>8176918465</v>
+        <v>0</v>
       </c>
       <c r="S24">
-        <v>3669182465</v>
+        <v>0</v>
       </c>
       <c r="T24">
-        <v>1851925471</v>
+        <v>0</v>
       </c>
       <c r="U24">
-        <v>590566592</v>
+        <v>0</v>
       </c>
       <c r="V24">
-        <v>3633973594</v>
+        <v>0</v>
       </c>
       <c r="W24">
-        <v>2205418963</v>
+        <v>0</v>
       </c>
       <c r="X24">
-        <v>592903151</v>
+        <v>0</v>
       </c>
       <c r="Y24" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F25">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="G25">
-        <v>1640000</v>
+        <v>1500000</v>
       </c>
       <c r="H25">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J25">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K25">
-        <v>10969386</v>
+        <v>5447675</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N25" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O25" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="P25">
-        <v>22818451349</v>
+        <v>18408761227</v>
       </c>
       <c r="Q25">
-        <v>30491967755</v>
+        <v>21902816604</v>
       </c>
       <c r="R25">
-        <v>18040053709</v>
+        <v>8176918465</v>
       </c>
       <c r="S25">
-        <v>2313787613</v>
+        <v>3669182465</v>
       </c>
       <c r="T25">
-        <v>4014101926</v>
+        <v>1851925471</v>
       </c>
       <c r="U25">
-        <v>1878997667</v>
+        <v>590566592</v>
       </c>
       <c r="V25">
-        <v>559427078</v>
+        <v>3633973594</v>
       </c>
       <c r="W25">
-        <v>-711183147</v>
+        <v>2205418963</v>
       </c>
       <c r="X25">
-        <v>1929682988</v>
+        <v>592903151</v>
       </c>
       <c r="Y25" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F26">
+        <v>2240000</v>
+      </c>
+      <c r="G26">
+        <v>1640000</v>
+      </c>
+      <c r="H26">
+        <v>600000</v>
+      </c>
+      <c r="I26">
+        <v>11500</v>
+      </c>
+      <c r="J26">
+        <v>13200</v>
+      </c>
+      <c r="K26">
+        <v>10969386</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>15000</v>
+      </c>
+      <c r="N26" t="s">
+        <v>127</v>
+      </c>
+      <c r="O26" t="s">
+        <v>151</v>
+      </c>
+      <c r="P26">
+        <v>22818451349</v>
+      </c>
+      <c r="Q26">
+        <v>30491967755</v>
+      </c>
+      <c r="R26">
+        <v>18040053709</v>
+      </c>
+      <c r="S26">
+        <v>2313787613</v>
+      </c>
+      <c r="T26">
+        <v>4014101926</v>
+      </c>
+      <c r="U26">
+        <v>1878997667</v>
+      </c>
+      <c r="V26">
+        <v>559427078</v>
+      </c>
+      <c r="W26">
+        <v>-711183147</v>
+      </c>
+      <c r="X26">
+        <v>1929682988</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27">
         <v>1580000</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>1580000</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
         <v>10500</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <v>12000</v>
       </c>
-      <c r="K26">
+      <c r="K27">
         <v>7874611</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>14000</v>
       </c>
-      <c r="N26" t="s">
-        <v>125</v>
-      </c>
-      <c r="O26" t="s">
-        <v>148</v>
-      </c>
-      <c r="P26">
+      <c r="N27" t="s">
+        <v>128</v>
+      </c>
+      <c r="O27" t="s">
+        <v>152</v>
+      </c>
+      <c r="P27">
         <v>7327878427</v>
       </c>
-      <c r="Q26">
+      <c r="Q27">
         <v>10756717708</v>
       </c>
-      <c r="R26">
+      <c r="R27">
         <v>4113702647</v>
       </c>
-      <c r="S26">
+      <c r="S27">
         <v>-588932080</v>
       </c>
-      <c r="T26">
+      <c r="T27">
         <v>254042570</v>
       </c>
-      <c r="U26">
+      <c r="U27">
         <v>-738698858</v>
       </c>
-      <c r="V26">
+      <c r="V27">
         <v>-569358529</v>
       </c>
-      <c r="W26">
+      <c r="W27">
         <v>-429546963</v>
       </c>
-      <c r="X26">
+      <c r="X27">
         <v>-550600734</v>
       </c>
-      <c r="Y26" t="s">
-        <v>172</v>
+      <c r="Y27" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3157,422 +3246,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E2">
         <v>14000</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E3">
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E4">
         <v>96380</v>
       </c>
       <c r="F4" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E5">
         <v>21000</v>
       </c>
       <c r="F5" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E6">
         <v>64350</v>
       </c>
       <c r="F6" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E7">
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E8">
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E9">
         <v>14250</v>
       </c>
       <c r="F9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E10">
         <v>16000</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D11" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E11">
         <v>13500</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E12">
         <v>14950</v>
       </c>
       <c r="F12" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E13">
         <v>29547</v>
       </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E14">
         <v>18040</v>
       </c>
       <c r="F14" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D15" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E15">
         <v>22100</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E16">
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E17">
         <v>60654</v>
       </c>
       <c r="F17" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E18">
         <v>26800</v>
       </c>
       <c r="F18" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D19" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E19">
         <v>524031</v>
       </c>
       <c r="F19" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E20">
         <v>6384</v>
       </c>
       <c r="F20" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D21" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E21">
         <v>8000</v>
       </c>
       <c r="F21" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-01
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="266">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,12 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2023-11-09</t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
     <t>2023-11-07</t>
   </si>
   <si>
@@ -155,12 +161,12 @@
     <t>2023-09-06</t>
   </si>
   <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
     <t>2023-11-13</t>
   </si>
   <si>
-    <t>2023-11-09</t>
-  </si>
-  <si>
     <t>2023-11-06</t>
   </si>
   <si>
@@ -182,6 +188,9 @@
     <t>2023-09-12</t>
   </si>
   <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
     <t>2023-11-28</t>
   </si>
   <si>
@@ -194,9 +203,6 @@
     <t>2023-11-21</t>
   </si>
   <si>
-    <t>2023-11-15</t>
-  </si>
-  <si>
     <t>2023-11-14</t>
   </si>
   <si>
@@ -206,12 +212,15 @@
     <t>2023-10-10</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>하이</t>
   </si>
   <si>
@@ -239,15 +248,18 @@
     <t>키움</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>한국, 미래</t>
   </si>
   <si>
     <t>유안타</t>
   </si>
   <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
     <t>에이에스텍</t>
   </si>
   <si>
@@ -326,6 +338,12 @@
     <t>아이엠티</t>
   </si>
   <si>
+    <t>136.4:1</t>
+  </si>
+  <si>
+    <t>52.70:1</t>
+  </si>
+  <si>
     <t>629.95:1</t>
   </si>
   <si>
@@ -404,6 +422,12 @@
     <t>753.50:1</t>
   </si>
   <si>
+    <t>0.43%</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>8.66%</t>
   </si>
   <si>
@@ -428,9 +452,6 @@
     <t>22.38%</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>6.69%</t>
   </si>
   <si>
@@ -476,6 +497,12 @@
     <t>22.20%</t>
   </si>
   <si>
+    <t>평판형 트랜스</t>
+  </si>
+  <si>
+    <t>금융지원서비스업</t>
+  </si>
+  <si>
     <t>자외선 차단제 유기 원료</t>
   </si>
   <si>
@@ -569,12 +596,12 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>포스뱅크</t>
+  </si>
+  <si>
     <t>하나스팩30호</t>
   </si>
   <si>
-    <t>키움스팩9호</t>
-  </si>
-  <si>
     <t>디에스단석(구,단석산업)</t>
   </si>
   <si>
@@ -599,9 +626,6 @@
     <t>와이바이오로직스</t>
   </si>
   <si>
-    <t>에이텀</t>
-  </si>
-  <si>
     <t>동인기연(유가)</t>
   </si>
   <si>
@@ -611,12 +635,12 @@
     <t>한국스팩13호</t>
   </si>
   <si>
+    <t>2024.01.05~01.11</t>
+  </si>
+  <si>
     <t>2023.12.08~12.11</t>
   </si>
   <si>
-    <t>2023.12.07~12.08</t>
-  </si>
-  <si>
     <t>2023.12.05~12.11</t>
   </si>
   <si>
@@ -662,6 +686,9 @@
     <t>2023.10.25~10.26</t>
   </si>
   <si>
+    <t>13,000~15,000</t>
+  </si>
+  <si>
     <t>2,000~2,000</t>
   </si>
   <si>
@@ -744,9 +771,6 @@
   </si>
   <si>
     <t>하나증권</t>
-  </si>
-  <si>
-    <t>키움증권</t>
   </si>
   <si>
     <t>KB증권,NH투자증권</t>
@@ -1146,7 +1170,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1234,76 +1258,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2">
-        <v>1407000</v>
+        <v>650000</v>
       </c>
       <c r="G2">
-        <v>844000</v>
+        <v>650000</v>
       </c>
       <c r="H2">
-        <v>563000</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>21000</v>
+        <v>23000</v>
       </c>
       <c r="J2">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="K2">
-        <v>5657215</v>
+        <v>5345180</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>28000</v>
+        <v>18000</v>
       </c>
       <c r="N2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>55809022</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>53633878</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>47971262</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>-4601725</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>-7645858</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>-5922868</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>-20523948</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>-12027347</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>-8387901</v>
       </c>
       <c r="Y2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1311,76 +1335,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F3">
-        <v>1640000</v>
+        <v>8000000</v>
       </c>
       <c r="G3">
-        <v>1640000</v>
+        <v>8000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>8183944</v>
+        <v>9100000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="O3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="P3">
-        <v>13660</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>25085</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>8905</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>3108</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>3731</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>2219</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1157</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>3465</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>1666</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1388,76 +1412,76 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F4">
-        <v>3350000</v>
+        <v>1407000</v>
       </c>
       <c r="G4">
-        <v>3350000</v>
+        <v>844000</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>563000</v>
       </c>
       <c r="I4">
-        <v>8000</v>
+        <v>21000</v>
       </c>
       <c r="J4">
-        <v>9500</v>
+        <v>25000</v>
       </c>
       <c r="K4">
-        <v>13436499</v>
+        <v>5657215</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>11000</v>
+        <v>28000</v>
       </c>
       <c r="N4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="O4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="P4">
-        <v>47984</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>51031</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>29425</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>10526</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>11804</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>7008</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>8661</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>9582</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>5612</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1465,76 +1489,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F5">
-        <v>4250000</v>
+        <v>1640000</v>
       </c>
       <c r="G5">
-        <v>4250000</v>
+        <v>1640000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>5200</v>
+        <v>11000</v>
       </c>
       <c r="J5">
-        <v>6000</v>
+        <v>14000</v>
       </c>
       <c r="K5">
-        <v>17002500</v>
+        <v>8183944</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="P5">
-        <v>27199897007</v>
+        <v>13660</v>
       </c>
       <c r="Q5">
-        <v>40971122327</v>
+        <v>25085</v>
       </c>
       <c r="R5">
-        <v>25300714406</v>
+        <v>8905</v>
       </c>
       <c r="S5">
-        <v>2887034102</v>
+        <v>3108</v>
       </c>
       <c r="T5">
-        <v>7167697077</v>
+        <v>3731</v>
       </c>
       <c r="U5">
-        <v>4740280453</v>
+        <v>2219</v>
       </c>
       <c r="V5">
-        <v>2399514033</v>
+        <v>1157</v>
       </c>
       <c r="W5">
-        <v>5498221693</v>
+        <v>3465</v>
       </c>
       <c r="X5">
-        <v>3402334635</v>
+        <v>1666</v>
       </c>
       <c r="Y5" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1542,76 +1566,76 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6">
-        <v>2079000</v>
+        <v>3350000</v>
       </c>
       <c r="G6">
-        <v>2079000</v>
+        <v>3350000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>28500</v>
+        <v>8000</v>
       </c>
       <c r="J6">
-        <v>34700</v>
+        <v>9500</v>
       </c>
       <c r="K6">
-        <v>9877043</v>
+        <v>13436499</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>34700</v>
+        <v>11000</v>
       </c>
       <c r="N6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="O6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="P6">
-        <v>26994234332</v>
+        <v>47984</v>
       </c>
       <c r="Q6">
-        <v>60121142197</v>
+        <v>51031</v>
       </c>
       <c r="R6">
-        <v>53305665235</v>
+        <v>29425</v>
       </c>
       <c r="S6">
-        <v>10162848799</v>
+        <v>10526</v>
       </c>
       <c r="T6">
-        <v>20033029594</v>
+        <v>11804</v>
       </c>
       <c r="U6">
-        <v>19806683734</v>
+        <v>7008</v>
       </c>
       <c r="V6">
-        <v>7996520497</v>
+        <v>8661</v>
       </c>
       <c r="W6">
-        <v>15559454518</v>
+        <v>9582</v>
       </c>
       <c r="X6">
-        <v>15932218050</v>
+        <v>5612</v>
       </c>
       <c r="Y6" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1619,76 +1643,76 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7">
-        <v>1596000</v>
+        <v>4250000</v>
       </c>
       <c r="G7">
-        <v>1596000</v>
+        <v>4250000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>3200</v>
+        <v>5200</v>
       </c>
       <c r="J7">
-        <v>3600</v>
+        <v>6000</v>
       </c>
       <c r="K7">
-        <v>13346380</v>
+        <v>17002500</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>4000</v>
+        <v>7000</v>
       </c>
       <c r="N7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="O7" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="P7">
-        <v>7668281979</v>
+        <v>27199897007</v>
       </c>
       <c r="Q7">
-        <v>7100921456</v>
+        <v>40971122327</v>
       </c>
       <c r="R7">
-        <v>1207846478</v>
+        <v>25300714406</v>
       </c>
       <c r="S7">
-        <v>5659403971</v>
+        <v>2887034102</v>
       </c>
       <c r="T7">
-        <v>6124121466</v>
+        <v>7167697077</v>
       </c>
       <c r="U7">
-        <v>940668827</v>
+        <v>4740280453</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>2399514033</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>5498221693</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>3402334635</v>
       </c>
       <c r="Y7" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1696,76 +1720,76 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F8">
-        <v>1600000</v>
+        <v>2079000</v>
       </c>
       <c r="G8">
-        <v>1600000</v>
+        <v>2079000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>29800</v>
+        <v>28500</v>
       </c>
       <c r="J8">
-        <v>33500</v>
+        <v>34700</v>
       </c>
       <c r="K8">
-        <v>13612736</v>
+        <v>9877043</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>20000</v>
+        <v>34700</v>
       </c>
       <c r="N8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O8" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>26994234332</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>60121142197</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>53305665235</v>
       </c>
       <c r="S8">
-        <v>-15286512079</v>
+        <v>10162848799</v>
       </c>
       <c r="T8">
-        <v>-21424611321</v>
+        <v>20033029594</v>
       </c>
       <c r="U8">
-        <v>-139745251263</v>
+        <v>19806683734</v>
       </c>
       <c r="V8">
-        <v>-53575668634</v>
+        <v>7996520497</v>
       </c>
       <c r="W8">
-        <v>-38885125426</v>
+        <v>15559454518</v>
       </c>
       <c r="X8">
-        <v>-12610702106</v>
+        <v>15932218050</v>
       </c>
       <c r="Y8" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1773,76 +1797,76 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F9">
-        <v>2636330</v>
+        <v>1596000</v>
       </c>
       <c r="G9">
-        <v>2636330</v>
+        <v>1596000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>19100</v>
+        <v>3200</v>
       </c>
       <c r="J9">
-        <v>21400</v>
+        <v>3600</v>
       </c>
       <c r="K9">
-        <v>10585320</v>
+        <v>13346380</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>25000</v>
+        <v>4000</v>
       </c>
       <c r="N9" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="O9" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="P9">
-        <v>45195788</v>
+        <v>7668281979</v>
       </c>
       <c r="Q9">
-        <v>69629209</v>
+        <v>7100921456</v>
       </c>
       <c r="R9">
-        <v>35634471</v>
+        <v>1207846478</v>
       </c>
       <c r="S9">
-        <v>2751277</v>
+        <v>5659403971</v>
       </c>
       <c r="T9">
-        <v>11449731</v>
+        <v>6124121466</v>
       </c>
       <c r="U9">
-        <v>2482194</v>
+        <v>940668827</v>
       </c>
       <c r="V9">
-        <v>2092692</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>5149538</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>2327401</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1850,46 +1874,46 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F10">
-        <v>4000000</v>
+        <v>1600000</v>
       </c>
       <c r="G10">
-        <v>4000000</v>
+        <v>1600000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>29800</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>33500</v>
       </c>
       <c r="K10">
-        <v>4320000</v>
+        <v>13612736</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N10" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="O10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1901,338 +1925,338 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>-15286512079</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>-21424611321</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>-139745251263</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>-53575668634</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>-38885125426</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>-12610702106</v>
       </c>
       <c r="Y10" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F11">
-        <v>7000000</v>
+        <v>2636330</v>
       </c>
       <c r="G11">
-        <v>7000000</v>
+        <v>2636330</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1200</v>
+        <v>19100</v>
       </c>
       <c r="J11">
-        <v>1500</v>
+        <v>21400</v>
       </c>
       <c r="K11">
-        <v>30610000</v>
+        <v>10585320</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="O11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="P11">
-        <v>67332006578</v>
+        <v>45195788</v>
       </c>
       <c r="Q11">
-        <v>100050838794</v>
+        <v>69629209</v>
       </c>
       <c r="R11">
-        <v>63366010569</v>
+        <v>35634471</v>
       </c>
       <c r="S11">
-        <v>1140243099</v>
+        <v>2751277</v>
       </c>
       <c r="T11">
-        <v>8333440685</v>
+        <v>11449731</v>
       </c>
       <c r="U11">
-        <v>7415958936</v>
+        <v>2482194</v>
       </c>
       <c r="V11">
-        <v>668088159</v>
+        <v>2092692</v>
       </c>
       <c r="W11">
-        <v>5930478364</v>
+        <v>5149538</v>
       </c>
       <c r="X11">
-        <v>5666583221</v>
+        <v>2327401</v>
       </c>
       <c r="Y11" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F12">
-        <v>5200000</v>
+        <v>4000000</v>
       </c>
       <c r="G12">
-        <v>5200000</v>
+        <v>4000000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>20771000</v>
+        <v>4320000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="O12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P12">
-        <v>39450601</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>49044883</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>21826468</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>2477559</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>8094900</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>215154</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>3427734</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>6575528</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>349843</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F13">
-        <v>2060000</v>
+        <v>7000000</v>
       </c>
       <c r="G13">
-        <v>2000000</v>
+        <v>7000000</v>
       </c>
       <c r="H13">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>20300</v>
+        <v>1200</v>
       </c>
       <c r="J13">
-        <v>22500</v>
+        <v>1500</v>
       </c>
       <c r="K13">
-        <v>14384224</v>
+        <v>30610000</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N13" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="O13" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="P13">
-        <v>5787300240</v>
+        <v>67332006578</v>
       </c>
       <c r="Q13">
-        <v>1914633847</v>
+        <v>100050838794</v>
       </c>
       <c r="R13">
-        <v>3156092272</v>
+        <v>63366010569</v>
       </c>
       <c r="S13">
-        <v>-1798278694</v>
+        <v>1140243099</v>
       </c>
       <c r="T13">
-        <v>-1453689952</v>
+        <v>8333440685</v>
       </c>
       <c r="U13">
-        <v>-4067648306</v>
+        <v>7415958936</v>
       </c>
       <c r="V13">
-        <v>-12449932055</v>
+        <v>668088159</v>
       </c>
       <c r="W13">
-        <v>-7426231074</v>
+        <v>5930478364</v>
       </c>
       <c r="X13">
-        <v>-52132058866</v>
+        <v>5666583221</v>
       </c>
       <c r="Y13" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F14">
-        <v>1200000</v>
+        <v>5200000</v>
       </c>
       <c r="G14">
-        <v>1200000</v>
+        <v>5200000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>9100</v>
+        <v>3500</v>
       </c>
       <c r="J14">
-        <v>11000</v>
+        <v>4000</v>
       </c>
       <c r="K14">
-        <v>7206940</v>
+        <v>20771000</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N14" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="O14" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="P14">
-        <v>20924</v>
+        <v>39450601</v>
       </c>
       <c r="Q14">
-        <v>27659</v>
+        <v>49044883</v>
       </c>
       <c r="R14">
-        <v>11818</v>
+        <v>21826468</v>
       </c>
       <c r="S14">
-        <v>2838</v>
+        <v>2477559</v>
       </c>
       <c r="T14">
-        <v>4563</v>
+        <v>8094900</v>
       </c>
       <c r="U14">
-        <v>-1222</v>
+        <v>215154</v>
       </c>
       <c r="V14">
-        <v>2413</v>
+        <v>3427734</v>
       </c>
       <c r="W14">
-        <v>3190</v>
+        <v>6575528</v>
       </c>
       <c r="X14">
-        <v>-862</v>
+        <v>349843</v>
       </c>
       <c r="Y14" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -2241,301 +2265,301 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F15">
-        <v>3600000</v>
+        <v>2060000</v>
       </c>
       <c r="G15">
-        <v>3600000</v>
+        <v>2000000</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I15">
-        <v>5000</v>
+        <v>20300</v>
       </c>
       <c r="J15">
-        <v>7000</v>
+        <v>22500</v>
       </c>
       <c r="K15">
-        <v>17306490</v>
+        <v>14384224</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N15" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="O15" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="P15">
-        <v>21976760922</v>
+        <v>5787300240</v>
       </c>
       <c r="Q15">
-        <v>15839004968</v>
+        <v>1914633847</v>
       </c>
       <c r="R15">
-        <v>6887755932</v>
+        <v>3156092272</v>
       </c>
       <c r="S15">
-        <v>-2217897363</v>
+        <v>-1798278694</v>
       </c>
       <c r="T15">
-        <v>-3403228196</v>
+        <v>-1453689952</v>
       </c>
       <c r="U15">
-        <v>-2758864194</v>
+        <v>-4067648306</v>
       </c>
       <c r="V15">
-        <v>-5110677395</v>
+        <v>-12449932055</v>
       </c>
       <c r="W15">
-        <v>-29510193610</v>
+        <v>-7426231074</v>
       </c>
       <c r="X15">
-        <v>-2514471056</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F16">
-        <v>12500000</v>
+        <v>1200000</v>
       </c>
       <c r="G16">
-        <v>12500000</v>
+        <v>1200000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>2000</v>
+        <v>9100</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K16">
-        <v>12905000</v>
+        <v>7206940</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N16" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O16" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>20924</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>27659</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>11818</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>2838</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>4563</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>-1222</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>2413</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>3190</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>-862</v>
       </c>
       <c r="Y16" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F17">
-        <v>1049482</v>
+        <v>3600000</v>
       </c>
       <c r="G17">
-        <v>944534</v>
+        <v>3600000</v>
       </c>
       <c r="H17">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>12800</v>
+        <v>5000</v>
       </c>
       <c r="J17">
-        <v>14500</v>
+        <v>7000</v>
       </c>
       <c r="K17">
-        <v>6261485</v>
+        <v>17306490</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N17" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="O17" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="P17">
-        <v>34557425427</v>
+        <v>21976760922</v>
       </c>
       <c r="Q17">
-        <v>39824841246</v>
+        <v>15839004968</v>
       </c>
       <c r="R17">
-        <v>23231897516</v>
+        <v>6887755932</v>
       </c>
       <c r="S17">
-        <v>3011651602</v>
+        <v>-2217897363</v>
       </c>
       <c r="T17">
-        <v>2384643399</v>
+        <v>-3403228196</v>
       </c>
       <c r="U17">
-        <v>4436005255</v>
+        <v>-2758864194</v>
       </c>
       <c r="V17">
-        <v>2755379556</v>
+        <v>-5110677395</v>
       </c>
       <c r="W17">
-        <v>1176755354</v>
+        <v>-29510193610</v>
       </c>
       <c r="X17">
-        <v>4046949430</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y17" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F18">
-        <v>1128720</v>
+        <v>12500000</v>
       </c>
       <c r="G18">
-        <v>1128720</v>
+        <v>12500000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>3300</v>
+        <v>2000</v>
       </c>
       <c r="J18">
-        <v>3900</v>
+        <v>2000</v>
       </c>
       <c r="K18">
-        <v>11287196</v>
+        <v>12905000</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N18" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="O18" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="P18">
-        <v>50552623684</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>69013134090</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>16887814423</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>9027232647</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>15707796256</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>555562560</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>9236341465</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>13159994846</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>1236029732</v>
+        <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2543,34 +2567,34 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F19">
-        <v>1800000</v>
+        <v>1049482</v>
       </c>
       <c r="G19">
-        <v>1800000</v>
+        <v>944534</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I19">
-        <v>13000</v>
+        <v>12800</v>
       </c>
       <c r="J19">
-        <v>15000</v>
+        <v>14500</v>
       </c>
       <c r="K19">
-        <v>10193520</v>
+        <v>6261485</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2579,40 +2603,40 @@
         <v>17000</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="O19" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="P19">
-        <v>3952070068</v>
+        <v>34557425427</v>
       </c>
       <c r="Q19">
-        <v>10789274729</v>
+        <v>39824841246</v>
       </c>
       <c r="R19">
-        <v>6040367765</v>
+        <v>23231897516</v>
       </c>
       <c r="S19">
-        <v>-4741577598</v>
+        <v>3011651602</v>
       </c>
       <c r="T19">
-        <v>-3671026788</v>
+        <v>2384643399</v>
       </c>
       <c r="U19">
-        <v>-3292521363</v>
+        <v>4436005255</v>
       </c>
       <c r="V19">
-        <v>-3654889267</v>
+        <v>2755379556</v>
       </c>
       <c r="W19">
-        <v>-2281074471</v>
+        <v>1176755354</v>
       </c>
       <c r="X19">
-        <v>-2539505707</v>
+        <v>4046949430</v>
       </c>
       <c r="Y19" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2626,70 +2650,70 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F20">
-        <v>4000000</v>
+        <v>1128720</v>
       </c>
       <c r="G20">
-        <v>4000000</v>
+        <v>1128720</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>5000</v>
+        <v>3300</v>
       </c>
       <c r="J20">
-        <v>5600</v>
+        <v>3900</v>
       </c>
       <c r="K20">
-        <v>16120000</v>
+        <v>11287196</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N20" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="P20">
-        <v>26691070764</v>
+        <v>50552623684</v>
       </c>
       <c r="Q20">
-        <v>22835113396</v>
+        <v>69013134090</v>
       </c>
       <c r="R20">
-        <v>7519073723</v>
+        <v>16887814423</v>
       </c>
       <c r="S20">
-        <v>6041270235</v>
+        <v>9027232647</v>
       </c>
       <c r="T20">
-        <v>6705120210</v>
+        <v>15707796256</v>
       </c>
       <c r="U20">
-        <v>982044017</v>
+        <v>555562560</v>
       </c>
       <c r="V20">
-        <v>5119066139</v>
+        <v>9236341465</v>
       </c>
       <c r="W20">
-        <v>5870093710</v>
+        <v>13159994846</v>
       </c>
       <c r="X20">
-        <v>1198587470</v>
+        <v>1236029732</v>
       </c>
       <c r="Y20" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2697,76 +2721,76 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F21">
-        <v>770000</v>
+        <v>1800000</v>
       </c>
       <c r="G21">
-        <v>770000</v>
+        <v>1800000</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>8200</v>
+        <v>13000</v>
       </c>
       <c r="J21">
-        <v>9400</v>
+        <v>15000</v>
       </c>
       <c r="K21">
-        <v>7674103</v>
+        <v>10193520</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N21" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="O21" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="P21">
-        <v>8242508010</v>
+        <v>3952070068</v>
       </c>
       <c r="Q21">
-        <v>10751900430</v>
+        <v>10789274729</v>
       </c>
       <c r="R21">
-        <v>4416778965</v>
+        <v>6040367765</v>
       </c>
       <c r="S21">
-        <v>426234451</v>
+        <v>-4741577598</v>
       </c>
       <c r="T21">
-        <v>2423749751</v>
+        <v>-3671026788</v>
       </c>
       <c r="U21">
-        <v>677048172</v>
+        <v>-3292521363</v>
       </c>
       <c r="V21">
-        <v>57890953</v>
+        <v>-3654889267</v>
       </c>
       <c r="W21">
-        <v>2826043673</v>
+        <v>-2281074471</v>
       </c>
       <c r="X21">
-        <v>990121873</v>
+        <v>-2539505707</v>
       </c>
       <c r="Y21" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2774,76 +2798,76 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F22">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="G22">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>22000</v>
+        <v>5000</v>
       </c>
       <c r="J22">
-        <v>25000</v>
+        <v>5600</v>
       </c>
       <c r="K22">
-        <v>9039778</v>
+        <v>16120000</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N22" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O22" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="P22">
-        <v>104225113285</v>
+        <v>26691070764</v>
       </c>
       <c r="Q22">
-        <v>106505634411</v>
+        <v>22835113396</v>
       </c>
       <c r="R22">
-        <v>66424930568</v>
+        <v>7519073723</v>
       </c>
       <c r="S22">
-        <v>6291020806</v>
+        <v>6041270235</v>
       </c>
       <c r="T22">
-        <v>7893242769</v>
+        <v>6705120210</v>
       </c>
       <c r="U22">
-        <v>7661497240</v>
+        <v>982044017</v>
       </c>
       <c r="V22">
-        <v>7319368873</v>
+        <v>5119066139</v>
       </c>
       <c r="W22">
-        <v>9286891982</v>
+        <v>5870093710</v>
       </c>
       <c r="X22">
-        <v>7334816490</v>
+        <v>1198587470</v>
       </c>
       <c r="Y22" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2851,76 +2875,76 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F23">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="G23">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>21000</v>
+        <v>8200</v>
       </c>
       <c r="J23">
-        <v>26000</v>
+        <v>9400</v>
       </c>
       <c r="K23">
-        <v>64819980</v>
+        <v>7674103</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N23" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="O23" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="P23">
-        <v>36980</v>
+        <v>8242508010</v>
       </c>
       <c r="Q23">
-        <v>44954</v>
+        <v>10751900430</v>
       </c>
       <c r="R23">
-        <v>23652</v>
+        <v>4416778965</v>
       </c>
       <c r="S23">
-        <v>-7085</v>
+        <v>426234451</v>
       </c>
       <c r="T23">
-        <v>-13228</v>
+        <v>2423749751</v>
       </c>
       <c r="U23">
-        <v>-9932</v>
+        <v>677048172</v>
       </c>
       <c r="V23">
-        <v>-7417</v>
+        <v>57890953</v>
       </c>
       <c r="W23">
-        <v>-12548</v>
+        <v>2826043673</v>
       </c>
       <c r="X23">
-        <v>-9333</v>
+        <v>990121873</v>
       </c>
       <c r="Y23" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2928,76 +2952,76 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F24">
-        <v>18000000</v>
+        <v>2000000</v>
       </c>
       <c r="G24">
-        <v>18000000</v>
+        <v>2000000</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="K24">
-        <v>18905000</v>
+        <v>9039778</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N24" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O24" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>104225113285</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>106505634411</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>66424930568</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>6291020806</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>7893242769</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>7661497240</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>7319368873</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>9286891982</v>
       </c>
       <c r="X24">
-        <v>0</v>
+        <v>7334816490</v>
       </c>
       <c r="Y24" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -3005,230 +3029,384 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F25">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="G25">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>8900</v>
+        <v>21000</v>
       </c>
       <c r="J25">
-        <v>11000</v>
+        <v>26000</v>
       </c>
       <c r="K25">
-        <v>5447675</v>
+        <v>64819980</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N25" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="O25" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="P25">
-        <v>18408761227</v>
+        <v>36980</v>
       </c>
       <c r="Q25">
-        <v>21902816604</v>
+        <v>44954</v>
       </c>
       <c r="R25">
-        <v>8176918465</v>
+        <v>23652</v>
       </c>
       <c r="S25">
-        <v>3669182465</v>
+        <v>-7085</v>
       </c>
       <c r="T25">
-        <v>1851925471</v>
+        <v>-13228</v>
       </c>
       <c r="U25">
-        <v>590566592</v>
+        <v>-9932</v>
       </c>
       <c r="V25">
-        <v>3633973594</v>
+        <v>-7417</v>
       </c>
       <c r="W25">
-        <v>2205418963</v>
+        <v>-12548</v>
       </c>
       <c r="X25">
-        <v>592903151</v>
+        <v>-9333</v>
       </c>
       <c r="Y25" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F26">
-        <v>2240000</v>
+        <v>18000000</v>
       </c>
       <c r="G26">
-        <v>1640000</v>
+        <v>18000000</v>
       </c>
       <c r="H26">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="J26">
-        <v>13200</v>
+        <v>2000</v>
       </c>
       <c r="K26">
-        <v>10969386</v>
+        <v>18905000</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="N26" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="O26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P26">
-        <v>22818451349</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>30491967755</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>18040053709</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>2313787613</v>
+        <v>0</v>
       </c>
       <c r="T26">
-        <v>4014101926</v>
+        <v>0</v>
       </c>
       <c r="U26">
-        <v>1878997667</v>
+        <v>0</v>
       </c>
       <c r="V26">
-        <v>559427078</v>
+        <v>0</v>
       </c>
       <c r="W26">
-        <v>-711183147</v>
+        <v>0</v>
       </c>
       <c r="X26">
-        <v>1929682988</v>
+        <v>0</v>
       </c>
       <c r="Y26" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:25">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>54</v>
       </c>
-      <c r="C27" t="s">
-        <v>62</v>
-      </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F27">
+        <v>1500000</v>
+      </c>
+      <c r="G27">
+        <v>1500000</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>8900</v>
+      </c>
+      <c r="J27">
+        <v>11000</v>
+      </c>
+      <c r="K27">
+        <v>5447675</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>12500</v>
+      </c>
+      <c r="N27" t="s">
+        <v>132</v>
+      </c>
+      <c r="O27" t="s">
+        <v>157</v>
+      </c>
+      <c r="P27">
+        <v>18408761227</v>
+      </c>
+      <c r="Q27">
+        <v>21902816604</v>
+      </c>
+      <c r="R27">
+        <v>8176918465</v>
+      </c>
+      <c r="S27">
+        <v>3669182465</v>
+      </c>
+      <c r="T27">
+        <v>1851925471</v>
+      </c>
+      <c r="U27">
+        <v>590566592</v>
+      </c>
+      <c r="V27">
+        <v>3633973594</v>
+      </c>
+      <c r="W27">
+        <v>2205418963</v>
+      </c>
+      <c r="X27">
+        <v>592903151</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28">
+        <v>2240000</v>
+      </c>
+      <c r="G28">
+        <v>1640000</v>
+      </c>
+      <c r="H28">
+        <v>600000</v>
+      </c>
+      <c r="I28">
+        <v>11500</v>
+      </c>
+      <c r="J28">
+        <v>13200</v>
+      </c>
+      <c r="K28">
+        <v>10969386</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>15000</v>
+      </c>
+      <c r="N28" t="s">
+        <v>133</v>
+      </c>
+      <c r="O28" t="s">
+        <v>158</v>
+      </c>
+      <c r="P28">
+        <v>22818451349</v>
+      </c>
+      <c r="Q28">
+        <v>30491967755</v>
+      </c>
+      <c r="R28">
+        <v>18040053709</v>
+      </c>
+      <c r="S28">
+        <v>2313787613</v>
+      </c>
+      <c r="T28">
+        <v>4014101926</v>
+      </c>
+      <c r="U28">
+        <v>1878997667</v>
+      </c>
+      <c r="V28">
+        <v>559427078</v>
+      </c>
+      <c r="W28">
+        <v>-711183147</v>
+      </c>
+      <c r="X28">
+        <v>1929682988</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29">
         <v>1580000</v>
       </c>
-      <c r="G27">
+      <c r="G29">
         <v>1580000</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>10500</v>
       </c>
-      <c r="J27">
+      <c r="J29">
         <v>12000</v>
       </c>
-      <c r="K27">
+      <c r="K29">
         <v>7874611</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>14000</v>
       </c>
-      <c r="N27" t="s">
-        <v>128</v>
-      </c>
-      <c r="O27" t="s">
-        <v>152</v>
-      </c>
-      <c r="P27">
+      <c r="N29" t="s">
+        <v>134</v>
+      </c>
+      <c r="O29" t="s">
+        <v>159</v>
+      </c>
+      <c r="P29">
         <v>7327878427</v>
       </c>
-      <c r="Q27">
+      <c r="Q29">
         <v>10756717708</v>
       </c>
-      <c r="R27">
+      <c r="R29">
         <v>4113702647</v>
       </c>
-      <c r="S27">
+      <c r="S29">
         <v>-588932080</v>
       </c>
-      <c r="T27">
+      <c r="T29">
         <v>254042570</v>
       </c>
-      <c r="U27">
+      <c r="U29">
         <v>-738698858</v>
       </c>
-      <c r="V27">
+      <c r="V29">
         <v>-569358529</v>
       </c>
-      <c r="W27">
+      <c r="W29">
         <v>-429546963</v>
       </c>
-      <c r="X27">
+      <c r="X29">
         <v>-550600734</v>
       </c>
-      <c r="Y27" t="s">
-        <v>177</v>
+      <c r="Y29" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3246,422 +3424,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2">
-        <v>14000</v>
+        <v>19500</v>
       </c>
       <c r="F2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E3">
-        <v>6000</v>
+        <v>14000</v>
       </c>
       <c r="F3" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>96380</v>
       </c>
       <c r="F4" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E5">
         <v>21000</v>
       </c>
       <c r="F5" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6">
         <v>64350</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="E7">
         <v>20000</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="E8">
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="D9" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E9">
         <v>14250</v>
       </c>
       <c r="F9" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="E10">
         <v>16000</v>
       </c>
       <c r="F10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="E11">
         <v>13500</v>
       </c>
       <c r="F11" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="E12">
         <v>14950</v>
       </c>
       <c r="F12" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E13">
         <v>29547</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="E14">
         <v>18040</v>
       </c>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="E15">
         <v>22100</v>
       </c>
       <c r="F15" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D16" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="E16">
         <v>59251</v>
       </c>
       <c r="F16" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="E17">
         <v>60654</v>
       </c>
       <c r="F17" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="E18">
         <v>26800</v>
       </c>
       <c r="F18" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="E19">
         <v>524031</v>
       </c>
       <c r="F19" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="E20">
         <v>6384</v>
       </c>
       <c r="F20" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="E21">
         <v>8000</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-10
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="255">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -158,9 +158,6 @@
     <t>2023-09-22</t>
   </si>
   <si>
-    <t>2023-09-06</t>
-  </si>
-  <si>
     <t>2023-11-21</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>2023-10-04</t>
   </si>
   <si>
-    <t>2023-09-12</t>
-  </si>
-  <si>
     <t>2023-12-05</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>2023-11-14</t>
   </si>
   <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
     <t>교보</t>
   </si>
   <si>
@@ -338,9 +329,6 @@
     <t>신성에스티</t>
   </si>
   <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
     <t>819.05</t>
   </si>
   <si>
@@ -422,9 +410,6 @@
     <t>583.50:1</t>
   </si>
   <si>
-    <t>753.50:1</t>
-  </si>
-  <si>
     <t>0.18%</t>
   </si>
   <si>
@@ -497,9 +482,6 @@
     <t>13.57%</t>
   </si>
   <si>
-    <t>22.20%</t>
-  </si>
-  <si>
     <t>기업인수합병</t>
   </si>
   <si>
@@ -572,9 +554,6 @@
     <t>전기차/2차전지 Busbar 및 배터리모듈 보호 부품 등</t>
   </si>
   <si>
-    <t>건식세정 장비 및 EUV Mask Baking Laser</t>
-  </si>
-  <si>
     <t>종목명</t>
   </si>
   <si>
@@ -593,6 +572,9 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>이닉스(구.이닉스정호)</t>
+  </si>
+  <si>
     <t>에이치비인베스트먼트</t>
   </si>
   <si>
@@ -623,7 +605,7 @@
     <t>동인기연(유가)</t>
   </si>
   <si>
-    <t>에코프로머티리얼즈(유가)</t>
+    <t>2024.01.11~01.17</t>
   </si>
   <si>
     <t>2024.01.08~01.12</t>
@@ -674,7 +656,7 @@
     <t>2023.10.31~11.06</t>
   </si>
   <si>
-    <t>2023.10.30~11.03</t>
+    <t>9,200~11,000</t>
   </si>
   <si>
     <t>2,400~2,800</t>
@@ -722,9 +704,6 @@
     <t>8,000~9,500</t>
   </si>
   <si>
-    <t>36,200~44,000</t>
-  </si>
-  <si>
     <t>19000</t>
   </si>
   <si>
@@ -761,7 +740,7 @@
     <t>11000</t>
   </si>
   <si>
-    <t>36200</t>
+    <t>삼성증권</t>
   </si>
   <si>
     <t>NH투자증권</t>
@@ -782,9 +761,6 @@
     <t>키움증권,KB증권,이베스트투자증권,하이투자증권,NH투자증권</t>
   </si>
   <si>
-    <t>삼성증권</t>
-  </si>
-  <si>
     <t>교보증권</t>
   </si>
   <si>
@@ -804,9 +780,6 @@
   </si>
   <si>
     <t>하이투자증권</t>
-  </si>
-  <si>
-    <t>미래에셋증권,NH투자증권,하이투자증권</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1252,16 +1225,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2">
         <v>3500000</v>
@@ -1288,10 +1261,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="O2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1321,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1329,16 +1302,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F3">
         <v>750000</v>
@@ -1365,10 +1338,10 @@
         <v>23000</v>
       </c>
       <c r="N3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="O3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="P3">
         <v>28564316</v>
@@ -1398,7 +1371,7 @@
         <v>2876182</v>
       </c>
       <c r="Y3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1409,13 +1382,13 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4">
         <v>1500000</v>
@@ -1442,10 +1415,10 @@
         <v>9000</v>
       </c>
       <c r="N4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1475,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1483,16 +1456,16 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5">
         <v>10000000</v>
@@ -1519,10 +1492,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1552,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1563,13 +1536,13 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>650000</v>
@@ -1596,10 +1569,10 @@
         <v>18000</v>
       </c>
       <c r="N6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="O6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="P6">
         <v>55809022</v>
@@ -1629,7 +1602,7 @@
         <v>-8387901</v>
       </c>
       <c r="Y6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1640,13 +1613,13 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F7">
         <v>8000000</v>
@@ -1673,10 +1646,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="O7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1706,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1714,16 +1687,16 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>1407000</v>
@@ -1750,10 +1723,10 @@
         <v>28000</v>
       </c>
       <c r="N8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1783,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1794,13 +1767,13 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>1640000</v>
@@ -1827,10 +1800,10 @@
         <v>17000</v>
       </c>
       <c r="N9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="P9">
         <v>13660</v>
@@ -1860,7 +1833,7 @@
         <v>1666</v>
       </c>
       <c r="Y9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1868,16 +1841,16 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F10">
         <v>3350000</v>
@@ -1904,10 +1877,10 @@
         <v>11000</v>
       </c>
       <c r="N10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="O10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P10">
         <v>47984</v>
@@ -1937,7 +1910,7 @@
         <v>5612</v>
       </c>
       <c r="Y10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1945,16 +1918,16 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F11">
         <v>4250000</v>
@@ -1981,10 +1954,10 @@
         <v>7000</v>
       </c>
       <c r="N11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="O11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="P11">
         <v>27199897007</v>
@@ -2014,7 +1987,7 @@
         <v>3402334635</v>
       </c>
       <c r="Y11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -2025,13 +1998,13 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12">
         <v>2079000</v>
@@ -2058,10 +2031,10 @@
         <v>34700</v>
       </c>
       <c r="N12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="P12">
         <v>26994234332</v>
@@ -2091,7 +2064,7 @@
         <v>15932218050</v>
       </c>
       <c r="Y12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2105,10 +2078,10 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F13">
         <v>1596000</v>
@@ -2135,10 +2108,10 @@
         <v>4000</v>
       </c>
       <c r="N13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="P13">
         <v>7668281979</v>
@@ -2168,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2182,10 +2155,10 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14">
         <v>1600000</v>
@@ -2212,10 +2185,10 @@
         <v>20000</v>
       </c>
       <c r="N14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2245,7 +2218,7 @@
         <v>-12610702106</v>
       </c>
       <c r="Y14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2253,16 +2226,16 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F15">
         <v>2636330</v>
@@ -2289,10 +2262,10 @@
         <v>25000</v>
       </c>
       <c r="N15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="P15">
         <v>45195788</v>
@@ -2322,7 +2295,7 @@
         <v>2327401</v>
       </c>
       <c r="Y15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2333,13 +2306,13 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F16">
         <v>4000000</v>
@@ -2366,10 +2339,10 @@
         <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2399,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2407,16 +2380,16 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F17">
         <v>7000000</v>
@@ -2443,10 +2416,10 @@
         <v>1800</v>
       </c>
       <c r="N17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="P17">
         <v>67332006578</v>
@@ -2476,7 +2449,7 @@
         <v>5666583221</v>
       </c>
       <c r="Y17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2490,10 +2463,10 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F18">
         <v>5200000</v>
@@ -2520,10 +2493,10 @@
         <v>4800</v>
       </c>
       <c r="N18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="P18">
         <v>39450601</v>
@@ -2553,7 +2526,7 @@
         <v>349843</v>
       </c>
       <c r="Y18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2567,10 +2540,10 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F19">
         <v>2060000</v>
@@ -2597,10 +2570,10 @@
         <v>22500</v>
       </c>
       <c r="N19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P19">
         <v>5787300240</v>
@@ -2630,7 +2603,7 @@
         <v>-52132058866</v>
       </c>
       <c r="Y19" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2644,10 +2617,10 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>1200000</v>
@@ -2674,10 +2647,10 @@
         <v>13000</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O20" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="P20">
         <v>20924</v>
@@ -2707,7 +2680,7 @@
         <v>-862</v>
       </c>
       <c r="Y20" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2721,10 +2694,10 @@
         <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F21">
         <v>3600000</v>
@@ -2751,10 +2724,10 @@
         <v>7500</v>
       </c>
       <c r="N21" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O21" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="P21">
         <v>21976760922</v>
@@ -2784,7 +2757,7 @@
         <v>-2514471056</v>
       </c>
       <c r="Y21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2798,10 +2771,10 @@
         <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F22">
         <v>12500000</v>
@@ -2828,10 +2801,10 @@
         <v>2000</v>
       </c>
       <c r="N22" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O22" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -2861,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="Y22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2875,10 +2848,10 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F23">
         <v>1049482</v>
@@ -2905,10 +2878,10 @@
         <v>17000</v>
       </c>
       <c r="N23" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O23" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="P23">
         <v>34557425427</v>
@@ -2938,7 +2911,7 @@
         <v>4046949430</v>
       </c>
       <c r="Y23" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2952,10 +2925,10 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F24">
         <v>1128720</v>
@@ -2982,10 +2955,10 @@
         <v>4400</v>
       </c>
       <c r="N24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O24" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="P24">
         <v>50552623684</v>
@@ -3015,7 +2988,7 @@
         <v>1236029732</v>
       </c>
       <c r="Y24" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -3023,16 +2996,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F25">
         <v>1800000</v>
@@ -3059,10 +3032,10 @@
         <v>17000</v>
       </c>
       <c r="N25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O25" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="P25">
         <v>3952070068</v>
@@ -3092,7 +3065,7 @@
         <v>-2539505707</v>
       </c>
       <c r="Y25" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -3106,10 +3079,10 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F26">
         <v>4000000</v>
@@ -3136,10 +3109,10 @@
         <v>6500</v>
       </c>
       <c r="N26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="O26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="P26">
         <v>26691070764</v>
@@ -3169,7 +3142,7 @@
         <v>1198587470</v>
       </c>
       <c r="Y26" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -3183,10 +3156,10 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F27">
         <v>770000</v>
@@ -3213,10 +3186,10 @@
         <v>7000</v>
       </c>
       <c r="N27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O27" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="P27">
         <v>8242508010</v>
@@ -3246,7 +3219,7 @@
         <v>990121873</v>
       </c>
       <c r="Y27" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -3254,16 +3227,16 @@
         <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F28">
         <v>2000000</v>
@@ -3290,10 +3263,10 @@
         <v>26000</v>
       </c>
       <c r="N28" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="P28">
         <v>104225113285</v>
@@ -3323,84 +3296,7 @@
         <v>7334816490</v>
       </c>
       <c r="Y28" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29">
-        <v>1580000</v>
-      </c>
-      <c r="G29">
-        <v>1580000</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>10500</v>
-      </c>
-      <c r="J29">
-        <v>12000</v>
-      </c>
-      <c r="K29">
-        <v>7874611</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>14000</v>
-      </c>
-      <c r="N29" t="s">
-        <v>135</v>
-      </c>
-      <c r="O29" t="s">
-        <v>160</v>
-      </c>
-      <c r="P29">
-        <v>7327878427</v>
-      </c>
-      <c r="Q29">
-        <v>10756717708</v>
-      </c>
-      <c r="R29">
-        <v>4113702647</v>
-      </c>
-      <c r="S29">
-        <v>-588932080</v>
-      </c>
-      <c r="T29">
-        <v>254042570</v>
-      </c>
-      <c r="U29">
-        <v>-738698858</v>
-      </c>
-      <c r="V29">
-        <v>-569358529</v>
-      </c>
-      <c r="W29">
-        <v>-429546963</v>
-      </c>
-      <c r="X29">
-        <v>-550600734</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3418,239 +3314,239 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E2">
-        <v>16000</v>
+        <v>27600</v>
       </c>
       <c r="F2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E3">
-        <v>19500</v>
+        <v>16000</v>
       </c>
       <c r="F3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E4">
-        <v>14000</v>
+        <v>19500</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E5">
-        <v>96380</v>
+        <v>14000</v>
       </c>
       <c r="F5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E6">
-        <v>8000</v>
+        <v>96380</v>
       </c>
       <c r="F6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>236</v>
+        <v>134</v>
       </c>
       <c r="E7">
-        <v>21000</v>
+        <v>8000</v>
       </c>
       <c r="F7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E8">
-        <v>64350</v>
+        <v>21000</v>
       </c>
       <c r="F8" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E9">
-        <v>20000</v>
+        <v>64350</v>
       </c>
       <c r="F9" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D10" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E10">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="F10" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D11" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E11">
-        <v>14250</v>
+        <v>7000</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E12">
-        <v>16000</v>
+        <v>14250</v>
       </c>
       <c r="F12" t="s">
         <v>249</v>
@@ -3658,39 +3554,39 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E13">
-        <v>13500</v>
+        <v>16000</v>
       </c>
       <c r="F13" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E14">
-        <v>14950</v>
+        <v>13500</v>
       </c>
       <c r="F14" t="s">
         <v>250</v>
@@ -3698,142 +3594,142 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E15">
-        <v>29547</v>
+        <v>14950</v>
       </c>
       <c r="F15" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D16" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E16">
-        <v>18040</v>
+        <v>29547</v>
       </c>
       <c r="F16" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D17" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E17">
-        <v>22100</v>
+        <v>18040</v>
       </c>
       <c r="F17" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D18" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E18">
-        <v>59251</v>
+        <v>22100</v>
       </c>
       <c r="F18" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D19" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E19">
-        <v>60654</v>
+        <v>59251</v>
       </c>
       <c r="F19" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C20" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D20" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E20">
-        <v>26800</v>
+        <v>60654</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C21" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E21">
-        <v>524031</v>
+        <v>26800</v>
       </c>
       <c r="F21" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-12
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="253">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -578,6 +578,9 @@
     <t>에이치비인베스트먼트</t>
   </si>
   <si>
+    <t>현대힘스</t>
+  </si>
+  <si>
     <t>포스뱅크</t>
   </si>
   <si>
@@ -653,15 +656,15 @@
     <t>2023.11.01~11.07</t>
   </si>
   <si>
-    <t>2023.10.31~11.06</t>
-  </si>
-  <si>
     <t>9,200~11,000</t>
   </si>
   <si>
     <t>2,400~2,800</t>
   </si>
   <si>
+    <t>5,000~6,300</t>
+  </si>
+  <si>
     <t>13,000~15,000</t>
   </si>
   <si>
@@ -701,7 +704,7 @@
     <t>33,000~37,000</t>
   </si>
   <si>
-    <t>8,000~9,500</t>
+    <t>2000</t>
   </si>
   <si>
     <t>19000</t>
@@ -710,9 +713,6 @@
     <t>6000</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>23000</t>
   </si>
   <si>
@@ -737,15 +737,15 @@
     <t>30000</t>
   </si>
   <si>
-    <t>11000</t>
-  </si>
-  <si>
     <t>삼성증권</t>
   </si>
   <si>
     <t>NH투자증권</t>
   </si>
   <si>
+    <t>미래에셋증권</t>
+  </si>
+  <si>
     <t>하나증권</t>
   </si>
   <si>
@@ -770,16 +770,10 @@
     <t>유안타증권</t>
   </si>
   <si>
-    <t>미래에셋증권</t>
-  </si>
-  <si>
     <t>대신증권</t>
   </si>
   <si>
     <t>KB증권</t>
-  </si>
-  <si>
-    <t>하이투자증권</t>
   </si>
 </sst>
 </file>
@@ -3337,7 +3331,7 @@
         <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
         <v>213</v>
@@ -3349,7 +3343,7 @@
         <v>27600</v>
       </c>
       <c r="F2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3357,7 +3351,7 @@
         <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>214</v>
@@ -3369,7 +3363,7 @@
         <v>16000</v>
       </c>
       <c r="F3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3386,10 +3380,10 @@
         <v>134</v>
       </c>
       <c r="E4">
-        <v>19500</v>
+        <v>43535</v>
       </c>
       <c r="F4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3406,7 +3400,7 @@
         <v>134</v>
       </c>
       <c r="E5">
-        <v>14000</v>
+        <v>19500</v>
       </c>
       <c r="F5" t="s">
         <v>243</v>
@@ -3426,10 +3420,10 @@
         <v>134</v>
       </c>
       <c r="E6">
-        <v>96380</v>
+        <v>14000</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3440,16 +3434,16 @@
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
         <v>134</v>
       </c>
       <c r="E7">
-        <v>8000</v>
+        <v>96380</v>
       </c>
       <c r="F7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3460,16 +3454,16 @@
         <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D8" t="s">
         <v>229</v>
       </c>
       <c r="E8">
-        <v>21000</v>
+        <v>8000</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3477,7 +3471,7 @@
         <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
         <v>219</v>
@@ -3486,115 +3480,115 @@
         <v>230</v>
       </c>
       <c r="E9">
-        <v>64350</v>
+        <v>21000</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D10" t="s">
         <v>231</v>
       </c>
       <c r="E10">
-        <v>20000</v>
+        <v>64350</v>
       </c>
       <c r="F10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E11">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="F11" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
         <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E12">
-        <v>14250</v>
+        <v>7000</v>
       </c>
       <c r="F12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E13">
-        <v>16000</v>
+        <v>14250</v>
       </c>
       <c r="F13" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
         <v>206</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E14">
-        <v>13500</v>
+        <v>16000</v>
       </c>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>207</v>
@@ -3603,18 +3597,18 @@
         <v>222</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E15">
-        <v>14950</v>
+        <v>13500</v>
       </c>
       <c r="F15" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>208</v>
@@ -3623,18 +3617,18 @@
         <v>223</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E16">
-        <v>29547</v>
+        <v>14950</v>
       </c>
       <c r="F16" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>209</v>
@@ -3643,10 +3637,10 @@
         <v>224</v>
       </c>
       <c r="D17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E17">
-        <v>18040</v>
+        <v>29547</v>
       </c>
       <c r="F17" t="s">
         <v>242</v>
@@ -3654,7 +3648,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>210</v>
@@ -3663,18 +3657,18 @@
         <v>225</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E18">
-        <v>22100</v>
+        <v>18040</v>
       </c>
       <c r="F18" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
         <v>211</v>
@@ -3683,38 +3677,38 @@
         <v>226</v>
       </c>
       <c r="D19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E19">
-        <v>59251</v>
+        <v>22100</v>
       </c>
       <c r="F19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
         <v>227</v>
       </c>
       <c r="D20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E20">
-        <v>60654</v>
+        <v>59251</v>
       </c>
       <c r="F20" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
         <v>212</v>
@@ -3723,13 +3717,13 @@
         <v>228</v>
       </c>
       <c r="D21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E21">
-        <v>26800</v>
+        <v>60654</v>
       </c>
       <c r="F21" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-16
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="261">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -608,6 +608,9 @@
     <t>이닉스(구.이닉스정호)</t>
   </si>
   <si>
+    <t>대신밸런스스팩17호</t>
+  </si>
+  <si>
     <t>에이치비인베스트먼트</t>
   </si>
   <si>
@@ -617,6 +620,9 @@
     <t>포스뱅크</t>
   </si>
   <si>
+    <t>스튜디오삼익</t>
+  </si>
+  <si>
     <t>하나스팩30호</t>
   </si>
   <si>
@@ -632,12 +638,12 @@
     <t>NH스팩30호</t>
   </si>
   <si>
-    <t>동인기연(유가)</t>
-  </si>
-  <si>
     <t>2024.01.11~01.17</t>
   </si>
   <si>
+    <t>2024.01.09~01.10</t>
+  </si>
+  <si>
     <t>2024.01.08~01.12</t>
   </si>
   <si>
@@ -680,12 +686,12 @@
     <t>2023.11.02~11.08</t>
   </si>
   <si>
-    <t>2023.11.01~11.07</t>
-  </si>
-  <si>
     <t>9,200~11,000</t>
   </si>
   <si>
+    <t>2,000~2,000</t>
+  </si>
+  <si>
     <t>2,400~2,800</t>
   </si>
   <si>
@@ -695,7 +701,7 @@
     <t>13,000~15,000</t>
   </si>
   <si>
-    <t>2,000~2,000</t>
+    <t>14,500~16,500</t>
   </si>
   <si>
     <t>79,000~89,000</t>
@@ -725,12 +731,6 @@
     <t>5,200~6,000</t>
   </si>
   <si>
-    <t>28,500~34,700</t>
-  </si>
-  <si>
-    <t>33,000~37,000</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -761,15 +761,12 @@
     <t>7000</t>
   </si>
   <si>
-    <t>34700</t>
-  </si>
-  <si>
-    <t>30000</t>
-  </si>
-  <si>
     <t>삼성증권</t>
   </si>
   <si>
+    <t>대신증권</t>
+  </si>
+  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -779,6 +776,9 @@
     <t>하나증권</t>
   </si>
   <si>
+    <t>DB금융투자</t>
+  </si>
+  <si>
     <t>KB증권,NH투자증권</t>
   </si>
   <si>
@@ -798,12 +798,6 @@
   </si>
   <si>
     <t>유안타증권</t>
-  </si>
-  <si>
-    <t>대신증권</t>
-  </si>
-  <si>
-    <t>KB증권</t>
   </si>
 </sst>
 </file>
@@ -3515,10 +3509,10 @@
         <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
         <v>143</v>
@@ -3527,7 +3521,7 @@
         <v>27600</v>
       </c>
       <c r="F2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3535,19 +3529,19 @@
         <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D3" t="s">
         <v>143</v>
       </c>
       <c r="E3">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="F3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3555,19 +3549,19 @@
         <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
         <v>143</v>
       </c>
       <c r="E4">
-        <v>43535</v>
+        <v>16000</v>
       </c>
       <c r="F4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3575,19 +3569,19 @@
         <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
         <v>143</v>
       </c>
       <c r="E5">
-        <v>19500</v>
+        <v>43535</v>
       </c>
       <c r="F5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3595,19 +3589,19 @@
         <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>143</v>
       </c>
       <c r="E6">
-        <v>14000</v>
+        <v>19500</v>
       </c>
       <c r="F6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3618,16 +3612,16 @@
         <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>143</v>
       </c>
       <c r="E7">
-        <v>96380</v>
+        <v>12325</v>
       </c>
       <c r="F7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3638,181 +3632,181 @@
         <v>211</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
         <v>238</v>
       </c>
       <c r="E8">
-        <v>8000</v>
+        <v>14000</v>
       </c>
       <c r="F8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s">
         <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E9">
-        <v>21000</v>
+        <v>96380</v>
       </c>
       <c r="F9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>204</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E10">
-        <v>64350</v>
+        <v>8000</v>
       </c>
       <c r="F10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E11">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="F11" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="D12" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E12">
-        <v>7000</v>
+        <v>64350</v>
       </c>
       <c r="F12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E13">
-        <v>14250</v>
+        <v>20000</v>
       </c>
       <c r="F13" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
         <v>238</v>
       </c>
       <c r="E14">
-        <v>16000</v>
+        <v>7000</v>
       </c>
       <c r="F14" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
         <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E15">
-        <v>13500</v>
+        <v>14250</v>
       </c>
       <c r="F15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
         <v>217</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E16">
-        <v>14950</v>
+        <v>16000</v>
       </c>
       <c r="F16" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>218</v>
@@ -3821,18 +3815,18 @@
         <v>233</v>
       </c>
       <c r="D17" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E17">
-        <v>29547</v>
+        <v>13500</v>
       </c>
       <c r="F17" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
         <v>219</v>
@@ -3841,18 +3835,18 @@
         <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E18">
-        <v>18040</v>
+        <v>14950</v>
       </c>
       <c r="F18" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
         <v>220</v>
@@ -3861,18 +3855,18 @@
         <v>235</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E19">
-        <v>22100</v>
+        <v>29547</v>
       </c>
       <c r="F19" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
         <v>221</v>
@@ -3881,33 +3875,33 @@
         <v>236</v>
       </c>
       <c r="D20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E20">
-        <v>59251</v>
+        <v>18040</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
         <v>237</v>
       </c>
       <c r="D21" t="s">
+        <v>247</v>
+      </c>
+      <c r="E21">
+        <v>22100</v>
+      </c>
+      <c r="F21" t="s">
         <v>249</v>
-      </c>
-      <c r="E21">
-        <v>60654</v>
-      </c>
-      <c r="F21" t="s">
-        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-20
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="250">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -155,9 +155,6 @@
     <t>2023-10-05</t>
   </si>
   <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
     <t>2023-11-28</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>2023-10-13</t>
   </si>
   <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
     <t>2023-12-12</t>
   </si>
   <si>
@@ -335,9 +329,6 @@
     <t>워트</t>
   </si>
   <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
     <t>396.84</t>
   </si>
   <si>
@@ -419,9 +410,6 @@
     <t>793.26:1</t>
   </si>
   <si>
-    <t>235.14:1</t>
-  </si>
-  <si>
     <t>12.02%</t>
   </si>
   <si>
@@ -494,9 +482,6 @@
     <t>10.06%</t>
   </si>
   <si>
-    <t>16.63%</t>
-  </si>
-  <si>
     <t>울트라커패시터(셀 및 모듈)</t>
   </si>
   <si>
@@ -567,9 +552,6 @@
   </si>
   <si>
     <t>초정밀 온습도 제어장비</t>
-  </si>
-  <si>
-    <t>의약품 품질관리, 신약개발지원, 체외진단기기</t>
   </si>
   <si>
     <t>종목명</t>
@@ -1140,7 +1122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1228,16 +1210,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F2">
         <v>14625000</v>
@@ -1264,10 +1246,10 @@
         <v>6000</v>
       </c>
       <c r="N2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1297,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1305,16 +1287,16 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3">
         <v>1400000</v>
@@ -1341,10 +1323,10 @@
         <v>19000</v>
       </c>
       <c r="N3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P3">
         <v>49637696375</v>
@@ -1374,7 +1356,7 @@
         <v>286239267</v>
       </c>
       <c r="Y3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1382,16 +1364,16 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F4">
         <v>3500000</v>
@@ -1418,10 +1400,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1451,7 +1433,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1462,13 +1444,13 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5">
         <v>750000</v>
@@ -1495,10 +1477,10 @@
         <v>23000</v>
       </c>
       <c r="N5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P5">
         <v>28564316</v>
@@ -1528,7 +1510,7 @@
         <v>2876182</v>
       </c>
       <c r="Y5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1539,13 +1521,13 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>1500000</v>
@@ -1572,10 +1554,10 @@
         <v>9000</v>
       </c>
       <c r="N6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1605,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1613,16 +1595,16 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7">
         <v>10000000</v>
@@ -1649,10 +1631,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="O7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1682,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1693,13 +1675,13 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>650000</v>
@@ -1726,10 +1708,10 @@
         <v>18000</v>
       </c>
       <c r="N8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="O8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P8">
         <v>55809022</v>
@@ -1759,7 +1741,7 @@
         <v>-8387901</v>
       </c>
       <c r="Y8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1770,13 +1752,13 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>8000000</v>
@@ -1803,10 +1785,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="O9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1836,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1844,16 +1826,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F10">
         <v>1407000</v>
@@ -1880,10 +1862,10 @@
         <v>28000</v>
       </c>
       <c r="N10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="O10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1913,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1924,13 +1906,13 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F11">
         <v>1640000</v>
@@ -1957,10 +1939,10 @@
         <v>17000</v>
       </c>
       <c r="N11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="O11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="P11">
         <v>13660</v>
@@ -1990,7 +1972,7 @@
         <v>1666</v>
       </c>
       <c r="Y11" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1998,16 +1980,16 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F12">
         <v>3350000</v>
@@ -2034,10 +2016,10 @@
         <v>11000</v>
       </c>
       <c r="N12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P12">
         <v>47984</v>
@@ -2067,7 +2049,7 @@
         <v>5612</v>
       </c>
       <c r="Y12" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2075,16 +2057,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F13">
         <v>4250000</v>
@@ -2111,10 +2093,10 @@
         <v>7000</v>
       </c>
       <c r="N13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="P13">
         <v>27199897007</v>
@@ -2144,7 +2126,7 @@
         <v>3402334635</v>
       </c>
       <c r="Y13" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2155,13 +2137,13 @@
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F14">
         <v>2079000</v>
@@ -2188,10 +2170,10 @@
         <v>34700</v>
       </c>
       <c r="N14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="P14">
         <v>26994234332</v>
@@ -2221,7 +2203,7 @@
         <v>15932218050</v>
       </c>
       <c r="Y14" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2235,10 +2217,10 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F15">
         <v>1596000</v>
@@ -2265,10 +2247,10 @@
         <v>4000</v>
       </c>
       <c r="N15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="O15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="P15">
         <v>7668281979</v>
@@ -2298,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2312,10 +2294,10 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F16">
         <v>1600000</v>
@@ -2342,10 +2324,10 @@
         <v>20000</v>
       </c>
       <c r="N16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="O16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2375,7 +2357,7 @@
         <v>-12610702106</v>
       </c>
       <c r="Y16" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2383,16 +2365,16 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F17">
         <v>2636330</v>
@@ -2419,10 +2401,10 @@
         <v>25000</v>
       </c>
       <c r="N17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P17">
         <v>45195788</v>
@@ -2452,7 +2434,7 @@
         <v>2327401</v>
       </c>
       <c r="Y17" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2463,13 +2445,13 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F18">
         <v>4000000</v>
@@ -2496,10 +2478,10 @@
         <v>2000</v>
       </c>
       <c r="N18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -2529,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2537,16 +2519,16 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F19">
         <v>7000000</v>
@@ -2573,10 +2555,10 @@
         <v>1800</v>
       </c>
       <c r="N19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P19">
         <v>67332006578</v>
@@ -2606,7 +2588,7 @@
         <v>5666583221</v>
       </c>
       <c r="Y19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2620,10 +2602,10 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>5200000</v>
@@ -2650,10 +2632,10 @@
         <v>4800</v>
       </c>
       <c r="N20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P20">
         <v>39450601</v>
@@ -2683,7 +2665,7 @@
         <v>349843</v>
       </c>
       <c r="Y20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2697,10 +2679,10 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F21">
         <v>2060000</v>
@@ -2727,10 +2709,10 @@
         <v>22500</v>
       </c>
       <c r="N21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P21">
         <v>5787300240</v>
@@ -2760,7 +2742,7 @@
         <v>-52132058866</v>
       </c>
       <c r="Y21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2774,10 +2756,10 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22">
         <v>1200000</v>
@@ -2804,10 +2786,10 @@
         <v>13000</v>
       </c>
       <c r="N22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P22">
         <v>20924</v>
@@ -2837,7 +2819,7 @@
         <v>-862</v>
       </c>
       <c r="Y22" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2851,10 +2833,10 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F23">
         <v>3600000</v>
@@ -2881,10 +2863,10 @@
         <v>7500</v>
       </c>
       <c r="N23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O23" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P23">
         <v>21976760922</v>
@@ -2914,7 +2896,7 @@
         <v>-2514471056</v>
       </c>
       <c r="Y23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2928,10 +2910,10 @@
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F24">
         <v>12500000</v>
@@ -2958,10 +2940,10 @@
         <v>2000</v>
       </c>
       <c r="N24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O24" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P24">
         <v>0</v>
@@ -2991,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="Y24" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -3005,10 +2987,10 @@
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25">
         <v>1049482</v>
@@ -3035,10 +3017,10 @@
         <v>17000</v>
       </c>
       <c r="N25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="O25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="P25">
         <v>34557425427</v>
@@ -3068,7 +3050,7 @@
         <v>4046949430</v>
       </c>
       <c r="Y25" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -3082,10 +3064,10 @@
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F26">
         <v>1128720</v>
@@ -3112,10 +3094,10 @@
         <v>4400</v>
       </c>
       <c r="N26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="P26">
         <v>50552623684</v>
@@ -3145,7 +3127,7 @@
         <v>1236029732</v>
       </c>
       <c r="Y26" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -3153,16 +3135,16 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F27">
         <v>1800000</v>
@@ -3189,10 +3171,10 @@
         <v>17000</v>
       </c>
       <c r="N27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O27" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P27">
         <v>3952070068</v>
@@ -3222,7 +3204,7 @@
         <v>-2539505707</v>
       </c>
       <c r="Y27" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -3236,10 +3218,10 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F28">
         <v>4000000</v>
@@ -3266,10 +3248,10 @@
         <v>6500</v>
       </c>
       <c r="N28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="O28" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="P28">
         <v>26691070764</v>
@@ -3299,84 +3281,7 @@
         <v>1198587470</v>
       </c>
       <c r="Y28" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29">
-        <v>770000</v>
-      </c>
-      <c r="G29">
-        <v>770000</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>8200</v>
-      </c>
-      <c r="J29">
-        <v>9400</v>
-      </c>
-      <c r="K29">
-        <v>7674103</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>7000</v>
-      </c>
-      <c r="N29" t="s">
-        <v>134</v>
-      </c>
-      <c r="O29" t="s">
-        <v>159</v>
-      </c>
-      <c r="P29">
-        <v>8242508010</v>
-      </c>
-      <c r="Q29">
-        <v>10751900430</v>
-      </c>
-      <c r="R29">
-        <v>4416778965</v>
-      </c>
-      <c r="S29">
-        <v>426234451</v>
-      </c>
-      <c r="T29">
-        <v>2423749751</v>
-      </c>
-      <c r="U29">
-        <v>677048172</v>
-      </c>
-      <c r="V29">
-        <v>57890953</v>
-      </c>
-      <c r="W29">
-        <v>2826043673</v>
-      </c>
-      <c r="X29">
-        <v>990121873</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3394,422 +3299,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E2">
         <v>27600</v>
       </c>
       <c r="F2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E3">
         <v>11000</v>
       </c>
       <c r="F3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E4">
         <v>16000</v>
       </c>
       <c r="F4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E5">
         <v>43535</v>
       </c>
       <c r="F5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E6">
         <v>8858</v>
       </c>
       <c r="F6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E7">
         <v>19500</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E8">
         <v>12325</v>
       </c>
       <c r="F8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E9">
         <v>14000</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E10">
         <v>96380</v>
       </c>
       <c r="F10" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E11">
         <v>8000</v>
       </c>
       <c r="F11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E12">
         <v>21000</v>
       </c>
       <c r="F12" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E13">
         <v>64350</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E14">
         <v>20000</v>
       </c>
       <c r="F14" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E15">
         <v>7000</v>
       </c>
       <c r="F15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E16">
         <v>14250</v>
       </c>
       <c r="F16" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" t="s">
         <v>213</v>
       </c>
-      <c r="C17" t="s">
-        <v>219</v>
-      </c>
       <c r="D17" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E17">
         <v>16000</v>
       </c>
       <c r="F17" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E18">
         <v>13500</v>
       </c>
       <c r="F18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E19">
         <v>14950</v>
       </c>
       <c r="F19" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E20">
         <v>29547</v>
       </c>
       <c r="F20" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D21" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E21">
         <v>18040</v>
       </c>
       <c r="F21" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-22
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="254">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2023-12-08</t>
+  </si>
+  <si>
     <t>2023-11-22</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
     <t>2023-10-05</t>
   </si>
   <si>
+    <t>2023-12-12</t>
+  </si>
+  <si>
     <t>2023-11-28</t>
   </si>
   <si>
@@ -176,7 +182,7 @@
     <t>2023-10-13</t>
   </si>
   <si>
-    <t>2023-12-12</t>
+    <t>2023-12-22</t>
   </si>
   <si>
     <t>2023-12-13</t>
@@ -200,12 +206,12 @@
     <t>2023-11-14</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
     <t>키움, KB</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>교보</t>
   </si>
   <si>
@@ -248,6 +254,9 @@
     <t>키움</t>
   </si>
   <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
     <t>LS머트리얼즈</t>
   </si>
   <si>
@@ -329,6 +338,9 @@
     <t>워트</t>
   </si>
   <si>
+    <t>708.35:1</t>
+  </si>
+  <si>
     <t>396.84</t>
   </si>
   <si>
@@ -410,6 +422,9 @@
     <t>793.26:1</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>12.02%</t>
   </si>
   <si>
@@ -425,9 +440,6 @@
     <t>14.47%</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>0.43%</t>
   </si>
   <si>
@@ -482,13 +494,13 @@
     <t>10.06%</t>
   </si>
   <si>
+    <t>기업인수합병</t>
+  </si>
+  <si>
     <t>울트라커패시터(셀 및 모듈)</t>
   </si>
   <si>
     <t>의약품 유통업</t>
-  </si>
-  <si>
-    <t>기업인수합병</t>
   </si>
   <si>
     <t>이차전지 자동화 설비</t>
@@ -1122,7 +1134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y28"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1210,46 +1222,46 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2">
-        <v>14625000</v>
+        <v>7000000</v>
       </c>
       <c r="G2">
-        <v>8775000</v>
+        <v>7000000</v>
       </c>
       <c r="H2">
-        <v>5850000</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>5500</v>
+        <v>2000</v>
       </c>
       <c r="K2">
-        <v>67652659</v>
+        <v>7305000</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1279,84 +1291,84 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F3">
-        <v>1400000</v>
+        <v>14625000</v>
       </c>
       <c r="G3">
-        <v>1400000</v>
+        <v>8775000</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>5850000</v>
       </c>
       <c r="I3">
-        <v>15000</v>
+        <v>4400</v>
       </c>
       <c r="J3">
-        <v>19000</v>
+        <v>5500</v>
       </c>
       <c r="K3">
-        <v>10650189</v>
+        <v>67652659</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>19000</v>
+        <v>6000</v>
       </c>
       <c r="N3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="P3">
-        <v>49637696375</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>77146751918</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>41854695636</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>-2726643993</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>890609048</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>176442923</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>-7688787420</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>-14330655532</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>286239267</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1364,76 +1376,76 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F4">
-        <v>3500000</v>
+        <v>1400000</v>
       </c>
       <c r="G4">
-        <v>3500000</v>
+        <v>1400000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>19000</v>
       </c>
       <c r="K4">
-        <v>3810000</v>
+        <v>10650189</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>19000</v>
       </c>
       <c r="N4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="O4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>49637696375</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>77146751918</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>41854695636</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>-2726643993</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>890609048</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>176442923</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>-7688787420</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>-14330655532</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>286239267</v>
       </c>
       <c r="Y4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1441,76 +1453,76 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F5">
-        <v>750000</v>
+        <v>3500000</v>
       </c>
       <c r="G5">
-        <v>750000</v>
+        <v>3500000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>19000</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>22000</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>3883557</v>
+        <v>3810000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>23000</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="O5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="P5">
-        <v>28564316</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>34734790</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>19566070</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>4032783</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>6075261</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>3863017</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>3909264</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>4830718</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>2876182</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1518,123 +1530,123 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F6">
-        <v>1500000</v>
+        <v>750000</v>
       </c>
       <c r="G6">
-        <v>1500000</v>
+        <v>750000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>9000</v>
+        <v>19000</v>
       </c>
       <c r="J6">
-        <v>11000</v>
+        <v>22000</v>
       </c>
       <c r="K6">
-        <v>13866898</v>
+        <v>3883557</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>9000</v>
+        <v>23000</v>
       </c>
       <c r="N6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>28564316</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>34734790</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>19566070</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>4032783</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>6075261</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>3863017</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>3909264</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>4830718</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>2876182</v>
       </c>
       <c r="Y6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7">
-        <v>10000000</v>
+        <v>1500000</v>
       </c>
       <c r="G7">
-        <v>10000000</v>
+        <v>1500000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K7">
-        <v>11050000</v>
+        <v>13866898</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="N7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O7" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1664,84 +1676,84 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F8">
-        <v>650000</v>
+        <v>10000000</v>
       </c>
       <c r="G8">
-        <v>650000</v>
+        <v>10000000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>23000</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K8">
-        <v>5345180</v>
+        <v>11050000</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="O8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P8">
-        <v>55809022</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>53633878</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>47971262</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>-4601725</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>-7645858</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>-5922868</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>-20523948</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>-12027347</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>-8387901</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1749,76 +1761,76 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F9">
-        <v>8000000</v>
+        <v>650000</v>
       </c>
       <c r="G9">
-        <v>8000000</v>
+        <v>650000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K9">
-        <v>9100000</v>
+        <v>5345180</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="O9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>55809022</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>53633878</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>47971262</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>-4601725</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>-7645858</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>-5922868</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>-20523948</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>-12027347</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>-8387901</v>
       </c>
       <c r="Y9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1826,46 +1838,46 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F10">
-        <v>1407000</v>
+        <v>8000000</v>
       </c>
       <c r="G10">
-        <v>844000</v>
+        <v>8000000</v>
       </c>
       <c r="H10">
-        <v>563000</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>25000</v>
+        <v>2000</v>
       </c>
       <c r="K10">
-        <v>5657215</v>
+        <v>9100000</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>28000</v>
+        <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="O10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1895,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1903,76 +1915,76 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F11">
-        <v>1640000</v>
+        <v>1407000</v>
       </c>
       <c r="G11">
-        <v>1640000</v>
+        <v>844000</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>563000</v>
       </c>
       <c r="I11">
-        <v>11000</v>
+        <v>21000</v>
       </c>
       <c r="J11">
-        <v>14000</v>
+        <v>25000</v>
       </c>
       <c r="K11">
-        <v>8183944</v>
+        <v>5657215</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>17000</v>
+        <v>28000</v>
       </c>
       <c r="N11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O11" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="P11">
-        <v>13660</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>25085</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>8905</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>3108</v>
+        <v>0</v>
       </c>
       <c r="T11">
-        <v>3731</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>2219</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>1157</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>3465</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>1666</v>
+        <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1980,76 +1992,76 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
         <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F12">
-        <v>3350000</v>
+        <v>1640000</v>
       </c>
       <c r="G12">
-        <v>3350000</v>
+        <v>1640000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>8000</v>
+        <v>11000</v>
       </c>
       <c r="J12">
-        <v>9500</v>
+        <v>14000</v>
       </c>
       <c r="K12">
-        <v>13436499</v>
+        <v>8183944</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="O12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="P12">
-        <v>47984</v>
+        <v>13660</v>
       </c>
       <c r="Q12">
-        <v>51031</v>
+        <v>25085</v>
       </c>
       <c r="R12">
-        <v>29425</v>
+        <v>8905</v>
       </c>
       <c r="S12">
-        <v>10526</v>
+        <v>3108</v>
       </c>
       <c r="T12">
-        <v>11804</v>
+        <v>3731</v>
       </c>
       <c r="U12">
-        <v>7008</v>
+        <v>2219</v>
       </c>
       <c r="V12">
-        <v>8661</v>
+        <v>1157</v>
       </c>
       <c r="W12">
-        <v>9582</v>
+        <v>3465</v>
       </c>
       <c r="X12">
-        <v>5612</v>
+        <v>1666</v>
       </c>
       <c r="Y12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -2057,76 +2069,76 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F13">
-        <v>4250000</v>
+        <v>3350000</v>
       </c>
       <c r="G13">
-        <v>4250000</v>
+        <v>3350000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>5200</v>
+        <v>8000</v>
       </c>
       <c r="J13">
-        <v>6000</v>
+        <v>9500</v>
       </c>
       <c r="K13">
-        <v>17002500</v>
+        <v>13436499</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="N13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="O13" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="P13">
-        <v>27199897007</v>
+        <v>47984</v>
       </c>
       <c r="Q13">
-        <v>40971122327</v>
+        <v>51031</v>
       </c>
       <c r="R13">
-        <v>25300714406</v>
+        <v>29425</v>
       </c>
       <c r="S13">
-        <v>2887034102</v>
+        <v>10526</v>
       </c>
       <c r="T13">
-        <v>7167697077</v>
+        <v>11804</v>
       </c>
       <c r="U13">
-        <v>4740280453</v>
+        <v>7008</v>
       </c>
       <c r="V13">
-        <v>2399514033</v>
+        <v>8661</v>
       </c>
       <c r="W13">
-        <v>5498221693</v>
+        <v>9582</v>
       </c>
       <c r="X13">
-        <v>3402334635</v>
+        <v>5612</v>
       </c>
       <c r="Y13" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2134,76 +2146,76 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F14">
-        <v>2079000</v>
+        <v>4250000</v>
       </c>
       <c r="G14">
-        <v>2079000</v>
+        <v>4250000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>28500</v>
+        <v>5200</v>
       </c>
       <c r="J14">
-        <v>34700</v>
+        <v>6000</v>
       </c>
       <c r="K14">
-        <v>9877043</v>
+        <v>17002500</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>34700</v>
+        <v>7000</v>
       </c>
       <c r="N14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="O14" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="P14">
-        <v>26994234332</v>
+        <v>27199897007</v>
       </c>
       <c r="Q14">
-        <v>60121142197</v>
+        <v>40971122327</v>
       </c>
       <c r="R14">
-        <v>53305665235</v>
+        <v>25300714406</v>
       </c>
       <c r="S14">
-        <v>10162848799</v>
+        <v>2887034102</v>
       </c>
       <c r="T14">
-        <v>20033029594</v>
+        <v>7167697077</v>
       </c>
       <c r="U14">
-        <v>19806683734</v>
+        <v>4740280453</v>
       </c>
       <c r="V14">
-        <v>7996520497</v>
+        <v>2399514033</v>
       </c>
       <c r="W14">
-        <v>15559454518</v>
+        <v>5498221693</v>
       </c>
       <c r="X14">
-        <v>15932218050</v>
+        <v>3402334635</v>
       </c>
       <c r="Y14" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2211,76 +2223,76 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F15">
-        <v>1596000</v>
+        <v>2079000</v>
       </c>
       <c r="G15">
-        <v>1596000</v>
+        <v>2079000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>3200</v>
+        <v>28500</v>
       </c>
       <c r="J15">
-        <v>3600</v>
+        <v>34700</v>
       </c>
       <c r="K15">
-        <v>13346380</v>
+        <v>9877043</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>4000</v>
+        <v>34700</v>
       </c>
       <c r="N15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O15" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="P15">
-        <v>7668281979</v>
+        <v>26994234332</v>
       </c>
       <c r="Q15">
-        <v>7100921456</v>
+        <v>60121142197</v>
       </c>
       <c r="R15">
-        <v>1207846478</v>
+        <v>53305665235</v>
       </c>
       <c r="S15">
-        <v>5659403971</v>
+        <v>10162848799</v>
       </c>
       <c r="T15">
-        <v>6124121466</v>
+        <v>20033029594</v>
       </c>
       <c r="U15">
-        <v>940668827</v>
+        <v>19806683734</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>7996520497</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>15559454518</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>15932218050</v>
       </c>
       <c r="Y15" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2291,73 +2303,73 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F16">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="G16">
-        <v>1600000</v>
+        <v>1596000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>29800</v>
+        <v>3200</v>
       </c>
       <c r="J16">
-        <v>33500</v>
+        <v>3600</v>
       </c>
       <c r="K16">
-        <v>13612736</v>
+        <v>13346380</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N16" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="O16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>7668281979</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>7100921456</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>1207846478</v>
       </c>
       <c r="S16">
-        <v>-15286512079</v>
+        <v>5659403971</v>
       </c>
       <c r="T16">
-        <v>-21424611321</v>
+        <v>6124121466</v>
       </c>
       <c r="U16">
-        <v>-139745251263</v>
+        <v>940668827</v>
       </c>
       <c r="V16">
-        <v>-53575668634</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>-38885125426</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>-12610702106</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2365,76 +2377,76 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F17">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="G17">
-        <v>2636330</v>
+        <v>1600000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>19100</v>
+        <v>29800</v>
       </c>
       <c r="J17">
-        <v>21400</v>
+        <v>33500</v>
       </c>
       <c r="K17">
-        <v>10585320</v>
+        <v>13612736</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N17" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="O17" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="P17">
-        <v>45195788</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>69629209</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>35634471</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>2751277</v>
+        <v>-15286512079</v>
       </c>
       <c r="T17">
-        <v>11449731</v>
+        <v>-21424611321</v>
       </c>
       <c r="U17">
-        <v>2482194</v>
+        <v>-139745251263</v>
       </c>
       <c r="V17">
-        <v>2092692</v>
+        <v>-53575668634</v>
       </c>
       <c r="W17">
-        <v>5149538</v>
+        <v>-38885125426</v>
       </c>
       <c r="X17">
-        <v>2327401</v>
+        <v>-12610702106</v>
       </c>
       <c r="Y17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2442,384 +2454,384 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F18">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="G18">
-        <v>4000000</v>
+        <v>2636330</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>2000</v>
+        <v>19100</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>21400</v>
       </c>
       <c r="K18">
-        <v>4320000</v>
+        <v>10585320</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N18" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O18" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>45195788</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>69629209</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>35634471</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>2751277</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>11449731</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>2482194</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>2092692</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>5149538</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>2327401</v>
       </c>
       <c r="Y18" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F19">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="G19">
-        <v>7000000</v>
+        <v>4000000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="J19">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="K19">
-        <v>30610000</v>
+        <v>4320000</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N19" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="O19" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="P19">
-        <v>67332006578</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>100050838794</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>63366010569</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>1140243099</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <v>8333440685</v>
+        <v>0</v>
       </c>
       <c r="U19">
-        <v>7415958936</v>
+        <v>0</v>
       </c>
       <c r="V19">
-        <v>668088159</v>
+        <v>0</v>
       </c>
       <c r="W19">
-        <v>5930478364</v>
+        <v>0</v>
       </c>
       <c r="X19">
-        <v>5666583221</v>
+        <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F20">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="G20">
-        <v>5200000</v>
+        <v>7000000</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>3500</v>
+        <v>1200</v>
       </c>
       <c r="J20">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="K20">
-        <v>20771000</v>
+        <v>30610000</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="P20">
-        <v>39450601</v>
+        <v>67332006578</v>
       </c>
       <c r="Q20">
-        <v>49044883</v>
+        <v>100050838794</v>
       </c>
       <c r="R20">
-        <v>21826468</v>
+        <v>63366010569</v>
       </c>
       <c r="S20">
-        <v>2477559</v>
+        <v>1140243099</v>
       </c>
       <c r="T20">
-        <v>8094900</v>
+        <v>8333440685</v>
       </c>
       <c r="U20">
-        <v>215154</v>
+        <v>7415958936</v>
       </c>
       <c r="V20">
-        <v>3427734</v>
+        <v>668088159</v>
       </c>
       <c r="W20">
-        <v>6575528</v>
+        <v>5930478364</v>
       </c>
       <c r="X20">
-        <v>349843</v>
+        <v>5666583221</v>
       </c>
       <c r="Y20" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
         <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F21">
-        <v>2060000</v>
+        <v>5200000</v>
       </c>
       <c r="G21">
-        <v>2000000</v>
+        <v>5200000</v>
       </c>
       <c r="H21">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>20300</v>
+        <v>3500</v>
       </c>
       <c r="J21">
-        <v>22500</v>
+        <v>4000</v>
       </c>
       <c r="K21">
-        <v>14384224</v>
+        <v>20771000</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N21" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="O21" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="P21">
-        <v>5787300240</v>
+        <v>39450601</v>
       </c>
       <c r="Q21">
-        <v>1914633847</v>
+        <v>49044883</v>
       </c>
       <c r="R21">
-        <v>3156092272</v>
+        <v>21826468</v>
       </c>
       <c r="S21">
-        <v>-1798278694</v>
+        <v>2477559</v>
       </c>
       <c r="T21">
-        <v>-1453689952</v>
+        <v>8094900</v>
       </c>
       <c r="U21">
-        <v>-4067648306</v>
+        <v>215154</v>
       </c>
       <c r="V21">
-        <v>-12449932055</v>
+        <v>3427734</v>
       </c>
       <c r="W21">
-        <v>-7426231074</v>
+        <v>6575528</v>
       </c>
       <c r="X21">
-        <v>-52132058866</v>
+        <v>349843</v>
       </c>
       <c r="Y21" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F22">
-        <v>1200000</v>
+        <v>2060000</v>
       </c>
       <c r="G22">
-        <v>1200000</v>
+        <v>2000000</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="I22">
-        <v>9100</v>
+        <v>20300</v>
       </c>
       <c r="J22">
-        <v>11000</v>
+        <v>22500</v>
       </c>
       <c r="K22">
-        <v>7206940</v>
+        <v>14384224</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="O22" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="P22">
-        <v>20924</v>
+        <v>5787300240</v>
       </c>
       <c r="Q22">
-        <v>27659</v>
+        <v>1914633847</v>
       </c>
       <c r="R22">
-        <v>11818</v>
+        <v>3156092272</v>
       </c>
       <c r="S22">
-        <v>2838</v>
+        <v>-1798278694</v>
       </c>
       <c r="T22">
-        <v>4563</v>
+        <v>-1453689952</v>
       </c>
       <c r="U22">
-        <v>-1222</v>
+        <v>-4067648306</v>
       </c>
       <c r="V22">
-        <v>2413</v>
+        <v>-12449932055</v>
       </c>
       <c r="W22">
-        <v>3190</v>
+        <v>-7426231074</v>
       </c>
       <c r="X22">
-        <v>-862</v>
+        <v>-52132058866</v>
       </c>
       <c r="Y22" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2827,230 +2839,230 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F23">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="G23">
-        <v>3600000</v>
+        <v>1200000</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>5000</v>
+        <v>9100</v>
       </c>
       <c r="J23">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="K23">
-        <v>17306490</v>
+        <v>7206940</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="O23" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="P23">
-        <v>21976760922</v>
+        <v>20924</v>
       </c>
       <c r="Q23">
-        <v>15839004968</v>
+        <v>27659</v>
       </c>
       <c r="R23">
-        <v>6887755932</v>
+        <v>11818</v>
       </c>
       <c r="S23">
-        <v>-2217897363</v>
+        <v>2838</v>
       </c>
       <c r="T23">
-        <v>-3403228196</v>
+        <v>4563</v>
       </c>
       <c r="U23">
-        <v>-2758864194</v>
+        <v>-1222</v>
       </c>
       <c r="V23">
-        <v>-5110677395</v>
+        <v>2413</v>
       </c>
       <c r="W23">
-        <v>-29510193610</v>
+        <v>3190</v>
       </c>
       <c r="X23">
-        <v>-2514471056</v>
+        <v>-862</v>
       </c>
       <c r="Y23" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F24">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="G24">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K24">
-        <v>12905000</v>
+        <v>17306490</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N24" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="O24" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>21976760922</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>15839004968</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>6887755932</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>-2217897363</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>-3403228196</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>-2758864194</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>-5110677395</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>-29510193610</v>
       </c>
       <c r="X24">
-        <v>0</v>
+        <v>-2514471056</v>
       </c>
       <c r="Y24" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F25">
-        <v>1049482</v>
+        <v>12500000</v>
       </c>
       <c r="G25">
-        <v>944534</v>
+        <v>12500000</v>
       </c>
       <c r="H25">
-        <v>104948</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>12800</v>
+        <v>2000</v>
       </c>
       <c r="J25">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="K25">
-        <v>6261485</v>
+        <v>12905000</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N25" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="O25" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="P25">
-        <v>34557425427</v>
+        <v>0</v>
       </c>
       <c r="Q25">
-        <v>39824841246</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>23231897516</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>3011651602</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>2384643399</v>
+        <v>0</v>
       </c>
       <c r="U25">
-        <v>4436005255</v>
+        <v>0</v>
       </c>
       <c r="V25">
-        <v>2755379556</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <v>1176755354</v>
+        <v>0</v>
       </c>
       <c r="X25">
-        <v>4046949430</v>
+        <v>0</v>
       </c>
       <c r="Y25" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -3058,76 +3070,76 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F26">
-        <v>1128720</v>
+        <v>1049482</v>
       </c>
       <c r="G26">
-        <v>1128720</v>
+        <v>944534</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>104948</v>
       </c>
       <c r="I26">
-        <v>3300</v>
+        <v>12800</v>
       </c>
       <c r="J26">
-        <v>3900</v>
+        <v>14500</v>
       </c>
       <c r="K26">
-        <v>11287196</v>
+        <v>6261485</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N26" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="O26" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="P26">
-        <v>50552623684</v>
+        <v>34557425427</v>
       </c>
       <c r="Q26">
-        <v>69013134090</v>
+        <v>39824841246</v>
       </c>
       <c r="R26">
-        <v>16887814423</v>
+        <v>23231897516</v>
       </c>
       <c r="S26">
-        <v>9027232647</v>
+        <v>3011651602</v>
       </c>
       <c r="T26">
-        <v>15707796256</v>
+        <v>2384643399</v>
       </c>
       <c r="U26">
-        <v>555562560</v>
+        <v>4436005255</v>
       </c>
       <c r="V26">
-        <v>9236341465</v>
+        <v>2755379556</v>
       </c>
       <c r="W26">
-        <v>13159994846</v>
+        <v>1176755354</v>
       </c>
       <c r="X26">
-        <v>1236029732</v>
+        <v>4046949430</v>
       </c>
       <c r="Y26" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -3135,76 +3147,76 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F27">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="G27">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>13000</v>
+        <v>3300</v>
       </c>
       <c r="J27">
-        <v>15000</v>
+        <v>3900</v>
       </c>
       <c r="K27">
-        <v>10193520</v>
+        <v>11287196</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N27" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="O27" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="P27">
-        <v>3952070068</v>
+        <v>50552623684</v>
       </c>
       <c r="Q27">
-        <v>10789274729</v>
+        <v>69013134090</v>
       </c>
       <c r="R27">
-        <v>6040367765</v>
+        <v>16887814423</v>
       </c>
       <c r="S27">
-        <v>-4741577598</v>
+        <v>9027232647</v>
       </c>
       <c r="T27">
-        <v>-3671026788</v>
+        <v>15707796256</v>
       </c>
       <c r="U27">
-        <v>-3292521363</v>
+        <v>555562560</v>
       </c>
       <c r="V27">
-        <v>-3654889267</v>
+        <v>9236341465</v>
       </c>
       <c r="W27">
-        <v>-2281074471</v>
+        <v>13159994846</v>
       </c>
       <c r="X27">
-        <v>-2539505707</v>
+        <v>1236029732</v>
       </c>
       <c r="Y27" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:25">
@@ -3212,76 +3224,153 @@
         <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F28">
+        <v>1800000</v>
+      </c>
+      <c r="G28">
+        <v>1800000</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>13000</v>
+      </c>
+      <c r="J28">
+        <v>15000</v>
+      </c>
+      <c r="K28">
+        <v>10193520</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>17000</v>
+      </c>
+      <c r="N28" t="s">
+        <v>133</v>
+      </c>
+      <c r="O28" t="s">
+        <v>157</v>
+      </c>
+      <c r="P28">
+        <v>3952070068</v>
+      </c>
+      <c r="Q28">
+        <v>10789274729</v>
+      </c>
+      <c r="R28">
+        <v>6040367765</v>
+      </c>
+      <c r="S28">
+        <v>-4741577598</v>
+      </c>
+      <c r="T28">
+        <v>-3671026788</v>
+      </c>
+      <c r="U28">
+        <v>-3292521363</v>
+      </c>
+      <c r="V28">
+        <v>-3654889267</v>
+      </c>
+      <c r="W28">
+        <v>-2281074471</v>
+      </c>
+      <c r="X28">
+        <v>-2539505707</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29">
         <v>4000000</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>4000000</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>5000</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <v>5600</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>16120000</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>6500</v>
       </c>
-      <c r="N28" t="s">
-        <v>130</v>
-      </c>
-      <c r="O28" t="s">
-        <v>154</v>
-      </c>
-      <c r="P28">
+      <c r="N29" t="s">
+        <v>134</v>
+      </c>
+      <c r="O29" t="s">
+        <v>158</v>
+      </c>
+      <c r="P29">
         <v>26691070764</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>22835113396</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>7519073723</v>
       </c>
-      <c r="S28">
+      <c r="S29">
         <v>6041270235</v>
       </c>
-      <c r="T28">
+      <c r="T29">
         <v>6705120210</v>
       </c>
-      <c r="U28">
+      <c r="U29">
         <v>982044017</v>
       </c>
-      <c r="V28">
+      <c r="V29">
         <v>5119066139</v>
       </c>
-      <c r="W28">
+      <c r="W29">
         <v>5870093710</v>
       </c>
-      <c r="X28">
+      <c r="X29">
         <v>1198587470</v>
       </c>
-      <c r="Y28" t="s">
-        <v>178</v>
+      <c r="Y29" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3299,422 +3388,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2">
         <v>27600</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3">
         <v>11000</v>
       </c>
       <c r="F3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4">
         <v>16000</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5">
         <v>43535</v>
       </c>
       <c r="F5" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6">
         <v>8858</v>
       </c>
       <c r="F6" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7">
         <v>19500</v>
       </c>
       <c r="F7" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8">
         <v>12325</v>
       </c>
       <c r="F8" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E9">
         <v>14000</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D10" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E10">
         <v>96380</v>
       </c>
       <c r="F10" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E11">
         <v>8000</v>
       </c>
       <c r="F11" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D12" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E12">
         <v>21000</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E13">
         <v>64350</v>
       </c>
       <c r="F13" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E14">
         <v>20000</v>
       </c>
       <c r="F14" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E15">
         <v>7000</v>
       </c>
       <c r="F15" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E16">
         <v>14250</v>
       </c>
       <c r="F16" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E17">
         <v>16000</v>
       </c>
       <c r="F17" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E18">
         <v>13500</v>
       </c>
       <c r="F18" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D19" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E19">
         <v>14950</v>
       </c>
       <c r="F19" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D20" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E20">
         <v>29547</v>
       </c>
       <c r="F20" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D21" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E21">
         <v>18040</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-28
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="245">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -563,6 +563,9 @@
     <t>에이피알</t>
   </si>
   <si>
+    <t>IBKS스팩24호</t>
+  </si>
+  <si>
     <t>케이웨더</t>
   </si>
   <si>
@@ -608,6 +611,9 @@
     <t>2024.01.22~01.26</t>
   </si>
   <si>
+    <t>2024.01.17~01.18</t>
+  </si>
+  <si>
     <t>2024.01.12~01.18</t>
   </si>
   <si>
@@ -644,12 +650,12 @@
     <t>2023.11.15~11.16</t>
   </si>
   <si>
-    <t>2023.11.10~11.16</t>
-  </si>
-  <si>
     <t>147,000~200,000</t>
   </si>
   <si>
+    <t>2,000~2,000</t>
+  </si>
+  <si>
     <t>4,800~5,800</t>
   </si>
   <si>
@@ -659,9 +665,6 @@
     <t>9,200~11,000</t>
   </si>
   <si>
-    <t>2,000~2,000</t>
-  </si>
-  <si>
     <t>2,400~2,800</t>
   </si>
   <si>
@@ -689,9 +692,6 @@
     <t>19,000~22,000</t>
   </si>
   <si>
-    <t>9,000~11,000</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -707,12 +707,12 @@
     <t>23000</t>
   </si>
   <si>
-    <t>9000</t>
-  </si>
-  <si>
     <t>신한투자증권,하나증권</t>
   </si>
   <si>
+    <t>아이비케이투자증권</t>
+  </si>
+  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -740,9 +740,6 @@
     <t>KB증권,NH투자증권</t>
   </si>
   <si>
-    <t>아이비케이투자증권</t>
-  </si>
-  <si>
     <t>하나증권,키움증권</t>
   </si>
   <si>
@@ -753,9 +750,6 @@
   </si>
   <si>
     <t>신영증권</t>
-  </si>
-  <si>
-    <t>유안타증권</t>
   </si>
 </sst>
 </file>
@@ -3313,10 +3307,10 @@
         <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>130</v>
@@ -3325,7 +3319,7 @@
         <v>55713</v>
       </c>
       <c r="F2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3333,19 +3327,19 @@
         <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
         <v>130</v>
       </c>
       <c r="E3">
-        <v>4800</v>
+        <v>2147483647</v>
       </c>
       <c r="F3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3353,19 +3347,19 @@
         <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
         <v>130</v>
       </c>
       <c r="E4">
-        <v>7200</v>
+        <v>4800</v>
       </c>
       <c r="F4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3373,19 +3367,19 @@
         <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
         <v>130</v>
       </c>
       <c r="E5">
-        <v>27600</v>
+        <v>7200</v>
       </c>
       <c r="F5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3393,19 +3387,19 @@
         <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
         <v>130</v>
       </c>
       <c r="E6">
-        <v>11000</v>
+        <v>27600</v>
       </c>
       <c r="F6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3413,19 +3407,19 @@
         <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D7" t="s">
         <v>130</v>
       </c>
       <c r="E7">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="F7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3433,7 +3427,7 @@
         <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
         <v>216</v>
@@ -3442,10 +3436,10 @@
         <v>130</v>
       </c>
       <c r="E8">
-        <v>43535</v>
+        <v>16000</v>
       </c>
       <c r="F8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3453,7 +3447,7 @@
         <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
         <v>217</v>
@@ -3462,10 +3456,10 @@
         <v>130</v>
       </c>
       <c r="E9">
-        <v>8858</v>
+        <v>43535</v>
       </c>
       <c r="F9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3473,7 +3467,7 @@
         <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
         <v>218</v>
@@ -3482,10 +3476,10 @@
         <v>130</v>
       </c>
       <c r="E10">
-        <v>19500</v>
+        <v>8858</v>
       </c>
       <c r="F10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3493,7 +3487,7 @@
         <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
         <v>219</v>
@@ -3502,10 +3496,10 @@
         <v>130</v>
       </c>
       <c r="E11">
-        <v>12325</v>
+        <v>19500</v>
       </c>
       <c r="F11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3513,19 +3507,19 @@
         <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>130</v>
       </c>
       <c r="E12">
-        <v>14000</v>
+        <v>12325</v>
       </c>
       <c r="F12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3533,19 +3527,19 @@
         <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E13">
-        <v>96380</v>
+        <v>14000</v>
       </c>
       <c r="F13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3553,159 +3547,159 @@
         <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E14">
-        <v>8000</v>
+        <v>96380</v>
       </c>
       <c r="F14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E15">
-        <v>21000</v>
+        <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
         <v>222</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E16">
-        <v>64350</v>
+        <v>21000</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E17">
-        <v>20000</v>
+        <v>64350</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
         <v>225</v>
       </c>
       <c r="E18">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="F18" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E19">
-        <v>14250</v>
+        <v>7000</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E20">
-        <v>16000</v>
+        <v>14250</v>
       </c>
       <c r="F20" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E21">
-        <v>13500</v>
+        <v>16000</v>
       </c>
       <c r="F21" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-29
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -563,6 +563,9 @@
     <t>에이피알</t>
   </si>
   <si>
+    <t>신영스팩10호</t>
+  </si>
+  <si>
     <t>IBKS스팩24호</t>
   </si>
   <si>
@@ -605,12 +608,12 @@
     <t>교보스팩15호</t>
   </si>
   <si>
-    <t>NH스팩30호</t>
-  </si>
-  <si>
     <t>2024.01.22~01.26</t>
   </si>
   <si>
+    <t>2024.01.22~01.23</t>
+  </si>
+  <si>
     <t>2024.01.17~01.18</t>
   </si>
   <si>
@@ -647,9 +650,6 @@
     <t>2023.11.16~11.22</t>
   </si>
   <si>
-    <t>2023.11.15~11.16</t>
-  </si>
-  <si>
     <t>147,000~200,000</t>
   </si>
   <si>
@@ -710,6 +710,9 @@
     <t>신한투자증권,하나증권</t>
   </si>
   <si>
+    <t>신영증권</t>
+  </si>
+  <si>
     <t>아이비케이투자증권</t>
   </si>
   <si>
@@ -747,9 +750,6 @@
   </si>
   <si>
     <t>교보증권</t>
-  </si>
-  <si>
-    <t>신영증권</t>
   </si>
 </sst>
 </file>
@@ -3336,7 +3336,7 @@
         <v>130</v>
       </c>
       <c r="E3">
-        <v>2147483647</v>
+        <v>9150</v>
       </c>
       <c r="F3" t="s">
         <v>231</v>
@@ -3350,13 +3350,13 @@
         <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>130</v>
       </c>
       <c r="E4">
-        <v>4800</v>
+        <v>2147483647</v>
       </c>
       <c r="F4" t="s">
         <v>232</v>
@@ -3367,16 +3367,16 @@
         <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>130</v>
       </c>
       <c r="E5">
-        <v>7200</v>
+        <v>4800</v>
       </c>
       <c r="F5" t="s">
         <v>233</v>
@@ -3390,13 +3390,13 @@
         <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
         <v>130</v>
       </c>
       <c r="E6">
-        <v>27600</v>
+        <v>7200</v>
       </c>
       <c r="F6" t="s">
         <v>234</v>
@@ -3410,13 +3410,13 @@
         <v>201</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
         <v>130</v>
       </c>
       <c r="E7">
-        <v>11000</v>
+        <v>27600</v>
       </c>
       <c r="F7" t="s">
         <v>235</v>
@@ -3430,16 +3430,16 @@
         <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D8" t="s">
         <v>130</v>
       </c>
       <c r="E8">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="F8" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3447,19 +3447,19 @@
         <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
         <v>130</v>
       </c>
       <c r="E9">
-        <v>43535</v>
+        <v>16000</v>
       </c>
       <c r="F9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3467,16 +3467,16 @@
         <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D10" t="s">
         <v>130</v>
       </c>
       <c r="E10">
-        <v>8858</v>
+        <v>43535</v>
       </c>
       <c r="F10" t="s">
         <v>237</v>
@@ -3490,13 +3490,13 @@
         <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
         <v>130</v>
       </c>
       <c r="E11">
-        <v>19500</v>
+        <v>8858</v>
       </c>
       <c r="F11" t="s">
         <v>238</v>
@@ -3507,16 +3507,16 @@
         <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D12" t="s">
         <v>130</v>
       </c>
       <c r="E12">
-        <v>12325</v>
+        <v>19500</v>
       </c>
       <c r="F12" t="s">
         <v>239</v>
@@ -3530,16 +3530,16 @@
         <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>130</v>
       </c>
       <c r="E13">
-        <v>14000</v>
+        <v>12325</v>
       </c>
       <c r="F13" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3550,16 +3550,16 @@
         <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E14">
-        <v>96380</v>
+        <v>14000</v>
       </c>
       <c r="F14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3570,53 +3570,53 @@
         <v>206</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E15">
-        <v>8000</v>
+        <v>96380</v>
       </c>
       <c r="F15" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
         <v>207</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E16">
-        <v>21000</v>
+        <v>8000</v>
       </c>
       <c r="F16" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E17">
-        <v>64350</v>
+        <v>21000</v>
       </c>
       <c r="F17" t="s">
         <v>242</v>
@@ -3624,30 +3624,30 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E18">
-        <v>20000</v>
+        <v>64350</v>
       </c>
       <c r="F18" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
         <v>212</v>
@@ -3656,27 +3656,27 @@
         <v>225</v>
       </c>
       <c r="E19">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="F19" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
         <v>209</v>
       </c>
       <c r="C20" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E20">
-        <v>14250</v>
+        <v>7000</v>
       </c>
       <c r="F20" t="s">
         <v>244</v>
@@ -3684,22 +3684,22 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>210</v>
       </c>
       <c r="C21" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E21">
-        <v>16000</v>
+        <v>14250</v>
       </c>
       <c r="F21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-12
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="196">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>14,500~18,500</t>
+  </si>
+  <si>
+    <t>30000</t>
   </si>
   <si>
     <t>20000</t>
@@ -2322,7 +2325,7 @@
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2342,7 +2345,7 @@
         <v>16500</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2362,7 +2365,7 @@
         <v>19500</v>
       </c>
       <c r="F4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2382,7 +2385,7 @@
         <v>10000</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2402,7 +2405,7 @@
         <v>19250</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2422,7 +2425,7 @@
         <v>6000</v>
       </c>
       <c r="F7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2442,7 +2445,7 @@
         <v>17400</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2462,7 +2465,7 @@
         <v>17600</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2476,13 +2479,13 @@
         <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>174</v>
       </c>
       <c r="E10">
         <v>40000</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2496,13 +2499,13 @@
         <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E11">
         <v>12870</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2516,13 +2519,13 @@
         <v>163</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E12">
         <v>10000</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2536,13 +2539,13 @@
         <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E13">
         <v>18936</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2556,13 +2559,13 @@
         <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E14">
         <v>8000</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2576,13 +2579,13 @@
         <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E15">
         <v>13000</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2596,13 +2599,13 @@
         <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E16">
         <v>8000</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2616,13 +2619,13 @@
         <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E17">
         <v>8000</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2636,13 +2639,13 @@
         <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E18">
         <v>55713</v>
       </c>
       <c r="F18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2656,13 +2659,13 @@
         <v>171</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E19">
         <v>4800</v>
       </c>
       <c r="F19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2676,13 +2679,13 @@
         <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E20">
         <v>7200</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2696,13 +2699,13 @@
         <v>173</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E21">
         <v>16385</v>
       </c>
       <c r="F21" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="202">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-02-21</t>
+  </si>
+  <si>
     <t>2024-02-16</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
     <t>2024-01-09</t>
   </si>
   <si>
+    <t>2024-02-27</t>
+  </si>
+  <si>
     <t>2024-02-22</t>
   </si>
   <si>
@@ -152,6 +158,9 @@
     <t>2024-01-10</t>
   </si>
   <si>
+    <t>2024-03-13</t>
+  </si>
+  <si>
     <t>2024-03-07</t>
   </si>
   <si>
@@ -176,6 +185,9 @@
     <t>2024-01-24</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>DB, NH</t>
   </si>
   <si>
@@ -197,9 +209,6 @@
     <t>키움</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>한화</t>
   </si>
   <si>
@@ -221,6 +230,9 @@
     <t>대신</t>
   </si>
   <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
     <t>케이엔알시스템</t>
   </si>
   <si>
@@ -269,6 +281,9 @@
     <t>대신밸런스제17호스팩</t>
   </si>
   <si>
+    <t>993.21:1</t>
+  </si>
+  <si>
     <t>873.20:1</t>
   </si>
   <si>
@@ -317,6 +332,9 @@
     <t>892.06:1</t>
   </si>
   <si>
+    <t>2.85%</t>
+  </si>
+  <si>
     <t>31.86%</t>
   </si>
   <si>
@@ -344,6 +362,9 @@
     <t>17.01%</t>
   </si>
   <si>
+    <t>생화학 측정기 및 센서, 면역진단기기 및 마커, 분자진단기기 및 시약 등</t>
+  </si>
+  <si>
     <t>특수목적 시험장비, 산업용로봇</t>
   </si>
   <si>
@@ -407,6 +428,9 @@
     <t>민테크</t>
   </si>
   <si>
+    <t>신한스팩13호</t>
+  </si>
+  <si>
     <t>신한스팩12호</t>
   </si>
   <si>
@@ -425,9 +449,6 @@
     <t>삼현</t>
   </si>
   <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
     <t>하나스팩31호</t>
   </si>
   <si>
@@ -452,6 +473,9 @@
     <t>2024.04.12~04.18</t>
   </si>
   <si>
+    <t>2024.04.04~04.05</t>
+  </si>
+  <si>
     <t>2024.03.27~03.28</t>
   </si>
   <si>
@@ -536,9 +560,6 @@
     <t>12,000~14,000</t>
   </si>
   <si>
-    <t>14,500~18,500</t>
-  </si>
-  <si>
     <t>30000</t>
   </si>
   <si>
@@ -600,9 +621,6 @@
   </si>
   <si>
     <t>키움증권</t>
-  </si>
-  <si>
-    <t>한화투자증권</t>
   </si>
 </sst>
 </file>
@@ -960,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1048,153 +1066,153 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F2">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="G2">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J2">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K2">
-        <v>10867713</v>
+        <v>14104416</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="P2">
-        <v>13884202433</v>
+        <v>132326879204</v>
       </c>
       <c r="Q2">
-        <v>51182177917</v>
+        <v>193893072828</v>
       </c>
       <c r="R2">
-        <v>8127683890</v>
+        <v>341250572142</v>
       </c>
       <c r="S2">
-        <v>-2233716995</v>
+        <v>-7083727446</v>
       </c>
       <c r="T2">
-        <v>2983031122</v>
+        <v>49300174288</v>
       </c>
       <c r="U2">
-        <v>-6655066594</v>
+        <v>150061283068</v>
       </c>
       <c r="V2">
-        <v>-5046530611</v>
+        <v>1473132550</v>
       </c>
       <c r="W2">
-        <v>1523272163</v>
+        <v>40660749810</v>
       </c>
       <c r="X2">
-        <v>-6716915237</v>
+        <v>120676291668</v>
       </c>
       <c r="Y2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F3">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="G3">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K3">
-        <v>5605000</v>
+        <v>10867713</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>13884202433</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>51182177917</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>8127683890</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>-2233716995</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>2983031122</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>-6655066594</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>-5046530611</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1523272163</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>-6716915237</v>
       </c>
       <c r="Y3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1202,22 +1220,22 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F4">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="G4">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1229,7 +1247,7 @@
         <v>2000</v>
       </c>
       <c r="K4">
-        <v>7010000</v>
+        <v>5605000</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1238,10 +1256,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1271,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1279,22 +1297,22 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1306,7 +1324,7 @@
         <v>2000</v>
       </c>
       <c r="K5">
-        <v>4155000</v>
+        <v>7010000</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1315,10 +1333,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1348,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1359,13 +1377,13 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F6">
         <v>4000000</v>
@@ -1383,7 +1401,7 @@
         <v>2000</v>
       </c>
       <c r="K6">
-        <v>4210000</v>
+        <v>4155000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1392,10 +1410,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1425,24 +1443,24 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F7">
         <v>4000000</v>
@@ -1460,7 +1478,7 @@
         <v>2000</v>
       </c>
       <c r="K7">
-        <v>4240000</v>
+        <v>4210000</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1469,10 +1487,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="O7" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1502,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1510,76 +1528,76 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="G8">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K8">
-        <v>5661970</v>
+        <v>4240000</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O8" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="P8">
-        <v>9490</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>12525</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>8916</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>1716</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>876</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1587,218 +1605,218 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F9">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="G9">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>4800</v>
+        <v>12000</v>
       </c>
       <c r="J9">
-        <v>5800</v>
+        <v>14000</v>
       </c>
       <c r="K9">
-        <v>9939614</v>
+        <v>5661970</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>7000</v>
+        <v>16000</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="P9">
-        <v>11728856090</v>
+        <v>9490</v>
       </c>
       <c r="Q9">
-        <v>17398754684</v>
+        <v>12525</v>
       </c>
       <c r="R9">
-        <v>9950753269</v>
+        <v>8916</v>
       </c>
       <c r="S9">
-        <v>210467803</v>
+        <v>154</v>
       </c>
       <c r="T9">
-        <v>768643625</v>
+        <v>1780</v>
       </c>
       <c r="U9">
-        <v>-2057246152</v>
+        <v>502</v>
       </c>
       <c r="V9">
-        <v>-1402142802</v>
+        <v>496</v>
       </c>
       <c r="W9">
-        <v>708681523</v>
+        <v>1716</v>
       </c>
       <c r="X9">
-        <v>-2027030543</v>
+        <v>876</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="G10">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J10">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K10">
-        <v>9465149</v>
+        <v>9939614</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="O10" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="P10">
-        <v>-7085110800</v>
+        <v>11728856090</v>
       </c>
       <c r="Q10">
-        <v>-7707829743</v>
+        <v>17398754684</v>
       </c>
       <c r="R10">
-        <v>-4353776321</v>
+        <v>9950753269</v>
       </c>
       <c r="S10">
-        <v>-7444566078</v>
+        <v>210467803</v>
       </c>
       <c r="T10">
-        <v>-8116734518</v>
+        <v>768643625</v>
       </c>
       <c r="U10">
-        <v>-4808043488</v>
+        <v>-2057246152</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>-1402142802</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>708681523</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>-2027030543</v>
       </c>
       <c r="Y10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="G11">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K11">
-        <v>4690000</v>
+        <v>9465149</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="O11" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>-7085110800</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>-7707829743</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>-4353776321</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>-7444566078</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>-8116734518</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>-4808043488</v>
       </c>
       <c r="V11">
         <v>0</v>
@@ -1810,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1818,73 +1836,73 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="G12">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>4225498</v>
+        <v>4690000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P12">
-        <v>84448377049</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>86585909893</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>71141473670</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>4232543828</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>2396516104</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>2260522008</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>3768461107</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>1925269107</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>1937996182</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
         <v>117</v>
@@ -1892,79 +1910,79 @@
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F13">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="G13">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>16500</v>
       </c>
       <c r="K13">
-        <v>4230000</v>
+        <v>4225498</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>84448377049</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>86585909893</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>71141473670</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>4232543828</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>2396516104</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>2260522008</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>3768461107</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>1925269107</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>1937996182</v>
       </c>
       <c r="Y13" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1972,76 +1990,76 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F14">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="G14">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J14">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K14">
-        <v>9355485</v>
+        <v>4230000</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P14">
-        <v>91496346476</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>91488384999</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>63460787949</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>9436568051</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>11992232752</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>8323875572</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <v>8609153489</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>6967992579</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <v>7769366120</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2049,153 +2067,153 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F15">
-        <v>8707000</v>
+        <v>1500000</v>
       </c>
       <c r="G15">
-        <v>5224000</v>
+        <v>1500000</v>
       </c>
       <c r="H15">
-        <v>3483000</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J15">
-        <v>6300</v>
+        <v>15000</v>
       </c>
       <c r="K15">
-        <v>34824000</v>
+        <v>9355485</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>7300</v>
+        <v>18000</v>
       </c>
       <c r="N15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="O15" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P15">
-        <v>120971135005</v>
+        <v>91496346476</v>
       </c>
       <c r="Q15">
-        <v>144752544468</v>
+        <v>91488384999</v>
       </c>
       <c r="R15">
-        <v>134349576051</v>
+        <v>63460787949</v>
       </c>
       <c r="S15">
-        <v>6228818073</v>
+        <v>9436568051</v>
       </c>
       <c r="T15">
-        <v>3756954475</v>
+        <v>11992232752</v>
       </c>
       <c r="U15">
-        <v>11092990558</v>
+        <v>8323875572</v>
       </c>
       <c r="V15">
-        <v>4708568182</v>
+        <v>8609153489</v>
       </c>
       <c r="W15">
-        <v>4366217534</v>
+        <v>6967992579</v>
       </c>
       <c r="X15">
-        <v>7277173431</v>
+        <v>7769366120</v>
       </c>
       <c r="Y15" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F16">
-        <v>2060000</v>
+        <v>8707000</v>
       </c>
       <c r="G16">
-        <v>2060000</v>
+        <v>5224000</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>3483000</v>
       </c>
       <c r="I16">
-        <v>4300</v>
+        <v>5000</v>
       </c>
       <c r="J16">
-        <v>4900</v>
+        <v>6300</v>
       </c>
       <c r="K16">
-        <v>9271339</v>
+        <v>34824000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>5300</v>
+        <v>7300</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O16" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P16">
-        <v>31236794775</v>
+        <v>120971135005</v>
       </c>
       <c r="Q16">
-        <v>37364336431</v>
+        <v>144752544468</v>
       </c>
       <c r="R16">
-        <v>30398728955</v>
+        <v>134349576051</v>
       </c>
       <c r="S16">
-        <v>4950804374</v>
+        <v>6228818073</v>
       </c>
       <c r="T16">
-        <v>5673304262</v>
+        <v>3756954475</v>
       </c>
       <c r="U16">
-        <v>5874298651</v>
+        <v>11092990558</v>
       </c>
       <c r="V16">
-        <v>4470133667</v>
+        <v>4708568182</v>
       </c>
       <c r="W16">
-        <v>4761400117</v>
+        <v>4366217534</v>
       </c>
       <c r="X16">
-        <v>4532708708</v>
+        <v>7277173431</v>
       </c>
       <c r="Y16" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2203,76 +2221,153 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F17">
+        <v>2060000</v>
+      </c>
+      <c r="G17">
+        <v>2060000</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>4300</v>
+      </c>
+      <c r="J17">
+        <v>4900</v>
+      </c>
+      <c r="K17">
+        <v>9271339</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>5300</v>
+      </c>
+      <c r="N17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P17">
+        <v>31236794775</v>
+      </c>
+      <c r="Q17">
+        <v>37364336431</v>
+      </c>
+      <c r="R17">
+        <v>30398728955</v>
+      </c>
+      <c r="S17">
+        <v>4950804374</v>
+      </c>
+      <c r="T17">
+        <v>5673304262</v>
+      </c>
+      <c r="U17">
+        <v>5874298651</v>
+      </c>
+      <c r="V17">
+        <v>4470133667</v>
+      </c>
+      <c r="W17">
+        <v>4761400117</v>
+      </c>
+      <c r="X17">
+        <v>4532708708</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18">
         <v>5500000</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>5500000</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>2000</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>2000</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>6060000</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>2000</v>
       </c>
-      <c r="N17" t="s">
-        <v>99</v>
-      </c>
-      <c r="O17" t="s">
-        <v>101</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>113</v>
+      <c r="N18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O18" t="s">
+        <v>107</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2290,399 +2385,399 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E3">
         <v>16500</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E4">
         <v>19500</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E5">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E6">
-        <v>19250</v>
+        <v>10000</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E7">
-        <v>6000</v>
+        <v>19250</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E8">
-        <v>17400</v>
+        <v>6000</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E9">
-        <v>17600</v>
+        <v>17400</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>107</v>
       </c>
       <c r="E10">
-        <v>40000</v>
+        <v>17600</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E11">
-        <v>12870</v>
+        <v>40000</v>
       </c>
       <c r="F11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="E12">
-        <v>10000</v>
+        <v>12870</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E13">
-        <v>18936</v>
+        <v>10000</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E14">
-        <v>8000</v>
+        <v>18936</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E15">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E16">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="F16" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E17">
         <v>8000</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E18">
-        <v>55713</v>
+        <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E19">
-        <v>4800</v>
+        <v>55713</v>
       </c>
       <c r="F19" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E20">
-        <v>7200</v>
+        <v>4800</v>
       </c>
       <c r="F20" t="s">
         <v>194</v>
@@ -2690,22 +2785,22 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E21">
-        <v>16385</v>
+        <v>7200</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-16
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="200">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -428,6 +428,9 @@
     <t>민테크</t>
   </si>
   <si>
+    <t>하나스팩33호</t>
+  </si>
+  <si>
     <t>신한스팩13호</t>
   </si>
   <si>
@@ -473,6 +476,9 @@
     <t>2024.04.12~04.18</t>
   </si>
   <si>
+    <t>2024.04.08~04.09</t>
+  </si>
+  <si>
     <t>2024.04.04~04.05</t>
   </si>
   <si>
@@ -518,9 +524,6 @@
     <t>2024.02.01~02.07</t>
   </si>
   <si>
-    <t>2024.01.29~02.02</t>
-  </si>
-  <si>
     <t>8,700~11,500</t>
   </si>
   <si>
@@ -557,7 +560,7 @@
     <t>4,800~5,800</t>
   </si>
   <si>
-    <t>12,000~14,000</t>
+    <t>2000</t>
   </si>
   <si>
     <t>20000</t>
@@ -566,9 +569,6 @@
     <t>30000</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>13500</t>
   </si>
   <si>
@@ -578,9 +578,6 @@
     <t>7000</t>
   </si>
   <si>
-    <t>16000</t>
-  </si>
-  <si>
     <t>삼성증권</t>
   </si>
   <si>
@@ -590,15 +587,15 @@
     <t>KB증권</t>
   </si>
   <si>
+    <t>하나증권</t>
+  </si>
+  <si>
     <t>신한투자증권</t>
   </si>
   <si>
     <t>미래에셋증권</t>
   </si>
   <si>
-    <t>하나증권</t>
-  </si>
-  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -618,9 +615,6 @@
   </si>
   <si>
     <t>신한투자증권,하나증권</t>
-  </si>
-  <si>
-    <t>키움증권</t>
   </si>
 </sst>
 </file>
@@ -2408,10 +2402,10 @@
         <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
         <v>107</v>
@@ -2420,7 +2414,7 @@
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2428,10 +2422,10 @@
         <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
         <v>107</v>
@@ -2440,7 +2434,7 @@
         <v>16500</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2448,10 +2442,10 @@
         <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
         <v>107</v>
@@ -2460,7 +2454,7 @@
         <v>19500</v>
       </c>
       <c r="F4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2468,19 +2462,19 @@
         <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
         <v>107</v>
       </c>
       <c r="E5">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2488,16 +2482,16 @@
         <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
         <v>107</v>
       </c>
       <c r="E6">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="F6" t="s">
         <v>191</v>
@@ -2508,7 +2502,7 @@
         <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>172</v>
@@ -2517,10 +2511,10 @@
         <v>107</v>
       </c>
       <c r="E7">
-        <v>19250</v>
+        <v>10000</v>
       </c>
       <c r="F7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2528,19 +2522,19 @@
         <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
         <v>107</v>
       </c>
       <c r="E8">
-        <v>6000</v>
+        <v>19250</v>
       </c>
       <c r="F8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2548,19 +2542,19 @@
         <v>141</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>181</v>
       </c>
       <c r="E9">
-        <v>17400</v>
+        <v>6000</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2568,19 +2562,19 @@
         <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
         <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="E10">
-        <v>17600</v>
+        <v>17400</v>
       </c>
       <c r="F10" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2588,7 +2582,7 @@
         <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
         <v>175</v>
@@ -2597,47 +2591,47 @@
         <v>182</v>
       </c>
       <c r="E11">
-        <v>40000</v>
+        <v>17600</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
         <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E12">
-        <v>12870</v>
+        <v>40000</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13">
-        <v>10000</v>
+        <v>12870</v>
       </c>
       <c r="F13" t="s">
         <v>193</v>
@@ -2645,42 +2639,42 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14">
-        <v>18936</v>
+        <v>10000</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E15">
-        <v>8000</v>
+        <v>18936</v>
       </c>
       <c r="F15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2688,59 +2682,59 @@
         <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E16">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="F16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E17">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="F17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2748,59 +2742,59 @@
         <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E19">
-        <v>55713</v>
+        <v>8000</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
         <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E20">
-        <v>4800</v>
+        <v>55713</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C21" t="s">
         <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21">
-        <v>7200</v>
+        <v>4800</v>
       </c>
       <c r="F21" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-21
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="206">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-02-29</t>
+  </si>
+  <si>
     <t>2024-02-21</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>2024-01-09</t>
   </si>
   <si>
+    <t>2024-03-07</t>
+  </si>
+  <si>
     <t>2024-02-27</t>
   </si>
   <si>
@@ -158,18 +164,15 @@
     <t>2024-01-10</t>
   </si>
   <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
     <t>2024-03-13</t>
   </si>
   <si>
-    <t>2024-03-07</t>
-  </si>
-  <si>
     <t>2024-03-05</t>
   </si>
   <si>
-    <t>2024-02-29</t>
-  </si>
-  <si>
     <t>2024-03-04</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
     <t>2024-01-24</t>
   </si>
   <si>
+    <t>한국</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -230,6 +236,9 @@
     <t>대신</t>
   </si>
   <si>
+    <t>삼현</t>
+  </si>
+  <si>
     <t>오상헬스케어</t>
   </si>
   <si>
@@ -281,6 +290,9 @@
     <t>대신밸런스제17호스팩</t>
   </si>
   <si>
+    <t>649.11:1</t>
+  </si>
+  <si>
     <t>993.21:1</t>
   </si>
   <si>
@@ -332,6 +344,9 @@
     <t>892.06:1</t>
   </si>
   <si>
+    <t>10.64%</t>
+  </si>
+  <si>
     <t>2.85%</t>
   </si>
   <si>
@@ -362,6 +377,9 @@
     <t>17.01%</t>
   </si>
   <si>
+    <t>스마트 액추에이터, 스마트 파워유닛</t>
+  </si>
+  <si>
     <t>생화학 측정기 및 센서, 면역진단기기 및 마커, 분자진단기기 및 시약 등</t>
   </si>
   <si>
@@ -450,9 +468,6 @@
   </si>
   <si>
     <t>엔젤로보틱스</t>
-  </si>
-  <si>
-    <t>삼현</t>
   </si>
   <si>
     <t>하나스팩31호</t>
@@ -975,7 +990,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1063,76 +1078,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="G2">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J2">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K2">
-        <v>14104416</v>
+        <v>10569189</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="P2">
-        <v>132326879204</v>
+        <v>59096247022</v>
       </c>
       <c r="Q2">
-        <v>193893072828</v>
+        <v>68617808568</v>
       </c>
       <c r="R2">
-        <v>341250572142</v>
+        <v>72737982928</v>
       </c>
       <c r="S2">
-        <v>-7083727446</v>
+        <v>3774225460</v>
       </c>
       <c r="T2">
-        <v>49300174288</v>
+        <v>2753382474</v>
       </c>
       <c r="U2">
-        <v>150061283068</v>
+        <v>8000270581</v>
       </c>
       <c r="V2">
-        <v>1473132550</v>
+        <v>3791818673</v>
       </c>
       <c r="W2">
-        <v>40660749810</v>
+        <v>3322524020</v>
       </c>
       <c r="X2">
-        <v>120676291668</v>
+        <v>7223298574</v>
       </c>
       <c r="Y2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1140,153 +1155,153 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F3">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="G3">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J3">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K3">
-        <v>10867713</v>
+        <v>14104416</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="P3">
-        <v>13884202433</v>
+        <v>132326879204</v>
       </c>
       <c r="Q3">
-        <v>51182177917</v>
+        <v>193893072828</v>
       </c>
       <c r="R3">
-        <v>8127683890</v>
+        <v>341250572142</v>
       </c>
       <c r="S3">
-        <v>-2233716995</v>
+        <v>-7083727446</v>
       </c>
       <c r="T3">
-        <v>2983031122</v>
+        <v>49300174288</v>
       </c>
       <c r="U3">
-        <v>-6655066594</v>
+        <v>150061283068</v>
       </c>
       <c r="V3">
-        <v>-5046530611</v>
+        <v>1473132550</v>
       </c>
       <c r="W3">
-        <v>1523272163</v>
+        <v>40660749810</v>
       </c>
       <c r="X3">
-        <v>-6716915237</v>
+        <v>120676291668</v>
       </c>
       <c r="Y3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="G4">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K4">
-        <v>5605000</v>
+        <v>10867713</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="O4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>13884202433</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>51182177917</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>8127683890</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>-2233716995</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>2983031122</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>-6655066594</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>-5046530611</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1523272163</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>-6716915237</v>
       </c>
       <c r="Y4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1294,22 +1309,22 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="G5">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1321,7 +1336,7 @@
         <v>2000</v>
       </c>
       <c r="K5">
-        <v>7010000</v>
+        <v>5605000</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1330,10 +1345,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1363,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1371,22 +1386,22 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="G6">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1398,7 +1413,7 @@
         <v>2000</v>
       </c>
       <c r="K6">
-        <v>4155000</v>
+        <v>7010000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1407,10 +1422,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="O6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1440,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1451,13 +1466,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F7">
         <v>4000000</v>
@@ -1475,7 +1490,7 @@
         <v>2000</v>
       </c>
       <c r="K7">
-        <v>4210000</v>
+        <v>4155000</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1484,10 +1499,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1517,24 +1532,24 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F8">
         <v>4000000</v>
@@ -1552,7 +1567,7 @@
         <v>2000</v>
       </c>
       <c r="K8">
-        <v>4240000</v>
+        <v>4210000</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1561,10 +1576,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1594,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1602,76 +1617,76 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="G9">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J9">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K9">
-        <v>5661970</v>
+        <v>4240000</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="P9">
-        <v>9490</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>12525</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>8916</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>1716</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>876</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1679,158 +1694,158 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F10">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="G10">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>4800</v>
+        <v>12000</v>
       </c>
       <c r="J10">
-        <v>5800</v>
+        <v>14000</v>
       </c>
       <c r="K10">
-        <v>9939614</v>
+        <v>5661970</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>7000</v>
+        <v>16000</v>
       </c>
       <c r="N10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P10">
-        <v>11728856090</v>
+        <v>9490</v>
       </c>
       <c r="Q10">
-        <v>17398754684</v>
+        <v>12525</v>
       </c>
       <c r="R10">
-        <v>9950753269</v>
+        <v>8916</v>
       </c>
       <c r="S10">
-        <v>210467803</v>
+        <v>154</v>
       </c>
       <c r="T10">
-        <v>768643625</v>
+        <v>1780</v>
       </c>
       <c r="U10">
-        <v>-2057246152</v>
+        <v>502</v>
       </c>
       <c r="V10">
-        <v>-1402142802</v>
+        <v>496</v>
       </c>
       <c r="W10">
-        <v>708681523</v>
+        <v>1716</v>
       </c>
       <c r="X10">
-        <v>-2027030543</v>
+        <v>876</v>
       </c>
       <c r="Y10" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F11">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="G11">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J11">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K11">
-        <v>9465149</v>
+        <v>9939614</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="P11">
-        <v>-7085110800</v>
+        <v>11728856090</v>
       </c>
       <c r="Q11">
-        <v>-7707829743</v>
+        <v>17398754684</v>
       </c>
       <c r="R11">
-        <v>-4353776321</v>
+        <v>9950753269</v>
       </c>
       <c r="S11">
-        <v>-7444566078</v>
+        <v>210467803</v>
       </c>
       <c r="T11">
-        <v>-8116734518</v>
+        <v>768643625</v>
       </c>
       <c r="U11">
-        <v>-4808043488</v>
+        <v>-2057246152</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>-1402142802</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>708681523</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>-2027030543</v>
       </c>
       <c r="Y11" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -1839,58 +1854,58 @@
         <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="G12">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K12">
-        <v>4690000</v>
+        <v>9465149</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O12" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>-7085110800</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>-7707829743</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>-4353776321</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>-7444566078</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>-8116734518</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>-4808043488</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1902,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1910,153 +1925,153 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F13">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="G13">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J13">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K13">
-        <v>4225498</v>
+        <v>4690000</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="P13">
-        <v>84448377049</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>86585909893</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>71141473670</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>4232543828</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>2396516104</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>2260522008</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>3768461107</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>1925269107</v>
+        <v>0</v>
       </c>
       <c r="X13">
-        <v>1937996182</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F14">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="G14">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>16500</v>
       </c>
       <c r="K14">
-        <v>4230000</v>
+        <v>4225498</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O14" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>84448377049</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>86585909893</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>71141473670</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>4232543828</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>2396516104</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>2260522008</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>3768461107</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>1925269107</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>1937996182</v>
       </c>
       <c r="Y14" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2064,76 +2079,76 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F15">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="G15">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J15">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
-        <v>9355485</v>
+        <v>4230000</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O15" t="s">
         <v>112</v>
       </c>
       <c r="P15">
-        <v>91496346476</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>91488384999</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>63460787949</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>9436568051</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>11992232752</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>8323875572</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>8609153489</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>6967992579</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>7769366120</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2141,153 +2156,153 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F16">
-        <v>8707000</v>
+        <v>1500000</v>
       </c>
       <c r="G16">
-        <v>5224000</v>
+        <v>1500000</v>
       </c>
       <c r="H16">
-        <v>3483000</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J16">
-        <v>6300</v>
+        <v>15000</v>
       </c>
       <c r="K16">
-        <v>34824000</v>
+        <v>9355485</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>7300</v>
+        <v>18000</v>
       </c>
       <c r="N16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="P16">
-        <v>120971135005</v>
+        <v>91496346476</v>
       </c>
       <c r="Q16">
-        <v>144752544468</v>
+        <v>91488384999</v>
       </c>
       <c r="R16">
-        <v>134349576051</v>
+        <v>63460787949</v>
       </c>
       <c r="S16">
-        <v>6228818073</v>
+        <v>9436568051</v>
       </c>
       <c r="T16">
-        <v>3756954475</v>
+        <v>11992232752</v>
       </c>
       <c r="U16">
-        <v>11092990558</v>
+        <v>8323875572</v>
       </c>
       <c r="V16">
-        <v>4708568182</v>
+        <v>8609153489</v>
       </c>
       <c r="W16">
-        <v>4366217534</v>
+        <v>6967992579</v>
       </c>
       <c r="X16">
-        <v>7277173431</v>
+        <v>7769366120</v>
       </c>
       <c r="Y16" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F17">
-        <v>2060000</v>
+        <v>8707000</v>
       </c>
       <c r="G17">
-        <v>2060000</v>
+        <v>5224000</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>3483000</v>
       </c>
       <c r="I17">
-        <v>4300</v>
+        <v>5000</v>
       </c>
       <c r="J17">
-        <v>4900</v>
+        <v>6300</v>
       </c>
       <c r="K17">
-        <v>9271339</v>
+        <v>34824000</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>5300</v>
+        <v>7300</v>
       </c>
       <c r="N17" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O17" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="P17">
-        <v>31236794775</v>
+        <v>120971135005</v>
       </c>
       <c r="Q17">
-        <v>37364336431</v>
+        <v>144752544468</v>
       </c>
       <c r="R17">
-        <v>30398728955</v>
+        <v>134349576051</v>
       </c>
       <c r="S17">
-        <v>4950804374</v>
+        <v>6228818073</v>
       </c>
       <c r="T17">
-        <v>5673304262</v>
+        <v>3756954475</v>
       </c>
       <c r="U17">
-        <v>5874298651</v>
+        <v>11092990558</v>
       </c>
       <c r="V17">
-        <v>4470133667</v>
+        <v>4708568182</v>
       </c>
       <c r="W17">
-        <v>4761400117</v>
+        <v>4366217534</v>
       </c>
       <c r="X17">
-        <v>4532708708</v>
+        <v>7277173431</v>
       </c>
       <c r="Y17" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2295,76 +2310,153 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F18">
+        <v>2060000</v>
+      </c>
+      <c r="G18">
+        <v>2060000</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>4300</v>
+      </c>
+      <c r="J18">
+        <v>4900</v>
+      </c>
+      <c r="K18">
+        <v>9271339</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>5300</v>
+      </c>
+      <c r="N18" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" t="s">
+        <v>119</v>
+      </c>
+      <c r="P18">
+        <v>31236794775</v>
+      </c>
+      <c r="Q18">
+        <v>37364336431</v>
+      </c>
+      <c r="R18">
+        <v>30398728955</v>
+      </c>
+      <c r="S18">
+        <v>4950804374</v>
+      </c>
+      <c r="T18">
+        <v>5673304262</v>
+      </c>
+      <c r="U18">
+        <v>5874298651</v>
+      </c>
+      <c r="V18">
+        <v>4470133667</v>
+      </c>
+      <c r="W18">
+        <v>4761400117</v>
+      </c>
+      <c r="X18">
+        <v>4532708708</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19">
         <v>5500000</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>5500000</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>2000</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>2000</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <v>6060000</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>2000</v>
       </c>
-      <c r="N18" t="s">
-        <v>104</v>
-      </c>
-      <c r="O18" t="s">
-        <v>107</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>120</v>
+      <c r="N19" t="s">
+        <v>108</v>
+      </c>
+      <c r="O19" t="s">
+        <v>112</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2382,422 +2474,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E3">
         <v>17400</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E4">
         <v>16500</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E5">
         <v>19500</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E6">
         <v>7000</v>
       </c>
       <c r="F6" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E7">
         <v>36000</v>
       </c>
       <c r="F7" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E8">
         <v>6000</v>
       </c>
       <c r="F8" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E9">
         <v>10000</v>
       </c>
       <c r="F9" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E10">
         <v>19250</v>
       </c>
       <c r="F10" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E11">
         <v>6000</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E12">
         <v>17600</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E13">
         <v>40000</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E14">
         <v>12870</v>
       </c>
       <c r="F14" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E15">
         <v>10000</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E16">
         <v>18936</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E17">
         <v>8000</v>
       </c>
       <c r="F17" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E18">
         <v>13000</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E19">
         <v>8000</v>
       </c>
       <c r="F19" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E21">
         <v>55713</v>
       </c>
       <c r="F21" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-25
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="193">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -128,9 +128,6 @@
     <t>2024-01-08</t>
   </si>
   <si>
-    <t>2024-01-09</t>
-  </si>
-  <si>
     <t>2024-03-07</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>2024-01-12</t>
   </si>
   <si>
-    <t>2024-01-10</t>
-  </si>
-  <si>
     <t>2024-03-21</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>2024-01-26</t>
   </si>
   <si>
-    <t>2024-01-24</t>
-  </si>
-  <si>
     <t>한국</t>
   </si>
   <si>
@@ -230,12 +221,6 @@
     <t>미래</t>
   </si>
   <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
     <t>삼현</t>
   </si>
   <si>
@@ -284,12 +269,6 @@
     <t>현대힘스</t>
   </si>
   <si>
-    <t>우진엔텍</t>
-  </si>
-  <si>
-    <t>대신밸런스제17호스팩</t>
-  </si>
-  <si>
     <t>649.11:1</t>
   </si>
   <si>
@@ -338,12 +317,6 @@
     <t>680.82:1</t>
   </si>
   <si>
-    <t>1,263.32:1</t>
-  </si>
-  <si>
-    <t>892.06:1</t>
-  </si>
-  <si>
     <t>10.64%</t>
   </si>
   <si>
@@ -374,9 +347,6 @@
     <t>11.98%</t>
   </si>
   <si>
-    <t>17.01%</t>
-  </si>
-  <si>
     <t>스마트 액추에이터, 스마트 파워유닛</t>
   </si>
   <si>
@@ -414,9 +384,6 @@
   </si>
   <si>
     <t>선박기자재 (선박 블록, 보강재, 도장 등)</t>
-  </si>
-  <si>
-    <t>발전소 계측제어설비 정비 서비스</t>
   </si>
   <si>
     <t>종목명</t>
@@ -984,7 +951,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1072,16 +1039,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F2">
         <v>2000000</v>
@@ -1108,10 +1075,10 @@
         <v>30000</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P2">
         <v>59096247022</v>
@@ -1141,7 +1108,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1149,16 +1116,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F3">
         <v>990000</v>
@@ -1185,10 +1152,10 @@
         <v>20000</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="P3">
         <v>132326879204</v>
@@ -1218,7 +1185,7 @@
         <v>120676291668</v>
       </c>
       <c r="Y3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1226,16 +1193,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F4">
         <v>2104000</v>
@@ -1262,10 +1229,10 @@
         <v>13500</v>
       </c>
       <c r="N4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="P4">
         <v>13884202433</v>
@@ -1295,7 +1262,7 @@
         <v>-6716915237</v>
       </c>
       <c r="Y4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1303,16 +1270,16 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F5">
         <v>5000000</v>
@@ -1339,10 +1306,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="O5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1372,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1386,10 +1353,10 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F6">
         <v>6500000</v>
@@ -1416,10 +1383,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="O6" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1449,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1460,13 +1427,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F7">
         <v>4000000</v>
@@ -1493,10 +1460,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="O7" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1526,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1537,13 +1504,13 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F8">
         <v>4000000</v>
@@ -1570,10 +1537,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="O8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1603,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1617,10 +1584,10 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1647,10 +1614,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="O9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1680,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1688,16 +1655,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <v>600000</v>
@@ -1724,10 +1691,10 @@
         <v>16000</v>
       </c>
       <c r="N10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="O10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="P10">
         <v>9490</v>
@@ -1757,7 +1724,7 @@
         <v>876</v>
       </c>
       <c r="Y10" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1765,16 +1732,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>1000000</v>
@@ -1801,10 +1768,10 @@
         <v>7000</v>
       </c>
       <c r="N11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="P11">
         <v>11728856090</v>
@@ -1834,7 +1801,7 @@
         <v>-2027030543</v>
       </c>
       <c r="Y11" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1842,16 +1809,16 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F12">
         <v>1130000</v>
@@ -1878,10 +1845,10 @@
         <v>20000</v>
       </c>
       <c r="N12" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="O12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="P12">
         <v>-7085110800</v>
@@ -1911,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1919,16 +1886,16 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F13">
         <v>4575000</v>
@@ -1955,10 +1922,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="O13" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1988,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1996,16 +1963,16 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F14">
         <v>850000</v>
@@ -2032,10 +1999,10 @@
         <v>18000</v>
       </c>
       <c r="N14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="P14">
         <v>84448377049</v>
@@ -2065,7 +2032,7 @@
         <v>1937996182</v>
       </c>
       <c r="Y14" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2073,16 +2040,16 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>4000000</v>
@@ -2109,10 +2076,10 @@
         <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="O15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2142,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2150,16 +2117,16 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <v>1500000</v>
@@ -2186,10 +2153,10 @@
         <v>18000</v>
       </c>
       <c r="N16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="P16">
         <v>91496346476</v>
@@ -2219,7 +2186,7 @@
         <v>7769366120</v>
       </c>
       <c r="Y16" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2227,16 +2194,16 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F17">
         <v>8707000</v>
@@ -2263,10 +2230,10 @@
         <v>7300</v>
       </c>
       <c r="N17" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="O17" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="P17">
         <v>120971135005</v>
@@ -2296,161 +2263,7 @@
         <v>7277173431</v>
       </c>
       <c r="Y17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18">
-        <v>2060000</v>
-      </c>
-      <c r="G18">
-        <v>2060000</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>4300</v>
-      </c>
-      <c r="J18">
-        <v>4900</v>
-      </c>
-      <c r="K18">
-        <v>9271339</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>5300</v>
-      </c>
-      <c r="N18" t="s">
-        <v>107</v>
-      </c>
-      <c r="O18" t="s">
-        <v>119</v>
-      </c>
-      <c r="P18">
-        <v>31236794775</v>
-      </c>
-      <c r="Q18">
-        <v>37364336431</v>
-      </c>
-      <c r="R18">
-        <v>30398728955</v>
-      </c>
-      <c r="S18">
-        <v>4950804374</v>
-      </c>
-      <c r="T18">
-        <v>5673304262</v>
-      </c>
-      <c r="U18">
-        <v>5874298651</v>
-      </c>
-      <c r="V18">
-        <v>4470133667</v>
-      </c>
-      <c r="W18">
-        <v>4761400117</v>
-      </c>
-      <c r="X18">
-        <v>4532708708</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19">
-        <v>5500000</v>
-      </c>
-      <c r="G19">
-        <v>5500000</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>2000</v>
-      </c>
-      <c r="J19">
-        <v>2000</v>
-      </c>
-      <c r="K19">
-        <v>6060000</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>2000</v>
-      </c>
-      <c r="N19" t="s">
-        <v>108</v>
-      </c>
-      <c r="O19" t="s">
-        <v>112</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2468,422 +2281,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E3">
         <v>25610</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E4">
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <v>16500</v>
       </c>
       <c r="F5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E6">
         <v>10300</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <v>19500</v>
       </c>
       <c r="F7" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>7000</v>
       </c>
       <c r="F8" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E9">
         <v>36000</v>
       </c>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>6000</v>
       </c>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E11">
         <v>10000</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E12">
         <v>19250</v>
       </c>
       <c r="F12" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E13">
         <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E14">
         <v>17600</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E15">
         <v>40000</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E16">
         <v>12870</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E17">
         <v>10000</v>
       </c>
       <c r="F17" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D18" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E18">
         <v>18936</v>
       </c>
       <c r="F18" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E19">
         <v>8000</v>
       </c>
       <c r="F19" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E20">
         <v>13000</v>
       </c>
       <c r="F20" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E21">
         <v>8000</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-26
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="199">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-03-06</t>
+  </si>
+  <si>
     <t>2024-02-29</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>2024-01-08</t>
   </si>
   <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
     <t>2024-03-07</t>
   </si>
   <si>
@@ -158,6 +164,9 @@
     <t>2024-01-12</t>
   </si>
   <si>
+    <t>2024-03-26</t>
+  </si>
+  <si>
     <t>2024-03-21</t>
   </si>
   <si>
@@ -179,12 +188,12 @@
     <t>2024-01-26</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>한국</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>DB, NH</t>
   </si>
   <si>
@@ -221,6 +230,9 @@
     <t>미래</t>
   </si>
   <si>
+    <t>엔젤로보틱스</t>
+  </si>
+  <si>
     <t>삼현</t>
   </si>
   <si>
@@ -269,6 +281,9 @@
     <t>현대힘스</t>
   </si>
   <si>
+    <t>1,157.0:1</t>
+  </si>
+  <si>
     <t>649.11:1</t>
   </si>
   <si>
@@ -317,6 +332,9 @@
     <t>680.82:1</t>
   </si>
   <si>
+    <t>16.67%</t>
+  </si>
+  <si>
     <t>10.64%</t>
   </si>
   <si>
@@ -347,6 +365,9 @@
     <t>11.98%</t>
   </si>
   <si>
+    <t>재활 전문 웨어러블 로봇, 근력 보조 무동력 웨어러블 슈트, 일상생활 보조 웨어러블 로봇 등</t>
+  </si>
+  <si>
     <t>스마트 액추에이터, 스마트 파워유닛</t>
   </si>
   <si>
@@ -413,6 +434,9 @@
     <t>이노그리드</t>
   </si>
   <si>
+    <t>SK증권스팩12호</t>
+  </si>
+  <si>
     <t>코칩</t>
   </si>
   <si>
@@ -440,9 +464,6 @@
     <t>하나스팩32호</t>
   </si>
   <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
     <t>하나스팩31호</t>
   </si>
   <si>
@@ -461,6 +482,9 @@
     <t>2024.04.18~04.24</t>
   </si>
   <si>
+    <t>2024.04.17~04.18</t>
+  </si>
+  <si>
     <t>2024.04.15~04.19</t>
   </si>
   <si>
@@ -509,9 +533,6 @@
     <t>2024.02.14~02.15</t>
   </si>
   <si>
-    <t>2024.02.13~02.14</t>
-  </si>
-  <si>
     <t>8,700~11,500</t>
   </si>
   <si>
@@ -521,12 +542,12 @@
     <t>29,000~35,000</t>
   </si>
   <si>
+    <t>2,000~2,000</t>
+  </si>
+  <si>
     <t>11,000~14,000</t>
   </si>
   <si>
-    <t>2,000~2,000</t>
-  </si>
-  <si>
     <t>6,500~8,500</t>
   </si>
   <si>
@@ -548,6 +569,9 @@
     <t>9,000~11,000</t>
   </si>
   <si>
+    <t>13000</t>
+  </si>
+  <si>
     <t>2000</t>
   </si>
   <si>
@@ -569,6 +593,9 @@
     <t>한국투자증권</t>
   </si>
   <si>
+    <t>SK증권</t>
+  </si>
+  <si>
     <t>유안타증권</t>
   </si>
   <si>
@@ -578,9 +605,6 @@
     <t>하나증권</t>
   </si>
   <si>
-    <t>케이비증권</t>
-  </si>
-  <si>
     <t>신한투자증권</t>
   </si>
   <si>
@@ -588,12 +612,6 @@
   </si>
   <si>
     <t>DB금융투자,NH투자증권</t>
-  </si>
-  <si>
-    <t>SK증권</t>
-  </si>
-  <si>
-    <t>유진증권</t>
   </si>
 </sst>
 </file>
@@ -951,7 +969,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1039,76 +1057,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F2">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="G2">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
+        <v>11000</v>
+      </c>
+      <c r="J2">
+        <v>15000</v>
+      </c>
+      <c r="K2">
+        <v>14014976</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
         <v>20000</v>
       </c>
-      <c r="J2">
-        <v>25000</v>
-      </c>
-      <c r="K2">
-        <v>10569189</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>30000</v>
-      </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="P2">
-        <v>59096247022</v>
+        <v>813929</v>
       </c>
       <c r="Q2">
-        <v>68617808568</v>
+        <v>2184312</v>
       </c>
       <c r="R2">
-        <v>72737982928</v>
+        <v>3744252</v>
       </c>
       <c r="S2">
-        <v>3774225460</v>
+        <v>-4828658</v>
       </c>
       <c r="T2">
-        <v>2753382474</v>
+        <v>-7101029</v>
       </c>
       <c r="U2">
-        <v>8000270581</v>
+        <v>-4926381</v>
       </c>
       <c r="V2">
-        <v>3791818673</v>
+        <v>-24094044</v>
       </c>
       <c r="W2">
-        <v>3322524020</v>
+        <v>-6797310</v>
       </c>
       <c r="X2">
-        <v>7223298574</v>
+        <v>-7817567</v>
       </c>
       <c r="Y2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1116,76 +1134,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F3">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="G3">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J3">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K3">
-        <v>14104416</v>
+        <v>10569189</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="P3">
-        <v>132326879204</v>
+        <v>59096247022</v>
       </c>
       <c r="Q3">
-        <v>193893072828</v>
+        <v>68617808568</v>
       </c>
       <c r="R3">
-        <v>341250572142</v>
+        <v>72737982928</v>
       </c>
       <c r="S3">
-        <v>-7083727446</v>
+        <v>3774225460</v>
       </c>
       <c r="T3">
-        <v>49300174288</v>
+        <v>2753382474</v>
       </c>
       <c r="U3">
-        <v>150061283068</v>
+        <v>8000270581</v>
       </c>
       <c r="V3">
-        <v>1473132550</v>
+        <v>3791818673</v>
       </c>
       <c r="W3">
-        <v>40660749810</v>
+        <v>3322524020</v>
       </c>
       <c r="X3">
-        <v>120676291668</v>
+        <v>7223298574</v>
       </c>
       <c r="Y3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1193,153 +1211,153 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F4">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="G4">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J4">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K4">
-        <v>10867713</v>
+        <v>14104416</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="P4">
-        <v>13884202433</v>
+        <v>132326879204</v>
       </c>
       <c r="Q4">
-        <v>51182177917</v>
+        <v>193893072828</v>
       </c>
       <c r="R4">
-        <v>8127683890</v>
+        <v>341250572142</v>
       </c>
       <c r="S4">
-        <v>-2233716995</v>
+        <v>-7083727446</v>
       </c>
       <c r="T4">
-        <v>2983031122</v>
+        <v>49300174288</v>
       </c>
       <c r="U4">
-        <v>-6655066594</v>
+        <v>150061283068</v>
       </c>
       <c r="V4">
-        <v>-5046530611</v>
+        <v>1473132550</v>
       </c>
       <c r="W4">
-        <v>1523272163</v>
+        <v>40660749810</v>
       </c>
       <c r="X4">
-        <v>-6716915237</v>
+        <v>120676291668</v>
       </c>
       <c r="Y4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="G5">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K5">
-        <v>5605000</v>
+        <v>10867713</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>13884202433</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>51182177917</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>8127683890</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>-2233716995</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>2983031122</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>-6655066594</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>-5046530611</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>1523272163</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>-6716915237</v>
       </c>
       <c r="Y5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1347,22 +1365,22 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F6">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="G6">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1374,7 +1392,7 @@
         <v>2000</v>
       </c>
       <c r="K6">
-        <v>7010000</v>
+        <v>5605000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1383,10 +1401,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1416,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1424,22 +1442,22 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F7">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="G7">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1451,7 +1469,7 @@
         <v>2000</v>
       </c>
       <c r="K7">
-        <v>4155000</v>
+        <v>7010000</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1460,10 +1478,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="O7" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1493,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1504,13 +1522,13 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>4000000</v>
@@ -1528,7 +1546,7 @@
         <v>2000</v>
       </c>
       <c r="K8">
-        <v>4210000</v>
+        <v>4155000</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1537,10 +1555,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O8" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1570,24 +1588,24 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1605,7 +1623,7 @@
         <v>2000</v>
       </c>
       <c r="K9">
-        <v>4240000</v>
+        <v>4210000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1614,10 +1632,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1647,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1655,76 +1673,76 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="G10">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K10">
-        <v>5661970</v>
+        <v>4240000</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="O10" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="P10">
-        <v>9490</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>12525</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>8916</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>1716</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>876</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1732,218 +1750,218 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="G11">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>4800</v>
+        <v>12000</v>
       </c>
       <c r="J11">
-        <v>5800</v>
+        <v>14000</v>
       </c>
       <c r="K11">
-        <v>9939614</v>
+        <v>5661970</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>7000</v>
+        <v>16000</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="O11" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="P11">
-        <v>11728856090</v>
+        <v>9490</v>
       </c>
       <c r="Q11">
-        <v>17398754684</v>
+        <v>12525</v>
       </c>
       <c r="R11">
-        <v>9950753269</v>
+        <v>8916</v>
       </c>
       <c r="S11">
-        <v>210467803</v>
+        <v>154</v>
       </c>
       <c r="T11">
-        <v>768643625</v>
+        <v>1780</v>
       </c>
       <c r="U11">
-        <v>-2057246152</v>
+        <v>502</v>
       </c>
       <c r="V11">
-        <v>-1402142802</v>
+        <v>496</v>
       </c>
       <c r="W11">
-        <v>708681523</v>
+        <v>1716</v>
       </c>
       <c r="X11">
-        <v>-2027030543</v>
+        <v>876</v>
       </c>
       <c r="Y11" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="G12">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J12">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K12">
-        <v>9465149</v>
+        <v>9939614</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P12">
-        <v>-7085110800</v>
+        <v>11728856090</v>
       </c>
       <c r="Q12">
-        <v>-7707829743</v>
+        <v>17398754684</v>
       </c>
       <c r="R12">
-        <v>-4353776321</v>
+        <v>9950753269</v>
       </c>
       <c r="S12">
-        <v>-7444566078</v>
+        <v>210467803</v>
       </c>
       <c r="T12">
-        <v>-8116734518</v>
+        <v>768643625</v>
       </c>
       <c r="U12">
-        <v>-4808043488</v>
+        <v>-2057246152</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>-1402142802</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>708681523</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>-2027030543</v>
       </c>
       <c r="Y12" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F13">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="G13">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K13">
-        <v>4690000</v>
+        <v>9465149</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="O13" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>-7085110800</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>-7707829743</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>-4353776321</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>-7444566078</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>-8116734518</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>-4808043488</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1955,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1963,73 +1981,73 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F14">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="G14">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J14">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K14">
-        <v>4225498</v>
+        <v>4690000</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="P14">
-        <v>84448377049</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>86585909893</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>71141473670</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>4232543828</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>2396516104</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>2260522008</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <v>3768461107</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>1925269107</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <v>1937996182</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="s">
         <v>120</v>
@@ -2037,79 +2055,79 @@
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F15">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="G15">
-        <v>4000000</v>
+        <v>850000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>16500</v>
       </c>
       <c r="K15">
-        <v>4230000</v>
+        <v>4225498</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="O15" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>84448377049</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>86585909893</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>71141473670</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>4232543828</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>2396516104</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>2260522008</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>3768461107</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>1925269107</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>1937996182</v>
       </c>
       <c r="Y15" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2117,76 +2135,76 @@
         <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F16">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="G16">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
-        <v>9355485</v>
+        <v>4230000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P16">
-        <v>91496346476</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>91488384999</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>63460787949</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>9436568051</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>11992232752</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>8323875572</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>8609153489</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>6967992579</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>7769366120</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2194,76 +2212,153 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F17">
+        <v>1500000</v>
+      </c>
+      <c r="G17">
+        <v>1500000</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>13000</v>
+      </c>
+      <c r="J17">
+        <v>15000</v>
+      </c>
+      <c r="K17">
+        <v>9355485</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>18000</v>
+      </c>
+      <c r="N17" t="s">
+        <v>103</v>
+      </c>
+      <c r="O17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P17">
+        <v>91496346476</v>
+      </c>
+      <c r="Q17">
+        <v>91488384999</v>
+      </c>
+      <c r="R17">
+        <v>63460787949</v>
+      </c>
+      <c r="S17">
+        <v>9436568051</v>
+      </c>
+      <c r="T17">
+        <v>11992232752</v>
+      </c>
+      <c r="U17">
+        <v>8323875572</v>
+      </c>
+      <c r="V17">
+        <v>8609153489</v>
+      </c>
+      <c r="W17">
+        <v>6967992579</v>
+      </c>
+      <c r="X17">
+        <v>7769366120</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18">
         <v>8707000</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>5224000</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>3483000</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>5000</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>6300</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>34824000</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>7300</v>
       </c>
-      <c r="N17" t="s">
-        <v>99</v>
-      </c>
-      <c r="O17" t="s">
-        <v>109</v>
-      </c>
-      <c r="P17">
+      <c r="N18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O18" t="s">
+        <v>115</v>
+      </c>
+      <c r="P18">
         <v>120971135005</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>144752544468</v>
       </c>
-      <c r="R17">
+      <c r="R18">
         <v>134349576051</v>
       </c>
-      <c r="S17">
+      <c r="S18">
         <v>6228818073</v>
       </c>
-      <c r="T17">
+      <c r="T18">
         <v>3756954475</v>
       </c>
-      <c r="U17">
+      <c r="U18">
         <v>11092990558</v>
       </c>
-      <c r="V17">
+      <c r="V18">
         <v>4708568182</v>
       </c>
-      <c r="W17">
+      <c r="W18">
         <v>4366217534</v>
       </c>
-      <c r="X17">
+      <c r="X18">
         <v>7277173431</v>
       </c>
-      <c r="Y17" t="s">
-        <v>122</v>
+      <c r="Y18" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2281,422 +2376,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E3">
         <v>25610</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E4">
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E5">
-        <v>16500</v>
+        <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E6">
-        <v>10300</v>
+        <v>16500</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E7">
-        <v>19500</v>
+        <v>10300</v>
       </c>
       <c r="F7" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E8">
-        <v>7000</v>
+        <v>19500</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E9">
-        <v>36000</v>
+        <v>7000</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E10">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="F10" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E11">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E12">
-        <v>19250</v>
+        <v>10000</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E13">
-        <v>6000</v>
+        <v>19250</v>
       </c>
       <c r="F13" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E14">
-        <v>17600</v>
+        <v>6000</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="E15">
-        <v>40000</v>
+        <v>17600</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="E16">
-        <v>12870</v>
+        <v>40000</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E17">
-        <v>10000</v>
+        <v>12870</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E18">
-        <v>18936</v>
+        <v>10000</v>
       </c>
       <c r="F18" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="E19">
-        <v>8000</v>
+        <v>18936</v>
       </c>
       <c r="F19" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E20">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E21">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="F21" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-30
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="190">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -128,9 +128,6 @@
     <t>2024-01-17</t>
   </si>
   <si>
-    <t>2024-01-05</t>
-  </si>
-  <si>
     <t>2024-03-13</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>2024-01-18</t>
   </si>
   <si>
-    <t>2024-01-11</t>
-  </si>
-  <si>
     <t>2024-03-27</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
     <t>IBKS제24호스팩</t>
   </si>
   <si>
-    <t>포스뱅크</t>
-  </si>
-  <si>
     <t>1247.72:1</t>
   </si>
   <si>
@@ -320,9 +311,6 @@
     <t>955.19:1</t>
   </si>
   <si>
-    <t>839.03:1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -350,9 +338,6 @@
     <t>5.55%</t>
   </si>
   <si>
-    <t>6.21%</t>
-  </si>
-  <si>
     <t>기업인수합병</t>
   </si>
   <si>
@@ -387,9 +372,6 @@
   </si>
   <si>
     <t>침실가구, 거실가구, 옷장/수납, 주방가구 등</t>
-  </si>
-  <si>
-    <t>POS 단말기, KIOSK 단말기</t>
   </si>
   <si>
     <t>종목명</t>
@@ -960,7 +942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1048,16 +1030,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2">
         <v>3000000</v>
@@ -1084,10 +1066,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1117,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1128,13 +1110,13 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3">
         <v>1600000</v>
@@ -1161,10 +1143,10 @@
         <v>20000</v>
       </c>
       <c r="N3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="P3">
         <v>813929</v>
@@ -1194,7 +1176,7 @@
         <v>-7817567</v>
       </c>
       <c r="Y3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1202,16 +1184,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4">
         <v>2000000</v>
@@ -1238,10 +1220,10 @@
         <v>30000</v>
       </c>
       <c r="N4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="P4">
         <v>59096247022</v>
@@ -1271,7 +1253,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1279,16 +1261,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>990000</v>
@@ -1315,10 +1297,10 @@
         <v>20000</v>
       </c>
       <c r="N5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P5">
         <v>132326879204</v>
@@ -1348,7 +1330,7 @@
         <v>120676291668</v>
       </c>
       <c r="Y5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1356,16 +1338,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6">
         <v>2104000</v>
@@ -1392,10 +1374,10 @@
         <v>13500</v>
       </c>
       <c r="N6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="P6">
         <v>13884202433</v>
@@ -1425,7 +1407,7 @@
         <v>-6716915237</v>
       </c>
       <c r="Y6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1433,16 +1415,16 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7">
         <v>5000000</v>
@@ -1469,10 +1451,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1502,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1516,10 +1498,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8">
         <v>6500000</v>
@@ -1546,10 +1528,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1579,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1590,13 +1572,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1623,10 +1605,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1656,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1667,13 +1649,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10">
         <v>4000000</v>
@@ -1700,10 +1682,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1733,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1747,10 +1729,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11">
         <v>4000000</v>
@@ -1777,10 +1759,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1810,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1818,16 +1800,16 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12">
         <v>600000</v>
@@ -1854,10 +1836,10 @@
         <v>16000</v>
       </c>
       <c r="N12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P12">
         <v>9490</v>
@@ -1887,7 +1869,7 @@
         <v>876</v>
       </c>
       <c r="Y12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1895,16 +1877,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>1000000</v>
@@ -1931,10 +1913,10 @@
         <v>7000</v>
       </c>
       <c r="N13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="P13">
         <v>11728856090</v>
@@ -1964,7 +1946,7 @@
         <v>-2027030543</v>
       </c>
       <c r="Y13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1972,16 +1954,16 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14">
         <v>1130000</v>
@@ -2008,10 +1990,10 @@
         <v>20000</v>
       </c>
       <c r="N14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P14">
         <v>-7085110800</v>
@@ -2041,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2049,16 +2031,16 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15">
         <v>4575000</v>
@@ -2085,11 +2067,11 @@
         <v>2000</v>
       </c>
       <c r="N15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O15" t="s">
         <v>98</v>
       </c>
-      <c r="O15" t="s">
-        <v>102</v>
-      </c>
       <c r="P15">
         <v>0</v>
       </c>
@@ -2118,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2126,16 +2108,16 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16">
         <v>850000</v>
@@ -2162,10 +2144,10 @@
         <v>18000</v>
       </c>
       <c r="N16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P16">
         <v>84448377049</v>
@@ -2195,7 +2177,7 @@
         <v>1937996182</v>
       </c>
       <c r="Y16" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2203,16 +2185,16 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F17">
         <v>4000000</v>
@@ -2239,10 +2221,10 @@
         <v>2000</v>
       </c>
       <c r="N17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -2272,84 +2254,7 @@
         <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18">
-        <v>1500000</v>
-      </c>
-      <c r="G18">
-        <v>1500000</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>13000</v>
-      </c>
-      <c r="J18">
-        <v>15000</v>
-      </c>
-      <c r="K18">
-        <v>9355485</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>18000</v>
-      </c>
-      <c r="N18" t="s">
-        <v>101</v>
-      </c>
-      <c r="O18" t="s">
-        <v>111</v>
-      </c>
-      <c r="P18">
-        <v>91496346476</v>
-      </c>
-      <c r="Q18">
-        <v>91488384999</v>
-      </c>
-      <c r="R18">
-        <v>63460787949</v>
-      </c>
-      <c r="S18">
-        <v>9436568051</v>
-      </c>
-      <c r="T18">
-        <v>11992232752</v>
-      </c>
-      <c r="U18">
-        <v>8323875572</v>
-      </c>
-      <c r="V18">
-        <v>8609153489</v>
-      </c>
-      <c r="W18">
-        <v>6967992579</v>
-      </c>
-      <c r="X18">
-        <v>7769366120</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2367,422 +2272,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>25610</v>
       </c>
       <c r="F3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E4">
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>652370</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E7">
         <v>16500</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E8">
         <v>10300</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E9">
         <v>19500</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E10">
         <v>24200</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E11">
         <v>7000</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E12">
         <v>36000</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E13">
         <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E14">
         <v>10000</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E15">
         <v>19250</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E16">
         <v>6000</v>
       </c>
       <c r="F16" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" t="s">
         <v>176</v>
-      </c>
-      <c r="D17" t="s">
-        <v>182</v>
       </c>
       <c r="E17">
         <v>17600</v>
       </c>
       <c r="F17" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" t="s">
         <v>177</v>
-      </c>
-      <c r="D18" t="s">
-        <v>183</v>
       </c>
       <c r="E18">
         <v>40000</v>
       </c>
       <c r="F18" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E19">
         <v>12870</v>
       </c>
       <c r="F19" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E20">
         <v>10000</v>
       </c>
       <c r="F20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D21" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E21">
         <v>18936</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-02
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="186">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -152,9 +152,6 @@
     <t>2024-01-23</t>
   </si>
   <si>
-    <t>2024-01-18</t>
-  </si>
-  <si>
     <t>2024-03-27</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>DB</t>
   </si>
   <si>
-    <t>IBK</t>
-  </si>
-  <si>
     <t>하나32호스팩</t>
   </si>
   <si>
@@ -260,9 +254,6 @@
     <t>스튜디오삼익</t>
   </si>
   <si>
-    <t>IBKS제24호스팩</t>
-  </si>
-  <si>
     <t>1247.72:1</t>
   </si>
   <si>
@@ -308,9 +299,6 @@
     <t>966.90:1</t>
   </si>
   <si>
-    <t>955.19:1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -446,7 +434,7 @@
     <t>2024.04.24~04.30</t>
   </si>
   <si>
-    <t>2024.04.18~04.24</t>
+    <t>2024.04.22~04.26</t>
   </si>
   <si>
     <t>2024.04.17~04.18</t>
@@ -539,10 +527,10 @@
     <t>9,000~11,000</t>
   </si>
   <si>
+    <t>2000</t>
+  </si>
+  <si>
     <t>13000</t>
-  </si>
-  <si>
-    <t>2000</t>
   </si>
   <si>
     <t>20000</t>
@@ -942,7 +930,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1033,13 +1021,13 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2">
         <v>3000000</v>
@@ -1066,10 +1054,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1099,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1110,13 +1098,13 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <v>1600000</v>
@@ -1143,10 +1131,10 @@
         <v>20000</v>
       </c>
       <c r="N3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="P3">
         <v>813929</v>
@@ -1176,7 +1164,7 @@
         <v>-7817567</v>
       </c>
       <c r="Y3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1187,13 +1175,13 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>2000000</v>
@@ -1220,10 +1208,10 @@
         <v>30000</v>
       </c>
       <c r="N4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="P4">
         <v>59096247022</v>
@@ -1253,7 +1241,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1267,10 +1255,10 @@
         <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <v>990000</v>
@@ -1297,10 +1285,10 @@
         <v>20000</v>
       </c>
       <c r="N5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="P5">
         <v>132326879204</v>
@@ -1330,7 +1318,7 @@
         <v>120676291668</v>
       </c>
       <c r="Y5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1344,10 +1332,10 @@
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6">
         <v>2104000</v>
@@ -1374,10 +1362,10 @@
         <v>13500</v>
       </c>
       <c r="N6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P6">
         <v>13884202433</v>
@@ -1407,7 +1395,7 @@
         <v>-6716915237</v>
       </c>
       <c r="Y6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1418,13 +1406,13 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F7">
         <v>5000000</v>
@@ -1451,10 +1439,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1484,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1498,10 +1486,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8">
         <v>6500000</v>
@@ -1528,10 +1516,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="O8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1561,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1572,13 +1560,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1605,10 +1593,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1638,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1649,13 +1637,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10">
         <v>4000000</v>
@@ -1682,10 +1670,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1715,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1729,10 +1717,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11">
         <v>4000000</v>
@@ -1759,10 +1747,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1792,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1803,13 +1791,13 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F12">
         <v>600000</v>
@@ -1836,10 +1824,10 @@
         <v>16000</v>
       </c>
       <c r="N12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="P12">
         <v>9490</v>
@@ -1869,7 +1857,7 @@
         <v>876</v>
       </c>
       <c r="Y12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1883,10 +1871,10 @@
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13">
         <v>1000000</v>
@@ -1913,10 +1901,10 @@
         <v>7000</v>
       </c>
       <c r="N13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="P13">
         <v>11728856090</v>
@@ -1946,7 +1934,7 @@
         <v>-2027030543</v>
       </c>
       <c r="Y13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1957,13 +1945,13 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14">
         <v>1130000</v>
@@ -1990,10 +1978,10 @@
         <v>20000</v>
       </c>
       <c r="N14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P14">
         <v>-7085110800</v>
@@ -2023,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2034,13 +2022,13 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F15">
         <v>4575000</v>
@@ -2067,10 +2055,10 @@
         <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2100,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2111,13 +2099,13 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F16">
         <v>850000</v>
@@ -2144,10 +2132,10 @@
         <v>18000</v>
       </c>
       <c r="N16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="P16">
         <v>84448377049</v>
@@ -2177,83 +2165,6 @@
         <v>1937996182</v>
       </c>
       <c r="Y16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17">
-        <v>4000000</v>
-      </c>
-      <c r="G17">
-        <v>4000000</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>2000</v>
-      </c>
-      <c r="J17">
-        <v>2000</v>
-      </c>
-      <c r="K17">
-        <v>4230000</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>2000</v>
-      </c>
-      <c r="N17" t="s">
-        <v>97</v>
-      </c>
-      <c r="O17" t="s">
-        <v>98</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2272,422 +2183,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E3">
         <v>25610</v>
       </c>
       <c r="F3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E4">
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E5">
         <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E6">
         <v>652370</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E7">
         <v>16500</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E8">
         <v>10300</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E9">
         <v>19500</v>
       </c>
       <c r="F9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E10">
         <v>24200</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E11">
         <v>7000</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E12">
         <v>36000</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E13">
         <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="E14">
         <v>10000</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E15">
         <v>19250</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E16">
         <v>6000</v>
       </c>
       <c r="F16" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E17">
         <v>17600</v>
       </c>
       <c r="F17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E18">
         <v>40000</v>
       </c>
       <c r="F18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
         <v>172</v>
-      </c>
-      <c r="D19" t="s">
-        <v>176</v>
       </c>
       <c r="E19">
         <v>12870</v>
       </c>
       <c r="F19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E20">
         <v>10000</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E21">
         <v>18936</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-03
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="192">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
     <t>2024-03-12</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>2024-01-17</t>
   </si>
   <si>
+    <t>2024-03-20</t>
+  </si>
+  <si>
     <t>2024-03-13</t>
   </si>
   <si>
@@ -152,6 +158,9 @@
     <t>2024-01-23</t>
   </si>
   <si>
+    <t>2024-04-03</t>
+  </si>
+  <si>
     <t>2024-03-27</t>
   </si>
   <si>
@@ -173,6 +182,9 @@
     <t>2024-02-06</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>하나</t>
   </si>
   <si>
@@ -209,6 +221,9 @@
     <t>DB</t>
   </si>
   <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
     <t>하나32호스팩</t>
   </si>
   <si>
@@ -254,6 +269,9 @@
     <t>스튜디오삼익</t>
   </si>
   <si>
+    <t>865.73 :1</t>
+  </si>
+  <si>
     <t>1247.72:1</t>
   </si>
   <si>
@@ -326,6 +344,9 @@
     <t>5.55%</t>
   </si>
   <si>
+    <t>알파리퀴드ⓡ 100, 알파리퀴드ⓡ HRR, 알파리퀴드ⓡ 디텍트, 알파리퀴드ⓡ 스크리닝</t>
+  </si>
+  <si>
     <t>기업인수합병</t>
   </si>
   <si>
@@ -419,9 +440,6 @@
     <t>신한스팩12호</t>
   </si>
   <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
     <t>하나스팩32호</t>
   </si>
   <si>
@@ -485,7 +503,7 @@
     <t>2024.02.16~02.22</t>
   </si>
   <si>
-    <t>8,700~11,500</t>
+    <t>8,700~11,000</t>
   </si>
   <si>
     <t>13,000~16,000</t>
@@ -930,7 +948,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1018,76 +1036,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F2">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="G2">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K2">
-        <v>3200000</v>
+        <v>13992625</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1230336508</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>2624739502</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>2926965114</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>-5277789009</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>-8667658271</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>-4923399541</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>-9788525741</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>-10436419054</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>-7563224846</v>
       </c>
       <c r="Y2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1095,76 +1113,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F3">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="G3">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>14014976</v>
+        <v>3200000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="P3">
-        <v>813929</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>2184312</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>3744252</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>-4828658</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>-7101029</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>-4926381</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>-24094044</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>-6797310</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>-7817567</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1172,76 +1190,76 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F4">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="G4">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
+        <v>11000</v>
+      </c>
+      <c r="J4">
+        <v>15000</v>
+      </c>
+      <c r="K4">
+        <v>14014976</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>20000</v>
       </c>
-      <c r="J4">
-        <v>25000</v>
-      </c>
-      <c r="K4">
-        <v>10569189</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>30000</v>
-      </c>
       <c r="N4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="P4">
-        <v>59096247022</v>
+        <v>813929</v>
       </c>
       <c r="Q4">
-        <v>68617808568</v>
+        <v>2184312</v>
       </c>
       <c r="R4">
-        <v>72737982928</v>
+        <v>3744252</v>
       </c>
       <c r="S4">
-        <v>3774225460</v>
+        <v>-4828658</v>
       </c>
       <c r="T4">
-        <v>2753382474</v>
+        <v>-7101029</v>
       </c>
       <c r="U4">
-        <v>8000270581</v>
+        <v>-4926381</v>
       </c>
       <c r="V4">
-        <v>3791818673</v>
+        <v>-24094044</v>
       </c>
       <c r="W4">
-        <v>3322524020</v>
+        <v>-6797310</v>
       </c>
       <c r="X4">
-        <v>7223298574</v>
+        <v>-7817567</v>
       </c>
       <c r="Y4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1249,76 +1267,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F5">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="G5">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J5">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K5">
-        <v>14104416</v>
+        <v>10569189</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="O5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="P5">
-        <v>132326879204</v>
+        <v>59096247022</v>
       </c>
       <c r="Q5">
-        <v>193893072828</v>
+        <v>68617808568</v>
       </c>
       <c r="R5">
-        <v>341250572142</v>
+        <v>72737982928</v>
       </c>
       <c r="S5">
-        <v>-7083727446</v>
+        <v>3774225460</v>
       </c>
       <c r="T5">
-        <v>49300174288</v>
+        <v>2753382474</v>
       </c>
       <c r="U5">
-        <v>150061283068</v>
+        <v>8000270581</v>
       </c>
       <c r="V5">
-        <v>1473132550</v>
+        <v>3791818673</v>
       </c>
       <c r="W5">
-        <v>40660749810</v>
+        <v>3322524020</v>
       </c>
       <c r="X5">
-        <v>120676291668</v>
+        <v>7223298574</v>
       </c>
       <c r="Y5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1326,153 +1344,153 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F6">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="G6">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J6">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K6">
-        <v>10867713</v>
+        <v>14104416</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="O6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="P6">
-        <v>13884202433</v>
+        <v>132326879204</v>
       </c>
       <c r="Q6">
-        <v>51182177917</v>
+        <v>193893072828</v>
       </c>
       <c r="R6">
-        <v>8127683890</v>
+        <v>341250572142</v>
       </c>
       <c r="S6">
-        <v>-2233716995</v>
+        <v>-7083727446</v>
       </c>
       <c r="T6">
-        <v>2983031122</v>
+        <v>49300174288</v>
       </c>
       <c r="U6">
-        <v>-6655066594</v>
+        <v>150061283068</v>
       </c>
       <c r="V6">
-        <v>-5046530611</v>
+        <v>1473132550</v>
       </c>
       <c r="W6">
-        <v>1523272163</v>
+        <v>40660749810</v>
       </c>
       <c r="X6">
-        <v>-6716915237</v>
+        <v>120676291668</v>
       </c>
       <c r="Y6" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F7">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="G7">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K7">
-        <v>5605000</v>
+        <v>10867713</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="O7" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>13884202433</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>51182177917</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>8127683890</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>-2233716995</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>2983031122</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>-6655066594</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>-5046530611</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>1523272163</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>-6716915237</v>
       </c>
       <c r="Y7" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1480,22 +1498,22 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F8">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="G8">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1507,7 +1525,7 @@
         <v>2000</v>
       </c>
       <c r="K8">
-        <v>7010000</v>
+        <v>5605000</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1516,10 +1534,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="O8" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1549,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1557,22 +1575,22 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F9">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="G9">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1584,7 +1602,7 @@
         <v>2000</v>
       </c>
       <c r="K9">
-        <v>4155000</v>
+        <v>7010000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1593,10 +1611,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="O9" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1626,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1637,13 +1655,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <v>4000000</v>
@@ -1661,7 +1679,7 @@
         <v>2000</v>
       </c>
       <c r="K10">
-        <v>4210000</v>
+        <v>4155000</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1670,10 +1688,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O10" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1703,24 +1721,24 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>4000000</v>
@@ -1738,7 +1756,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>4240000</v>
+        <v>4210000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1747,10 +1765,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="O11" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1780,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1788,76 +1806,76 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F12">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="G12">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>5661970</v>
+        <v>4240000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P12">
-        <v>9490</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>12525</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>8916</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>502</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>1716</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>876</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1865,218 +1883,218 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F13">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="G13">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>4800</v>
+        <v>12000</v>
       </c>
       <c r="J13">
-        <v>5800</v>
+        <v>14000</v>
       </c>
       <c r="K13">
-        <v>9939614</v>
+        <v>5661970</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>7000</v>
+        <v>16000</v>
       </c>
       <c r="N13" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="O13" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="P13">
-        <v>11728856090</v>
+        <v>9490</v>
       </c>
       <c r="Q13">
-        <v>17398754684</v>
+        <v>12525</v>
       </c>
       <c r="R13">
-        <v>9950753269</v>
+        <v>8916</v>
       </c>
       <c r="S13">
-        <v>210467803</v>
+        <v>154</v>
       </c>
       <c r="T13">
-        <v>768643625</v>
+        <v>1780</v>
       </c>
       <c r="U13">
-        <v>-2057246152</v>
+        <v>502</v>
       </c>
       <c r="V13">
-        <v>-1402142802</v>
+        <v>496</v>
       </c>
       <c r="W13">
-        <v>708681523</v>
+        <v>1716</v>
       </c>
       <c r="X13">
-        <v>-2027030543</v>
+        <v>876</v>
       </c>
       <c r="Y13" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F14">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="G14">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J14">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K14">
-        <v>9465149</v>
+        <v>9939614</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N14" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="O14" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="P14">
-        <v>-7085110800</v>
+        <v>11728856090</v>
       </c>
       <c r="Q14">
-        <v>-7707829743</v>
+        <v>17398754684</v>
       </c>
       <c r="R14">
-        <v>-4353776321</v>
+        <v>9950753269</v>
       </c>
       <c r="S14">
-        <v>-7444566078</v>
+        <v>210467803</v>
       </c>
       <c r="T14">
-        <v>-8116734518</v>
+        <v>768643625</v>
       </c>
       <c r="U14">
-        <v>-4808043488</v>
+        <v>-2057246152</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>-1402142802</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>708681523</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>-2027030543</v>
       </c>
       <c r="Y14" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F15">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="G15">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K15">
-        <v>4690000</v>
+        <v>9465149</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N15" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="O15" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>-7085110800</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>-7707829743</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>-4353776321</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>-7444566078</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>-8116734518</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>-4808043488</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -2088,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2096,76 +2114,153 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F16">
+        <v>4575000</v>
+      </c>
+      <c r="G16">
+        <v>4575000</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>2000</v>
+      </c>
+      <c r="J16">
+        <v>2000</v>
+      </c>
+      <c r="K16">
+        <v>4690000</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>2000</v>
+      </c>
+      <c r="N16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17">
         <v>850000</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>850000</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>14500</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>16500</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>4225498</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>18000</v>
       </c>
-      <c r="N16" t="s">
-        <v>93</v>
-      </c>
-      <c r="O16" t="s">
-        <v>102</v>
-      </c>
-      <c r="P16">
+      <c r="N17" t="s">
+        <v>99</v>
+      </c>
+      <c r="O17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P17">
         <v>84448377049</v>
       </c>
-      <c r="Q16">
+      <c r="Q17">
         <v>86585909893</v>
       </c>
-      <c r="R16">
+      <c r="R17">
         <v>71141473670</v>
       </c>
-      <c r="S16">
+      <c r="S17">
         <v>4232543828</v>
       </c>
-      <c r="T16">
+      <c r="T17">
         <v>2396516104</v>
       </c>
-      <c r="U16">
+      <c r="U17">
         <v>2260522008</v>
       </c>
-      <c r="V16">
+      <c r="V17">
         <v>3768461107</v>
       </c>
-      <c r="W16">
+      <c r="W17">
         <v>1925269107</v>
       </c>
-      <c r="X16">
+      <c r="X17">
         <v>1937996182</v>
       </c>
-      <c r="Y16" t="s">
-        <v>114</v>
+      <c r="Y17" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2183,422 +2278,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E2">
         <v>10440</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E3">
         <v>25610</v>
       </c>
       <c r="F3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E4">
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E5">
         <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E6">
         <v>652370</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>16500</v>
       </c>
       <c r="F7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E8">
         <v>10300</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <v>19500</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E10">
         <v>24200</v>
       </c>
       <c r="F10" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E11">
         <v>7000</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E12">
         <v>36000</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E13">
         <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E14">
         <v>10000</v>
       </c>
       <c r="F14" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E15">
         <v>19250</v>
       </c>
       <c r="F15" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E16">
         <v>6000</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="E17">
         <v>17600</v>
       </c>
       <c r="F17" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="E18">
         <v>40000</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="E19">
         <v>12870</v>
       </c>
       <c r="F19" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E20">
         <v>10000</v>
       </c>
       <c r="F20" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E21">
         <v>18936</v>
       </c>
       <c r="F21" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-09
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="179">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -125,12 +125,6 @@
     <t>2024-02-01</t>
   </si>
   <si>
-    <t>2024-01-22</t>
-  </si>
-  <si>
-    <t>2024-01-17</t>
-  </si>
-  <si>
     <t>2024-03-20</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>2024-02-07</t>
   </si>
   <si>
-    <t>2024-01-23</t>
-  </si>
-  <si>
     <t>2024-04-03</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>2024-02-23</t>
   </si>
   <si>
-    <t>2024-02-06</t>
-  </si>
-  <si>
     <t>미래</t>
   </si>
   <si>
@@ -215,12 +203,6 @@
     <t>한화</t>
   </si>
   <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
     <t>아이엠비디엑스</t>
   </si>
   <si>
@@ -263,12 +245,6 @@
     <t>이에이트</t>
   </si>
   <si>
-    <t>신영스팩10호</t>
-  </si>
-  <si>
-    <t>스튜디오삼익</t>
-  </si>
-  <si>
     <t>865.73 :1</t>
   </si>
   <si>
@@ -311,12 +287,6 @@
     <t>630.64:1</t>
   </si>
   <si>
-    <t>949.18:1</t>
-  </si>
-  <si>
-    <t>966.90:1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -341,9 +311,6 @@
     <t>2.35%</t>
   </si>
   <si>
-    <t>5.55%</t>
-  </si>
-  <si>
     <t>알파리퀴드ⓡ 100, 알파리퀴드ⓡ HRR, 알파리퀴드ⓡ 디텍트, 알파리퀴드ⓡ 스크리닝</t>
   </si>
   <si>
@@ -380,9 +347,6 @@
     <t>CFD 시뮬레이션 소프트웨어, 디지털트윈 플랫폼</t>
   </si>
   <si>
-    <t>침실가구, 거실가구, 옷장/수납, 주방가구 등</t>
-  </si>
-  <si>
     <t>종목명</t>
   </si>
   <si>
@@ -401,9 +365,15 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>하스</t>
+  </si>
+  <si>
     <t>노브랜드</t>
   </si>
   <si>
+    <t>KB스팩28호</t>
+  </si>
+  <si>
     <t>아이씨티케이</t>
   </si>
   <si>
@@ -443,12 +413,15 @@
     <t>하나스팩32호</t>
   </si>
   <si>
-    <t>하나스팩31호</t>
+    <t>2024.05.16~05.22</t>
   </si>
   <si>
     <t>2024.04.30~05.08</t>
   </si>
   <si>
+    <t>2024.04.29~04.30</t>
+  </si>
+  <si>
     <t>2024.04.24~04.30</t>
   </si>
   <si>
@@ -497,24 +470,21 @@
     <t>2024.02.21~02.27</t>
   </si>
   <si>
-    <t>2024.02.16~02.19</t>
-  </si>
-  <si>
-    <t>2024.02.16~02.22</t>
+    <t>9,000~12,000</t>
   </si>
   <si>
     <t>8,700~11,000</t>
   </si>
   <si>
+    <t>2,000~2,000</t>
+  </si>
+  <si>
     <t>13,000~16,000</t>
   </si>
   <si>
     <t>29,000~35,000</t>
   </si>
   <si>
-    <t>2,000~2,000</t>
-  </si>
-  <si>
     <t>73,300~83,400</t>
   </si>
   <si>
@@ -542,9 +512,6 @@
     <t>13,000~15,000</t>
   </si>
   <si>
-    <t>9,000~11,000</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -557,12 +524,12 @@
     <t>30000</t>
   </si>
   <si>
-    <t>13500</t>
-  </si>
-  <si>
     <t>삼성증권</t>
   </si>
   <si>
+    <t>KB증권</t>
+  </si>
+  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -578,9 +545,6 @@
     <t>유안타증권</t>
   </si>
   <si>
-    <t>KB증권</t>
-  </si>
-  <si>
     <t>하나증권</t>
   </si>
   <si>
@@ -588,9 +552,6 @@
   </si>
   <si>
     <t>미래에셋증권</t>
-  </si>
-  <si>
-    <t>DB금융투자,NH투자증권</t>
   </si>
 </sst>
 </file>
@@ -948,7 +909,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1036,16 +997,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <v>2500000</v>
@@ -1072,10 +1033,10 @@
         <v>13000</v>
       </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P2">
         <v>1230336508</v>
@@ -1105,7 +1066,7 @@
         <v>-7563224846</v>
       </c>
       <c r="Y2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1113,16 +1074,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F3">
         <v>3000000</v>
@@ -1149,10 +1110,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1182,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1193,13 +1154,13 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F4">
         <v>1600000</v>
@@ -1226,10 +1187,10 @@
         <v>20000</v>
       </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="O4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="P4">
         <v>813929</v>
@@ -1259,7 +1220,7 @@
         <v>-7817567</v>
       </c>
       <c r="Y4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1267,16 +1228,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F5">
         <v>2000000</v>
@@ -1303,10 +1264,10 @@
         <v>30000</v>
       </c>
       <c r="N5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="O5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P5">
         <v>59096247022</v>
@@ -1336,7 +1297,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1344,16 +1305,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F6">
         <v>990000</v>
@@ -1380,10 +1341,10 @@
         <v>20000</v>
       </c>
       <c r="N6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="O6" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="P6">
         <v>132326879204</v>
@@ -1413,7 +1374,7 @@
         <v>120676291668</v>
       </c>
       <c r="Y6" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1421,16 +1382,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F7">
         <v>2104000</v>
@@ -1457,10 +1418,10 @@
         <v>13500</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="O7" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="P7">
         <v>13884202433</v>
@@ -1490,7 +1451,7 @@
         <v>-6716915237</v>
       </c>
       <c r="Y7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1498,16 +1459,16 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>5000000</v>
@@ -1534,11 +1495,11 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8" t="s">
         <v>90</v>
       </c>
-      <c r="O8" t="s">
-        <v>100</v>
-      </c>
       <c r="P8">
         <v>0</v>
       </c>
@@ -1567,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1581,10 +1542,10 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F9">
         <v>6500000</v>
@@ -1611,10 +1572,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="O9" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1644,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1655,13 +1616,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F10">
         <v>4000000</v>
@@ -1688,10 +1649,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1721,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1732,13 +1693,13 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F11">
         <v>4000000</v>
@@ -1765,10 +1726,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="O11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1798,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1812,10 +1773,10 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F12">
         <v>4000000</v>
@@ -1842,10 +1803,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="O12" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1875,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1883,16 +1844,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F13">
         <v>600000</v>
@@ -1919,10 +1880,10 @@
         <v>16000</v>
       </c>
       <c r="N13" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" t="s">
         <v>95</v>
-      </c>
-      <c r="O13" t="s">
-        <v>105</v>
       </c>
       <c r="P13">
         <v>9490</v>
@@ -1952,7 +1913,7 @@
         <v>876</v>
       </c>
       <c r="Y13" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1960,16 +1921,16 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F14">
         <v>1000000</v>
@@ -1996,10 +1957,10 @@
         <v>7000</v>
       </c>
       <c r="N14" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" t="s">
         <v>96</v>
-      </c>
-      <c r="O14" t="s">
-        <v>106</v>
       </c>
       <c r="P14">
         <v>11728856090</v>
@@ -2029,7 +1990,7 @@
         <v>-2027030543</v>
       </c>
       <c r="Y14" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2037,16 +1998,16 @@
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F15">
         <v>1130000</v>
@@ -2073,10 +2034,10 @@
         <v>20000</v>
       </c>
       <c r="N15" t="s">
+        <v>89</v>
+      </c>
+      <c r="O15" t="s">
         <v>97</v>
-      </c>
-      <c r="O15" t="s">
-        <v>107</v>
       </c>
       <c r="P15">
         <v>-7085110800</v>
@@ -2106,161 +2067,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16">
-        <v>4575000</v>
-      </c>
-      <c r="G16">
-        <v>4575000</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>2000</v>
-      </c>
-      <c r="J16">
-        <v>2000</v>
-      </c>
-      <c r="K16">
-        <v>4690000</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>2000</v>
-      </c>
-      <c r="N16" t="s">
-        <v>98</v>
-      </c>
-      <c r="O16" t="s">
-        <v>100</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17">
-        <v>850000</v>
-      </c>
-      <c r="G17">
-        <v>850000</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>14500</v>
-      </c>
-      <c r="J17">
-        <v>16500</v>
-      </c>
-      <c r="K17">
-        <v>4225498</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>18000</v>
-      </c>
-      <c r="N17" t="s">
-        <v>99</v>
-      </c>
-      <c r="O17" t="s">
-        <v>108</v>
-      </c>
-      <c r="P17">
-        <v>84448377049</v>
-      </c>
-      <c r="Q17">
-        <v>86585909893</v>
-      </c>
-      <c r="R17">
-        <v>71141473670</v>
-      </c>
-      <c r="S17">
-        <v>4232543828</v>
-      </c>
-      <c r="T17">
-        <v>2396516104</v>
-      </c>
-      <c r="U17">
-        <v>2260522008</v>
-      </c>
-      <c r="V17">
-        <v>3768461107</v>
-      </c>
-      <c r="W17">
-        <v>1925269107</v>
-      </c>
-      <c r="X17">
-        <v>1937996182</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2278,422 +2085,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E2">
-        <v>10440</v>
+        <v>16290</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E3">
-        <v>25610</v>
+        <v>10440</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E4">
-        <v>17400</v>
+        <v>10000</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E5">
-        <v>6000</v>
+        <v>25610</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E6">
-        <v>652370</v>
+        <v>17400</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E7">
-        <v>16500</v>
+        <v>6000</v>
       </c>
       <c r="F7" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E8">
-        <v>10300</v>
+        <v>652370</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>19500</v>
+        <v>16500</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E10">
-        <v>24200</v>
+        <v>10300</v>
       </c>
       <c r="F10" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E11">
-        <v>7000</v>
+        <v>19500</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E12">
-        <v>36000</v>
+        <v>24200</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
         <v>153</v>
       </c>
-      <c r="C13" t="s">
-        <v>165</v>
-      </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E13">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>90</v>
       </c>
       <c r="E14">
-        <v>10000</v>
+        <v>36000</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15">
+        <v>6000</v>
+      </c>
+      <c r="F15" t="s">
         <v>177</v>
-      </c>
-      <c r="E15">
-        <v>19250</v>
-      </c>
-      <c r="F15" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" t="s">
         <v>165</v>
       </c>
-      <c r="D16" t="s">
-        <v>176</v>
-      </c>
       <c r="E16">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17">
+        <v>19250</v>
+      </c>
+      <c r="F17" t="s">
         <v>178</v>
-      </c>
-      <c r="E17">
-        <v>17600</v>
-      </c>
-      <c r="F17" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E18">
-        <v>40000</v>
+        <v>6000</v>
       </c>
       <c r="F18" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E19">
-        <v>12870</v>
+        <v>17600</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E20">
-        <v>10000</v>
+        <v>40000</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E21">
-        <v>18936</v>
+        <v>12870</v>
       </c>
       <c r="F21" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -371,6 +371,9 @@
     <t>노브랜드</t>
   </si>
   <si>
+    <t>에스오에스랩</t>
+  </si>
+  <si>
     <t>KB스팩28호</t>
   </si>
   <si>
@@ -467,15 +470,15 @@
     <t>2024.02.29~03.07</t>
   </si>
   <si>
-    <t>2024.02.21~02.27</t>
-  </si>
-  <si>
     <t>9,000~12,000</t>
   </si>
   <si>
     <t>8,700~11,000</t>
   </si>
   <si>
+    <t>7,500~9,000</t>
+  </si>
+  <si>
     <t>2,000~2,000</t>
   </si>
   <si>
@@ -509,9 +512,6 @@
     <t>20,000~25,000</t>
   </si>
   <si>
-    <t>13,000~15,000</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -527,13 +527,13 @@
     <t>삼성증권</t>
   </si>
   <si>
+    <t>한국투자증권</t>
+  </si>
+  <si>
     <t>KB증권</t>
   </si>
   <si>
     <t>NH투자증권</t>
-  </si>
-  <si>
-    <t>한국투자증권</t>
   </si>
   <si>
     <t>SK증권</t>
@@ -2108,7 +2108,7 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>151</v>
@@ -2128,7 +2128,7 @@
         <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>152</v>
@@ -2157,7 +2157,7 @@
         <v>90</v>
       </c>
       <c r="E4">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="F4" t="s">
         <v>170</v>
@@ -2177,7 +2177,7 @@
         <v>90</v>
       </c>
       <c r="E5">
-        <v>25610</v>
+        <v>10000</v>
       </c>
       <c r="F5" t="s">
         <v>171</v>
@@ -2197,7 +2197,7 @@
         <v>90</v>
       </c>
       <c r="E6">
-        <v>17400</v>
+        <v>25610</v>
       </c>
       <c r="F6" t="s">
         <v>172</v>
@@ -2211,16 +2211,16 @@
         <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
         <v>90</v>
       </c>
       <c r="E7">
-        <v>6000</v>
+        <v>17400</v>
       </c>
       <c r="F7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2231,16 +2231,16 @@
         <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
         <v>90</v>
       </c>
       <c r="E8">
-        <v>652370</v>
+        <v>6000</v>
       </c>
       <c r="F8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2257,10 +2257,10 @@
         <v>90</v>
       </c>
       <c r="E9">
-        <v>16500</v>
+        <v>652370</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2271,16 +2271,16 @@
         <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
         <v>90</v>
       </c>
       <c r="E10">
-        <v>10300</v>
+        <v>16500</v>
       </c>
       <c r="F10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2291,16 +2291,16 @@
         <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
         <v>90</v>
       </c>
       <c r="E11">
-        <v>19500</v>
+        <v>10300</v>
       </c>
       <c r="F11" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2308,7 +2308,7 @@
         <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>159</v>
@@ -2317,10 +2317,10 @@
         <v>90</v>
       </c>
       <c r="E12">
-        <v>24200</v>
+        <v>19500</v>
       </c>
       <c r="F12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2331,16 +2331,16 @@
         <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D13" t="s">
         <v>90</v>
       </c>
       <c r="E13">
-        <v>7000</v>
+        <v>24200</v>
       </c>
       <c r="F13" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2351,16 +2351,16 @@
         <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="E14">
-        <v>36000</v>
+        <v>7000</v>
       </c>
       <c r="F14" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2371,16 +2371,16 @@
         <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="E15">
-        <v>6000</v>
+        <v>36000</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2391,13 +2391,13 @@
         <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s">
         <v>165</v>
       </c>
       <c r="E16">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="F16" t="s">
         <v>177</v>
@@ -2405,67 +2405,67 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
         <v>146</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E17">
-        <v>19250</v>
+        <v>10000</v>
       </c>
       <c r="F17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
         <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E18">
-        <v>6000</v>
+        <v>19250</v>
       </c>
       <c r="F18" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E19">
-        <v>17600</v>
+        <v>6000</v>
       </c>
       <c r="F19" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>149</v>
@@ -2474,10 +2474,10 @@
         <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E20">
-        <v>40000</v>
+        <v>17600</v>
       </c>
       <c r="F20" t="s">
         <v>172</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>150</v>
@@ -2494,13 +2494,13 @@
         <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E21">
-        <v>12870</v>
+        <v>40000</v>
       </c>
       <c r="F21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-02
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="204">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,12 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-04-12</t>
+  </si>
+  <si>
+    <t>2024-04-15</t>
+  </si>
+  <si>
     <t>2024-04-08</t>
   </si>
   <si>
@@ -125,6 +131,12 @@
     <t>2024-02-13</t>
   </si>
   <si>
+    <t>2024-04-18</t>
+  </si>
+  <si>
+    <t>2024-04-16</t>
+  </si>
+  <si>
     <t>2024-04-09</t>
   </si>
   <si>
@@ -155,15 +167,15 @@
     <t>2024-02-14</t>
   </si>
   <si>
+    <t>2024-05-02</t>
+  </si>
+  <si>
     <t>2024-04-24</t>
   </si>
   <si>
     <t>2024-04-22</t>
   </si>
   <si>
-    <t>2024-04-15</t>
-  </si>
-  <si>
     <t>2024-04-03</t>
   </si>
   <si>
@@ -179,6 +191,12 @@
     <t>2024-03-04</t>
   </si>
   <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
     <t>하나</t>
   </si>
   <si>
@@ -191,9 +209,6 @@
     <t>NH</t>
   </si>
   <si>
-    <t>한국</t>
-  </si>
-  <si>
     <t>DB, NH</t>
   </si>
   <si>
@@ -203,6 +218,12 @@
     <t>BNK</t>
   </si>
   <si>
+    <t>디앤디파마텍</t>
+  </si>
+  <si>
+    <t>유안타제16호스팩</t>
+  </si>
+  <si>
     <t>하나33호스팩</t>
   </si>
   <si>
@@ -239,6 +260,12 @@
     <t>비엔케이제2호스팩</t>
   </si>
   <si>
+    <t>848.50:1</t>
+  </si>
+  <si>
+    <t>1,050.42:1</t>
+  </si>
+  <si>
     <t>1277.22:1</t>
   </si>
   <si>
@@ -275,6 +302,9 @@
     <t>703.99:1</t>
   </si>
   <si>
+    <t>10.96%</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -293,6 +323,12 @@
     <t>31.86%</t>
   </si>
   <si>
+    <t>대사성질환 치료제 등</t>
+  </si>
+  <si>
+    <t>금융 지원 서비스(기업인수목적회사)</t>
+  </si>
+  <si>
     <t>기업인수합병</t>
   </si>
   <si>
@@ -381,9 +417,6 @@
   </si>
   <si>
     <t>민테크</t>
-  </si>
-  <si>
-    <t>디앤디파마텍</t>
   </si>
   <si>
     <t>하나스팩33호</t>
@@ -951,7 +984,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1039,64 +1072,64 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F2">
-        <v>3500000</v>
+        <v>1100000</v>
       </c>
       <c r="G2">
-        <v>3500000</v>
+        <v>1100000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K2">
-        <v>3700000</v>
+        <v>10429232</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>33000</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="O2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-75676750274</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>-68652978862</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-9506668082</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>-69862474811</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>-137025491259</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>3014576074</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1108,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1116,22 +1149,22 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F3">
-        <v>3000000</v>
+        <v>5150000</v>
       </c>
       <c r="G3">
-        <v>3000000</v>
+        <v>5150000</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1143,7 +1176,7 @@
         <v>2000</v>
       </c>
       <c r="K3">
-        <v>3620000</v>
+        <v>5510000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1152,10 +1185,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1185,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1193,22 +1226,22 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F4">
-        <v>5000000</v>
+        <v>3500000</v>
       </c>
       <c r="G4">
-        <v>5000000</v>
+        <v>3500000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1220,7 +1253,7 @@
         <v>2000</v>
       </c>
       <c r="K4">
-        <v>5520000</v>
+        <v>3700000</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1229,10 +1262,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="O4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1262,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1270,76 +1303,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F5">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="G5">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>9900</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>13992625</v>
+        <v>3620000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="P5">
-        <v>1230336508</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>2624739502</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>2926965114</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>-5277789009</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>-8667658271</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>-4923399541</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>-9788525741</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>-10436419054</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>-7563224846</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1347,22 +1380,22 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F6">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="G6">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1374,7 +1407,7 @@
         <v>2000</v>
       </c>
       <c r="K6">
-        <v>3200000</v>
+        <v>5520000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1383,10 +1416,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="O6" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1416,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1424,76 +1457,76 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F7">
-        <v>1600000</v>
+        <v>2500000</v>
       </c>
       <c r="G7">
-        <v>1600000</v>
+        <v>2500000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>11000</v>
+        <v>7700</v>
       </c>
       <c r="J7">
-        <v>15000</v>
+        <v>9900</v>
       </c>
       <c r="K7">
-        <v>14014976</v>
+        <v>13992625</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>20000</v>
+        <v>13000</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="O7" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="P7">
-        <v>813929</v>
+        <v>1230336508</v>
       </c>
       <c r="Q7">
-        <v>2184312</v>
+        <v>2624739502</v>
       </c>
       <c r="R7">
-        <v>3744252</v>
+        <v>2926965114</v>
       </c>
       <c r="S7">
-        <v>-4828658</v>
+        <v>-5277789009</v>
       </c>
       <c r="T7">
-        <v>-7101029</v>
+        <v>-8667658271</v>
       </c>
       <c r="U7">
-        <v>-4926381</v>
+        <v>-4923399541</v>
       </c>
       <c r="V7">
-        <v>-24094044</v>
+        <v>-9788525741</v>
       </c>
       <c r="W7">
-        <v>-6797310</v>
+        <v>-10436419054</v>
       </c>
       <c r="X7">
-        <v>-7817567</v>
+        <v>-7563224846</v>
       </c>
       <c r="Y7" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1501,76 +1534,76 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F8">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
       <c r="G8">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>25000</v>
+        <v>2000</v>
       </c>
       <c r="K8">
-        <v>10569189</v>
+        <v>3200000</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="O8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="P8">
-        <v>59096247022</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>68617808568</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>72737982928</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>3774225460</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>2753382474</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>8000270581</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>3791818673</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>3322524020</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>7223298574</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1578,34 +1611,34 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F9">
-        <v>990000</v>
+        <v>1600000</v>
       </c>
       <c r="G9">
-        <v>990000</v>
+        <v>1600000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>13000</v>
+        <v>11000</v>
       </c>
       <c r="J9">
         <v>15000</v>
       </c>
       <c r="K9">
-        <v>14104416</v>
+        <v>14014976</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1614,40 +1647,40 @@
         <v>20000</v>
       </c>
       <c r="N9" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="O9" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="P9">
-        <v>132326879204</v>
+        <v>813929</v>
       </c>
       <c r="Q9">
-        <v>193893072828</v>
+        <v>2184312</v>
       </c>
       <c r="R9">
-        <v>341250572142</v>
+        <v>3744252</v>
       </c>
       <c r="S9">
-        <v>-7083727446</v>
+        <v>-4828658</v>
       </c>
       <c r="T9">
-        <v>49300174288</v>
+        <v>-7101029</v>
       </c>
       <c r="U9">
-        <v>150061283068</v>
+        <v>-4926381</v>
       </c>
       <c r="V9">
-        <v>1473132550</v>
+        <v>-24094044</v>
       </c>
       <c r="W9">
-        <v>40660749810</v>
+        <v>-6797310</v>
       </c>
       <c r="X9">
-        <v>120676291668</v>
+        <v>-7817567</v>
       </c>
       <c r="Y9" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1655,230 +1688,230 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F10">
-        <v>2104000</v>
+        <v>2000000</v>
       </c>
       <c r="G10">
-        <v>2104000</v>
+        <v>2000000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>9000</v>
+        <v>20000</v>
       </c>
       <c r="J10">
-        <v>11000</v>
+        <v>25000</v>
       </c>
       <c r="K10">
-        <v>10867713</v>
+        <v>10569189</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>13500</v>
+        <v>30000</v>
       </c>
       <c r="N10" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="O10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="P10">
-        <v>13884202433</v>
+        <v>59096247022</v>
       </c>
       <c r="Q10">
-        <v>51182177917</v>
+        <v>68617808568</v>
       </c>
       <c r="R10">
-        <v>8127683890</v>
+        <v>72737982928</v>
       </c>
       <c r="S10">
-        <v>-2233716995</v>
+        <v>3774225460</v>
       </c>
       <c r="T10">
-        <v>2983031122</v>
+        <v>2753382474</v>
       </c>
       <c r="U10">
-        <v>-6655066594</v>
+        <v>8000270581</v>
       </c>
       <c r="V10">
-        <v>-5046530611</v>
+        <v>3791818673</v>
       </c>
       <c r="W10">
-        <v>1523272163</v>
+        <v>3322524020</v>
       </c>
       <c r="X10">
-        <v>-6716915237</v>
+        <v>7223298574</v>
       </c>
       <c r="Y10" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F11">
-        <v>5000000</v>
+        <v>990000</v>
       </c>
       <c r="G11">
-        <v>5000000</v>
+        <v>990000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="K11">
-        <v>5605000</v>
+        <v>14104416</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N11" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="O11" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>132326879204</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>193893072828</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>341250572142</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>-7083727446</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>49300174288</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>150061283068</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>1473132550</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>40660749810</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>120676291668</v>
       </c>
       <c r="Y11" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F12">
-        <v>4000000</v>
+        <v>2104000</v>
       </c>
       <c r="G12">
-        <v>4000000</v>
+        <v>2104000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K12">
-        <v>4155000</v>
+        <v>10867713</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="O12" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>13884202433</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>51182177917</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>8127683890</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>-2233716995</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>2983031122</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>-6655066594</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>-5046530611</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1523272163</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>-6716915237</v>
       </c>
       <c r="Y12" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1886,22 +1919,22 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F13">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="G13">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1913,7 +1946,7 @@
         <v>2000</v>
       </c>
       <c r="K13">
-        <v>4210000</v>
+        <v>5605000</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1922,10 +1955,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1955,7 +1988,161 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14">
+        <v>4000000</v>
+      </c>
+      <c r="G14">
+        <v>4000000</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2000</v>
+      </c>
+      <c r="J14">
+        <v>2000</v>
+      </c>
+      <c r="K14">
+        <v>4155000</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+      <c r="N14" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <v>4000000</v>
+      </c>
+      <c r="G15">
+        <v>4000000</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2000</v>
+      </c>
+      <c r="J15">
+        <v>2000</v>
+      </c>
+      <c r="K15">
+        <v>4210000</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>2000</v>
+      </c>
+      <c r="N15" t="s">
+        <v>94</v>
+      </c>
+      <c r="O15" t="s">
+        <v>96</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1973,422 +2160,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E13" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="F15" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="F16" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E17" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F19" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F20" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E21" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="F21" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-05
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="195">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -125,9 +125,6 @@
     <t>2024-02-16</t>
   </si>
   <si>
-    <t>2024-02-13</t>
-  </si>
-  <si>
     <t>2024-04-18</t>
   </si>
   <si>
@@ -158,12 +155,6 @@
     <t>2024-02-22</t>
   </si>
   <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
-    <t>2024-02-14</t>
-  </si>
-  <si>
     <t>2024-05-03</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>2024-03-21</t>
   </si>
   <si>
-    <t>2024-03-05</t>
-  </si>
-  <si>
     <t>KB</t>
   </si>
   <si>
@@ -212,9 +200,6 @@
     <t>DB, NH</t>
   </si>
   <si>
-    <t>BNK</t>
-  </si>
-  <si>
     <t>민테크</t>
   </si>
   <si>
@@ -251,12 +236,6 @@
     <t>케이엔알시스템</t>
   </si>
   <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
     <t>946.72:1</t>
   </si>
   <si>
@@ -293,12 +272,6 @@
     <t>873.20:1</t>
   </si>
   <si>
-    <t>1,018.60:1</t>
-  </si>
-  <si>
-    <t>703.99:1</t>
-  </si>
-  <si>
     <t>4.23%</t>
   </si>
   <si>
@@ -354,9 +327,6 @@
   </si>
   <si>
     <t>특수목적 시험장비, 산업용로봇</t>
-  </si>
-  <si>
-    <t>금융 지원 서비스업</t>
   </si>
   <si>
     <t>종목명</t>
@@ -987,7 +957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1075,16 +1045,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F2">
         <v>3000000</v>
@@ -1111,10 +1081,10 @@
         <v>10500</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="O2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="P2">
         <v>9576212189</v>
@@ -1144,7 +1114,7 @@
         <v>-7501425172</v>
       </c>
       <c r="Y2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1152,16 +1122,16 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3">
         <v>1100000</v>
@@ -1188,10 +1158,10 @@
         <v>33000</v>
       </c>
       <c r="N3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="P3">
         <v>-75676750274</v>
@@ -1221,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1229,16 +1199,16 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F4">
         <v>5150000</v>
@@ -1265,10 +1235,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="O4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1298,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1306,16 +1276,16 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F5">
         <v>3500000</v>
@@ -1342,40 +1312,40 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="O5" t="s">
+        <v>87</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
         <v>96</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1383,16 +1353,16 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F6">
         <v>3000000</v>
@@ -1419,10 +1389,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="O6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1452,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1460,16 +1430,16 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F7">
         <v>5000000</v>
@@ -1496,10 +1466,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="O7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1529,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1537,16 +1507,16 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F8">
         <v>2500000</v>
@@ -1573,10 +1543,10 @@
         <v>13000</v>
       </c>
       <c r="N8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="P8">
         <v>1230336508</v>
@@ -1606,7 +1576,7 @@
         <v>-7563224846</v>
       </c>
       <c r="Y8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1614,16 +1584,16 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F9">
         <v>3000000</v>
@@ -1650,40 +1620,40 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
+        <v>80</v>
+      </c>
+      <c r="O9" t="s">
         <v>87</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
         <v>96</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1694,13 +1664,13 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F10">
         <v>1600000</v>
@@ -1727,10 +1697,10 @@
         <v>20000</v>
       </c>
       <c r="N10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="O10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="P10">
         <v>813929</v>
@@ -1760,7 +1730,7 @@
         <v>-7817567</v>
       </c>
       <c r="Y10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1768,16 +1738,16 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F11">
         <v>2000000</v>
@@ -1804,10 +1774,10 @@
         <v>30000</v>
       </c>
       <c r="N11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="O11" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="P11">
         <v>59096247022</v>
@@ -1837,7 +1807,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1845,16 +1815,16 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F12">
         <v>990000</v>
@@ -1881,10 +1851,10 @@
         <v>20000</v>
       </c>
       <c r="N12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="O12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="P12">
         <v>132326879204</v>
@@ -1914,7 +1884,7 @@
         <v>120676291668</v>
       </c>
       <c r="Y12" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1922,16 +1892,16 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F13">
         <v>2104000</v>
@@ -1958,10 +1928,10 @@
         <v>13500</v>
       </c>
       <c r="N13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="O13" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="P13">
         <v>13884202433</v>
@@ -1991,161 +1961,7 @@
         <v>-6716915237</v>
       </c>
       <c r="Y13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14">
-        <v>5000000</v>
-      </c>
-      <c r="G14">
-        <v>5000000</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>2000</v>
-      </c>
-      <c r="J14">
-        <v>2000</v>
-      </c>
-      <c r="K14">
-        <v>5605000</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>2000</v>
-      </c>
-      <c r="N14" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" t="s">
-        <v>96</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15">
-        <v>4000000</v>
-      </c>
-      <c r="G15">
-        <v>4000000</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>2000</v>
-      </c>
-      <c r="J15">
-        <v>2000</v>
-      </c>
-      <c r="K15">
-        <v>4210000</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>2000</v>
-      </c>
-      <c r="N15" t="s">
-        <v>93</v>
-      </c>
-      <c r="O15" t="s">
-        <v>96</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2163,422 +1979,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F5" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F8" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" t="s">
         <v>149</v>
       </c>
-      <c r="C13" t="s">
-        <v>159</v>
-      </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" t="s">
         <v>188</v>
-      </c>
-      <c r="F14" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="F16" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F19" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="F20" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="F21" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-10
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="197">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -362,6 +362,9 @@
     <t>하이젠알앤엠</t>
   </si>
   <si>
+    <t>미래에셋비전스팩5호</t>
+  </si>
+  <si>
     <t>한국스팩14호</t>
   </si>
   <si>
@@ -380,9 +383,6 @@
     <t>라메디텍</t>
   </si>
   <si>
-    <t>미래에셋비전스팩5호</t>
-  </si>
-  <si>
     <t>그리드위즈</t>
   </si>
   <si>
@@ -434,9 +434,6 @@
     <t>2024.05.27~05.31</t>
   </si>
   <si>
-    <t>2024.05.23~05.24</t>
-  </si>
-  <si>
     <t>2024.05.23~05.29</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
     <t>15300</t>
   </si>
   <si>
+    <t>9500</t>
+  </si>
+  <si>
     <t>8000</t>
   </si>
   <si>
@@ -545,9 +545,6 @@
     <t>13499</t>
   </si>
   <si>
-    <t>9500</t>
-  </si>
-  <si>
     <t>47600</t>
   </si>
   <si>
@@ -581,13 +578,13 @@
     <t>한국투자증권</t>
   </si>
   <si>
+    <t>미래에셋증권</t>
+  </si>
+  <si>
     <t>DB금융투자</t>
   </si>
   <si>
     <t>대신증권</t>
-  </si>
-  <si>
-    <t>미래에셋증권</t>
   </si>
   <si>
     <t>삼성증권</t>
@@ -2091,16 +2088,16 @@
         <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
         <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2111,13 +2108,13 @@
         <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
         <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F3" t="s">
         <v>187</v>
@@ -2128,19 +2125,19 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2148,19 +2145,19 @@
         <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2168,19 +2165,19 @@
         <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
         <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2188,19 +2185,19 @@
         <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
         <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2211,16 +2208,16 @@
         <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
         <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2228,19 +2225,19 @@
         <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
         <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2248,19 +2245,19 @@
         <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
         <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2268,19 +2265,19 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
         <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2288,19 +2285,19 @@
         <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2308,19 +2305,19 @@
         <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2328,10 +2325,10 @@
         <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14" t="s">
         <v>89</v>
@@ -2340,7 +2337,7 @@
         <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2348,19 +2345,19 @@
         <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
         <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2368,19 +2365,19 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
         <v>173</v>
       </c>
       <c r="F16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2388,19 +2385,19 @@
         <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2408,19 +2405,19 @@
         <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2428,19 +2425,19 @@
         <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2448,19 +2445,19 @@
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2468,19 +2465,19 @@
         <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-11
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="198">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -509,6 +509,9 @@
     <t>11,000~14,000</t>
   </si>
   <si>
+    <t>14000</t>
+  </si>
+  <si>
     <t>2000</t>
   </si>
   <si>
@@ -557,7 +560,7 @@
     <t>16290</t>
   </si>
   <si>
-    <t>10440</t>
+    <t>16800</t>
   </si>
   <si>
     <t>25610</t>
@@ -2094,10 +2097,10 @@
         <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2114,10 +2117,10 @@
         <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2134,10 +2137,10 @@
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2154,10 +2157,10 @@
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2174,10 +2177,10 @@
         <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2194,10 +2197,10 @@
         <v>89</v>
       </c>
       <c r="E7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2214,10 +2217,10 @@
         <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2234,10 +2237,10 @@
         <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2254,10 +2257,10 @@
         <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2274,10 +2277,10 @@
         <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2294,10 +2297,10 @@
         <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2314,10 +2317,10 @@
         <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2337,7 +2340,7 @@
         <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2351,13 +2354,13 @@
         <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2371,13 +2374,13 @@
         <v>151</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2391,13 +2394,13 @@
         <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2411,13 +2414,13 @@
         <v>151</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2431,13 +2434,13 @@
         <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2451,13 +2454,13 @@
         <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2471,13 +2474,13 @@
         <v>151</v>
       </c>
       <c r="D21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E21" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-13
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="192">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -122,9 +122,6 @@
     <t>2024-02-29</t>
   </si>
   <si>
-    <t>2024-02-21</t>
-  </si>
-  <si>
     <t>2024-04-19</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>2024-03-07</t>
   </si>
   <si>
-    <t>2024-02-27</t>
-  </si>
-  <si>
     <t>2024-05-07</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>삼현</t>
   </si>
   <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
     <t>988.32:1</t>
   </si>
   <si>
@@ -278,9 +269,6 @@
     <t>649.11:1</t>
   </si>
   <si>
-    <t>993.21:1</t>
-  </si>
-  <si>
     <t>13.19%</t>
   </si>
   <si>
@@ -302,9 +290,6 @@
     <t>10.64%</t>
   </si>
   <si>
-    <t>2.85%</t>
-  </si>
-  <si>
     <t>소형 및 초소형 슈퍼커패시터</t>
   </si>
   <si>
@@ -336,9 +321,6 @@
   </si>
   <si>
     <t>스마트 액추에이터, 스마트 파워유닛</t>
-  </si>
-  <si>
-    <t>생화학 측정기 및 센서, 면역진단기기 및 마커, 분자진단기기 및 시약 등</t>
   </si>
   <si>
     <t>종목명</t>
@@ -966,7 +948,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1054,16 +1036,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>1500000</v>
@@ -1090,10 +1072,10 @@
         <v>18000</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P2">
         <v>47284698907</v>
@@ -1123,7 +1105,7 @@
         <v>4195570793</v>
       </c>
       <c r="Y2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1131,16 +1113,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>3000000</v>
@@ -1167,10 +1149,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1200,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1208,16 +1190,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4">
         <v>3000000</v>
@@ -1244,10 +1226,10 @@
         <v>10500</v>
       </c>
       <c r="N4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P4">
         <v>9576212189</v>
@@ -1277,7 +1259,7 @@
         <v>-7501425172</v>
       </c>
       <c r="Y4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1285,16 +1267,16 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5">
         <v>1100000</v>
@@ -1321,10 +1303,10 @@
         <v>33000</v>
       </c>
       <c r="N5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P5">
         <v>-75676750274</v>
@@ -1354,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1362,16 +1344,16 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6">
         <v>5150000</v>
@@ -1398,10 +1380,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1431,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1439,16 +1421,16 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>3500000</v>
@@ -1475,10 +1457,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1508,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1516,16 +1498,16 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>3000000</v>
@@ -1552,10 +1534,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1585,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1593,16 +1575,16 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>5000000</v>
@@ -1629,10 +1611,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1662,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1670,16 +1652,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F10">
         <v>2500000</v>
@@ -1706,10 +1688,10 @@
         <v>13000</v>
       </c>
       <c r="N10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P10">
         <v>1230336508</v>
@@ -1739,7 +1721,7 @@
         <v>-7563224846</v>
       </c>
       <c r="Y10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1747,16 +1729,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>3000000</v>
@@ -1783,10 +1765,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1816,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1827,13 +1809,13 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F12">
         <v>1600000</v>
@@ -1860,10 +1842,10 @@
         <v>20000</v>
       </c>
       <c r="N12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="O12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="P12">
         <v>813929</v>
@@ -1893,7 +1875,7 @@
         <v>-7817567</v>
       </c>
       <c r="Y12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1901,16 +1883,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>2000000</v>
@@ -1937,10 +1919,10 @@
         <v>30000</v>
       </c>
       <c r="N13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="O13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P13">
         <v>59096247022</v>
@@ -1970,84 +1952,7 @@
         <v>7223298574</v>
       </c>
       <c r="Y13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14">
-        <v>990000</v>
-      </c>
-      <c r="G14">
-        <v>990000</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>13000</v>
-      </c>
-      <c r="J14">
-        <v>15000</v>
-      </c>
-      <c r="K14">
-        <v>14104416</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>20000</v>
-      </c>
-      <c r="N14" t="s">
-        <v>87</v>
-      </c>
-      <c r="O14" t="s">
-        <v>95</v>
-      </c>
-      <c r="P14">
-        <v>132326879204</v>
-      </c>
-      <c r="Q14">
-        <v>193893072828</v>
-      </c>
-      <c r="R14">
-        <v>341250572142</v>
-      </c>
-      <c r="S14">
-        <v>-7083727446</v>
-      </c>
-      <c r="T14">
-        <v>49300174288</v>
-      </c>
-      <c r="U14">
-        <v>150061283068</v>
-      </c>
-      <c r="V14">
-        <v>1473132550</v>
-      </c>
-      <c r="W14">
-        <v>40660749810</v>
-      </c>
-      <c r="X14">
-        <v>120676291668</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2065,422 +1970,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F8" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F11" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F17" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F18" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F21" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-14
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="189">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -344,6 +344,12 @@
     <t>하이젠알앤엠</t>
   </si>
   <si>
+    <t>KB스팩29호</t>
+  </si>
+  <si>
+    <t>에이치엠씨아이비스팩7호</t>
+  </si>
+  <si>
     <t>미래에셋비전스팩5호</t>
   </si>
   <si>
@@ -395,12 +401,12 @@
     <t>HD현대마린솔루션(구.HD현대글로벌서비스)(유가)</t>
   </si>
   <si>
-    <t>유안타스팩16호</t>
-  </si>
-  <si>
     <t>2024.06.07~06.13</t>
   </si>
   <si>
+    <t>2024.06.04~06.05</t>
+  </si>
+  <si>
     <t>2024.06.03~06.04</t>
   </si>
   <si>
@@ -443,12 +449,6 @@
     <t>2024.04.16~04.22</t>
   </si>
   <si>
-    <t>2024.04.15~04.19</t>
-  </si>
-  <si>
-    <t>2024.04.15~04.16</t>
-  </si>
-  <si>
     <t>4,500~5,500</t>
   </si>
   <si>
@@ -488,9 +488,6 @@
     <t>73,300~83,400</t>
   </si>
   <si>
-    <t>11,000~14,000</t>
-  </si>
-  <si>
     <t>14000</t>
   </si>
   <si>
@@ -503,12 +500,12 @@
     <t>83400</t>
   </si>
   <si>
-    <t>18000</t>
-  </si>
-  <si>
     <t>15300</t>
   </si>
   <si>
+    <t>12000</t>
+  </si>
+  <si>
     <t>9500</t>
   </si>
   <si>
@@ -554,15 +551,15 @@
     <t>652370</t>
   </si>
   <si>
-    <t>16500</t>
-  </si>
-  <si>
-    <t>10300</t>
-  </si>
-  <si>
     <t>한국투자증권</t>
   </si>
   <si>
+    <t>KB증권</t>
+  </si>
+  <si>
+    <t>현대차증권</t>
+  </si>
+  <si>
     <t>미래에셋증권</t>
   </si>
   <si>
@@ -581,16 +578,10 @@
     <t>NH투자증권</t>
   </si>
   <si>
-    <t>KB증권</t>
-  </si>
-  <si>
     <t>SK증권</t>
   </si>
   <si>
     <t>KB증권,신한투자증권,하나증권,대신증권,삼성증권</t>
-  </si>
-  <si>
-    <t>유안타증권</t>
   </si>
 </sst>
 </file>
@@ -1993,7 +1984,7 @@
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>144</v>
@@ -2002,10 +1993,10 @@
         <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2013,7 +2004,7 @@
         <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
         <v>145</v>
@@ -2022,10 +2013,10 @@
         <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2033,7 +2024,7 @@
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
         <v>145</v>
@@ -2042,10 +2033,10 @@
         <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2053,16 +2044,16 @@
         <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
         <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
         <v>181</v>
@@ -2076,16 +2067,16 @@
         <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
         <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2096,16 +2087,16 @@
         <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
         <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2116,16 +2107,16 @@
         <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
         <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2133,19 +2124,19 @@
         <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
         <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2153,19 +2144,19 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
         <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F10" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2173,19 +2164,19 @@
         <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
         <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2193,19 +2184,19 @@
         <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
         <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2216,13 +2207,13 @@
         <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
         <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
         <v>185</v>
@@ -2236,16 +2227,16 @@
         <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
         <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2256,16 +2247,16 @@
         <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2279,13 +2270,13 @@
         <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2296,16 +2287,16 @@
         <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2319,13 +2310,13 @@
         <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2336,56 +2327,56 @@
         <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
         <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
         <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-22
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="189">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -380,6 +380,9 @@
     <t>엑셀세라퓨틱스</t>
   </si>
   <si>
+    <t>시프트업</t>
+  </si>
+  <si>
     <t>이노그리드</t>
   </si>
   <si>
@@ -407,9 +410,6 @@
     <t>노브랜드</t>
   </si>
   <si>
-    <t>KB스팩28호</t>
-  </si>
-  <si>
     <t>2024.06.13~06.19</t>
   </si>
   <si>
@@ -431,6 +431,9 @@
     <t>2024.06.03~06.04</t>
   </si>
   <si>
+    <t>2024.06.03~06.13</t>
+  </si>
+  <si>
     <t>2024.05.31~06.07</t>
   </si>
   <si>
@@ -452,9 +455,6 @@
     <t>2024.04.30~05.08</t>
   </si>
   <si>
-    <t>2024.04.29~04.30</t>
-  </si>
-  <si>
     <t>9,000~12,000</t>
   </si>
   <si>
@@ -470,6 +470,9 @@
     <t>6,200~7,700</t>
   </si>
   <si>
+    <t>47,000~60,000</t>
+  </si>
+  <si>
     <t>29,000~35,000</t>
   </si>
   <si>
@@ -524,6 +527,9 @@
     <t>10032</t>
   </si>
   <si>
+    <t>340750</t>
+  </si>
+  <si>
     <t>17400</t>
   </si>
   <si>
@@ -564,6 +570,9 @@
   </si>
   <si>
     <t>대신증권</t>
+  </si>
+  <si>
+    <t>한국투자증권,NH투자증권,신한투자증권</t>
   </si>
   <si>
     <t>DB금융투자</t>
@@ -2061,10 +2070,10 @@
         <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2081,10 +2090,10 @@
         <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2101,10 +2110,10 @@
         <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2121,10 +2130,10 @@
         <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2141,10 +2150,10 @@
         <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2161,10 +2170,10 @@
         <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2181,10 +2190,10 @@
         <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2201,10 +2210,10 @@
         <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2221,10 +2230,10 @@
         <v>87</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2241,10 +2250,10 @@
         <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2261,10 +2270,10 @@
         <v>87</v>
       </c>
       <c r="E12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2275,16 +2284,16 @@
         <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
         <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2295,16 +2304,16 @@
         <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
         <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2312,7 +2321,7 @@
         <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
         <v>153</v>
@@ -2321,10 +2330,10 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2341,10 +2350,10 @@
         <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F16" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2352,7 +2361,7 @@
         <v>126</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
         <v>155</v>
@@ -2361,10 +2370,10 @@
         <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2381,10 +2390,10 @@
         <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2395,16 +2404,16 @@
         <v>143</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>177</v>
       </c>
       <c r="F19" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2415,16 +2424,16 @@
         <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
         <v>159</v>
       </c>
       <c r="E20" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2435,16 +2444,16 @@
         <v>145</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-23
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="195">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-04-30</t>
+  </si>
+  <si>
     <t>2024-04-29</t>
   </si>
   <si>
@@ -125,7 +128,7 @@
     <t>2024-03-06</t>
   </si>
   <si>
-    <t>2024-04-30</t>
+    <t>2024-05-08</t>
   </si>
   <si>
     <t>2024-05-30</t>
@@ -155,6 +158,9 @@
     <t>2024-03-13</t>
   </si>
   <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
     <t>2024-05-17</t>
   </si>
   <si>
@@ -176,6 +182,9 @@
     <t>2024-03-26</t>
   </si>
   <si>
+    <t>삼성</t>
+  </si>
+  <si>
     <t>KB</t>
   </si>
   <si>
@@ -200,6 +209,9 @@
     <t>미래</t>
   </si>
   <si>
+    <t>노브랜드</t>
+  </si>
+  <si>
     <t>KB제28호스팩</t>
   </si>
   <si>
@@ -239,6 +251,9 @@
     <t>엔젤로보틱스</t>
   </si>
   <si>
+    <t>1075.61:1</t>
+  </si>
+  <si>
     <t>1118.39:1</t>
   </si>
   <si>
@@ -278,6 +293,9 @@
     <t>1,157.0:1</t>
   </si>
   <si>
+    <t>4.51%</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -299,6 +317,9 @@
     <t>16.67%</t>
   </si>
   <si>
+    <t>Knit, Woven 의류</t>
+  </si>
+  <si>
     <t>기업인수합병</t>
   </si>
   <si>
@@ -405,9 +426,6 @@
   </si>
   <si>
     <t>미래에셋비전스팩4호</t>
-  </si>
-  <si>
-    <t>노브랜드</t>
   </si>
   <si>
     <t>2024.06.13~06.19</t>
@@ -939,7 +957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1027,76 +1045,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F2">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="G2">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>8700</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K2">
-        <v>5505000</v>
+        <v>7651263</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1104,46 +1122,46 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F3">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="G3">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>13124496</v>
+        <v>5505000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="O3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1173,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1184,73 +1202,73 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F4">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="G4">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="J4">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="K4">
-        <v>8503460</v>
+        <v>13124496</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="N4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="P4">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1261,73 +1279,73 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F5">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="G5">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K5">
-        <v>3310000</v>
+        <v>8503460</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>47284698907</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>38750429966</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>25900014771</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>7595091433</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>5807002440</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>3668321605</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>5701880294</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>4780312126</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>4195570793</v>
       </c>
       <c r="Y5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1335,16 +1353,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6">
         <v>3000000</v>
@@ -1356,197 +1374,197 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>6500</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>8500</v>
+        <v>2000</v>
       </c>
       <c r="K6">
-        <v>21945300</v>
+        <v>3310000</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="O6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P6">
-        <v>9576212189</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>11914994171</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>7285537916</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1172310325</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>-2762203259</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>-4737405164</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>-7460336546</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>-7104430732</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>-7501425172</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F7">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="G7">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>22000</v>
+        <v>6500</v>
       </c>
       <c r="J7">
-        <v>26000</v>
+        <v>8500</v>
       </c>
       <c r="K7">
-        <v>10429232</v>
+        <v>21945300</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>33000</v>
+        <v>10500</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="P7">
-        <v>-75676750274</v>
+        <v>9576212189</v>
       </c>
       <c r="Q7">
-        <v>-68652978862</v>
+        <v>11914994171</v>
       </c>
       <c r="R7">
-        <v>-9506668082</v>
+        <v>7285537916</v>
       </c>
       <c r="S7">
-        <v>-69862474811</v>
+        <v>1172310325</v>
       </c>
       <c r="T7">
-        <v>-137025491259</v>
+        <v>-2762203259</v>
       </c>
       <c r="U7">
-        <v>3014576074</v>
+        <v>-4737405164</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>-7460336546</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>-7104430732</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>-7501425172</v>
       </c>
       <c r="Y7" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F8">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="G8">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J8">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K8">
-        <v>5510000</v>
+        <v>10429232</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>2000</v>
+        <v>33000</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O8" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>-75676750274</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>-68652978862</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>-9506668082</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>-69862474811</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>-137025491259</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>3014576074</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1558,30 +1576,30 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F9">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="G9">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1593,7 +1611,7 @@
         <v>2000</v>
       </c>
       <c r="K9">
-        <v>3700000</v>
+        <v>5510000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1602,10 +1620,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="O9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1635,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1646,19 +1664,19 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F10">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="G10">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1670,7 +1688,7 @@
         <v>2000</v>
       </c>
       <c r="K10">
-        <v>3620000</v>
+        <v>3700000</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1679,10 +1697,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="O10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1723,19 +1741,19 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F11">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="G11">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1747,7 +1765,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>5520000</v>
+        <v>3620000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1756,10 +1774,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="O11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1789,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1800,73 +1818,73 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F12">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="G12">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>9900</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>13992625</v>
+        <v>5520000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P12">
-        <v>1230336508</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>2624739502</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>2926965114</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>-5277789009</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>-8667658271</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>-4923399541</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>-9788525741</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>-10436419054</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>-7563224846</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1877,73 +1895,73 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F13">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="G13">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K13">
-        <v>3200000</v>
+        <v>13992625</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O13" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1230336508</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>2624739502</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>2926965114</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>-5277789009</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>-8667658271</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>-4923399541</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>-9788525741</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>-10436419054</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>-7563224846</v>
       </c>
       <c r="Y13" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1951,76 +1969,153 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F14">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="G14">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J14">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K14">
-        <v>14014976</v>
+        <v>3200000</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O14" t="s">
         <v>93</v>
       </c>
       <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15">
+        <v>1600000</v>
+      </c>
+      <c r="G15">
+        <v>1600000</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>11000</v>
+      </c>
+      <c r="J15">
+        <v>15000</v>
+      </c>
+      <c r="K15">
+        <v>14014976</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>20000</v>
+      </c>
+      <c r="N15" t="s">
+        <v>91</v>
+      </c>
+      <c r="O15" t="s">
+        <v>99</v>
+      </c>
+      <c r="P15">
         <v>813929</v>
       </c>
-      <c r="Q14">
+      <c r="Q15">
         <v>2184312</v>
       </c>
-      <c r="R14">
+      <c r="R15">
         <v>3744252</v>
       </c>
-      <c r="S14">
+      <c r="S15">
         <v>-4828658</v>
       </c>
-      <c r="T14">
+      <c r="T15">
         <v>-7101029</v>
       </c>
-      <c r="U14">
+      <c r="U15">
         <v>-4926381</v>
       </c>
-      <c r="V14">
+      <c r="V15">
         <v>-24094044</v>
       </c>
-      <c r="W14">
+      <c r="W15">
         <v>-6797310</v>
       </c>
-      <c r="X14">
+      <c r="X15">
         <v>-7817567</v>
       </c>
-      <c r="Y14" t="s">
-        <v>104</v>
+      <c r="Y15" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2038,422 +2133,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F8" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F10" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="F15" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F17" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="F18" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="F19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="F21" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-25
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -377,6 +377,12 @@
     <t>하스</t>
   </si>
   <si>
+    <t>에이치브이엠(구.한국진공야금)</t>
+  </si>
+  <si>
+    <t>이노스페이스</t>
+  </si>
+  <si>
     <t>한국스팩15호</t>
   </si>
   <si>
@@ -422,12 +428,6 @@
     <t>그리드위즈</t>
   </si>
   <si>
-    <t>이노스페이스</t>
-  </si>
-  <si>
-    <t>에이치브이엠(구.한국진공야금)</t>
-  </si>
-  <si>
     <t>미래에셋비전스팩4호</t>
   </si>
   <si>
@@ -437,6 +437,9 @@
     <t>2024.06.13~06.19</t>
   </si>
   <si>
+    <t>2024.06.11~06.17</t>
+  </si>
+  <si>
     <t>2024.06.10~06.11</t>
   </si>
   <si>
@@ -470,9 +473,6 @@
     <t>2024.05.23~05.29</t>
   </si>
   <si>
-    <t>2024.05.22~05.28</t>
-  </si>
-  <si>
     <t>2024.05.13~05.14</t>
   </si>
   <si>
@@ -482,6 +482,12 @@
     <t>9,000~12,000</t>
   </si>
   <si>
+    <t>11,000~14,200</t>
+  </si>
+  <si>
+    <t>36,400~43,300</t>
+  </si>
+  <si>
     <t>2,000~2,000</t>
   </si>
   <si>
@@ -509,12 +515,6 @@
     <t>34,000~40,000</t>
   </si>
   <si>
-    <t>36,400~45,600</t>
-  </si>
-  <si>
-    <t>11,000~14,200</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -524,6 +524,12 @@
     <t>16290</t>
   </si>
   <si>
+    <t>26400</t>
+  </si>
+  <si>
+    <t>48412</t>
+  </si>
+  <si>
     <t>12500</t>
   </si>
   <si>
@@ -569,18 +575,15 @@
     <t>47600</t>
   </si>
   <si>
-    <t>48412</t>
-  </si>
-  <si>
-    <t>26400</t>
-  </si>
-  <si>
     <t>NH투자증권</t>
   </si>
   <si>
     <t>삼성증권</t>
   </si>
   <si>
+    <t>미래에셋증권,신한투자증권</t>
+  </si>
+  <si>
     <t>한국투자증권</t>
   </si>
   <si>
@@ -600,9 +603,6 @@
   </si>
   <si>
     <t>DB금융투자</t>
-  </si>
-  <si>
-    <t>미래에셋증권,신한투자증권</t>
   </si>
 </sst>
 </file>
@@ -2211,7 +2211,7 @@
         <v>169</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2219,7 +2219,7 @@
         <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
         <v>156</v>
@@ -2239,10 +2239,10 @@
         <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
         <v>93</v>
@@ -2259,10 +2259,10 @@
         <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
         <v>93</v>
@@ -2271,7 +2271,7 @@
         <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2282,7 +2282,7 @@
         <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
         <v>93</v>
@@ -2291,7 +2291,7 @@
         <v>173</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2311,7 +2311,7 @@
         <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2319,10 +2319,10 @@
         <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
         <v>93</v>
@@ -2331,7 +2331,7 @@
         <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2342,7 +2342,7 @@
         <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
         <v>93</v>
@@ -2351,7 +2351,7 @@
         <v>176</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2359,10 +2359,10 @@
         <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
         <v>93</v>
@@ -2371,7 +2371,7 @@
         <v>177</v>
       </c>
       <c r="F12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2382,7 +2382,7 @@
         <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>93</v>
@@ -2391,7 +2391,7 @@
         <v>178</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2399,7 +2399,7 @@
         <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
         <v>160</v>
@@ -2411,7 +2411,7 @@
         <v>179</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2419,10 +2419,10 @@
         <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
         <v>93</v>
@@ -2439,10 +2439,10 @@
         <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
         <v>93</v>
@@ -2451,7 +2451,7 @@
         <v>181</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2462,7 +2462,7 @@
         <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>93</v>
@@ -2471,7 +2471,7 @@
         <v>182</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2491,7 +2491,7 @@
         <v>183</v>
       </c>
       <c r="F18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2511,7 +2511,7 @@
         <v>184</v>
       </c>
       <c r="F19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2531,7 +2531,7 @@
         <v>185</v>
       </c>
       <c r="F20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2542,7 +2542,7 @@
         <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D21" t="s">
         <v>166</v>
@@ -2551,7 +2551,7 @@
         <v>93</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-27
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="186">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -122,12 +122,6 @@
     <t>2024-03-14</t>
   </si>
   <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-03-06</t>
-  </si>
-  <si>
     <t>2024-05-08</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>2024-03-20</t>
   </si>
   <si>
-    <t>2024-03-13</t>
-  </si>
-  <si>
     <t>2024-05-23</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>2024-04-03</t>
   </si>
   <si>
-    <t>2024-03-26</t>
-  </si>
-  <si>
     <t>삼성</t>
   </si>
   <si>
@@ -245,12 +233,6 @@
     <t>아이엠비디엑스</t>
   </si>
   <si>
-    <t>하나32호스팩</t>
-  </si>
-  <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
     <t>1075.61:1</t>
   </si>
   <si>
@@ -287,12 +269,6 @@
     <t>865.73 :1</t>
   </si>
   <si>
-    <t>1247.72:1</t>
-  </si>
-  <si>
-    <t>1,157.0:1</t>
-  </si>
-  <si>
     <t>4.51%</t>
   </si>
   <si>
@@ -314,9 +290,6 @@
     <t>4.50%</t>
   </si>
   <si>
-    <t>16.67%</t>
-  </si>
-  <si>
     <t>Knit, Woven 의류</t>
   </si>
   <si>
@@ -348,9 +321,6 @@
   </si>
   <si>
     <t>알파리퀴드ⓡ 100, 알파리퀴드ⓡ HRR, 알파리퀴드ⓡ 디텍트, 알파리퀴드ⓡ 스크리닝</t>
-  </si>
-  <si>
-    <t>재활 전문 웨어러블 로봇, 근력 보조 무동력 웨어러블 슈트, 일상생활 보조 웨어러블 로봇 등</t>
   </si>
   <si>
     <t>종목명</t>
@@ -960,7 +930,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1048,16 +1018,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>1200000</v>
@@ -1084,10 +1054,10 @@
         <v>14000</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="P2">
         <v>468321534076</v>
@@ -1117,7 +1087,7 @@
         <v>4820429371</v>
       </c>
       <c r="Y2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1128,13 +1098,13 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>5000000</v>
@@ -1161,10 +1131,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="O3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1194,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1202,16 +1172,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F4">
         <v>1970000</v>
@@ -1238,10 +1208,10 @@
         <v>20000</v>
       </c>
       <c r="N4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1271,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1279,16 +1249,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F5">
         <v>1500000</v>
@@ -1315,10 +1285,10 @@
         <v>18000</v>
       </c>
       <c r="N5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="O5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="P5">
         <v>47284698907</v>
@@ -1348,7 +1318,7 @@
         <v>4195570793</v>
       </c>
       <c r="Y5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1356,16 +1326,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F6">
         <v>3000000</v>
@@ -1392,10 +1362,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1425,7 +1395,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1433,16 +1403,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>3000000</v>
@@ -1469,10 +1439,10 @@
         <v>10500</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="O7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="P7">
         <v>9576212189</v>
@@ -1502,7 +1472,7 @@
         <v>-7501425172</v>
       </c>
       <c r="Y7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1510,16 +1480,16 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>1100000</v>
@@ -1546,10 +1516,10 @@
         <v>33000</v>
       </c>
       <c r="N8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="P8">
         <v>-75676750274</v>
@@ -1579,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1587,16 +1557,16 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>5150000</v>
@@ -1623,10 +1593,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1656,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1664,16 +1634,16 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F10">
         <v>3500000</v>
@@ -1700,10 +1670,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="O10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1733,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1741,16 +1711,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>3000000</v>
@@ -1777,10 +1747,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="O11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1810,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1818,16 +1788,16 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F12">
         <v>5000000</v>
@@ -1854,10 +1824,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1887,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1895,16 +1865,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>2500000</v>
@@ -1931,10 +1901,10 @@
         <v>13000</v>
       </c>
       <c r="N13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="P13">
         <v>1230336508</v>
@@ -1964,161 +1934,7 @@
         <v>-7563224846</v>
       </c>
       <c r="Y13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14">
-        <v>3000000</v>
-      </c>
-      <c r="G14">
-        <v>3000000</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>2000</v>
-      </c>
-      <c r="J14">
-        <v>2000</v>
-      </c>
-      <c r="K14">
-        <v>3200000</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>2000</v>
-      </c>
-      <c r="N14" t="s">
-        <v>90</v>
-      </c>
-      <c r="O14" t="s">
-        <v>93</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15">
-        <v>1600000</v>
-      </c>
-      <c r="G15">
-        <v>1600000</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>11000</v>
-      </c>
-      <c r="J15">
-        <v>15000</v>
-      </c>
-      <c r="K15">
-        <v>14014976</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>20000</v>
-      </c>
-      <c r="N15" t="s">
-        <v>91</v>
-      </c>
-      <c r="O15" t="s">
-        <v>99</v>
-      </c>
-      <c r="P15">
-        <v>813929</v>
-      </c>
-      <c r="Q15">
-        <v>2184312</v>
-      </c>
-      <c r="R15">
-        <v>3744252</v>
-      </c>
-      <c r="S15">
-        <v>-4828658</v>
-      </c>
-      <c r="T15">
-        <v>-7101029</v>
-      </c>
-      <c r="U15">
-        <v>-4926381</v>
-      </c>
-      <c r="V15">
-        <v>-24094044</v>
-      </c>
-      <c r="W15">
-        <v>-6797310</v>
-      </c>
-      <c r="X15">
-        <v>-7817567</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2136,422 +1952,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-29
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="173">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-05-13</t>
+  </si>
+  <si>
     <t>2024-04-30</t>
   </si>
   <si>
@@ -122,6 +125,9 @@
     <t>2024-03-14</t>
   </si>
   <si>
+    <t>2024-05-14</t>
+  </si>
+  <si>
     <t>2024-05-08</t>
   </si>
   <si>
@@ -149,6 +155,9 @@
     <t>2024-03-20</t>
   </si>
   <si>
+    <t>2024-05-29</t>
+  </si>
+  <si>
     <t>2024-05-23</t>
   </si>
   <si>
@@ -170,6 +179,9 @@
     <t>2024-04-03</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>삼성</t>
   </si>
   <si>
@@ -194,7 +206,7 @@
     <t>신한</t>
   </si>
   <si>
-    <t>미래</t>
+    <t>미래에셋비전스팩4호</t>
   </si>
   <si>
     <t>노브랜드</t>
@@ -233,6 +245,9 @@
     <t>아이엠비디엑스</t>
   </si>
   <si>
+    <t>1011.2:1</t>
+  </si>
+  <si>
     <t>1075.61:1</t>
   </si>
   <si>
@@ -269,12 +284,12 @@
     <t>865.73 :1</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>4.51%</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>6.54%</t>
   </si>
   <si>
@@ -290,6 +305,9 @@
     <t>4.50%</t>
   </si>
   <si>
+    <t>기업인수목적회사(기타금융서비스)</t>
+  </si>
+  <si>
     <t>Knit, Woven 의류</t>
   </si>
   <si>
@@ -347,6 +365,9 @@
     <t>이엔셀</t>
   </si>
   <si>
+    <t>이노그리드</t>
+  </si>
+  <si>
     <t>하스</t>
   </si>
   <si>
@@ -386,9 +407,6 @@
     <t>시프트업</t>
   </si>
   <si>
-    <t>이노그리드</t>
-  </si>
-  <si>
     <t>한중엔시에스</t>
   </si>
   <si>
@@ -434,9 +452,6 @@
     <t>2024.06.03~06.13</t>
   </si>
   <si>
-    <t>2024.05.31~06.07</t>
-  </si>
-  <si>
     <t>2024.05.30~06.05</t>
   </si>
   <si>
@@ -452,6 +467,9 @@
     <t>13,600~15,300</t>
   </si>
   <si>
+    <t>29,000~35,000</t>
+  </si>
+  <si>
     <t>9,000~12,000</t>
   </si>
   <si>
@@ -473,9 +491,6 @@
     <t>47,000~60,000</t>
   </si>
   <si>
-    <t>29,000~35,000</t>
-  </si>
-  <si>
     <t>20,000~23,500</t>
   </si>
   <si>
@@ -491,13 +506,13 @@
     <t>NH투자증권</t>
   </si>
   <si>
+    <t>한국투자증권</t>
+  </si>
+  <si>
     <t>삼성증권</t>
   </si>
   <si>
     <t>미래에셋증권,신한투자증권</t>
-  </si>
-  <si>
-    <t>한국투자증권</t>
   </si>
   <si>
     <t>미래에셋증권</t>
@@ -876,7 +891,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -964,76 +979,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F2">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="G2">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>8700</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K2">
-        <v>7651263</v>
+        <v>8100000</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P2">
-        <v>468321534076</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>555936831337</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>359249623614</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>22403886436</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>33386727728</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>10411712773</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>10859975142</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>29346086803</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>4820429371</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1041,76 +1056,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F3">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="G3">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>8700</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K3">
-        <v>5505000</v>
+        <v>7651263</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1118,46 +1133,46 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F4">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="G4">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K4">
-        <v>13124496</v>
+        <v>5505000</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="O4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1187,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1195,76 +1210,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F5">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="G5">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="J5">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="K5">
-        <v>8503460</v>
+        <v>13124496</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="N5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="P5">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1272,76 +1287,76 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F6">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="G6">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K6">
-        <v>3310000</v>
+        <v>8503460</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="O6" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>47284698907</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>38750429966</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>25900014771</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>7595091433</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>5807002440</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>3668321605</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>5701880294</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>4780312126</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>4195570793</v>
       </c>
       <c r="Y6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1349,16 +1364,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>3000000</v>
@@ -1370,197 +1385,197 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>6500</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>8500</v>
+        <v>2000</v>
       </c>
       <c r="K7">
-        <v>21945300</v>
+        <v>3310000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P7">
-        <v>9576212189</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>11914994171</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>7285537916</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>1172310325</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>-2762203259</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>-4737405164</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>-7460336546</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>-7104430732</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>-7501425172</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F8">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="G8">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>22000</v>
+        <v>6500</v>
       </c>
       <c r="J8">
-        <v>26000</v>
+        <v>8500</v>
       </c>
       <c r="K8">
-        <v>10429232</v>
+        <v>21945300</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>33000</v>
+        <v>10500</v>
       </c>
       <c r="N8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="O8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="P8">
-        <v>-75676750274</v>
+        <v>9576212189</v>
       </c>
       <c r="Q8">
-        <v>-68652978862</v>
+        <v>11914994171</v>
       </c>
       <c r="R8">
-        <v>-9506668082</v>
+        <v>7285537916</v>
       </c>
       <c r="S8">
-        <v>-69862474811</v>
+        <v>1172310325</v>
       </c>
       <c r="T8">
-        <v>-137025491259</v>
+        <v>-2762203259</v>
       </c>
       <c r="U8">
-        <v>3014576074</v>
+        <v>-4737405164</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>-7460336546</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>-7104430732</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>-7501425172</v>
       </c>
       <c r="Y8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F9">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="G9">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K9">
-        <v>5510000</v>
+        <v>10429232</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>33000</v>
       </c>
       <c r="N9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>-75676750274</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>-68652978862</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>-9506668082</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>-69862474811</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>-137025491259</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>3014576074</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1572,30 +1587,30 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F10">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="G10">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1607,7 +1622,7 @@
         <v>2000</v>
       </c>
       <c r="K10">
-        <v>3700000</v>
+        <v>5510000</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1616,10 +1631,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1649,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1657,22 +1672,22 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F11">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="G11">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1684,7 +1699,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>3620000</v>
+        <v>3700000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1693,10 +1708,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="O11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1726,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1734,22 +1749,22 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F12">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="G12">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1761,7 +1776,7 @@
         <v>2000</v>
       </c>
       <c r="K12">
-        <v>5520000</v>
+        <v>3620000</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1770,10 +1785,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="O12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1803,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1811,76 +1826,153 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F13">
+        <v>5000000</v>
+      </c>
+      <c r="G13">
+        <v>5000000</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2000</v>
+      </c>
+      <c r="J13">
+        <v>2000</v>
+      </c>
+      <c r="K13">
+        <v>5520000</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>2000</v>
+      </c>
+      <c r="N13" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" t="s">
+        <v>89</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14">
         <v>2500000</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>2500000</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>7700</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>9900</v>
       </c>
-      <c r="K13">
+      <c r="K14">
         <v>13992625</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>13000</v>
       </c>
-      <c r="N13" t="s">
-        <v>83</v>
-      </c>
-      <c r="O13" t="s">
-        <v>90</v>
-      </c>
-      <c r="P13">
+      <c r="N14" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" t="s">
+        <v>95</v>
+      </c>
+      <c r="P14">
         <v>1230336508</v>
       </c>
-      <c r="Q13">
+      <c r="Q14">
         <v>2624739502</v>
       </c>
-      <c r="R13">
+      <c r="R14">
         <v>2926965114</v>
       </c>
-      <c r="S13">
+      <c r="S14">
         <v>-5277789009</v>
       </c>
-      <c r="T13">
+      <c r="T14">
         <v>-8667658271</v>
       </c>
-      <c r="U13">
+      <c r="U14">
         <v>-4923399541</v>
       </c>
-      <c r="V13">
+      <c r="V14">
         <v>-9788525741</v>
       </c>
-      <c r="W13">
+      <c r="W14">
         <v>-10436419054</v>
       </c>
-      <c r="X13">
+      <c r="X14">
         <v>-7563224846</v>
       </c>
-      <c r="Y13" t="s">
-        <v>101</v>
+      <c r="Y14" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1898,422 +1990,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E2">
         <v>8000</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E3">
         <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E4">
-        <v>16290</v>
+        <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E5">
-        <v>26400</v>
+        <v>16290</v>
       </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E6">
-        <v>48412</v>
+        <v>26400</v>
       </c>
       <c r="F6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E7">
-        <v>12500</v>
+        <v>48412</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
         <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E8">
-        <v>15300</v>
+        <v>12500</v>
       </c>
       <c r="F8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E9">
-        <v>12900</v>
+        <v>15300</v>
       </c>
       <c r="F9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E10">
-        <v>12000</v>
+        <v>12900</v>
       </c>
       <c r="F10" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E11">
-        <v>14000</v>
+        <v>12000</v>
       </c>
       <c r="F11" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E12">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E13">
-        <v>9500</v>
+        <v>15000</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E14">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="F14" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E15">
-        <v>10032</v>
+        <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E16">
-        <v>340750</v>
+        <v>10032</v>
       </c>
       <c r="F16" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E17">
-        <v>17400</v>
+        <v>340750</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E18">
         <v>32000</v>
       </c>
       <c r="F18" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E19">
         <v>10000</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E20">
         <v>13650</v>
       </c>
       <c r="F20" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E21">
         <v>13499</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-31
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="176">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -404,7 +404,7 @@
     <t>엑셀세라퓨틱스</t>
   </si>
   <si>
-    <t>시프트업</t>
+    <t>시프트업(유가)</t>
   </si>
   <si>
     <t>신한글로벌액티브</t>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>10,500~14,000</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
   <si>
     <t>이베스트 투자증권</t>
@@ -2031,7 +2034,7 @@
         <v>8000</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2051,7 +2054,7 @@
         <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2071,7 +2074,7 @@
         <v>17400</v>
       </c>
       <c r="F4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2091,7 +2094,7 @@
         <v>16290</v>
       </c>
       <c r="F5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2111,7 +2114,7 @@
         <v>26400</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2131,7 +2134,7 @@
         <v>48412</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2151,7 +2154,7 @@
         <v>12500</v>
       </c>
       <c r="F8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2171,7 +2174,7 @@
         <v>15300</v>
       </c>
       <c r="F9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2191,7 +2194,7 @@
         <v>12900</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2211,7 +2214,7 @@
         <v>12000</v>
       </c>
       <c r="F11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2231,7 +2234,7 @@
         <v>14000</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2251,7 +2254,7 @@
         <v>15000</v>
       </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2271,7 +2274,7 @@
         <v>9500</v>
       </c>
       <c r="F14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2291,7 +2294,7 @@
         <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2311,7 +2314,7 @@
         <v>10032</v>
       </c>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2331,7 +2334,7 @@
         <v>340750</v>
       </c>
       <c r="F17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2351,7 +2354,7 @@
         <v>70000</v>
       </c>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2371,7 +2374,7 @@
         <v>32000</v>
       </c>
       <c r="F19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2385,13 +2388,13 @@
         <v>149</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="E20">
         <v>10000</v>
       </c>
       <c r="F20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2411,7 +2414,7 @@
         <v>13650</v>
       </c>
       <c r="F21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-01
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -359,6 +359,9 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>아이빔테크놀로지</t>
+  </si>
+  <si>
     <t>이베스트스팩6호</t>
   </si>
   <si>
@@ -416,7 +419,7 @@
     <t>디비금융스팩12호</t>
   </si>
   <si>
-    <t>씨어스테크놀로지</t>
+    <t>2024.07.15~07.19</t>
   </si>
   <si>
     <t>2024.06.27~06.28</t>
@@ -461,7 +464,7 @@
     <t>2024.05.28~05.29</t>
   </si>
   <si>
-    <t>2024.05.27~05.31</t>
+    <t>7,300~8,500</t>
   </si>
   <si>
     <t>2,000~2,000</t>
@@ -500,12 +503,12 @@
     <t>20,000~23,500</t>
   </si>
   <si>
-    <t>10,500~14,000</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
+    <t>삼성증권</t>
+  </si>
+  <si>
     <t>이베스트 투자증권</t>
   </si>
   <si>
@@ -513,9 +516,6 @@
   </si>
   <si>
     <t>한국투자증권</t>
-  </si>
-  <si>
-    <t>삼성증권</t>
   </si>
   <si>
     <t>미래에셋증권,신한투자증권</t>
@@ -2031,7 +2031,7 @@
         <v>89</v>
       </c>
       <c r="E2">
-        <v>8000</v>
+        <v>16308</v>
       </c>
       <c r="F2" t="s">
         <v>163</v>
@@ -2051,7 +2051,7 @@
         <v>89</v>
       </c>
       <c r="E3">
-        <v>21308</v>
+        <v>8000</v>
       </c>
       <c r="F3" t="s">
         <v>164</v>
@@ -2071,7 +2071,7 @@
         <v>89</v>
       </c>
       <c r="E4">
-        <v>17400</v>
+        <v>21308</v>
       </c>
       <c r="F4" t="s">
         <v>165</v>
@@ -2082,7 +2082,7 @@
         <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>152</v>
@@ -2091,7 +2091,7 @@
         <v>89</v>
       </c>
       <c r="E5">
-        <v>16290</v>
+        <v>17400</v>
       </c>
       <c r="F5" t="s">
         <v>166</v>
@@ -2111,10 +2111,10 @@
         <v>89</v>
       </c>
       <c r="E6">
-        <v>26400</v>
+        <v>16290</v>
       </c>
       <c r="F6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2122,7 +2122,7 @@
         <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
         <v>154</v>
@@ -2131,10 +2131,10 @@
         <v>89</v>
       </c>
       <c r="E7">
-        <v>48412</v>
+        <v>26400</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2145,16 +2145,16 @@
         <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
         <v>89</v>
       </c>
       <c r="E8">
-        <v>12500</v>
+        <v>48412</v>
       </c>
       <c r="F8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2165,16 +2165,16 @@
         <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D9" t="s">
         <v>89</v>
       </c>
       <c r="E9">
-        <v>15300</v>
+        <v>12500</v>
       </c>
       <c r="F9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2185,16 +2185,16 @@
         <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
         <v>89</v>
       </c>
       <c r="E10">
-        <v>12900</v>
+        <v>15300</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2205,16 +2205,16 @@
         <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
         <v>89</v>
       </c>
       <c r="E11">
-        <v>12000</v>
+        <v>12900</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2222,19 +2222,19 @@
         <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
       </c>
       <c r="E12">
-        <v>14000</v>
+        <v>12000</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2245,16 +2245,16 @@
         <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
       </c>
       <c r="E13">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="F13" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2265,16 +2265,16 @@
         <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
         <v>89</v>
       </c>
       <c r="E14">
-        <v>9500</v>
+        <v>15000</v>
       </c>
       <c r="F14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2282,19 +2282,19 @@
         <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D15" t="s">
         <v>89</v>
       </c>
       <c r="E15">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="F15" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2302,19 +2302,19 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D16" t="s">
         <v>89</v>
       </c>
       <c r="E16">
-        <v>10032</v>
+        <v>8000</v>
       </c>
       <c r="F16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2322,7 +2322,7 @@
         <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
         <v>158</v>
@@ -2331,10 +2331,10 @@
         <v>89</v>
       </c>
       <c r="E17">
-        <v>340750</v>
+        <v>10032</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2351,10 +2351,10 @@
         <v>89</v>
       </c>
       <c r="E18">
-        <v>70000</v>
+        <v>340750</v>
       </c>
       <c r="F18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2371,10 +2371,10 @@
         <v>89</v>
       </c>
       <c r="E19">
-        <v>32000</v>
+        <v>70000</v>
       </c>
       <c r="F19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2385,16 +2385,16 @@
         <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>89</v>
       </c>
       <c r="E20">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2405,16 +2405,16 @@
         <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="E21">
-        <v>13650</v>
+        <v>10000</v>
       </c>
       <c r="F21" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-03
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="169">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -122,9 +122,6 @@
     <t>2024-03-27</t>
   </si>
   <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
     <t>2024-05-14</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>2024-03-28</t>
   </si>
   <si>
-    <t>2024-03-20</t>
-  </si>
-  <si>
     <t>2024-05-29</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>2024-04-22</t>
   </si>
   <si>
-    <t>2024-04-03</t>
-  </si>
-  <si>
     <t>미래</t>
   </si>
   <si>
@@ -242,9 +233,6 @@
     <t>신한제12호스팩</t>
   </si>
   <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
     <t>1011.2:1</t>
   </si>
   <si>
@@ -281,9 +269,6 @@
     <t>1,104.54:1</t>
   </si>
   <si>
-    <t>865.73 :1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -302,9 +287,6 @@
     <t>10.96%</t>
   </si>
   <si>
-    <t>4.50%</t>
-  </si>
-  <si>
     <t>기업인수목적회사(기타금융서비스)</t>
   </si>
   <si>
@@ -336,9 +318,6 @@
   </si>
   <si>
     <t>금융서비스(기업인수목적회사)</t>
-  </si>
-  <si>
-    <t>알파리퀴드ⓡ 100, 알파리퀴드ⓡ HRR, 알파리퀴드ⓡ 디텍트, 알파리퀴드ⓡ 스크리닝</t>
   </si>
   <si>
     <t>종목명</t>
@@ -900,7 +879,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -988,16 +967,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>6650000</v>
@@ -1024,10 +1003,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1057,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1065,16 +1044,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>1200000</v>
@@ -1101,10 +1080,10 @@
         <v>14000</v>
       </c>
       <c r="N3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="O3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="P3">
         <v>468321534076</v>
@@ -1134,7 +1113,7 @@
         <v>4820429371</v>
       </c>
       <c r="Y3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1145,13 +1124,13 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F4">
         <v>5000000</v>
@@ -1178,10 +1157,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1211,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1219,16 +1198,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F5">
         <v>1970000</v>
@@ -1255,10 +1234,10 @@
         <v>20000</v>
       </c>
       <c r="N5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1288,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1296,16 +1275,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6">
         <v>1500000</v>
@@ -1332,10 +1311,10 @@
         <v>18000</v>
       </c>
       <c r="N6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="P6">
         <v>47284698907</v>
@@ -1365,7 +1344,7 @@
         <v>4195570793</v>
       </c>
       <c r="Y6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1373,16 +1352,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>3000000</v>
@@ -1409,10 +1388,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="O7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1442,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1450,16 +1429,16 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>3000000</v>
@@ -1486,10 +1465,10 @@
         <v>10500</v>
       </c>
       <c r="N8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="P8">
         <v>9576212189</v>
@@ -1519,7 +1498,7 @@
         <v>-7501425172</v>
       </c>
       <c r="Y8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1527,16 +1506,16 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F9">
         <v>1100000</v>
@@ -1563,10 +1542,10 @@
         <v>33000</v>
       </c>
       <c r="N9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="P9">
         <v>-75676750274</v>
@@ -1596,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1604,16 +1583,16 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F10">
         <v>5150000</v>
@@ -1640,10 +1619,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1673,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1681,16 +1660,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11">
         <v>3500000</v>
@@ -1717,10 +1696,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="O11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1750,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1758,16 +1737,16 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F12">
         <v>3000000</v>
@@ -1794,10 +1773,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="O12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1827,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1835,16 +1814,16 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F13">
         <v>5000000</v>
@@ -1871,10 +1850,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="O13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1904,84 +1883,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14">
-        <v>2500000</v>
-      </c>
-      <c r="G14">
-        <v>2500000</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>7700</v>
-      </c>
-      <c r="J14">
-        <v>9900</v>
-      </c>
-      <c r="K14">
-        <v>13992625</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>13000</v>
-      </c>
-      <c r="N14" t="s">
-        <v>88</v>
-      </c>
-      <c r="O14" t="s">
-        <v>95</v>
-      </c>
-      <c r="P14">
-        <v>1230336508</v>
-      </c>
-      <c r="Q14">
-        <v>2624739502</v>
-      </c>
-      <c r="R14">
-        <v>2926965114</v>
-      </c>
-      <c r="S14">
-        <v>-5277789009</v>
-      </c>
-      <c r="T14">
-        <v>-8667658271</v>
-      </c>
-      <c r="U14">
-        <v>-4923399541</v>
-      </c>
-      <c r="V14">
-        <v>-9788525741</v>
-      </c>
-      <c r="W14">
-        <v>-10436419054</v>
-      </c>
-      <c r="X14">
-        <v>-7563224846</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1999,422 +1901,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E2">
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>8000</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E4">
         <v>21308</v>
       </c>
       <c r="F4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E5">
         <v>17400</v>
       </c>
       <c r="F5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E6">
         <v>16290</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E7">
         <v>26400</v>
       </c>
       <c r="F7" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E8">
         <v>48412</v>
       </c>
       <c r="F8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E9">
         <v>12500</v>
       </c>
       <c r="F9" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E10">
         <v>15300</v>
       </c>
       <c r="F10" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E11">
         <v>12900</v>
       </c>
       <c r="F11" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E12">
         <v>12000</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E13">
         <v>14000</v>
       </c>
       <c r="F13" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E14">
         <v>15000</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E15">
         <v>9500</v>
       </c>
       <c r="F15" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E16">
         <v>8000</v>
       </c>
       <c r="F16" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E17">
         <v>10032</v>
       </c>
       <c r="F17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E18">
         <v>340750</v>
       </c>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E19">
         <v>70000</v>
       </c>
       <c r="F19" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E20">
         <v>32000</v>
       </c>
       <c r="F20" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E21">
         <v>10000</v>
       </c>
       <c r="F21" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-06
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="170">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -344,6 +344,12 @@
     <t>이베스트스팩6호</t>
   </si>
   <si>
+    <t>엑셀세라퓨틱스</t>
+  </si>
+  <si>
+    <t>피앤에스미캐닉스</t>
+  </si>
+  <si>
     <t>이엔셀</t>
   </si>
   <si>
@@ -383,9 +389,6 @@
     <t>한국스팩14호</t>
   </si>
   <si>
-    <t>엑셀세라퓨틱스</t>
-  </si>
-  <si>
     <t>시프트업(유가)</t>
   </si>
   <si>
@@ -395,15 +398,15 @@
     <t>한중엔시에스</t>
   </si>
   <si>
-    <t>디비금융스팩12호</t>
-  </si>
-  <si>
     <t>2024.07.15~07.19</t>
   </si>
   <si>
     <t>2024.06.27~06.28</t>
   </si>
   <si>
+    <t>2024.06.24~06.28</t>
+  </si>
+  <si>
     <t>2024.06.17~06.21</t>
   </si>
   <si>
@@ -431,7 +434,7 @@
     <t>2024.06.03~06.04</t>
   </si>
   <si>
-    <t>2024.06.03~06.13</t>
+    <t>2024.06.03~06.27</t>
   </si>
   <si>
     <t>2024.06.03~06.05</t>
@@ -440,15 +443,18 @@
     <t>2024.05.30~06.05</t>
   </si>
   <si>
-    <t>2024.05.28~05.29</t>
-  </si>
-  <si>
     <t>7,300~8,500</t>
   </si>
   <si>
     <t>2,000~2,000</t>
   </si>
   <si>
+    <t>6,200~7,700</t>
+  </si>
+  <si>
+    <t>14,000~17,000</t>
+  </si>
+  <si>
     <t>13,600~15,300</t>
   </si>
   <si>
@@ -470,9 +476,6 @@
     <t>7,500~9,000</t>
   </si>
   <si>
-    <t>6,200~7,700</t>
-  </si>
-  <si>
     <t>47,000~60,000</t>
   </si>
   <si>
@@ -491,6 +494,12 @@
     <t>엘에스증권</t>
   </si>
   <si>
+    <t>대신증권</t>
+  </si>
+  <si>
+    <t>키움증권</t>
+  </si>
+  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -509,9 +518,6 @@
     <t>현대차증권</t>
   </si>
   <si>
-    <t>대신증권</t>
-  </si>
-  <si>
     <t>한국투자증권,NH투자증권,신한투자증권</t>
   </si>
   <si>
@@ -519,9 +525,6 @@
   </si>
   <si>
     <t>IBK투자증권</t>
-  </si>
-  <si>
-    <t>DB금융투자</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1939,7 @@
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1956,7 +1959,7 @@
         <v>8000</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1973,10 +1976,10 @@
         <v>84</v>
       </c>
       <c r="E4">
-        <v>21308</v>
+        <v>10032</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1984,7 +1987,7 @@
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
         <v>145</v>
@@ -1993,10 +1996,10 @@
         <v>84</v>
       </c>
       <c r="E5">
-        <v>17400</v>
+        <v>18900</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2013,10 +2016,10 @@
         <v>84</v>
       </c>
       <c r="E6">
-        <v>16290</v>
+        <v>21308</v>
       </c>
       <c r="F6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2033,10 +2036,10 @@
         <v>84</v>
       </c>
       <c r="E7">
-        <v>26400</v>
+        <v>17400</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2053,10 +2056,10 @@
         <v>84</v>
       </c>
       <c r="E8">
-        <v>48412</v>
+        <v>16290</v>
       </c>
       <c r="F8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2067,16 +2070,16 @@
         <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
         <v>84</v>
       </c>
       <c r="E9">
-        <v>12500</v>
+        <v>26400</v>
       </c>
       <c r="F9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2084,19 +2087,19 @@
         <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>
       </c>
       <c r="E10">
-        <v>15300</v>
+        <v>48412</v>
       </c>
       <c r="F10" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2104,7 +2107,7 @@
         <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>143</v>
@@ -2113,10 +2116,10 @@
         <v>84</v>
       </c>
       <c r="E11">
-        <v>12900</v>
+        <v>12500</v>
       </c>
       <c r="F11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2124,16 +2127,16 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12">
-        <v>12000</v>
+        <v>15300</v>
       </c>
       <c r="F12" t="s">
         <v>162</v>
@@ -2153,10 +2156,10 @@
         <v>84</v>
       </c>
       <c r="E13">
-        <v>14000</v>
+        <v>12900</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2167,16 +2170,16 @@
         <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
         <v>84</v>
       </c>
       <c r="E14">
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="F14" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2184,7 +2187,7 @@
         <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
         <v>143</v>
@@ -2193,10 +2196,10 @@
         <v>84</v>
       </c>
       <c r="E15">
-        <v>9500</v>
+        <v>14000</v>
       </c>
       <c r="F15" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2207,16 +2210,16 @@
         <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
         <v>84</v>
       </c>
       <c r="E16">
-        <v>8000</v>
+        <v>15000</v>
       </c>
       <c r="F16" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2224,16 +2227,16 @@
         <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C17" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D17" t="s">
         <v>84</v>
       </c>
       <c r="E17">
-        <v>10032</v>
+        <v>9500</v>
       </c>
       <c r="F17" t="s">
         <v>164</v>
@@ -2247,16 +2250,16 @@
         <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="E18">
-        <v>340750</v>
+        <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2273,10 +2276,10 @@
         <v>84</v>
       </c>
       <c r="E19">
-        <v>70000</v>
+        <v>340750</v>
       </c>
       <c r="F19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2293,10 +2296,10 @@
         <v>84</v>
       </c>
       <c r="E20">
-        <v>32000</v>
+        <v>70000</v>
       </c>
       <c r="F20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2307,16 +2310,16 @@
         <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="E21">
-        <v>10000</v>
+        <v>32000</v>
       </c>
       <c r="F21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-08
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="171">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>2000</t>
+  </si>
+  <si>
+    <t>30000</t>
   </si>
   <si>
     <t>삼성증권</t>
@@ -1939,7 +1942,7 @@
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1959,7 +1962,7 @@
         <v>8000</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1979,7 +1982,7 @@
         <v>10032</v>
       </c>
       <c r="F4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1999,7 +2002,7 @@
         <v>18900</v>
       </c>
       <c r="F5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2019,7 +2022,7 @@
         <v>21308</v>
       </c>
       <c r="F6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2039,7 +2042,7 @@
         <v>17400</v>
       </c>
       <c r="F7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2059,7 +2062,7 @@
         <v>16290</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2079,7 +2082,7 @@
         <v>26400</v>
       </c>
       <c r="F9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2099,7 +2102,7 @@
         <v>48412</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2119,7 +2122,7 @@
         <v>12500</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2139,7 +2142,7 @@
         <v>15300</v>
       </c>
       <c r="F12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2159,7 +2162,7 @@
         <v>12900</v>
       </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2179,7 +2182,7 @@
         <v>12000</v>
       </c>
       <c r="F14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2193,13 +2196,13 @@
         <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="E15">
         <v>14000</v>
       </c>
       <c r="F15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2219,7 +2222,7 @@
         <v>15000</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2233,13 +2236,13 @@
         <v>143</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="E17">
         <v>9500</v>
       </c>
       <c r="F17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2259,7 +2262,7 @@
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2279,7 +2282,7 @@
         <v>340750</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2299,7 +2302,7 @@
         <v>70000</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2313,13 +2316,13 @@
         <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="E21">
         <v>32000</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-11
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="172">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>2000</t>
+  </si>
+  <si>
+    <t>3000</t>
   </si>
   <si>
     <t>30000</t>
@@ -1942,7 +1945,7 @@
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1962,7 +1965,7 @@
         <v>8000</v>
       </c>
       <c r="F3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1982,7 +1985,7 @@
         <v>10032</v>
       </c>
       <c r="F4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2002,7 +2005,7 @@
         <v>18900</v>
       </c>
       <c r="F5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2022,7 +2025,7 @@
         <v>21308</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2042,7 +2045,7 @@
         <v>17400</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2062,7 +2065,7 @@
         <v>16290</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2082,7 +2085,7 @@
         <v>26400</v>
       </c>
       <c r="F9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2102,7 +2105,7 @@
         <v>48412</v>
       </c>
       <c r="F10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2122,7 +2125,7 @@
         <v>12500</v>
       </c>
       <c r="F11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2142,7 +2145,7 @@
         <v>15300</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2162,7 +2165,7 @@
         <v>12900</v>
       </c>
       <c r="F13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2176,13 +2179,13 @@
         <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="E14">
         <v>12000</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2202,7 +2205,7 @@
         <v>14000</v>
       </c>
       <c r="F15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2222,7 +2225,7 @@
         <v>15000</v>
       </c>
       <c r="F16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2242,7 +2245,7 @@
         <v>9500</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2262,7 +2265,7 @@
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2282,7 +2285,7 @@
         <v>340750</v>
       </c>
       <c r="F19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2296,13 +2299,13 @@
         <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="E20">
         <v>70000</v>
       </c>
       <c r="F20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2316,13 +2319,13 @@
         <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E21">
         <v>32000</v>
       </c>
       <c r="F21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-12
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -341,6 +341,12 @@
     <t>아이빔테크놀로지</t>
   </si>
   <si>
+    <t>키움스팩9호</t>
+  </si>
+  <si>
+    <t>넥스트바이오메디컬</t>
+  </si>
+  <si>
     <t>이베스트스팩6호</t>
   </si>
   <si>
@@ -392,15 +398,15 @@
     <t>시프트업(유가)</t>
   </si>
   <si>
-    <t>신한글로벌액티브</t>
-  </si>
-  <si>
-    <t>한중엔시에스</t>
-  </si>
-  <si>
     <t>2024.07.15~07.19</t>
   </si>
   <si>
+    <t>2024.07.02~07.03</t>
+  </si>
+  <si>
+    <t>2024.07.01~07.05</t>
+  </si>
+  <si>
     <t>2024.06.27~06.28</t>
   </si>
   <si>
@@ -437,18 +443,15 @@
     <t>2024.06.03~06.27</t>
   </si>
   <si>
-    <t>2024.06.03~06.05</t>
-  </si>
-  <si>
-    <t>2024.05.30~06.05</t>
-  </si>
-  <si>
     <t>7,300~8,500</t>
   </si>
   <si>
     <t>2,000~2,000</t>
   </si>
   <si>
+    <t>24,000~29,000</t>
+  </si>
+  <si>
     <t>6,200~7,700</t>
   </si>
   <si>
@@ -479,39 +482,27 @@
     <t>47,000~60,000</t>
   </si>
   <si>
-    <t>3,000~3,800</t>
-  </si>
-  <si>
-    <t>20,000~23,500</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>30000</t>
-  </si>
-  <si>
     <t>삼성증권</t>
   </si>
   <si>
+    <t>키움증권</t>
+  </si>
+  <si>
+    <t>한국투자증권</t>
+  </si>
+  <si>
     <t>엘에스증권</t>
   </si>
   <si>
     <t>대신증권</t>
   </si>
   <si>
-    <t>키움증권</t>
-  </si>
-  <si>
     <t>NH투자증권</t>
   </si>
   <si>
-    <t>한국투자증권</t>
-  </si>
-  <si>
     <t>미래에셋증권,신한투자증권</t>
   </si>
   <si>
@@ -525,12 +516,6 @@
   </si>
   <si>
     <t>한국투자증권,NH투자증권,신한투자증권</t>
-  </si>
-  <si>
-    <t>신한투자증권,한국투자증권</t>
-  </si>
-  <si>
-    <t>IBK투자증권</t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1930,7 @@
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1962,10 +1947,10 @@
         <v>84</v>
       </c>
       <c r="E3">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1982,10 +1967,10 @@
         <v>84</v>
       </c>
       <c r="E4">
-        <v>10032</v>
+        <v>24000</v>
       </c>
       <c r="F4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1993,19 +1978,19 @@
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
         <v>84</v>
       </c>
       <c r="E5">
-        <v>18900</v>
+        <v>8000</v>
       </c>
       <c r="F5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2013,19 +1998,19 @@
         <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
       </c>
       <c r="E6">
-        <v>21308</v>
+        <v>10032</v>
       </c>
       <c r="F6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2036,16 +2021,16 @@
         <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
         <v>84</v>
       </c>
       <c r="E7">
-        <v>17400</v>
+        <v>18900</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2053,19 +2038,19 @@
         <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
         <v>84</v>
       </c>
       <c r="E8">
-        <v>16290</v>
+        <v>21308</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2073,19 +2058,19 @@
         <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
         <v>84</v>
       </c>
       <c r="E9">
-        <v>26400</v>
+        <v>17400</v>
       </c>
       <c r="F9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2093,19 +2078,19 @@
         <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>
       </c>
       <c r="E10">
-        <v>48412</v>
+        <v>16290</v>
       </c>
       <c r="F10" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2113,19 +2098,19 @@
         <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D11" t="s">
         <v>84</v>
       </c>
       <c r="E11">
-        <v>12500</v>
+        <v>26400</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2142,10 +2127,10 @@
         <v>84</v>
       </c>
       <c r="E12">
-        <v>15300</v>
+        <v>48412</v>
       </c>
       <c r="F12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2162,10 +2147,10 @@
         <v>84</v>
       </c>
       <c r="E13">
-        <v>12900</v>
+        <v>12500</v>
       </c>
       <c r="F13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2176,16 +2161,16 @@
         <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
       <c r="E14">
-        <v>12000</v>
+        <v>15300</v>
       </c>
       <c r="F14" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2193,19 +2178,19 @@
         <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E15">
-        <v>14000</v>
+        <v>12900</v>
       </c>
       <c r="F15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2213,16 +2198,16 @@
         <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="E16">
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="F16" t="s">
         <v>164</v>
@@ -2239,13 +2224,13 @@
         <v>143</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17">
-        <v>9500</v>
+        <v>14000</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2253,19 +2238,19 @@
         <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
       <c r="E18">
-        <v>8000</v>
+        <v>15000</v>
       </c>
       <c r="F18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2273,19 +2258,19 @@
         <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="E19">
-        <v>340750</v>
+        <v>9500</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2296,16 +2281,16 @@
         <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E20">
-        <v>70000</v>
+        <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2316,16 +2301,16 @@
         <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="E21">
-        <v>32000</v>
+        <v>340750</v>
       </c>
       <c r="F21" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-14
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="173">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
     <t>2024-05-13</t>
   </si>
   <si>
@@ -122,6 +125,9 @@
     <t>2024-03-27</t>
   </si>
   <si>
+    <t>2024-05-29</t>
+  </si>
+  <si>
     <t>2024-05-14</t>
   </si>
   <si>
@@ -149,10 +155,7 @@
     <t>2024-03-28</t>
   </si>
   <si>
-    <t>2024-05-29</t>
-  </si>
-  <si>
-    <t>2024-05-23</t>
+    <t>2024-06-14</t>
   </si>
   <si>
     <t>2024-05-17</t>
@@ -170,12 +173,12 @@
     <t>2024-04-22</t>
   </si>
   <si>
+    <t>삼성</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
     <t>KB</t>
   </si>
   <si>
@@ -197,6 +200,9 @@
     <t>신한</t>
   </si>
   <si>
+    <t>그리드위즈</t>
+  </si>
+  <si>
     <t>미래에셋비전스팩4호</t>
   </si>
   <si>
@@ -233,6 +239,9 @@
     <t>신한제12호스팩</t>
   </si>
   <si>
+    <t>124.60:1</t>
+  </si>
+  <si>
     <t>1011.2:1</t>
   </si>
   <si>
@@ -269,6 +278,9 @@
     <t>1,104.54:1</t>
   </si>
   <si>
+    <t>0.95%</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -287,6 +299,9 @@
     <t>10.96%</t>
   </si>
   <si>
+    <t>수요관리 서비스, 전기차 충전기 모뎀 등</t>
+  </si>
+  <si>
     <t>기업인수목적회사(기타금융서비스)</t>
   </si>
   <si>
@@ -485,6 +500,9 @@
     <t>2000</t>
   </si>
   <si>
+    <t>11500</t>
+  </si>
+  <si>
     <t>삼성증권</t>
   </si>
   <si>
@@ -515,7 +533,7 @@
     <t>현대차증권</t>
   </si>
   <si>
-    <t>한국투자증권,NH투자증권,신한투자증권</t>
+    <t>한국투자.NH투자.신한투자증권</t>
   </si>
 </sst>
 </file>
@@ -873,7 +891,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -961,46 +979,46 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="G2">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>34000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="K2">
-        <v>8100000</v>
+        <v>7942750</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="N2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1030,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1038,76 +1056,76 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F3">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="G3">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>8700</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>7651263</v>
+        <v>8100000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="P3">
-        <v>468321534076</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>555936831337</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>359249623614</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>22403886436</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>33386727728</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>10411712773</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>10859975142</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>29346086803</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>4820429371</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1115,76 +1133,76 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="G4">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>8700</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K4">
-        <v>5505000</v>
+        <v>7651263</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1192,46 +1210,46 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="G5">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>13124496</v>
+        <v>5505000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1261,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1269,7 +1287,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>47</v>
@@ -1278,67 +1296,67 @@
         <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F6">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="G6">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="J6">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="K6">
-        <v>8503460</v>
+        <v>13124496</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="N6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P6">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1346,76 +1364,76 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="G7">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K7">
-        <v>3310000</v>
+        <v>8503460</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O7" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>47284698907</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>38750429966</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>25900014771</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>7595091433</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>5807002440</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>3668321605</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>5701880294</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>4780312126</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>4195570793</v>
       </c>
       <c r="Y7" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1423,16 +1441,16 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F8">
         <v>3000000</v>
@@ -1444,197 +1462,197 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>6500</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>8500</v>
+        <v>2000</v>
       </c>
       <c r="K8">
-        <v>21945300</v>
+        <v>3310000</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O8" t="s">
         <v>88</v>
       </c>
       <c r="P8">
-        <v>9576212189</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <v>11914994171</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>7285537916</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>1172310325</v>
+        <v>0</v>
       </c>
       <c r="T8">
-        <v>-2762203259</v>
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>-4737405164</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>-7460336546</v>
+        <v>0</v>
       </c>
       <c r="W8">
-        <v>-7104430732</v>
+        <v>0</v>
       </c>
       <c r="X8">
-        <v>-7501425172</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F9">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="G9">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>22000</v>
+        <v>6500</v>
       </c>
       <c r="J9">
-        <v>26000</v>
+        <v>8500</v>
       </c>
       <c r="K9">
-        <v>10429232</v>
+        <v>21945300</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>33000</v>
+        <v>10500</v>
       </c>
       <c r="N9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P9">
-        <v>-75676750274</v>
+        <v>9576212189</v>
       </c>
       <c r="Q9">
-        <v>-68652978862</v>
+        <v>11914994171</v>
       </c>
       <c r="R9">
-        <v>-9506668082</v>
+        <v>7285537916</v>
       </c>
       <c r="S9">
-        <v>-69862474811</v>
+        <v>1172310325</v>
       </c>
       <c r="T9">
-        <v>-137025491259</v>
+        <v>-2762203259</v>
       </c>
       <c r="U9">
-        <v>3014576074</v>
+        <v>-4737405164</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>-7460336546</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>-7104430732</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>-7501425172</v>
       </c>
       <c r="Y9" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="G10">
-        <v>5150000</v>
+        <v>1100000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K10">
-        <v>5510000</v>
+        <v>10429232</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>33000</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O10" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>-75676750274</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>-68652978862</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>-9506668082</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>-69862474811</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>-137025491259</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>3014576074</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1646,30 +1664,30 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F11">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="G11">
-        <v>3500000</v>
+        <v>5150000</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1681,7 +1699,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>3700000</v>
+        <v>5510000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1690,10 +1708,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="O11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1723,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1731,22 +1749,22 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F12">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="G12">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1758,7 +1776,7 @@
         <v>2000</v>
       </c>
       <c r="K12">
-        <v>3620000</v>
+        <v>3700000</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1767,10 +1785,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1800,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1808,22 +1826,22 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="G13">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1835,7 +1853,7 @@
         <v>2000</v>
       </c>
       <c r="K13">
-        <v>5520000</v>
+        <v>3620000</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1844,10 +1862,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="O13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1877,7 +1895,84 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14">
+        <v>5000000</v>
+      </c>
+      <c r="G14">
+        <v>5000000</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2000</v>
+      </c>
+      <c r="J14">
+        <v>2000</v>
+      </c>
+      <c r="K14">
+        <v>5520000</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+      <c r="N14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O14" t="s">
+        <v>88</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1895,422 +1990,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E2">
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>24000</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>8000</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E6">
         <v>10032</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E7">
         <v>18900</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E8">
         <v>21308</v>
       </c>
       <c r="F8" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E9">
         <v>17400</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E10">
         <v>16290</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E11">
         <v>26400</v>
       </c>
       <c r="F11" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E12">
         <v>48412</v>
       </c>
       <c r="F12" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <v>12500</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E14">
         <v>15300</v>
       </c>
       <c r="F14" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E15">
         <v>12900</v>
       </c>
       <c r="F15" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E16">
         <v>12000</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E17">
         <v>14000</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="E18">
-        <v>15000</v>
+        <v>23000</v>
       </c>
       <c r="F18" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E19">
         <v>9500</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E21">
         <v>340750</v>
       </c>
       <c r="F21" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-24
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="198">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-06-05</t>
+  </si>
+  <si>
     <t>2024-06-04</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
     <t>2024-05-27</t>
   </si>
   <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
     <t>2024-05-28</t>
   </si>
   <si>
@@ -128,10 +134,7 @@
     <t>2024-04-12</t>
   </si>
   <si>
-    <t>2024-04-08</t>
-  </si>
-  <si>
-    <t>2024-06-05</t>
+    <t>2024-06-07</t>
   </si>
   <si>
     <t>2024-05-31</t>
@@ -146,9 +149,6 @@
     <t>2024-05-08</t>
   </si>
   <si>
-    <t>2024-05-30</t>
-  </si>
-  <si>
     <t>2024-04-19</t>
   </si>
   <si>
@@ -158,7 +158,7 @@
     <t>2024-04-16</t>
   </si>
   <si>
-    <t>2024-04-09</t>
+    <t>2024-06-24</t>
   </si>
   <si>
     <t>2024-06-21</t>
@@ -188,13 +188,16 @@
     <t>2024-05-02</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>KB</t>
   </si>
   <si>
     <t>한국</t>
   </si>
   <si>
-    <t>미래</t>
+    <t>IBK</t>
   </si>
   <si>
     <t>대신</t>
@@ -215,7 +218,7 @@
     <t>유안타</t>
   </si>
   <si>
-    <t>하나</t>
+    <t>미래에셋비전스팩6호</t>
   </si>
   <si>
     <t>KB제29호스팩</t>
@@ -230,6 +233,9 @@
     <t>씨어스테크놀로지</t>
   </si>
   <si>
+    <t>한중엔시에스</t>
+  </si>
+  <si>
     <t>라메디텍</t>
   </si>
   <si>
@@ -266,7 +272,7 @@
     <t>유안타제16호스팩</t>
   </si>
   <si>
-    <t>하나33호스팩</t>
+    <t>1,107.2:1</t>
   </si>
   <si>
     <t>1100.48:1</t>
@@ -281,6 +287,9 @@
     <t>1084.39:1</t>
   </si>
   <si>
+    <t>725.94:1</t>
+  </si>
+  <si>
     <t>1115.44:1</t>
   </si>
   <si>
@@ -317,15 +326,15 @@
     <t>1,050.42:1</t>
   </si>
   <si>
-    <t>1277.22:1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>2.06%</t>
   </si>
   <si>
+    <t>12.44%</t>
+  </si>
+  <si>
     <t>9.93%</t>
   </si>
   <si>
@@ -353,6 +362,9 @@
     <t>심전도검사솔루션 입원환자모니터링솔루션</t>
   </si>
   <si>
+    <t>수냉식 냉각시스템 ESS Parts, 공랭식 ESS Module Parts, EV Module 및 내연기관 Parts</t>
+  </si>
+  <si>
     <t>초소형 레이저 의료기기 및 미용기기</t>
   </si>
   <si>
@@ -450,9 +462,6 @@
   </si>
   <si>
     <t>하이젠알앤엠</t>
-  </si>
-  <si>
-    <t>미래에셋비전스팩6호</t>
   </si>
   <si>
     <t>KB스팩29호</t>
@@ -957,7 +966,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1045,10 +1054,10 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -1057,10 +1066,10 @@
         <v>67</v>
       </c>
       <c r="F2">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="G2">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1072,7 +1081,7 @@
         <v>2000</v>
       </c>
       <c r="K2">
-        <v>6220000</v>
+        <v>6930000</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1081,10 +1090,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1114,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1125,7 +1134,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>58</v>
@@ -1134,10 +1143,10 @@
         <v>68</v>
       </c>
       <c r="F3">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G3">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1149,7 +1158,7 @@
         <v>2000</v>
       </c>
       <c r="K3">
-        <v>4810000</v>
+        <v>6220000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1158,10 +1167,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1191,15 +1200,15 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1211,10 +1220,10 @@
         <v>69</v>
       </c>
       <c r="F4">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="G4">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1226,7 +1235,7 @@
         <v>2000</v>
       </c>
       <c r="K4">
-        <v>5480000</v>
+        <v>4810000</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1235,10 +1244,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1268,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1276,200 +1285,200 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>70</v>
       </c>
       <c r="F5">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="G5">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>12293880</v>
+        <v>5480000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P5">
-        <v>1386123525</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>1152944128</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1885010467</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>-4388824706</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>-7990287699</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>-9803411085</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>-4430563401</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>-7988275689</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>-9916946238</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
         <v>71</v>
       </c>
       <c r="F6">
-        <v>1298000</v>
+        <v>1300000</v>
       </c>
       <c r="G6">
-        <v>1298000</v>
+        <v>1300000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>10400</v>
+        <v>10500</v>
       </c>
       <c r="J6">
-        <v>12700</v>
+        <v>14000</v>
       </c>
       <c r="K6">
-        <v>8650735</v>
+        <v>12293880</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>16000</v>
+        <v>17000</v>
       </c>
       <c r="N6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P6">
-        <v>2055746777</v>
+        <v>1386123525</v>
       </c>
       <c r="Q6">
-        <v>2918221978</v>
+        <v>1152944128</v>
       </c>
       <c r="R6">
-        <v>979078233</v>
+        <v>1885010467</v>
       </c>
       <c r="S6">
-        <v>-3343774083</v>
+        <v>-4388824706</v>
       </c>
       <c r="T6">
-        <v>-3525649863</v>
+        <v>-7990287699</v>
       </c>
       <c r="U6">
-        <v>-1713494359</v>
+        <v>-9803411085</v>
       </c>
       <c r="V6">
-        <v>-4430074915</v>
+        <v>-4430563401</v>
       </c>
       <c r="W6">
-        <v>-8304699942</v>
+        <v>-7988275689</v>
       </c>
       <c r="X6">
-        <v>-1627684107</v>
+        <v>-9916946238</v>
       </c>
       <c r="Y6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>72</v>
       </c>
       <c r="F7">
-        <v>5000000</v>
+        <v>1600000</v>
       </c>
       <c r="G7">
-        <v>5000000</v>
+        <v>1600000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>23500</v>
       </c>
       <c r="K7">
-        <v>5840000</v>
+        <v>8751446</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1499,84 +1508,84 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>73</v>
       </c>
       <c r="F8">
-        <v>1400000</v>
+        <v>1298000</v>
       </c>
       <c r="G8">
-        <v>1400000</v>
+        <v>1298000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>34000</v>
+        <v>10400</v>
       </c>
       <c r="J8">
-        <v>40000</v>
+        <v>12700</v>
       </c>
       <c r="K8">
-        <v>7942750</v>
+        <v>8650735</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>40000</v>
+        <v>16000</v>
       </c>
       <c r="N8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>2055746777</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>2918221978</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>979078233</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>-3343774083</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>-3525649863</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>-1713494359</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>-4430074915</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>-8304699942</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>-1627684107</v>
       </c>
       <c r="Y8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1587,19 +1596,19 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
         <v>74</v>
       </c>
       <c r="F9">
-        <v>6650000</v>
+        <v>5000000</v>
       </c>
       <c r="G9">
-        <v>6650000</v>
+        <v>5000000</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1611,7 +1620,7 @@
         <v>2000</v>
       </c>
       <c r="K9">
-        <v>8100000</v>
+        <v>5840000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1620,10 +1629,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1653,7 +1662,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1661,76 +1670,76 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
         <v>75</v>
       </c>
       <c r="F10">
-        <v>1200000</v>
+        <v>1400000</v>
       </c>
       <c r="G10">
-        <v>1200000</v>
+        <v>1400000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>8700</v>
+        <v>34000</v>
       </c>
       <c r="J10">
-        <v>11000</v>
+        <v>40000</v>
       </c>
       <c r="K10">
-        <v>7651263</v>
+        <v>7942750</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>14000</v>
+        <v>40000</v>
       </c>
       <c r="N10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P10">
-        <v>468321534076</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <v>555936831337</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>359249623614</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>22403886436</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>33386727728</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <v>10411712773</v>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>10859975142</v>
+        <v>0</v>
       </c>
       <c r="W10">
-        <v>29346086803</v>
+        <v>0</v>
       </c>
       <c r="X10">
-        <v>4820429371</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1738,10 +1747,10 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>57</v>
@@ -1750,10 +1759,10 @@
         <v>76</v>
       </c>
       <c r="F11">
-        <v>5000000</v>
+        <v>6650000</v>
       </c>
       <c r="G11">
-        <v>5000000</v>
+        <v>6650000</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1765,7 +1774,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>5505000</v>
+        <v>8100000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1774,10 +1783,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1807,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1818,7 +1827,7 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -1827,64 +1836,64 @@
         <v>77</v>
       </c>
       <c r="F12">
-        <v>1970000</v>
+        <v>1200000</v>
       </c>
       <c r="G12">
-        <v>1970000</v>
+        <v>1200000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>13000</v>
+        <v>8700</v>
       </c>
       <c r="J12">
-        <v>16000</v>
+        <v>11000</v>
       </c>
       <c r="K12">
-        <v>13124496</v>
+        <v>7651263</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>20000</v>
+        <v>14000</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1892,10 +1901,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
         <v>58</v>
@@ -1904,64 +1913,64 @@
         <v>78</v>
       </c>
       <c r="F13">
-        <v>1500000</v>
+        <v>5000000</v>
       </c>
       <c r="G13">
-        <v>1500000</v>
+        <v>5000000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J13">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
-        <v>8503460</v>
+        <v>5505000</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="P13">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X13">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1969,10 +1978,10 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
@@ -1981,34 +1990,34 @@
         <v>79</v>
       </c>
       <c r="F14">
-        <v>3000000</v>
+        <v>1970000</v>
       </c>
       <c r="G14">
-        <v>3000000</v>
+        <v>1970000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K14">
-        <v>3310000</v>
+        <v>13124496</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O14" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2038,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2046,141 +2055,141 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
         <v>80</v>
       </c>
       <c r="F15">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="G15">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>6500</v>
+        <v>11000</v>
       </c>
       <c r="J15">
-        <v>8500</v>
+        <v>14000</v>
       </c>
       <c r="K15">
-        <v>21945300</v>
+        <v>8503460</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>10500</v>
+        <v>18000</v>
       </c>
       <c r="N15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P15">
-        <v>9576212189</v>
+        <v>47284698907</v>
       </c>
       <c r="Q15">
-        <v>11914994171</v>
+        <v>38750429966</v>
       </c>
       <c r="R15">
-        <v>7285537916</v>
+        <v>25900014771</v>
       </c>
       <c r="S15">
-        <v>1172310325</v>
+        <v>7595091433</v>
       </c>
       <c r="T15">
-        <v>-2762203259</v>
+        <v>5807002440</v>
       </c>
       <c r="U15">
-        <v>-4737405164</v>
+        <v>3668321605</v>
       </c>
       <c r="V15">
-        <v>-7460336546</v>
+        <v>5701880294</v>
       </c>
       <c r="W15">
-        <v>-7104430732</v>
+        <v>4780312126</v>
       </c>
       <c r="X15">
-        <v>-7501425172</v>
+        <v>4195570793</v>
       </c>
       <c r="Y15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>81</v>
       </c>
       <c r="F16">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="G16">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>22000</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
-        <v>10429232</v>
+        <v>3310000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>33000</v>
+        <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O16" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P16">
-        <v>-75676750274</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>-68652978862</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>-9506668082</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>-69862474811</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>-137025491259</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>3014576074</v>
+        <v>0</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2192,161 +2201,238 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>82</v>
       </c>
       <c r="F17">
-        <v>5150000</v>
+        <v>3000000</v>
       </c>
       <c r="G17">
-        <v>5150000</v>
+        <v>3000000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2000</v>
+        <v>6500</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>8500</v>
       </c>
       <c r="K17">
-        <v>5510000</v>
+        <v>21945300</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>10500</v>
       </c>
       <c r="N17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>9576212189</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>11914994171</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>7285537916</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>1172310325</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>-2762203259</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>-4737405164</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>-7460336546</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>-7104430732</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>-7501425172</v>
       </c>
       <c r="Y17" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
         <v>83</v>
       </c>
       <c r="F18">
-        <v>3500000</v>
+        <v>1100000</v>
       </c>
       <c r="G18">
-        <v>3500000</v>
+        <v>1100000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
+        <v>22000</v>
+      </c>
+      <c r="J18">
+        <v>26000</v>
+      </c>
+      <c r="K18">
+        <v>10429232</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>33000</v>
+      </c>
+      <c r="N18" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" t="s">
+        <v>112</v>
+      </c>
+      <c r="P18">
+        <v>-75676750274</v>
+      </c>
+      <c r="Q18">
+        <v>-68652978862</v>
+      </c>
+      <c r="R18">
+        <v>-9506668082</v>
+      </c>
+      <c r="S18">
+        <v>-69862474811</v>
+      </c>
+      <c r="T18">
+        <v>-137025491259</v>
+      </c>
+      <c r="U18">
+        <v>3014576074</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19">
+        <v>5150000</v>
+      </c>
+      <c r="G19">
+        <v>5150000</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>2000</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>2000</v>
       </c>
-      <c r="K18">
-        <v>3700000</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="K19">
+        <v>5510000</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>2000</v>
       </c>
-      <c r="N18" t="s">
-        <v>100</v>
-      </c>
-      <c r="O18" t="s">
-        <v>101</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>110</v>
+      <c r="N19" t="s">
+        <v>102</v>
+      </c>
+      <c r="O19" t="s">
+        <v>103</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2364,422 +2450,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2">
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3">
         <v>9500</v>
       </c>
       <c r="F3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4">
         <v>12000</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E5">
         <v>8000</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E6">
         <v>22400</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <v>6000</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E8">
         <v>24000</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E9">
         <v>8000</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>10032</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E11">
         <v>18900</v>
       </c>
       <c r="F11" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E12">
         <v>21308</v>
       </c>
       <c r="F12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E13">
         <v>16290</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E14">
         <v>26400</v>
       </c>
       <c r="F14" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E15">
         <v>48412</v>
       </c>
       <c r="F15" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E16">
         <v>12500</v>
       </c>
       <c r="F16" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E17">
         <v>15300</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E18">
         <v>12900</v>
       </c>
       <c r="F18" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E19">
         <v>12000</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E20">
         <v>14000</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E21">
         <v>23000</v>
       </c>
       <c r="F21" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-06-27
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="211">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-06-07</t>
+  </si>
+  <si>
     <t>2024-06-03</t>
   </si>
   <si>
@@ -134,12 +137,12 @@
     <t>2024-04-12</t>
   </si>
   <si>
+    <t>2024-06-13</t>
+  </si>
+  <si>
     <t>2024-06-10</t>
   </si>
   <si>
-    <t>2024-06-07</t>
-  </si>
-  <si>
     <t>2024-05-31</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
     <t>2024-04-16</t>
   </si>
   <si>
+    <t>2024-06-27</t>
+  </si>
+  <si>
     <t>2024-06-25</t>
   </si>
   <si>
@@ -224,6 +230,9 @@
     <t>유안타</t>
   </si>
   <si>
+    <t>하이젠알앤엠</t>
+  </si>
+  <si>
     <t>에스오에스랩</t>
   </si>
   <si>
@@ -281,6 +290,9 @@
     <t>유안타제16호스팩</t>
   </si>
   <si>
+    <t>1099.21:1</t>
+  </si>
+  <si>
     <t>1072.30:1</t>
   </si>
   <si>
@@ -338,6 +350,9 @@
     <t>1,050.42:1</t>
   </si>
   <si>
+    <t>11.80%</t>
+  </si>
+  <si>
     <t>4.19%</t>
   </si>
   <si>
@@ -371,6 +386,9 @@
     <t>10.96%</t>
   </si>
   <si>
+    <t>전동기 및 발전기 (범용모터, 서보모터)</t>
+  </si>
+  <si>
     <t>산업용 및 차량용 라이다(LiDAR)</t>
   </si>
   <si>
@@ -483,9 +501,6 @@
   </si>
   <si>
     <t>한국스팩15호</t>
-  </si>
-  <si>
-    <t>하이젠알앤엠</t>
   </si>
   <si>
     <t>KB스팩29호</t>
@@ -990,7 +1005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1078,76 +1093,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2">
-        <v>2000000</v>
+        <v>3400000</v>
       </c>
       <c r="G2">
-        <v>2000000</v>
+        <v>3400000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>7500</v>
+        <v>4500</v>
       </c>
       <c r="J2">
-        <v>9000</v>
+        <v>5500</v>
       </c>
       <c r="K2">
-        <v>17529140</v>
+        <v>30888000</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>11500</v>
+        <v>7000</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>85187882584</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>87525689695</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>77247394706</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2205797752</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>4920387020</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>4336496285</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1613954566</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>3980493669</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>2646634321</v>
       </c>
       <c r="Y2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1155,46 +1170,46 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F3">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="G3">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="K3">
-        <v>6930000</v>
+        <v>17529140</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1224,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1232,22 +1247,22 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F4">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="G4">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1259,7 +1274,7 @@
         <v>2000</v>
       </c>
       <c r="K4">
-        <v>6220000</v>
+        <v>6930000</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1268,10 +1283,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="O4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1301,30 +1316,30 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1336,7 +1351,7 @@
         <v>2000</v>
       </c>
       <c r="K5">
-        <v>4810000</v>
+        <v>6220000</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1345,10 +1360,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1378,30 +1393,30 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F6">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="G6">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1413,7 +1428,7 @@
         <v>2000</v>
       </c>
       <c r="K6">
-        <v>5480000</v>
+        <v>4810000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1422,10 +1437,10 @@
         <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="O6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1455,84 +1470,84 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="G7">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K7">
-        <v>12293880</v>
+        <v>5480000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P7">
-        <v>1386123525</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>1152944128</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>1885010467</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>-4388824706</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>-7990287699</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>-9803411085</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>-4430563401</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>-7988275689</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>-9916946238</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1540,230 +1555,230 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F8">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="G8">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J8">
-        <v>23500</v>
+        <v>14000</v>
       </c>
       <c r="K8">
-        <v>8751446</v>
+        <v>12293880</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1386123525</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>1152944128</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1885010467</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>-4388824706</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>-7990287699</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>-9803411085</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>-4430563401</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>-7988275689</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>-9916946238</v>
       </c>
       <c r="Y8" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F9">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="G9">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>10400</v>
+        <v>20000</v>
       </c>
       <c r="J9">
-        <v>12700</v>
+        <v>23500</v>
       </c>
       <c r="K9">
-        <v>8650735</v>
+        <v>8751446</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P9">
-        <v>2055746777</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>2918221978</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>979078233</v>
+        <v>0</v>
       </c>
       <c r="S9">
-        <v>-3343774083</v>
+        <v>0</v>
       </c>
       <c r="T9">
-        <v>-3525649863</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>-1713494359</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>-4430074915</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>-8304699942</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>-1627684107</v>
+        <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="G10">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>10400</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>12700</v>
       </c>
       <c r="K10">
-        <v>5840000</v>
+        <v>8650735</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>2055746777</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>2918221978</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>979078233</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>-3343774083</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>-3525649863</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>-1713494359</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>-4430074915</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>-8304699942</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>-1627684107</v>
       </c>
       <c r="Y10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1771,46 +1786,46 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="G11">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>34000</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
-        <v>7942750</v>
+        <v>5840000</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1840,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1851,43 +1866,43 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="G12">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>34000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="K12">
-        <v>8100000</v>
+        <v>7942750</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="N12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O12" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1917,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1928,73 +1943,73 @@
         <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F13">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="G13">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>8700</v>
+        <v>2000</v>
       </c>
       <c r="J13">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
-        <v>7651263</v>
+        <v>8100000</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O13" t="s">
         <v>113</v>
       </c>
       <c r="P13">
-        <v>468321534076</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>555936831337</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>359249623614</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>22403886436</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>33386727728</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>10411712773</v>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>10859975142</v>
+        <v>0</v>
       </c>
       <c r="W13">
-        <v>29346086803</v>
+        <v>0</v>
       </c>
       <c r="X13">
-        <v>4820429371</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2002,76 +2017,76 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F14">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="G14">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>8700</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K14">
-        <v>5505000</v>
+        <v>7651263</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O14" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y14" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2079,46 +2094,46 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F15">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="G15">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J15">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
-        <v>13124496</v>
+        <v>5505000</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2148,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2156,76 +2171,76 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F16">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="G16">
-        <v>1500000</v>
+        <v>1970000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="J16">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="K16">
-        <v>8503460</v>
+        <v>13124496</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="N16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="P16">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2236,73 +2251,73 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F17">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="G17">
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K17">
-        <v>3310000</v>
+        <v>8503460</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N17" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O17" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>47284698907</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>38750429966</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>25900014771</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>7595091433</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>5807002440</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>3668321605</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>5701880294</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>4780312126</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>4195570793</v>
       </c>
       <c r="Y17" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2310,16 +2325,16 @@
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F18">
         <v>3000000</v>
@@ -2331,209 +2346,286 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>6500</v>
+        <v>2000</v>
       </c>
       <c r="J18">
-        <v>8500</v>
+        <v>2000</v>
       </c>
       <c r="K18">
-        <v>21945300</v>
+        <v>3310000</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="N18" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P18">
-        <v>9576212189</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>11914994171</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>7285537916</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>1172310325</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>-2762203259</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>-4737405164</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>-7460336546</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>-7104430732</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>-7501425172</v>
+        <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F19">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="G19">
-        <v>1100000</v>
+        <v>3000000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>22000</v>
+        <v>6500</v>
       </c>
       <c r="J19">
-        <v>26000</v>
+        <v>8500</v>
       </c>
       <c r="K19">
-        <v>10429232</v>
+        <v>21945300</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>33000</v>
+        <v>10500</v>
       </c>
       <c r="N19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O19" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P19">
-        <v>-75676750274</v>
+        <v>9576212189</v>
       </c>
       <c r="Q19">
-        <v>-68652978862</v>
+        <v>11914994171</v>
       </c>
       <c r="R19">
-        <v>-9506668082</v>
+        <v>7285537916</v>
       </c>
       <c r="S19">
-        <v>-69862474811</v>
+        <v>1172310325</v>
       </c>
       <c r="T19">
-        <v>-137025491259</v>
+        <v>-2762203259</v>
       </c>
       <c r="U19">
-        <v>3014576074</v>
+        <v>-4737405164</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>-7460336546</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>-7104430732</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>-7501425172</v>
       </c>
       <c r="Y19" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F20">
+        <v>1100000</v>
+      </c>
+      <c r="G20">
+        <v>1100000</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>22000</v>
+      </c>
+      <c r="J20">
+        <v>26000</v>
+      </c>
+      <c r="K20">
+        <v>10429232</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>33000</v>
+      </c>
+      <c r="N20" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" t="s">
+        <v>122</v>
+      </c>
+      <c r="P20">
+        <v>-75676750274</v>
+      </c>
+      <c r="Q20">
+        <v>-68652978862</v>
+      </c>
+      <c r="R20">
+        <v>-9506668082</v>
+      </c>
+      <c r="S20">
+        <v>-69862474811</v>
+      </c>
+      <c r="T20">
+        <v>-137025491259</v>
+      </c>
+      <c r="U20">
+        <v>3014576074</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21">
         <v>5150000</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>5150000</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>2000</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>2000</v>
       </c>
-      <c r="K20">
+      <c r="K21">
         <v>5510000</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>2000</v>
       </c>
-      <c r="N20" t="s">
-        <v>106</v>
-      </c>
-      <c r="O20" t="s">
-        <v>108</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>132</v>
+      <c r="N21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" t="s">
+        <v>113</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2551,422 +2643,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E2">
         <v>16308</v>
       </c>
       <c r="F2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E3">
         <v>18900</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E4">
         <v>9500</v>
       </c>
       <c r="F4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E5">
         <v>17500</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E6">
         <v>12000</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E7">
         <v>8000</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E8">
         <v>182400</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E9">
         <v>22400</v>
       </c>
       <c r="F9" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E10">
         <v>6000</v>
       </c>
       <c r="F10" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E11">
         <v>24000</v>
       </c>
       <c r="F11" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E12">
         <v>8000</v>
       </c>
       <c r="F12" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E13">
         <v>10032</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E14">
         <v>21308</v>
       </c>
       <c r="F14" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E15">
         <v>16290</v>
       </c>
       <c r="F15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E16">
         <v>26400</v>
       </c>
       <c r="F16" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C17" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E17">
         <v>48412</v>
       </c>
       <c r="F17" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>12500</v>
       </c>
       <c r="F18" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E19">
         <v>15300</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D20" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E20">
         <v>12900</v>
       </c>
       <c r="F20" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E21">
         <v>12000</v>
       </c>
       <c r="F21" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-05
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="212">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -470,6 +470,9 @@
     <t>키움스팩9호</t>
   </si>
   <si>
+    <t>뱅크웨어글로벌</t>
+  </si>
+  <si>
     <t>티디에스팜</t>
   </si>
   <si>
@@ -494,9 +497,6 @@
     <t>산일전기(유가)</t>
   </si>
   <si>
-    <t>뱅크웨어글로벌</t>
-  </si>
-  <si>
     <t>이베스트스팩6호</t>
   </si>
   <si>
@@ -536,9 +536,6 @@
     <t>2024.07.09~07.15</t>
   </si>
   <si>
-    <t>2024.07.08~07.12</t>
-  </si>
-  <si>
     <t>2024.06.27~06.28</t>
   </si>
   <si>
@@ -566,6 +563,9 @@
     <t>13,600~15,300</t>
   </si>
   <si>
+    <t>16,000~19,000</t>
+  </si>
+  <si>
     <t>9,500~10,700</t>
   </si>
   <si>
@@ -584,9 +584,6 @@
     <t>24,000~30,000</t>
   </si>
   <si>
-    <t>16,000~19,000</t>
-  </si>
-  <si>
     <t>6,200~7,700</t>
   </si>
   <si>
@@ -629,6 +626,9 @@
     <t>키움증권</t>
   </si>
   <si>
+    <t>미래에셋증권</t>
+  </si>
+  <si>
     <t>한국투자증권</t>
   </si>
   <si>
@@ -642,9 +642,6 @@
   </si>
   <si>
     <t>미래에셋증권,삼성증권</t>
-  </si>
-  <si>
-    <t>미래에셋증권</t>
   </si>
   <si>
     <t>엘에스증권</t>
@@ -2752,7 +2749,7 @@
         <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
         <v>117</v>
@@ -2761,7 +2758,7 @@
         <v>11600</v>
       </c>
       <c r="F2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2772,7 +2769,7 @@
         <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
         <v>117</v>
@@ -2781,7 +2778,7 @@
         <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2792,7 +2789,7 @@
         <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
         <v>117</v>
@@ -2801,7 +2798,7 @@
         <v>6000</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2809,19 +2806,19 @@
         <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
         <v>117</v>
       </c>
       <c r="E5">
-        <v>9500</v>
+        <v>22400</v>
       </c>
       <c r="F5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2829,19 +2826,19 @@
         <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
         <v>117</v>
       </c>
       <c r="E6">
-        <v>16308</v>
+        <v>9500</v>
       </c>
       <c r="F6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2852,16 +2849,16 @@
         <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
         <v>117</v>
       </c>
       <c r="E7">
-        <v>24000</v>
+        <v>16308</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2869,19 +2866,19 @@
         <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" t="s">
         <v>117</v>
       </c>
       <c r="E8">
-        <v>18900</v>
+        <v>24000</v>
       </c>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2889,19 +2886,19 @@
         <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
         <v>117</v>
       </c>
       <c r="E9">
-        <v>17500</v>
+        <v>18900</v>
       </c>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2909,19 +2906,19 @@
         <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
         <v>117</v>
       </c>
       <c r="E10">
-        <v>12000</v>
+        <v>17500</v>
       </c>
       <c r="F10" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2932,16 +2929,16 @@
         <v>171</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
         <v>117</v>
       </c>
       <c r="E11">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="F11" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2949,19 +2946,19 @@
         <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D12" t="s">
         <v>117</v>
       </c>
       <c r="E12">
-        <v>182400</v>
+        <v>8000</v>
       </c>
       <c r="F12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2969,19 +2966,19 @@
         <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
         <v>117</v>
       </c>
       <c r="E13">
-        <v>22400</v>
+        <v>182400</v>
       </c>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2989,19 +2986,19 @@
         <v>160</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E14">
         <v>8000</v>
       </c>
       <c r="F14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3009,19 +3006,19 @@
         <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E15">
         <v>10032</v>
       </c>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3029,13 +3026,13 @@
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E16">
         <v>16290</v>
@@ -3049,19 +3046,19 @@
         <v>162</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17">
         <v>26400</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3069,19 +3066,19 @@
         <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E18">
         <v>48412</v>
       </c>
       <c r="F18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3089,13 +3086,13 @@
         <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19">
         <v>12500</v>
@@ -3109,13 +3106,13 @@
         <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E20">
         <v>15300</v>
@@ -3129,19 +3126,19 @@
         <v>77</v>
       </c>
       <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" t="s">
         <v>180</v>
       </c>
-      <c r="C21" t="s">
-        <v>181</v>
-      </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21">
         <v>12900</v>
       </c>
       <c r="F21" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-06
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="215">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -461,6 +461,9 @@
     <t>주간사</t>
   </si>
   <si>
+    <t>에이치이엠파마(구.에이치이엠)</t>
+  </si>
+  <si>
     <t>교보스팩16호</t>
   </si>
   <si>
@@ -509,6 +512,9 @@
     <t>한국스팩15호</t>
   </si>
   <si>
+    <t>2024.08.26~08.30</t>
+  </si>
+  <si>
     <t>2024.07.29~07.30</t>
   </si>
   <si>
@@ -554,7 +560,7 @@
     <t>2024.06.07~06.13</t>
   </si>
   <si>
-    <t>2024.06.05~06.07</t>
+    <t>18,000~21,000</t>
   </si>
   <si>
     <t>2,000~2,000</t>
@@ -615,6 +621,9 @@
   </si>
   <si>
     <t>7000</t>
+  </si>
+  <si>
+    <t>신한투자증권</t>
   </si>
   <si>
     <t>교보증권</t>
@@ -2746,19 +2755,19 @@
         <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
         <v>117</v>
       </c>
       <c r="E2">
-        <v>11600</v>
+        <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2766,19 +2775,19 @@
         <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
         <v>117</v>
       </c>
       <c r="E3">
-        <v>21308</v>
+        <v>11600</v>
       </c>
       <c r="F3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2786,19 +2795,19 @@
         <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
         <v>117</v>
       </c>
       <c r="E4">
-        <v>6000</v>
+        <v>21308</v>
       </c>
       <c r="F4" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2806,7 +2815,7 @@
         <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>182</v>
@@ -2815,10 +2824,10 @@
         <v>117</v>
       </c>
       <c r="E5">
-        <v>22400</v>
+        <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2829,16 +2838,16 @@
         <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
         <v>117</v>
       </c>
       <c r="E6">
-        <v>9500</v>
+        <v>22400</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2846,19 +2855,19 @@
         <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
         <v>117</v>
       </c>
       <c r="E7">
-        <v>16308</v>
+        <v>9500</v>
       </c>
       <c r="F7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2866,19 +2875,19 @@
         <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
         <v>117</v>
       </c>
       <c r="E8">
-        <v>24000</v>
+        <v>16308</v>
       </c>
       <c r="F8" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2886,19 +2895,19 @@
         <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
         <v>117</v>
       </c>
       <c r="E9">
-        <v>18900</v>
+        <v>24000</v>
       </c>
       <c r="F9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2906,19 +2915,19 @@
         <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
         <v>117</v>
       </c>
       <c r="E10">
-        <v>17500</v>
+        <v>18900</v>
       </c>
       <c r="F10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2926,19 +2935,19 @@
         <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
         <v>117</v>
       </c>
       <c r="E11">
-        <v>12000</v>
+        <v>17500</v>
       </c>
       <c r="F11" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2946,19 +2955,19 @@
         <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
         <v>117</v>
       </c>
       <c r="E12">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="F12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2966,19 +2975,19 @@
         <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
         <v>117</v>
       </c>
       <c r="E13">
-        <v>182400</v>
+        <v>8000</v>
       </c>
       <c r="F13" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2986,19 +2995,19 @@
         <v>160</v>
       </c>
       <c r="B14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>117</v>
       </c>
       <c r="E14">
-        <v>8000</v>
+        <v>182400</v>
       </c>
       <c r="F14" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3006,139 +3015,139 @@
         <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E15">
-        <v>10032</v>
+        <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E16">
-        <v>16290</v>
+        <v>10032</v>
       </c>
       <c r="F16" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E17">
-        <v>26400</v>
+        <v>16290</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E18">
-        <v>48412</v>
+        <v>26400</v>
       </c>
       <c r="F18" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E19">
-        <v>12500</v>
+        <v>48412</v>
       </c>
       <c r="F19" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E20">
-        <v>15300</v>
+        <v>12500</v>
       </c>
       <c r="F20" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="E21">
-        <v>12900</v>
+        <v>15300</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-07
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="202">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -137,12 +137,6 @@
     <t>2024-04-24</t>
   </si>
   <si>
-    <t>2024-04-15</t>
-  </si>
-  <si>
-    <t>2024-04-17</t>
-  </si>
-  <si>
     <t>2024-06-19</t>
   </si>
   <si>
@@ -161,12 +155,6 @@
     <t>2024-05-08</t>
   </si>
   <si>
-    <t>2024-04-19</t>
-  </si>
-  <si>
-    <t>2024-04-18</t>
-  </si>
-  <si>
     <t>2024-07-03</t>
   </si>
   <si>
@@ -197,9 +185,6 @@
     <t>2024-05-17</t>
   </si>
   <si>
-    <t>2024-05-07</t>
-  </si>
-  <si>
     <t>2024-07-01</t>
   </si>
   <si>
@@ -227,9 +212,6 @@
     <t>NH</t>
   </si>
   <si>
-    <t>SK</t>
-  </si>
-  <si>
     <t>신한, 한국</t>
   </si>
   <si>
@@ -287,12 +269,6 @@
     <t>아이씨티케이</t>
   </si>
   <si>
-    <t>코칩</t>
-  </si>
-  <si>
-    <t>SK증권제12호스팩</t>
-  </si>
-  <si>
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
@@ -350,12 +326,6 @@
     <t>783.2:1</t>
   </si>
   <si>
-    <t>988.32:1</t>
-  </si>
-  <si>
-    <t>1,189.41:1</t>
-  </si>
-  <si>
     <t>38.7:1</t>
   </si>
   <si>
@@ -392,9 +362,6 @@
     <t>6.54%</t>
   </si>
   <si>
-    <t>13.19%</t>
-  </si>
-  <si>
     <t>리튬디실리케이트 수복소재(Amber block, Amber Ingot 등), 지르코니아 유치관</t>
   </si>
   <si>
@@ -432,12 +399,6 @@
   </si>
   <si>
     <t>PUF반도체,보안솔루션(보안반도체,정보통신모듈기기,정보통신용반도체) 제조,개발</t>
-  </si>
-  <si>
-    <t>소형 및 초소형 슈퍼커패시터</t>
-  </si>
-  <si>
-    <t>기업인수목적 주식회사</t>
   </si>
   <si>
     <t>신탁 및 집합투자</t>
@@ -1017,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1105,16 +1066,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F2">
         <v>1810000</v>
@@ -1141,10 +1102,10 @@
         <v>16000</v>
       </c>
       <c r="N2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="P2">
         <v>12596039842</v>
@@ -1174,7 +1135,7 @@
         <v>1795726428</v>
       </c>
       <c r="Y2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1182,16 +1143,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F3">
         <v>1330000</v>
@@ -1218,10 +1179,10 @@
         <v>43300</v>
       </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="P3">
         <v>103267682</v>
@@ -1251,7 +1212,7 @@
         <v>-83246975113</v>
       </c>
       <c r="Y3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1262,13 +1223,13 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F4">
         <v>3400000</v>
@@ -1295,10 +1256,10 @@
         <v>7000</v>
       </c>
       <c r="N4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="O4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="P4">
         <v>85187882584</v>
@@ -1328,7 +1289,7 @@
         <v>2646634321</v>
       </c>
       <c r="Y4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1339,13 +1300,13 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>6250000</v>
@@ -1372,10 +1333,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1405,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1416,13 +1377,13 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F6">
         <v>2000000</v>
@@ -1449,10 +1410,10 @@
         <v>11500</v>
       </c>
       <c r="N6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="O6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1482,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1493,13 +1454,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F7">
         <v>6450000</v>
@@ -1526,10 +1487,10 @@
         <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="O7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1559,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1570,13 +1531,13 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F8">
         <v>6000000</v>
@@ -1603,10 +1564,10 @@
         <v>2000</v>
       </c>
       <c r="N8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1636,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1647,13 +1608,13 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F9">
         <v>4000000</v>
@@ -1680,10 +1641,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="O9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1713,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1724,13 +1685,13 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F10">
         <v>4750000</v>
@@ -1757,10 +1718,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="O10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1790,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1798,16 +1759,16 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F11">
         <v>1300000</v>
@@ -1834,10 +1795,10 @@
         <v>17000</v>
       </c>
       <c r="N11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="P11">
         <v>1386123525</v>
@@ -1867,7 +1828,7 @@
         <v>-9916946238</v>
       </c>
       <c r="Y11" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1878,13 +1839,13 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F12">
         <v>1600000</v>
@@ -1911,10 +1872,10 @@
         <v>30000</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="O12" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1944,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1952,16 +1913,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>1298000</v>
@@ -1988,10 +1949,10 @@
         <v>16000</v>
       </c>
       <c r="N13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="O13" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="P13">
         <v>2055746777</v>
@@ -2021,7 +1982,7 @@
         <v>-1627684107</v>
       </c>
       <c r="Y13" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2029,16 +1990,16 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F14">
         <v>5000000</v>
@@ -2065,10 +2026,10 @@
         <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2098,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2106,16 +2067,16 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F15">
         <v>1400000</v>
@@ -2142,10 +2103,10 @@
         <v>40000</v>
       </c>
       <c r="N15" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="O15" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2175,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2183,16 +2144,16 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F16">
         <v>6650000</v>
@@ -2219,11 +2180,11 @@
         <v>2000</v>
       </c>
       <c r="N16" t="s">
+        <v>99</v>
+      </c>
+      <c r="O16" t="s">
         <v>107</v>
       </c>
-      <c r="O16" t="s">
-        <v>117</v>
-      </c>
       <c r="P16">
         <v>0</v>
       </c>
@@ -2252,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2260,16 +2221,16 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F17">
         <v>1200000</v>
@@ -2296,10 +2257,10 @@
         <v>14000</v>
       </c>
       <c r="N17" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="P17">
         <v>468321534076</v>
@@ -2329,7 +2290,7 @@
         <v>4820429371</v>
       </c>
       <c r="Y17" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2340,13 +2301,13 @@
         <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F18">
         <v>5000000</v>
@@ -2373,10 +2334,10 @@
         <v>2000</v>
       </c>
       <c r="N18" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="O18" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -2406,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2417,13 +2378,13 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F19">
         <v>1970000</v>
@@ -2450,10 +2411,10 @@
         <v>20000</v>
       </c>
       <c r="N19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="O19" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -2483,238 +2444,84 @@
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F20">
-        <v>1500000</v>
+        <v>23333334</v>
       </c>
       <c r="G20">
-        <v>1500000</v>
+        <v>23333334</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>11000</v>
+        <v>3000</v>
       </c>
       <c r="J20">
-        <v>14000</v>
+        <v>3800</v>
       </c>
       <c r="K20">
-        <v>8503460</v>
+        <v>43477664</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>18000</v>
+        <v>3000</v>
       </c>
       <c r="N20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="O20" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="P20">
-        <v>47284698907</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>38750429966</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>25900014771</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>7595091433</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>5807002440</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>3668321605</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>5701880294</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>4780312126</v>
+        <v>0</v>
       </c>
       <c r="X20">
-        <v>4195570793</v>
+        <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21">
-        <v>3000000</v>
-      </c>
-      <c r="G21">
-        <v>3000000</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>2000</v>
-      </c>
-      <c r="J21">
-        <v>2000</v>
-      </c>
-      <c r="K21">
-        <v>3310000</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>2000</v>
-      </c>
-      <c r="N21" t="s">
-        <v>112</v>
-      </c>
-      <c r="O21" t="s">
-        <v>117</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22">
-        <v>23333334</v>
-      </c>
-      <c r="G22">
-        <v>23333334</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>3000</v>
-      </c>
-      <c r="J22">
-        <v>3800</v>
-      </c>
-      <c r="K22">
-        <v>43477664</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>3000</v>
-      </c>
-      <c r="N22" t="s">
-        <v>113</v>
-      </c>
-      <c r="O22" t="s">
-        <v>117</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2732,422 +2539,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E2">
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E3">
         <v>11600</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E4">
         <v>21308</v>
       </c>
       <c r="F4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E5">
         <v>6000</v>
       </c>
       <c r="F5" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E6">
         <v>22400</v>
       </c>
       <c r="F6" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E7">
         <v>9500</v>
       </c>
       <c r="F7" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E8">
         <v>16308</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E9">
         <v>24000</v>
       </c>
       <c r="F9" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E10">
         <v>18900</v>
       </c>
       <c r="F10" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E11">
         <v>17500</v>
       </c>
       <c r="F11" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E12">
         <v>12000</v>
       </c>
       <c r="F12" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>8000</v>
       </c>
       <c r="F13" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E14">
         <v>182400</v>
       </c>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E15">
         <v>8000</v>
       </c>
       <c r="F15" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="E16">
         <v>10032</v>
       </c>
       <c r="F16" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E17">
         <v>16290</v>
       </c>
       <c r="F17" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E18">
         <v>26400</v>
       </c>
       <c r="F18" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="E19">
         <v>48412</v>
       </c>
       <c r="F19" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E20">
         <v>12500</v>
       </c>
       <c r="F20" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="E21">
         <v>15300</v>
       </c>
       <c r="F21" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-14
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="204">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -443,6 +443,9 @@
     <t>에이치이엠파마(구.에이치이엠)</t>
   </si>
   <si>
+    <t>아이스크림미디어(구.시공미디어)</t>
+  </si>
+  <si>
     <t>케이쓰리아이</t>
   </si>
   <si>
@@ -491,12 +494,12 @@
     <t>엑셀세라퓨틱스</t>
   </si>
   <si>
-    <t>에이치브이엠(구.한국진공야금)</t>
-  </si>
-  <si>
     <t>2024.08.26~08.30</t>
   </si>
   <si>
+    <t>2024.07.31~08.06</t>
+  </si>
+  <si>
     <t>2024.07.30~08.05</t>
   </si>
   <si>
@@ -536,12 +539,12 @@
     <t>2024.06.13~06.19</t>
   </si>
   <si>
-    <t>2024.06.11~06.17</t>
-  </si>
-  <si>
     <t>18,000~21,000</t>
   </si>
   <si>
+    <t>32,000~40,200</t>
+  </si>
+  <si>
     <t>12,500~15,500</t>
   </si>
   <si>
@@ -581,9 +584,6 @@
     <t>9,000~12,000</t>
   </si>
   <si>
-    <t>11,000~14,200</t>
-  </si>
-  <si>
     <t>2000</t>
   </si>
   <si>
@@ -593,12 +593,12 @@
     <t>16000</t>
   </si>
   <si>
-    <t>18000</t>
-  </si>
-  <si>
     <t>신한투자증권</t>
   </si>
   <si>
+    <t>삼성증권</t>
+  </si>
+  <si>
     <t>하나증권</t>
   </si>
   <si>
@@ -618,9 +618,6 @@
   </si>
   <si>
     <t>NH투자증권</t>
-  </si>
-  <si>
-    <t>삼성증권</t>
   </si>
   <si>
     <t>SK증권</t>
@@ -2660,7 +2657,7 @@
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2677,10 +2674,10 @@
         <v>109</v>
       </c>
       <c r="E3">
-        <v>17500</v>
+        <v>78720</v>
       </c>
       <c r="F3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2688,7 +2685,7 @@
         <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>176</v>
@@ -2697,10 +2694,10 @@
         <v>109</v>
       </c>
       <c r="E4">
-        <v>42471</v>
+        <v>17500</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2717,10 +2714,10 @@
         <v>109</v>
       </c>
       <c r="E5">
-        <v>11600</v>
+        <v>42471</v>
       </c>
       <c r="F5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2737,10 +2734,10 @@
         <v>109</v>
       </c>
       <c r="E6">
-        <v>24000</v>
+        <v>11600</v>
       </c>
       <c r="F6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2748,7 +2745,7 @@
         <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
         <v>179</v>
@@ -2757,10 +2754,10 @@
         <v>109</v>
       </c>
       <c r="E7">
-        <v>14700</v>
+        <v>24000</v>
       </c>
       <c r="F7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2768,19 +2765,19 @@
         <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
         <v>109</v>
       </c>
       <c r="E8">
-        <v>13518</v>
+        <v>14700</v>
       </c>
       <c r="F8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2791,16 +2788,16 @@
         <v>163</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
       </c>
       <c r="E9">
-        <v>21308</v>
+        <v>13518</v>
       </c>
       <c r="F9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2811,16 +2808,16 @@
         <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
         <v>109</v>
       </c>
       <c r="E10">
-        <v>6000</v>
+        <v>21308</v>
       </c>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2828,19 +2825,19 @@
         <v>150</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
         <v>109</v>
       </c>
       <c r="E11">
-        <v>22400</v>
+        <v>6000</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2848,7 +2845,7 @@
         <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>182</v>
@@ -2857,10 +2854,10 @@
         <v>109</v>
       </c>
       <c r="E12">
-        <v>9500</v>
+        <v>22400</v>
       </c>
       <c r="F12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2877,10 +2874,10 @@
         <v>109</v>
       </c>
       <c r="E13">
-        <v>16308</v>
+        <v>9500</v>
       </c>
       <c r="F13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2897,10 +2894,10 @@
         <v>109</v>
       </c>
       <c r="E14">
-        <v>18900</v>
+        <v>16308</v>
       </c>
       <c r="F14" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2911,16 +2908,16 @@
         <v>168</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
         <v>109</v>
       </c>
       <c r="E15">
-        <v>12000</v>
+        <v>18900</v>
       </c>
       <c r="F15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2928,19 +2925,19 @@
         <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
         <v>109</v>
       </c>
       <c r="E16">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2951,61 +2948,61 @@
         <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="E17">
-        <v>182400</v>
+        <v>8000</v>
       </c>
       <c r="F17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
         <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>109</v>
       </c>
       <c r="E18">
-        <v>8000</v>
+        <v>182400</v>
       </c>
       <c r="F18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E19">
-        <v>10032</v>
+        <v>8000</v>
       </c>
       <c r="F19" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="B20" t="s">
         <v>172</v>
@@ -3014,18 +3011,18 @@
         <v>187</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20">
-        <v>16290</v>
+        <v>10032</v>
       </c>
       <c r="F20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
         <v>173</v>
@@ -3034,13 +3031,13 @@
         <v>188</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E21">
-        <v>26400</v>
+        <v>16290</v>
       </c>
       <c r="F21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-15
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="208">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-06-24</t>
+  </si>
+  <si>
     <t>2024-06-27</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
     <t>2024-05-08</t>
   </si>
   <si>
+    <t>2024-07-15</t>
+  </si>
+  <si>
     <t>2024-07-12</t>
   </si>
   <si>
@@ -176,9 +182,6 @@
     <t>2024-06-25</t>
   </si>
   <si>
-    <t>2024-06-24</t>
-  </si>
-  <si>
     <t>2024-06-21</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>대신</t>
+  </si>
+  <si>
     <t>엘에스</t>
   </si>
   <si>
@@ -212,9 +218,6 @@
     <t>IBK</t>
   </si>
   <si>
-    <t>대신</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -224,6 +227,9 @@
     <t>신한, 한국</t>
   </si>
   <si>
+    <t>엑셀세라퓨틱스</t>
+  </si>
+  <si>
     <t>이베스트스팩6호</t>
   </si>
   <si>
@@ -284,6 +290,9 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>1233.80:1</t>
+  </si>
+  <si>
     <t>1131.75:1</t>
   </si>
   <si>
@@ -344,6 +353,9 @@
     <t>38.7:1</t>
   </si>
   <si>
+    <t>4.50%</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -377,6 +389,9 @@
     <t>6.54%</t>
   </si>
   <si>
+    <t>CellCor SFD/CD(세포배양배지)</t>
+  </si>
+  <si>
     <t>기업인수목적 주식회사</t>
   </si>
   <si>
@@ -489,9 +504,6 @@
   </si>
   <si>
     <t>산일전기(유가)</t>
-  </si>
-  <si>
-    <t>엑셀세라퓨틱스</t>
   </si>
   <si>
     <t>2024.08.26~08.30</t>
@@ -984,7 +996,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1072,46 +1084,46 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="G2">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>6200</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="K2">
-        <v>5020000</v>
+        <v>10830212</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1141,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1152,73 +1164,73 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F3">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="G3">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="K3">
-        <v>7836009</v>
+        <v>5020000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="P3">
-        <v>12596039842</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>14910346438</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>16039074617</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>1732604466</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>2893667787</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>1613779678</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1558081149</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>2643467726</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>1795726428</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1229,73 +1241,73 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F4">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="G4">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>36400</v>
+        <v>9000</v>
       </c>
       <c r="J4">
-        <v>43300</v>
+        <v>12000</v>
       </c>
       <c r="K4">
-        <v>9375694</v>
+        <v>7836009</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="P4">
-        <v>103267682</v>
+        <v>12596039842</v>
       </c>
       <c r="Q4">
-        <v>342201581</v>
+        <v>14910346438</v>
       </c>
       <c r="R4">
-        <v>231425455</v>
+        <v>16039074617</v>
       </c>
       <c r="S4">
-        <v>-7598692896</v>
+        <v>1732604466</v>
       </c>
       <c r="T4">
-        <v>-25822444575</v>
+        <v>2893667787</v>
       </c>
       <c r="U4">
-        <v>-15929213281</v>
+        <v>1613779678</v>
       </c>
       <c r="V4">
-        <v>-6973258680</v>
+        <v>1558081149</v>
       </c>
       <c r="W4">
-        <v>-48433907514</v>
+        <v>2643467726</v>
       </c>
       <c r="X4">
-        <v>-83246975113</v>
+        <v>1795726428</v>
       </c>
       <c r="Y4" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1303,76 +1315,76 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F5">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="G5">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>4500</v>
+        <v>36400</v>
       </c>
       <c r="J5">
-        <v>5500</v>
+        <v>43300</v>
       </c>
       <c r="K5">
-        <v>30888000</v>
+        <v>9375694</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>7000</v>
+        <v>43300</v>
       </c>
       <c r="N5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="P5">
-        <v>85187882584</v>
+        <v>103267682</v>
       </c>
       <c r="Q5">
-        <v>87525689695</v>
+        <v>342201581</v>
       </c>
       <c r="R5">
-        <v>77247394706</v>
+        <v>231425455</v>
       </c>
       <c r="S5">
-        <v>2205797752</v>
+        <v>-7598692896</v>
       </c>
       <c r="T5">
-        <v>4920387020</v>
+        <v>-25822444575</v>
       </c>
       <c r="U5">
-        <v>4336496285</v>
+        <v>-15929213281</v>
       </c>
       <c r="V5">
-        <v>1613954566</v>
+        <v>-6973258680</v>
       </c>
       <c r="W5">
-        <v>3980493669</v>
+        <v>-48433907514</v>
       </c>
       <c r="X5">
-        <v>2646634321</v>
+        <v>-83246975113</v>
       </c>
       <c r="Y5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1383,73 +1395,73 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F6">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="G6">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>4500</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>5500</v>
       </c>
       <c r="K6">
-        <v>6870000</v>
+        <v>30888000</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O6" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>85187882584</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>87525689695</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>77247394706</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>2205797752</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>4920387020</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>4336496285</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1613954566</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>3980493669</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>2646634321</v>
       </c>
       <c r="Y6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1457,43 +1469,43 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F7">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="G7">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="K7">
-        <v>17529140</v>
+        <v>6870000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s">
         <v>113</v>
@@ -1526,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1534,46 +1546,46 @@
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F8">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="G8">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="J8">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="K8">
-        <v>6930000</v>
+        <v>17529140</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O8" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1603,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1611,22 +1623,22 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="G9">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1638,7 +1650,7 @@
         <v>2000</v>
       </c>
       <c r="K9">
-        <v>6220000</v>
+        <v>6930000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1647,10 +1659,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1680,30 +1692,30 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F10">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G10">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1715,7 +1727,7 @@
         <v>2000</v>
       </c>
       <c r="K10">
-        <v>4810000</v>
+        <v>6220000</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1724,10 +1736,10 @@
         <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="O10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1757,30 +1769,30 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F11">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="G11">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1792,7 +1804,7 @@
         <v>2000</v>
       </c>
       <c r="K11">
-        <v>5480000</v>
+        <v>4810000</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1801,10 +1813,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1834,84 +1846,84 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F12">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="G12">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
-        <v>12293880</v>
+        <v>5480000</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="O12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P12">
-        <v>1386123525</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>1152944128</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>1885010467</v>
+        <v>0</v>
       </c>
       <c r="S12">
-        <v>-4388824706</v>
+        <v>0</v>
       </c>
       <c r="T12">
-        <v>-7990287699</v>
+        <v>0</v>
       </c>
       <c r="U12">
-        <v>-9803411085</v>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>-4430563401</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>-7988275689</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>-9916946238</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1919,230 +1931,230 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="G13">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J13">
-        <v>23500</v>
+        <v>14000</v>
       </c>
       <c r="K13">
-        <v>8751446</v>
+        <v>12293880</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1386123525</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1152944128</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>1885010467</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>-4388824706</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>-7990287699</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>-9803411085</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>-4430563401</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>-7988275689</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>-9916946238</v>
       </c>
       <c r="Y13" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F14">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="G14">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>10400</v>
+        <v>20000</v>
       </c>
       <c r="J14">
-        <v>12700</v>
+        <v>23500</v>
       </c>
       <c r="K14">
-        <v>8650735</v>
+        <v>8751446</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P14">
-        <v>2055746777</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>2918221978</v>
+        <v>0</v>
       </c>
       <c r="R14">
-        <v>979078233</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>-3343774083</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>-3525649863</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>-1713494359</v>
+        <v>0</v>
       </c>
       <c r="V14">
-        <v>-4430074915</v>
+        <v>0</v>
       </c>
       <c r="W14">
-        <v>-8304699942</v>
+        <v>0</v>
       </c>
       <c r="X14">
-        <v>-1627684107</v>
+        <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="G15">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>10400</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>12700</v>
       </c>
       <c r="K15">
-        <v>5840000</v>
+        <v>8650735</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O15" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>2055746777</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>2918221978</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>979078233</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>-3343774083</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>-3525649863</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>-1713494359</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>-4430074915</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>-8304699942</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>-1627684107</v>
       </c>
       <c r="Y15" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2150,46 +2162,46 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F16">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="G16">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>34000</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
-        <v>7942750</v>
+        <v>5840000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2219,7 +2231,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2230,43 +2242,43 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F17">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="G17">
-        <v>6650000</v>
+        <v>1400000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2000</v>
+        <v>34000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="K17">
-        <v>8100000</v>
+        <v>7942750</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="N17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O17" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="P17">
         <v>0</v>
@@ -2296,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2307,73 +2319,73 @@
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="G18">
-        <v>1200000</v>
+        <v>6650000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>8700</v>
+        <v>2000</v>
       </c>
       <c r="J18">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K18">
-        <v>7651263</v>
+        <v>8100000</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="P18">
-        <v>468321534076</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>555936831337</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>359249623614</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>22403886436</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>33386727728</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>10411712773</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>10859975142</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>29346086803</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>4820429371</v>
+        <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2381,76 +2393,76 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="G19">
-        <v>5000000</v>
+        <v>1200000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>2000</v>
+        <v>8700</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K19">
-        <v>5505000</v>
+        <v>7651263</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O19" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>468321534076</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>555936831337</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>359249623614</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>22403886436</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>33386727728</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>10411712773</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>10859975142</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>29346086803</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>4820429371</v>
       </c>
       <c r="Y19" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2458,46 +2470,46 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F20">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="G20">
-        <v>1970000</v>
+        <v>5000000</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J20">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K20">
-        <v>13124496</v>
+        <v>5505000</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="O20" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="P20">
         <v>0</v>
@@ -2527,15 +2539,15 @@
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>58</v>
@@ -2544,67 +2556,144 @@
         <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F21">
+        <v>1970000</v>
+      </c>
+      <c r="G21">
+        <v>1970000</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>13000</v>
+      </c>
+      <c r="J21">
+        <v>16000</v>
+      </c>
+      <c r="K21">
+        <v>13124496</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>20000</v>
+      </c>
+      <c r="N21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" t="s">
+        <v>123</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22">
         <v>23333334</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>23333334</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
         <v>3000</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>3800</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>43477664</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <v>3000</v>
       </c>
-      <c r="N21" t="s">
-        <v>108</v>
-      </c>
-      <c r="O21" t="s">
-        <v>109</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>134</v>
+      <c r="N22" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" t="s">
+        <v>113</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2622,422 +2711,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E2">
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E3">
         <v>78720</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E4">
         <v>17500</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E5">
         <v>42471</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E6">
         <v>11600</v>
       </c>
       <c r="F6" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E7">
         <v>24000</v>
       </c>
       <c r="F7" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E8">
         <v>14700</v>
       </c>
       <c r="F8" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E9">
         <v>13518</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E10">
         <v>21308</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E11">
         <v>6000</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E12">
         <v>22400</v>
       </c>
       <c r="F12" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E13">
         <v>9500</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E14">
         <v>16308</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E15">
         <v>18900</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E16">
         <v>12000</v>
       </c>
       <c r="F16" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E17">
         <v>8000</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>182400</v>
       </c>
       <c r="F18" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E19">
         <v>8000</v>
       </c>
       <c r="F19" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E20">
         <v>10032</v>
       </c>
       <c r="F20" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C21" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E21">
         <v>16290</v>
       </c>
       <c r="F21" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-18
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="201">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -428,6 +428,9 @@
     <t>에이치이엠파마(구.에이치이엠)</t>
   </si>
   <si>
+    <t>이엔셀</t>
+  </si>
+  <si>
     <t>엠83</t>
   </si>
   <si>
@@ -452,9 +455,6 @@
     <t>유라클</t>
   </si>
   <si>
-    <t>이엔셀</t>
-  </si>
-  <si>
     <t>키움스팩9호</t>
   </si>
   <si>
@@ -482,6 +482,9 @@
     <t>2024.08.26~08.30</t>
   </si>
   <si>
+    <t>2024.08.02~08.08</t>
+  </si>
+  <si>
     <t>2024.08.01~08.07</t>
   </si>
   <si>
@@ -497,12 +500,12 @@
     <t>2024.07.29~08.02</t>
   </si>
   <si>
+    <t>2024.07.23~07.24</t>
+  </si>
+  <si>
     <t>2024.07.23~07.29</t>
   </si>
   <si>
-    <t>2024.07.23~07.24</t>
-  </si>
-  <si>
     <t>2024.07.18~07.24</t>
   </si>
   <si>
@@ -527,6 +530,9 @@
     <t>18,000~21,000</t>
   </si>
   <si>
+    <t>13,600~15,300</t>
+  </si>
+  <si>
     <t>11,000~13,000</t>
   </si>
   <si>
@@ -548,9 +554,6 @@
     <t>4,900~5,700</t>
   </si>
   <si>
-    <t>13,600~15,300</t>
-  </si>
-  <si>
     <t>16,000~19,000</t>
   </si>
   <si>
@@ -572,12 +575,18 @@
     <t>2000</t>
   </si>
   <si>
+    <t>35000</t>
+  </si>
+  <si>
     <t>10000</t>
   </si>
   <si>
     <t>신한투자증권</t>
   </si>
   <si>
+    <t>NH투자증권</t>
+  </si>
+  <si>
     <t>신영증권,유진투자증권</t>
   </si>
   <si>
@@ -600,9 +609,6 @@
   </si>
   <si>
     <t>키움증권</t>
-  </si>
-  <si>
-    <t>NH투자증권</t>
   </si>
   <si>
     <t>SK증권</t>
@@ -2556,7 +2562,7 @@
         <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>105</v>
@@ -2565,7 +2571,7 @@
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2576,16 +2582,16 @@
         <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>105</v>
       </c>
       <c r="E3">
-        <v>16500</v>
+        <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2596,16 +2602,16 @@
         <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
         <v>105</v>
       </c>
       <c r="E4">
-        <v>78720</v>
+        <v>16500</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2616,16 +2622,16 @@
         <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
         <v>105</v>
       </c>
       <c r="E5">
-        <v>17500</v>
+        <v>78720</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2633,19 +2639,19 @@
         <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
       </c>
       <c r="E6">
-        <v>42471</v>
+        <v>17500</v>
       </c>
       <c r="F6" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2656,16 +2662,16 @@
         <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
         <v>105</v>
       </c>
       <c r="E7">
-        <v>11600</v>
+        <v>42471</v>
       </c>
       <c r="F7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2676,16 +2682,16 @@
         <v>159</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
       </c>
       <c r="E8">
-        <v>24000</v>
+        <v>11600</v>
       </c>
       <c r="F8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2693,19 +2699,19 @@
         <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
         <v>105</v>
       </c>
       <c r="E9">
-        <v>14700</v>
+        <v>24000</v>
       </c>
       <c r="F9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2713,19 +2719,19 @@
         <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="D10" t="s">
         <v>105</v>
       </c>
       <c r="E10">
-        <v>13518</v>
+        <v>14700</v>
       </c>
       <c r="F10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2736,16 +2742,16 @@
         <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D11" t="s">
         <v>105</v>
       </c>
       <c r="E11">
-        <v>21308</v>
+        <v>13518</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2756,7 +2762,7 @@
         <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D12" t="s">
         <v>105</v>
@@ -2765,7 +2771,7 @@
         <v>6000</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2773,10 +2779,10 @@
         <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
         <v>105</v>
@@ -2785,7 +2791,7 @@
         <v>22400</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2793,10 +2799,10 @@
         <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -2805,7 +2811,7 @@
         <v>9500</v>
       </c>
       <c r="F14" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2813,10 +2819,10 @@
         <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
         <v>105</v>
@@ -2825,7 +2831,7 @@
         <v>16308</v>
       </c>
       <c r="F15" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2833,10 +2839,10 @@
         <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
         <v>105</v>
@@ -2845,7 +2851,7 @@
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2853,19 +2859,19 @@
         <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2873,19 +2879,19 @@
         <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2893,19 +2899,19 @@
         <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>186</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2913,19 +2919,19 @@
         <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2933,19 +2939,19 @@
         <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-19
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="200">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -434,6 +434,9 @@
     <t>엠83</t>
   </si>
   <si>
+    <t>티디에스팜</t>
+  </si>
+  <si>
     <t>아이스크림미디어(구.시공미디어)</t>
   </si>
   <si>
@@ -461,9 +464,6 @@
     <t>뱅크웨어글로벌</t>
   </si>
   <si>
-    <t>티디에스팜</t>
-  </si>
-  <si>
     <t>아이빔테크놀로지</t>
   </si>
   <si>
@@ -506,9 +506,6 @@
     <t>2024.07.23~07.29</t>
   </si>
   <si>
-    <t>2024.07.18~07.24</t>
-  </si>
-  <si>
     <t>2024.07.15~07.19</t>
   </si>
   <si>
@@ -536,6 +533,9 @@
     <t>11,000~13,000</t>
   </si>
   <si>
+    <t>9,500~10,700</t>
+  </si>
+  <si>
     <t>32,000~40,200</t>
   </si>
   <si>
@@ -557,9 +557,6 @@
     <t>16,000~19,000</t>
   </si>
   <si>
-    <t>9,500~10,700</t>
-  </si>
-  <si>
     <t>7,300~8,500</t>
   </si>
   <si>
@@ -590,6 +587,9 @@
     <t>신영증권,유진투자증권</t>
   </si>
   <si>
+    <t>한국투자증권</t>
+  </si>
+  <si>
     <t>삼성증권</t>
   </si>
   <si>
@@ -600,9 +600,6 @@
   </si>
   <si>
     <t>교보증권</t>
-  </si>
-  <si>
-    <t>한국투자증권</t>
   </si>
   <si>
     <t>대신증권</t>
@@ -2562,7 +2559,7 @@
         <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
         <v>105</v>
@@ -2571,7 +2568,7 @@
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2582,7 +2579,7 @@
         <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
         <v>105</v>
@@ -2591,7 +2588,7 @@
         <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2602,7 +2599,7 @@
         <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
         <v>105</v>
@@ -2611,7 +2608,7 @@
         <v>16500</v>
       </c>
       <c r="F4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2622,16 +2619,16 @@
         <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
         <v>105</v>
       </c>
       <c r="E5">
-        <v>78720</v>
+        <v>9500</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2639,19 +2636,19 @@
         <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
         <v>105</v>
       </c>
       <c r="E6">
-        <v>17500</v>
+        <v>78720</v>
       </c>
       <c r="F6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2662,16 +2659,16 @@
         <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
         <v>105</v>
       </c>
       <c r="E7">
-        <v>42471</v>
+        <v>17500</v>
       </c>
       <c r="F7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2679,19 +2676,19 @@
         <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
         <v>105</v>
       </c>
       <c r="E8">
-        <v>11600</v>
+        <v>42471</v>
       </c>
       <c r="F8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2699,19 +2696,19 @@
         <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
         <v>105</v>
       </c>
       <c r="E9">
-        <v>24000</v>
+        <v>11600</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2722,16 +2719,16 @@
         <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
         <v>105</v>
       </c>
       <c r="E10">
-        <v>14700</v>
+        <v>24000</v>
       </c>
       <c r="F10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2742,16 +2739,16 @@
         <v>160</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
         <v>105</v>
       </c>
       <c r="E11">
-        <v>13518</v>
+        <v>14700</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2759,19 +2756,19 @@
         <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
         <v>105</v>
       </c>
       <c r="E12">
-        <v>6000</v>
+        <v>13518</v>
       </c>
       <c r="F12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2779,19 +2776,19 @@
         <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D13" t="s">
         <v>105</v>
       </c>
       <c r="E13">
-        <v>22400</v>
+        <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2799,19 +2796,19 @@
         <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
       </c>
       <c r="E14">
-        <v>9500</v>
+        <v>22400</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2819,10 +2816,10 @@
         <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
         <v>105</v>
@@ -2839,10 +2836,10 @@
         <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D16" t="s">
         <v>105</v>
@@ -2851,7 +2848,7 @@
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2859,19 +2856,19 @@
         <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
         <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2879,19 +2876,19 @@
         <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
         <v>176</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2899,19 +2896,19 @@
         <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2919,19 +2916,19 @@
         <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
         <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2939,19 +2936,19 @@
         <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-21
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="201">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>6,200~7,700</t>
+  </si>
+  <si>
+    <t>22000</t>
   </si>
   <si>
     <t>2000</t>
@@ -2568,7 +2571,7 @@
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2588,7 +2591,7 @@
         <v>21308</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2608,7 +2611,7 @@
         <v>16500</v>
       </c>
       <c r="F4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2628,7 +2631,7 @@
         <v>9500</v>
       </c>
       <c r="F5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2648,7 +2651,7 @@
         <v>78720</v>
       </c>
       <c r="F6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2668,7 +2671,7 @@
         <v>17500</v>
       </c>
       <c r="F7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2688,7 +2691,7 @@
         <v>42471</v>
       </c>
       <c r="F8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2708,7 +2711,7 @@
         <v>11600</v>
       </c>
       <c r="F9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2728,7 +2731,7 @@
         <v>24000</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2748,7 +2751,7 @@
         <v>14700</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2768,7 +2771,7 @@
         <v>13518</v>
       </c>
       <c r="F12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2788,7 +2791,7 @@
         <v>6000</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2808,7 +2811,7 @@
         <v>22400</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2828,7 +2831,7 @@
         <v>16308</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2842,13 +2845,13 @@
         <v>181</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>184</v>
       </c>
       <c r="E16">
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2862,13 +2865,13 @@
         <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2882,13 +2885,13 @@
         <v>176</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2902,13 +2905,13 @@
         <v>182</v>
       </c>
       <c r="D19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2922,13 +2925,13 @@
         <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2942,13 +2945,13 @@
         <v>183</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-25
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="196">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -413,6 +413,9 @@
     <t>키움스팩9호</t>
   </si>
   <si>
+    <t>아이스크림미디어(구.시공미디어)</t>
+  </si>
+  <si>
     <t>이엔셀</t>
   </si>
   <si>
@@ -422,9 +425,6 @@
     <t>티디에스팜</t>
   </si>
   <si>
-    <t>아이스크림미디어(구.시공미디어)</t>
-  </si>
-  <si>
     <t>케이쓰리아이</t>
   </si>
   <si>
@@ -467,6 +467,9 @@
     <t>2024.08.13~08.14</t>
   </si>
   <si>
+    <t>2024.08.09~08.16</t>
+  </si>
+  <si>
     <t>2024.08.02~08.08</t>
   </si>
   <si>
@@ -512,6 +515,9 @@
     <t>2,000~2,000</t>
   </si>
   <si>
+    <t>32,000~40,200</t>
+  </si>
+  <si>
     <t>13,600~15,300</t>
   </si>
   <si>
@@ -521,9 +527,6 @@
     <t>9,500~10,700</t>
   </si>
   <si>
-    <t>32,000~40,200</t>
-  </si>
-  <si>
     <t>12,500~15,500</t>
   </si>
   <si>
@@ -569,6 +572,9 @@
     <t>키움증권</t>
   </si>
   <si>
+    <t>삼성증권</t>
+  </si>
+  <si>
     <t>NH투자증권</t>
   </si>
   <si>
@@ -576,9 +582,6 @@
   </si>
   <si>
     <t>한국투자증권</t>
-  </si>
-  <si>
-    <t>삼성증권</t>
   </si>
   <si>
     <t>하나증권</t>
@@ -2467,7 +2470,7 @@
         <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
         <v>101</v>
@@ -2476,7 +2479,7 @@
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2487,7 +2490,7 @@
         <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
         <v>101</v>
@@ -2496,7 +2499,7 @@
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2507,16 +2510,16 @@
         <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
         <v>101</v>
       </c>
       <c r="E4">
-        <v>21308</v>
+        <v>78720</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2527,16 +2530,16 @@
         <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
         <v>101</v>
       </c>
       <c r="E5">
-        <v>16500</v>
+        <v>21308</v>
       </c>
       <c r="F5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2547,16 +2550,16 @@
         <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
         <v>101</v>
       </c>
       <c r="E6">
-        <v>9500</v>
+        <v>16500</v>
       </c>
       <c r="F6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2564,19 +2567,19 @@
         <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
         <v>101</v>
       </c>
       <c r="E7">
-        <v>78720</v>
+        <v>9500</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2584,10 +2587,10 @@
         <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
         <v>101</v>
@@ -2596,7 +2599,7 @@
         <v>17500</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2604,10 +2607,10 @@
         <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
         <v>101</v>
@@ -2616,7 +2619,7 @@
         <v>42471</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2624,10 +2627,10 @@
         <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
         <v>101</v>
@@ -2636,7 +2639,7 @@
         <v>11600</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2644,10 +2647,10 @@
         <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
@@ -2656,7 +2659,7 @@
         <v>24000</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2664,10 +2667,10 @@
         <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
         <v>101</v>
@@ -2676,7 +2679,7 @@
         <v>14700</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2684,10 +2687,10 @@
         <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
         <v>101</v>
@@ -2696,7 +2699,7 @@
         <v>13518</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2704,10 +2707,10 @@
         <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
         <v>101</v>
@@ -2716,7 +2719,7 @@
         <v>22400</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2724,19 +2727,19 @@
         <v>143</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E15">
         <v>16308</v>
       </c>
       <c r="F15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2744,19 +2747,19 @@
         <v>144</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E16">
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2764,19 +2767,19 @@
         <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2784,19 +2787,19 @@
         <v>146</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2804,19 +2807,19 @@
         <v>147</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2824,19 +2827,19 @@
         <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2844,19 +2847,19 @@
         <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-29
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="202">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -134,9 +134,6 @@
     <t>2024-05-23</t>
   </si>
   <si>
-    <t>2024-05-13</t>
-  </si>
-  <si>
     <t>2024-07-10</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>2024-05-29</t>
   </si>
   <si>
-    <t>2024-05-14</t>
-  </si>
-  <si>
     <t>2024-07-26</t>
   </si>
   <si>
@@ -281,9 +275,6 @@
     <t>그리드위즈</t>
   </si>
   <si>
-    <t>미래에셋비전스팩4호</t>
-  </si>
-  <si>
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
@@ -341,9 +332,6 @@
     <t>124.60:1</t>
   </si>
   <si>
-    <t>1011.2:1</t>
-  </si>
-  <si>
     <t>38.7:1</t>
   </si>
   <si>
@@ -414,9 +402,6 @@
   </si>
   <si>
     <t>수요관리 서비스, 전기차 충전기 모뎀 등</t>
-  </si>
-  <si>
-    <t>기업인수목적회사(기타금융서비스)</t>
   </si>
   <si>
     <t>신탁 및 집합투자</t>
@@ -993,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1081,16 +1066,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2">
         <v>6000000</v>
@@ -1117,10 +1102,10 @@
         <v>2000</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1150,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1158,16 +1143,16 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F3">
         <v>4000000</v>
@@ -1194,10 +1179,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1227,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1235,16 +1220,16 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4">
         <v>1618000</v>
@@ -1271,10 +1256,10 @@
         <v>10000</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1304,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1312,16 +1297,16 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5">
         <v>4000000</v>
@@ -1348,10 +1333,10 @@
         <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1381,7 +1366,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1389,16 +1374,16 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6">
         <v>1810000</v>
@@ -1425,10 +1410,10 @@
         <v>16000</v>
       </c>
       <c r="N6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P6">
         <v>12596039842</v>
@@ -1458,7 +1443,7 @@
         <v>1795726428</v>
       </c>
       <c r="Y6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1466,16 +1451,16 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7">
         <v>1330000</v>
@@ -1502,10 +1487,10 @@
         <v>43300</v>
       </c>
       <c r="N7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P7">
         <v>103267682</v>
@@ -1535,7 +1520,7 @@
         <v>-83246975113</v>
       </c>
       <c r="Y7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1549,10 +1534,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8">
         <v>3400000</v>
@@ -1579,10 +1564,10 @@
         <v>7000</v>
       </c>
       <c r="N8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="O8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P8">
         <v>85187882584</v>
@@ -1612,7 +1597,7 @@
         <v>2646634321</v>
       </c>
       <c r="Y8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1623,13 +1608,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <v>6250000</v>
@@ -1656,10 +1641,10 @@
         <v>2000</v>
       </c>
       <c r="N9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1689,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="Y9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1700,13 +1685,13 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <v>2000000</v>
@@ -1733,10 +1718,10 @@
         <v>11500</v>
       </c>
       <c r="N10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1766,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1780,10 +1765,10 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>6450000</v>
@@ -1810,10 +1795,10 @@
         <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="O11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1843,7 +1828,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1854,13 +1839,13 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F12">
         <v>6000000</v>
@@ -1887,10 +1872,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1920,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1931,13 +1916,13 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13">
         <v>4000000</v>
@@ -1964,10 +1949,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="O13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1997,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -2008,13 +1993,13 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F14">
         <v>4750000</v>
@@ -2041,10 +2026,10 @@
         <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2074,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -2082,16 +2067,16 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F15">
         <v>1300000</v>
@@ -2118,10 +2103,10 @@
         <v>17000</v>
       </c>
       <c r="N15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P15">
         <v>1386123525</v>
@@ -2151,7 +2136,7 @@
         <v>-9916946238</v>
       </c>
       <c r="Y15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2165,10 +2150,10 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16">
         <v>1600000</v>
@@ -2195,10 +2180,10 @@
         <v>30000</v>
       </c>
       <c r="N16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -2228,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2236,16 +2221,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F17">
         <v>1298000</v>
@@ -2272,10 +2257,10 @@
         <v>16000</v>
       </c>
       <c r="N17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="O17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="P17">
         <v>2055746777</v>
@@ -2305,7 +2290,7 @@
         <v>-1627684107</v>
       </c>
       <c r="Y17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2313,16 +2298,16 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F18">
         <v>5000000</v>
@@ -2349,11 +2334,11 @@
         <v>2000</v>
       </c>
       <c r="N18" t="s">
+        <v>103</v>
+      </c>
+      <c r="O18" t="s">
         <v>106</v>
       </c>
-      <c r="O18" t="s">
-        <v>110</v>
-      </c>
       <c r="P18">
         <v>0</v>
       </c>
@@ -2382,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2390,16 +2375,16 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F19">
         <v>1400000</v>
@@ -2426,10 +2411,10 @@
         <v>40000</v>
       </c>
       <c r="N19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O19" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -2459,54 +2444,54 @@
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F20">
-        <v>6650000</v>
+        <v>23333334</v>
       </c>
       <c r="G20">
-        <v>6650000</v>
+        <v>23333334</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J20">
-        <v>2000</v>
+        <v>3800</v>
       </c>
       <c r="K20">
-        <v>8100000</v>
+        <v>43477664</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="N20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P20">
         <v>0</v>
@@ -2536,84 +2521,7 @@
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21">
-        <v>23333334</v>
-      </c>
-      <c r="G21">
-        <v>23333334</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>3000</v>
-      </c>
-      <c r="J21">
-        <v>3800</v>
-      </c>
-      <c r="K21">
-        <v>43477664</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>3000</v>
-      </c>
-      <c r="N21" t="s">
-        <v>109</v>
-      </c>
-      <c r="O21" t="s">
-        <v>110</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2631,422 +2539,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2">
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3">
         <v>6000</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E4">
         <v>78720</v>
       </c>
       <c r="F4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5">
         <v>21308</v>
       </c>
       <c r="F5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6">
         <v>16500</v>
       </c>
       <c r="F6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E7">
         <v>9500</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8">
         <v>17500</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E9">
         <v>42471</v>
       </c>
       <c r="F9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E10">
         <v>11600</v>
       </c>
       <c r="F10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11">
         <v>24000</v>
       </c>
       <c r="F11" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12">
         <v>14700</v>
       </c>
       <c r="F12" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13">
         <v>13518</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14">
         <v>22400</v>
       </c>
       <c r="F14" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E15">
         <v>16308</v>
       </c>
       <c r="F15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E16">
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" t="s">
         <v>171</v>
       </c>
-      <c r="C17" t="s">
-        <v>176</v>
-      </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" t="s">
         <v>171</v>
       </c>
-      <c r="C18" t="s">
-        <v>176</v>
-      </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" t="s">
         <v>188</v>
-      </c>
-      <c r="D19" t="s">
-        <v>193</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D21" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-31
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="209">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-07-11</t>
+  </si>
+  <si>
     <t>2024-07-09</t>
   </si>
   <si>
@@ -134,6 +137,9 @@
     <t>2024-05-23</t>
   </si>
   <si>
+    <t>2024-07-17</t>
+  </si>
+  <si>
     <t>2024-07-10</t>
   </si>
   <si>
@@ -188,6 +194,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>키움</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -221,6 +230,9 @@
     <t>신한, 한국</t>
   </si>
   <si>
+    <t>피앤에스미캐닉스</t>
+  </si>
+  <si>
     <t>엔에이치스팩31호</t>
   </si>
   <si>
@@ -278,6 +290,9 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>986.08:1</t>
+  </si>
+  <si>
     <t>1123.43 :1</t>
   </si>
   <si>
@@ -335,6 +350,9 @@
     <t>38.7:1</t>
   </si>
   <si>
+    <t>5.60%</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -365,6 +383,9 @@
     <t>0.95%</t>
   </si>
   <si>
+    <t>보행재활로봇 시스템</t>
+  </si>
+  <si>
     <t>금융지원서비스업</t>
   </si>
   <si>
@@ -428,6 +449,9 @@
     <t>에이치이엠파마(구.에이치이엠)</t>
   </si>
   <si>
+    <t>아이언디바이스</t>
+  </si>
+  <si>
     <t>키움스팩9호</t>
   </si>
   <si>
@@ -455,9 +479,6 @@
     <t>넥스트바이오메디컬</t>
   </si>
   <si>
-    <t>아이언디바이스</t>
-  </si>
-  <si>
     <t>유라클</t>
   </si>
   <si>
@@ -467,9 +488,6 @@
     <t>아이빔테크놀로지</t>
   </si>
   <si>
-    <t>피앤에스미캐닉스</t>
-  </si>
-  <si>
     <t>NH스팩31호</t>
   </si>
   <si>
@@ -482,6 +500,9 @@
     <t>2024.08.26~08.30</t>
   </si>
   <si>
+    <t>2024.08.19~08.23</t>
+  </si>
+  <si>
     <t>2024.08.13~08.14</t>
   </si>
   <si>
@@ -530,6 +551,9 @@
     <t>18,000~21,000</t>
   </si>
   <si>
+    <t>4,900~5,700</t>
+  </si>
+  <si>
     <t>2,000~2,000</t>
   </si>
   <si>
@@ -554,9 +578,6 @@
     <t>24,000~29,000</t>
   </si>
   <si>
-    <t>4,900~5,700</t>
-  </si>
-  <si>
     <t>16,000~19,000</t>
   </si>
   <si>
@@ -587,6 +608,9 @@
     <t>신한투자증권</t>
   </si>
   <si>
+    <t>대신증권</t>
+  </si>
+  <si>
     <t>키움증권</t>
   </si>
   <si>
@@ -609,9 +633,6 @@
   </si>
   <si>
     <t>교보증권</t>
-  </si>
-  <si>
-    <t>대신증권</t>
   </si>
   <si>
     <t>SK증권</t>
@@ -978,7 +999,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1066,99 +1087,99 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F2">
-        <v>6000000</v>
+        <v>1350000</v>
       </c>
       <c r="G2">
-        <v>6000000</v>
+        <v>1350000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="K2">
-        <v>6345000</v>
+        <v>6471740</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="N2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>5214628820</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>6009352447</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>965797975</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2015081728</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1319755337</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>-44547594</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1503069100</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1410469786</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>24178632</v>
       </c>
       <c r="Y2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F3">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G3">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1170,7 +1191,7 @@
         <v>2000</v>
       </c>
       <c r="K3">
-        <v>4420000</v>
+        <v>6345000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1179,10 +1200,10 @@
         <v>2000</v>
       </c>
       <c r="N3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1212,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1220,46 +1241,46 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F4">
-        <v>1618000</v>
+        <v>4000000</v>
       </c>
       <c r="G4">
-        <v>1618000</v>
+        <v>4000000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>6200</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="K4">
-        <v>10830212</v>
+        <v>4420000</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="O4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1289,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1297,46 +1318,46 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>6200</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="K5">
-        <v>5020000</v>
+        <v>10830212</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1366,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1374,76 +1395,76 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F6">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="G6">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="K6">
-        <v>7836009</v>
+        <v>5020000</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="P6">
-        <v>12596039842</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>14910346438</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>16039074617</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1732604466</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>2893667787</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>1613779678</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1558081149</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>2643467726</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>1795726428</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1451,76 +1472,76 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F7">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="G7">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>36400</v>
+        <v>9000</v>
       </c>
       <c r="J7">
-        <v>43300</v>
+        <v>12000</v>
       </c>
       <c r="K7">
-        <v>9375694</v>
+        <v>7836009</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="O7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="P7">
-        <v>103267682</v>
+        <v>12596039842</v>
       </c>
       <c r="Q7">
-        <v>342201581</v>
+        <v>14910346438</v>
       </c>
       <c r="R7">
-        <v>231425455</v>
+        <v>16039074617</v>
       </c>
       <c r="S7">
-        <v>-7598692896</v>
+        <v>1732604466</v>
       </c>
       <c r="T7">
-        <v>-25822444575</v>
+        <v>2893667787</v>
       </c>
       <c r="U7">
-        <v>-15929213281</v>
+        <v>1613779678</v>
       </c>
       <c r="V7">
-        <v>-6973258680</v>
+        <v>1558081149</v>
       </c>
       <c r="W7">
-        <v>-48433907514</v>
+        <v>2643467726</v>
       </c>
       <c r="X7">
-        <v>-83246975113</v>
+        <v>1795726428</v>
       </c>
       <c r="Y7" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1528,76 +1549,76 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F8">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="G8">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>4500</v>
+        <v>36400</v>
       </c>
       <c r="J8">
-        <v>5500</v>
+        <v>43300</v>
       </c>
       <c r="K8">
-        <v>30888000</v>
+        <v>9375694</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>7000</v>
+        <v>43300</v>
       </c>
       <c r="N8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="O8" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="P8">
-        <v>85187882584</v>
+        <v>103267682</v>
       </c>
       <c r="Q8">
-        <v>87525689695</v>
+        <v>342201581</v>
       </c>
       <c r="R8">
-        <v>77247394706</v>
+        <v>231425455</v>
       </c>
       <c r="S8">
-        <v>2205797752</v>
+        <v>-7598692896</v>
       </c>
       <c r="T8">
-        <v>4920387020</v>
+        <v>-25822444575</v>
       </c>
       <c r="U8">
-        <v>4336496285</v>
+        <v>-15929213281</v>
       </c>
       <c r="V8">
-        <v>1613954566</v>
+        <v>-6973258680</v>
       </c>
       <c r="W8">
-        <v>3980493669</v>
+        <v>-48433907514</v>
       </c>
       <c r="X8">
-        <v>2646634321</v>
+        <v>-83246975113</v>
       </c>
       <c r="Y8" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1608,73 +1629,73 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F9">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="G9">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>4500</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>5500</v>
       </c>
       <c r="K9">
-        <v>6870000</v>
+        <v>30888000</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>85187882584</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>87525689695</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>77247394706</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>2205797752</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>4920387020</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>4336496285</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>1613954566</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>3980493669</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>2646634321</v>
       </c>
       <c r="Y9" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1682,46 +1703,46 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="G10">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="K10">
-        <v>17529140</v>
+        <v>6870000</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1751,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1759,46 +1780,46 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="G11">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="K11">
-        <v>6930000</v>
+        <v>17529140</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1828,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1836,22 +1857,22 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="G12">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1863,7 +1884,7 @@
         <v>2000</v>
       </c>
       <c r="K12">
-        <v>6220000</v>
+        <v>6930000</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1872,10 +1893,10 @@
         <v>2000</v>
       </c>
       <c r="N12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1905,30 +1926,30 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F13">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G13">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1940,7 +1961,7 @@
         <v>2000</v>
       </c>
       <c r="K13">
-        <v>4810000</v>
+        <v>6220000</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1949,10 +1970,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1982,30 +2003,30 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F14">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="G14">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2017,7 +2038,7 @@
         <v>2000</v>
       </c>
       <c r="K14">
-        <v>5480000</v>
+        <v>4810000</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2026,10 +2047,10 @@
         <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O14" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2059,84 +2080,84 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F15">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="G15">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J15">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
-        <v>12293880</v>
+        <v>5480000</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="O15" t="s">
         <v>112</v>
       </c>
       <c r="P15">
-        <v>1386123525</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1152944128</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>1885010467</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>-4388824706</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>-7990287699</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>-9803411085</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>-4430563401</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>-7988275689</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>-9916946238</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -2144,230 +2165,230 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F16">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="G16">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J16">
-        <v>23500</v>
+        <v>14000</v>
       </c>
       <c r="K16">
-        <v>8751446</v>
+        <v>12293880</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1386123525</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>1152944128</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>1885010467</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>-4388824706</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>-7990287699</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>-9803411085</v>
       </c>
       <c r="V16">
-        <v>0</v>
+        <v>-4430563401</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>-7988275689</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>-9916946238</v>
       </c>
       <c r="Y16" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F17">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="G17">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>10400</v>
+        <v>20000</v>
       </c>
       <c r="J17">
-        <v>12700</v>
+        <v>23500</v>
       </c>
       <c r="K17">
-        <v>8650735</v>
+        <v>8751446</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N17" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="O17" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="P17">
-        <v>2055746777</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>2918221978</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>979078233</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>-3343774083</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>-3525649863</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>-1713494359</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>-4430074915</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>-8304699942</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>-1627684107</v>
+        <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F18">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="G18">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>2000</v>
+        <v>10400</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>12700</v>
       </c>
       <c r="K18">
-        <v>5840000</v>
+        <v>8650735</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="O18" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>2055746777</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>2918221978</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>979078233</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>-3343774083</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>-3525649863</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>-1713494359</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>-4430074915</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>-8304699942</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>-1627684107</v>
       </c>
       <c r="Y18" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -2375,46 +2396,46 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F19">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="G19">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>34000</v>
+        <v>2000</v>
       </c>
       <c r="J19">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="K19">
-        <v>7942750</v>
+        <v>5840000</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N19" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="O19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -2444,84 +2465,161 @@
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20">
+        <v>1400000</v>
+      </c>
+      <c r="G20">
+        <v>1400000</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>34000</v>
+      </c>
+      <c r="J20">
+        <v>40000</v>
+      </c>
+      <c r="K20">
+        <v>7942750</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>40000</v>
+      </c>
+      <c r="N20" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" t="s">
+        <v>121</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21">
         <v>23333334</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>23333334</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <v>3000</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>3800</v>
       </c>
-      <c r="K20">
+      <c r="K21">
         <v>43477664</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>3000</v>
       </c>
-      <c r="N20" t="s">
-        <v>105</v>
-      </c>
-      <c r="O20" t="s">
-        <v>106</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>129</v>
+      <c r="N21" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" t="s">
+        <v>112</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2539,422 +2637,422 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E2">
         <v>12546</v>
       </c>
       <c r="F2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E3">
-        <v>6000</v>
+        <v>14700</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E4">
-        <v>78720</v>
+        <v>6000</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E5">
-        <v>21308</v>
+        <v>78720</v>
       </c>
       <c r="F5" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E6">
-        <v>16500</v>
+        <v>21308</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E7">
-        <v>9500</v>
+        <v>16500</v>
       </c>
       <c r="F7" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E8">
-        <v>17500</v>
+        <v>9500</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E9">
-        <v>42471</v>
+        <v>17500</v>
       </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E10">
-        <v>11600</v>
+        <v>42471</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E11">
-        <v>24000</v>
+        <v>11600</v>
       </c>
       <c r="F11" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E12">
-        <v>14700</v>
+        <v>24000</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E13">
         <v>13518</v>
       </c>
       <c r="F13" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E14">
         <v>22400</v>
       </c>
       <c r="F14" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E15">
         <v>16308</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="E16">
         <v>18900</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E17">
         <v>12000</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C18" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E18">
         <v>8000</v>
       </c>
       <c r="F18" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="E19">
         <v>182400</v>
       </c>
       <c r="F19" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E20">
         <v>8000</v>
       </c>
       <c r="F20" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E21">
         <v>10032</v>
       </c>
       <c r="F21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-08-06
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="235">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -92,6 +92,9 @@
     <t>주요제품</t>
   </si>
   <si>
+    <t>2024-07-15</t>
+  </si>
+  <si>
     <t>2024-07-11</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
     <t>2024-05-23</t>
   </si>
   <si>
+    <t>2024-07-19</t>
+  </si>
+  <si>
     <t>2024-07-17</t>
   </si>
   <si>
@@ -158,15 +164,15 @@
     <t>2024-05-29</t>
   </si>
   <si>
+    <t>2024-08-06</t>
+  </si>
+  <si>
     <t>2024-07-26</t>
   </si>
   <si>
     <t>2024-07-25</t>
   </si>
   <si>
-    <t>2024-07-15</t>
-  </si>
-  <si>
     <t>2024-07-12</t>
   </si>
   <si>
@@ -194,6 +200,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>삼성</t>
+  </si>
+  <si>
     <t>키움</t>
   </si>
   <si>
@@ -209,9 +218,6 @@
     <t>엘에스</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
     <t>미래</t>
   </si>
   <si>
@@ -230,6 +236,9 @@
     <t>신한, 한국</t>
   </si>
   <si>
+    <t>아이빔테크놀로지</t>
+  </si>
+  <si>
     <t>피앤에스미캐닉스</t>
   </si>
   <si>
@@ -290,6 +299,9 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>1011.50:1</t>
+  </si>
+  <si>
     <t>986.08:1</t>
   </si>
   <si>
@@ -350,6 +362,9 @@
     <t>38.7:1</t>
   </si>
   <si>
+    <t>0.49%</t>
+  </si>
+  <si>
     <t>5.60%</t>
   </si>
   <si>
@@ -383,6 +398,9 @@
     <t>0.95%</t>
   </si>
   <si>
+    <t>생체현미경, CRO 서비스</t>
+  </si>
+  <si>
     <t>보행재활로봇 시스템</t>
   </si>
   <si>
@@ -461,6 +479,9 @@
     <t>아이스크림미디어(구.시공미디어)</t>
   </si>
   <si>
+    <t>대신밸런스스팩18호</t>
+  </si>
+  <si>
     <t>이엔셀</t>
   </si>
   <si>
@@ -488,9 +509,6 @@
     <t>뱅크웨어글로벌</t>
   </si>
   <si>
-    <t>아이빔테크놀로지</t>
-  </si>
-  <si>
     <t>NH스팩31호</t>
   </si>
   <si>
@@ -515,6 +533,9 @@
     <t>2024.08.09~08.16</t>
   </si>
   <si>
+    <t>2024.08.05~08.06</t>
+  </si>
+  <si>
     <t>2024.08.02~08.08</t>
   </si>
   <si>
@@ -548,9 +569,6 @@
     <t>2024.07.09~07.15</t>
   </si>
   <si>
-    <t>2024.06.27~06.28</t>
-  </si>
-  <si>
     <t>18,000~21,000</t>
   </si>
   <si>
@@ -596,6 +614,9 @@
     <t>2000</t>
   </si>
   <si>
+    <t>21000</t>
+  </si>
+  <si>
     <t>16000</t>
   </si>
   <si>
@@ -620,6 +641,9 @@
     <t>78720</t>
   </si>
   <si>
+    <t>13000</t>
+  </si>
+  <si>
     <t>21308</t>
   </si>
   <si>
@@ -641,16 +665,16 @@
     <t>24000</t>
   </si>
   <si>
-    <t>13518</t>
+    <t>15771</t>
   </si>
   <si>
     <t>22400</t>
   </si>
   <si>
-    <t>16308</t>
-  </si>
-  <si>
-    <t>18900</t>
+    <t>22340</t>
+  </si>
+  <si>
+    <t>29700</t>
   </si>
   <si>
     <t>12000</t>
@@ -659,7 +683,7 @@
     <t>8000</t>
   </si>
   <si>
-    <t>182400</t>
+    <t>266000</t>
   </si>
   <si>
     <t>신한투자증권</t>
@@ -696,9 +720,6 @@
   </si>
   <si>
     <t>미래에셋증권,삼성증권</t>
-  </si>
-  <si>
-    <t>엘에스증권</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1077,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1144,76 +1165,76 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2">
-        <v>1350000</v>
+        <v>2234000</v>
       </c>
       <c r="G2">
-        <v>1350000</v>
+        <v>2234000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>14000</v>
+        <v>7300</v>
       </c>
       <c r="J2">
-        <v>17000</v>
+        <v>8500</v>
       </c>
       <c r="K2">
-        <v>6471740</v>
+        <v>14965620</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>22000</v>
+        <v>10000</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P2">
-        <v>5214628820</v>
+        <v>1337894447</v>
       </c>
       <c r="Q2">
-        <v>6009352447</v>
+        <v>4495088983</v>
       </c>
       <c r="R2">
-        <v>965797975</v>
+        <v>99398351</v>
       </c>
       <c r="S2">
-        <v>2015081728</v>
+        <v>-3330678562</v>
       </c>
       <c r="T2">
-        <v>1319755337</v>
+        <v>-2905069801</v>
       </c>
       <c r="U2">
-        <v>-44547594</v>
+        <v>-1314068310</v>
       </c>
       <c r="V2">
-        <v>1503069100</v>
+        <v>-9735376868</v>
       </c>
       <c r="W2">
-        <v>1410469786</v>
+        <v>-5043515600</v>
       </c>
       <c r="X2">
-        <v>24178632</v>
+        <v>-1257080998</v>
       </c>
       <c r="Y2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -1221,99 +1242,99 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F3">
-        <v>6000000</v>
+        <v>1350000</v>
       </c>
       <c r="G3">
-        <v>6000000</v>
+        <v>1350000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="K3">
-        <v>6345000</v>
+        <v>6471740</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="O3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>5214628820</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>6009352447</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>965797975</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>2015081728</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1319755337</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>-44547594</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1503069100</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1410469786</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>24178632</v>
       </c>
       <c r="Y3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G4">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1325,7 +1346,7 @@
         <v>2000</v>
       </c>
       <c r="K4">
-        <v>4420000</v>
+        <v>6345000</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1334,10 +1355,10 @@
         <v>2000</v>
       </c>
       <c r="N4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="O4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1367,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1375,46 +1396,46 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F5">
-        <v>1618000</v>
+        <v>4000000</v>
       </c>
       <c r="G5">
-        <v>1618000</v>
+        <v>4000000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>6200</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="K5">
-        <v>10830212</v>
+        <v>4420000</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="O5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1444,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1452,46 +1473,46 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="G6">
-        <v>4000000</v>
+        <v>1618000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>6200</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="K6">
-        <v>5020000</v>
+        <v>10830212</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>10000</v>
       </c>
       <c r="N6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="O6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1521,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1529,76 +1550,76 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F7">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="G7">
-        <v>1810000</v>
+        <v>4000000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="K7">
-        <v>7836009</v>
+        <v>5020000</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="P7">
-        <v>12596039842</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>14910346438</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>16039074617</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>1732604466</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>2893667787</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>1613779678</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>1558081149</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>2643467726</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>1795726428</v>
+        <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1606,76 +1627,76 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F8">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="G8">
-        <v>1330000</v>
+        <v>1810000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>36400</v>
+        <v>9000</v>
       </c>
       <c r="J8">
-        <v>43300</v>
+        <v>12000</v>
       </c>
       <c r="K8">
-        <v>9375694</v>
+        <v>7836009</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="P8">
-        <v>103267682</v>
+        <v>12596039842</v>
       </c>
       <c r="Q8">
-        <v>342201581</v>
+        <v>14910346438</v>
       </c>
       <c r="R8">
-        <v>231425455</v>
+        <v>16039074617</v>
       </c>
       <c r="S8">
-        <v>-7598692896</v>
+        <v>1732604466</v>
       </c>
       <c r="T8">
-        <v>-25822444575</v>
+        <v>2893667787</v>
       </c>
       <c r="U8">
-        <v>-15929213281</v>
+        <v>1613779678</v>
       </c>
       <c r="V8">
-        <v>-6973258680</v>
+        <v>1558081149</v>
       </c>
       <c r="W8">
-        <v>-48433907514</v>
+        <v>2643467726</v>
       </c>
       <c r="X8">
-        <v>-83246975113</v>
+        <v>1795726428</v>
       </c>
       <c r="Y8" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1683,76 +1704,76 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="G9">
-        <v>3400000</v>
+        <v>1330000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>4500</v>
+        <v>36400</v>
       </c>
       <c r="J9">
-        <v>5500</v>
+        <v>43300</v>
       </c>
       <c r="K9">
-        <v>30888000</v>
+        <v>9375694</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>7000</v>
+        <v>43300</v>
       </c>
       <c r="N9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O9" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P9">
-        <v>85187882584</v>
+        <v>103267682</v>
       </c>
       <c r="Q9">
-        <v>87525689695</v>
+        <v>342201581</v>
       </c>
       <c r="R9">
-        <v>77247394706</v>
+        <v>231425455</v>
       </c>
       <c r="S9">
-        <v>2205797752</v>
+        <v>-7598692896</v>
       </c>
       <c r="T9">
-        <v>4920387020</v>
+        <v>-25822444575</v>
       </c>
       <c r="U9">
-        <v>4336496285</v>
+        <v>-15929213281</v>
       </c>
       <c r="V9">
-        <v>1613954566</v>
+        <v>-6973258680</v>
       </c>
       <c r="W9">
-        <v>3980493669</v>
+        <v>-48433907514</v>
       </c>
       <c r="X9">
-        <v>2646634321</v>
+        <v>-83246975113</v>
       </c>
       <c r="Y9" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1763,73 +1784,73 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F10">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="G10">
-        <v>6250000</v>
+        <v>3400000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>4500</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>5500</v>
       </c>
       <c r="K10">
-        <v>6870000</v>
+        <v>30888000</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="O10" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>85187882584</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>87525689695</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>77247394706</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>2205797752</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>4920387020</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>4336496285</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>1613954566</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>3980493669</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>2646634321</v>
       </c>
       <c r="Y10" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1837,43 +1858,43 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F11">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="G11">
-        <v>2000000</v>
+        <v>6250000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
-        <v>17529140</v>
+        <v>6870000</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O11" t="s">
         <v>117</v>
@@ -1906,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1914,46 +1935,46 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="G12">
-        <v>6450000</v>
+        <v>2000000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="K12">
-        <v>6930000</v>
+        <v>17529140</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="O12" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1983,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1991,22 +2012,22 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F13">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="G13">
-        <v>6000000</v>
+        <v>6450000</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2018,7 +2039,7 @@
         <v>2000</v>
       </c>
       <c r="K13">
-        <v>6220000</v>
+        <v>6930000</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2027,10 +2048,10 @@
         <v>2000</v>
       </c>
       <c r="N13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="O13" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -2060,30 +2081,30 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F14">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="G14">
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2095,7 +2116,7 @@
         <v>2000</v>
       </c>
       <c r="K14">
-        <v>4810000</v>
+        <v>6220000</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2104,10 +2125,10 @@
         <v>2000</v>
       </c>
       <c r="N14" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2137,30 +2158,30 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F15">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="G15">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2172,7 +2193,7 @@
         <v>2000</v>
       </c>
       <c r="K15">
-        <v>5480000</v>
+        <v>4810000</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2181,10 +2202,10 @@
         <v>2000</v>
       </c>
       <c r="N15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="O15" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -2214,84 +2235,84 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F16">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="G16">
-        <v>1300000</v>
+        <v>4750000</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
-        <v>12293880</v>
+        <v>5480000</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="O16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P16">
-        <v>1386123525</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>1152944128</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>1885010467</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>-4388824706</v>
+        <v>0</v>
       </c>
       <c r="T16">
-        <v>-7990287699</v>
+        <v>0</v>
       </c>
       <c r="U16">
-        <v>-9803411085</v>
+        <v>0</v>
       </c>
       <c r="V16">
-        <v>-4430563401</v>
+        <v>0</v>
       </c>
       <c r="W16">
-        <v>-7988275689</v>
+        <v>0</v>
       </c>
       <c r="X16">
-        <v>-9916946238</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -2299,230 +2320,230 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F17">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="G17">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J17">
-        <v>23500</v>
+        <v>14000</v>
       </c>
       <c r="K17">
-        <v>8751446</v>
+        <v>12293880</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N17" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="O17" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1386123525</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>1152944128</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1885010467</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>-4388824706</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>-7990287699</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>-9803411085</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <v>-4430563401</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>-7988275689</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>-9916946238</v>
       </c>
       <c r="Y17" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F18">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="G18">
-        <v>1298000</v>
+        <v>1600000</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>10400</v>
+        <v>20000</v>
       </c>
       <c r="J18">
-        <v>12700</v>
+        <v>23500</v>
       </c>
       <c r="K18">
-        <v>8650735</v>
+        <v>8751446</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N18" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="O18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="P18">
-        <v>2055746777</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>2918221978</v>
+        <v>0</v>
       </c>
       <c r="R18">
-        <v>979078233</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>-3343774083</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>-3525649863</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>-1713494359</v>
+        <v>0</v>
       </c>
       <c r="V18">
-        <v>-4430074915</v>
+        <v>0</v>
       </c>
       <c r="W18">
-        <v>-8304699942</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>-1627684107</v>
+        <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F19">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="G19">
-        <v>5000000</v>
+        <v>1298000</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>2000</v>
+        <v>10400</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>12700</v>
       </c>
       <c r="K19">
-        <v>5840000</v>
+        <v>8650735</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O19" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>2055746777</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>2918221978</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>979078233</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>-3343774083</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>-3525649863</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>-1713494359</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>-4430074915</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>-8304699942</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>-1627684107</v>
       </c>
       <c r="Y19" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -2530,46 +2551,46 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F20">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="G20">
-        <v>1400000</v>
+        <v>5000000</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>34000</v>
+        <v>2000</v>
       </c>
       <c r="J20">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="K20">
-        <v>7942750</v>
+        <v>5840000</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N20" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="O20" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="P20">
         <v>0</v>
@@ -2599,84 +2620,161 @@
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21">
+        <v>1400000</v>
+      </c>
+      <c r="G21">
+        <v>1400000</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>34000</v>
+      </c>
+      <c r="J21">
+        <v>40000</v>
+      </c>
+      <c r="K21">
+        <v>7942750</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>40000</v>
+      </c>
+      <c r="N21" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" t="s">
+        <v>126</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22">
         <v>23333334</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>23333334</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
         <v>3000</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>3800</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>43477664</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <v>3000</v>
       </c>
-      <c r="N21" t="s">
-        <v>110</v>
-      </c>
-      <c r="O21" t="s">
-        <v>112</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>136</v>
+      <c r="N22" t="s">
+        <v>114</v>
+      </c>
+      <c r="O22" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2694,239 +2792,239 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F4" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F5" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F8" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F9" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F10" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C11" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F12" t="s">
         <v>224</v>
@@ -2934,182 +3032,182 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>198</v>
       </c>
       <c r="E13" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="F13" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C14" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="F14" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="E17" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F17" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E18" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="F18" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F19" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="E21" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="F21" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-08-09
</commit_message>
<xml_diff>
--- a/datasets/ib-strategy-data.xlsx
+++ b/datasets/ib-strategy-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="235">
   <si>
     <t>수요예측(시작일)</t>
   </si>
@@ -611,15 +611,18 @@
     <t>24,000~30,000</t>
   </si>
   <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>13000</t>
+  </si>
+  <si>
     <t>15500</t>
   </si>
   <si>
     <t>16500</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>29000</t>
   </si>
   <si>
@@ -650,16 +653,10 @@
     <t>78720</t>
   </si>
   <si>
-    <t>13000</t>
-  </si>
-  <si>
     <t>21308</t>
   </si>
   <si>
-    <t>9500</t>
-  </si>
-  <si>
-    <t>22351</t>
+    <t>21700</t>
   </si>
   <si>
     <t>50781</t>
@@ -2827,10 +2824,10 @@
         <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2850,7 +2847,7 @@
         <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2867,10 +2864,10 @@
         <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2887,10 +2884,10 @@
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2907,10 +2904,10 @@
         <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2924,13 +2921,13 @@
         <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>198</v>
       </c>
       <c r="E7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2950,7 +2947,7 @@
         <v>212</v>
       </c>
       <c r="F8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2967,10 +2964,10 @@
         <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2984,13 +2981,13 @@
         <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="E10" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3004,13 +3001,13 @@
         <v>191</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3024,13 +3021,13 @@
         <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3044,13 +3041,13 @@
         <v>185</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3064,13 +3061,13 @@
         <v>193</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3084,13 +3081,13 @@
         <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3104,13 +3101,13 @@
         <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3124,13 +3121,13 @@
         <v>195</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3144,13 +3141,13 @@
         <v>196</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3164,13 +3161,13 @@
         <v>185</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3184,13 +3181,13 @@
         <v>185</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3204,13 +3201,13 @@
         <v>197</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>